<commit_message>
Started designing UML diagrams
</commit_message>
<xml_diff>
--- a/User Stories/NataliaUserStories.xlsx
+++ b/User Stories/NataliaUserStories.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Palej\Desktop\Software Design with AI for Cloud\Year_3\agile-labs3\Newsagent-Project\User Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4705F05-D3A2-49F7-8710-6BA295CDD8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F60AF4E-D2D4-4579-98CE-1D3ED81398D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminUserStories" sheetId="1" r:id="rId1"/>
     <sheet name="NewsagentUserStories" sheetId="2" r:id="rId2"/>
+    <sheet name="UMLs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="176">
   <si>
     <t>As an admin</t>
   </si>
@@ -448,13 +449,130 @@
   </si>
   <si>
     <t>Role will grant user extra premissions, eg. Newsagent can generate invoices and Driver can only print them</t>
+  </si>
+  <si>
+    <t>Newsagent</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>+deactivateCustomer() : void</t>
+  </si>
+  <si>
+    <t>+generateInvoice() : void</t>
+  </si>
+  <si>
+    <t>+generateDeliveryDoc() : void</t>
+  </si>
+  <si>
+    <t>+givePermission() : void</t>
+  </si>
+  <si>
+    <t>- username : String</t>
+  </si>
+  <si>
+    <t>- role : String</t>
+  </si>
+  <si>
+    <t>- password : String</t>
+  </si>
+  <si>
+    <t>- customerDatabase: Database</t>
+  </si>
+  <si>
+    <t>- userDatabase : Database</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>+Newsagent : (username: String, password: String, role: String, customerDatabase: Database)</t>
+  </si>
+  <si>
+    <t>+Admin : (uesrname: String, password: String, role: String, userDatabase: Database)</t>
+  </si>
+  <si>
+    <t>+getCustID() : void</t>
+  </si>
+  <si>
+    <t>+getFirstName() : void</t>
+  </si>
+  <si>
+    <t>+getLastName() : void</t>
+  </si>
+  <si>
+    <t>+getCustAddress() : void</t>
+  </si>
+  <si>
+    <t>+getPhoneNo() : void</t>
+  </si>
+  <si>
+    <t>+setCustID() : int</t>
+  </si>
+  <si>
+    <t>+setFirstName() : String</t>
+  </si>
+  <si>
+    <t>+setLastName() : String</t>
+  </si>
+  <si>
+    <t>+setCustAddress() : String</t>
+  </si>
+  <si>
+    <t>- custID : int</t>
+  </si>
+  <si>
+    <t>- firstName : String</t>
+  </si>
+  <si>
+    <t>- lastName : String</t>
+  </si>
+  <si>
+    <t>- custAddress : String</t>
+  </si>
+  <si>
+    <t>- phoneNo : String</t>
+  </si>
+  <si>
+    <t>+Customer(custID: int, firstName: String, lastName: String, custAddress: String, phoneNo: String)</t>
+  </si>
+  <si>
+    <t>+setPhoneNo() : String</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>+ createUserAccount(username: String, password: String, role: String): void</t>
+  </si>
+  <si>
+    <t>+ updateUserAccount(username: String, password: String, role: String): void</t>
+  </si>
+  <si>
+    <t>+ deleteUserAccount(username: String): void</t>
+  </si>
+  <si>
+    <t>+ readUserAccount(username: String): void</t>
+  </si>
+  <si>
+    <t>+ printUserAccount(username: String): void</t>
+  </si>
+  <si>
+    <t>Admin extends User</t>
+  </si>
+  <si>
+    <t>Newsagent extends User</t>
+  </si>
+  <si>
+    <t>User and Customer standalone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -481,6 +599,12 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -638,7 +762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -753,12 +877,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -771,67 +949,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1157,7 +1285,7 @@
   <dimension ref="A1:F88"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1192,13 +1320,13 @@
       <c r="A2" s="38">
         <v>1</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="41" t="s">
         <v>40</v>
       </c>
       <c r="E2" s="15" t="s">
@@ -1210,9 +1338,9 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="39"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
       <c r="E3" s="15" t="s">
         <v>54</v>
       </c>
@@ -1222,9 +1350,9 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="39"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
       <c r="E4" s="15" t="s">
         <v>56</v>
       </c>
@@ -1232,9 +1360,9 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="39"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
       <c r="E5" s="15" t="s">
         <v>57</v>
       </c>
@@ -1242,9 +1370,9 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="39"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
       <c r="E6" s="15" t="s">
         <v>46</v>
       </c>
@@ -1252,9 +1380,9 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="39"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
       <c r="E7" s="15" t="s">
         <v>38</v>
       </c>
@@ -1272,13 +1400,13 @@
       <c r="A9" s="38">
         <v>2</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="41" t="s">
         <v>91</v>
       </c>
       <c r="E9" s="14" t="s">
@@ -1290,9 +1418,9 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="39"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
       <c r="E10" s="15" t="s">
         <v>97</v>
       </c>
@@ -1300,9 +1428,9 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="39"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
       <c r="E11" s="15" t="s">
         <v>100</v>
       </c>
@@ -1310,9 +1438,9 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="39"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
       <c r="E12" s="15" t="s">
         <v>98</v>
       </c>
@@ -1320,9 +1448,9 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="39"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
       <c r="E13" s="15" t="s">
         <v>99</v>
       </c>
@@ -1330,19 +1458,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="39"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
       <c r="E14" s="15" t="s">
         <v>93</v>
       </c>
       <c r="F14" s="24"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="52"/>
-      <c r="B15" s="53"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
       <c r="E15" s="15" t="s">
         <v>14</v>
       </c>
@@ -1360,13 +1488,13 @@
       <c r="A17" s="38">
         <v>3</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="41" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="15" t="s">
@@ -1378,19 +1506,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="39"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
       <c r="E18" s="15" t="s">
         <v>101</v>
       </c>
       <c r="F18" s="24"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="52"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
       <c r="E19" s="11" t="s">
         <v>58</v>
       </c>
@@ -1408,13 +1536,13 @@
       <c r="A21" s="38">
         <v>4</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="C21" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="40" t="s">
+      <c r="D21" s="41" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="15" t="s">
@@ -1426,9 +1554,9 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="39"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
       <c r="E22" s="15" t="s">
         <v>106</v>
       </c>
@@ -1436,9 +1564,9 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="39"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
       <c r="E23" s="15" t="s">
         <v>107</v>
       </c>
@@ -1446,9 +1574,9 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="39"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
       <c r="E24" s="15" t="s">
         <v>108</v>
       </c>
@@ -1456,9 +1584,9 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="39"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
       <c r="E25" s="15" t="s">
         <v>102</v>
       </c>
@@ -1466,19 +1594,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="39"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
       <c r="E26" s="15" t="s">
         <v>103</v>
       </c>
       <c r="F26" s="24"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" s="52"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
       <c r="E27" s="15" t="s">
         <v>11</v>
       </c>
@@ -1496,13 +1624,13 @@
       <c r="A29" s="38">
         <v>5</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="40" t="s">
+      <c r="C29" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="40" t="s">
+      <c r="D29" s="41" t="s">
         <v>92</v>
       </c>
       <c r="E29" s="15" t="s">
@@ -1512,19 +1640,19 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="39"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
       <c r="E30" s="15" t="s">
         <v>104</v>
       </c>
       <c r="F30" s="24"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31" s="52"/>
-      <c r="B31" s="53"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
       <c r="E31" s="15" t="s">
         <v>105</v>
       </c>
@@ -1542,13 +1670,13 @@
       <c r="A33" s="38">
         <v>6</v>
       </c>
-      <c r="B33" s="40" t="s">
+      <c r="B33" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="40" t="s">
+      <c r="C33" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="40" t="s">
+      <c r="D33" s="41" t="s">
         <v>16</v>
       </c>
       <c r="E33" s="15" t="s">
@@ -1559,10 +1687,10 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="52"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
       <c r="E34" s="15" t="s">
         <v>110</v>
       </c>
@@ -1577,80 +1705,80 @@
       <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="63">
+      <c r="A36" s="44">
         <v>7</v>
       </c>
-      <c r="B36" s="62" t="s">
+      <c r="B36" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="62" t="s">
+      <c r="C36" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="D36" s="62" t="s">
+      <c r="D36" s="45" t="s">
         <v>78</v>
       </c>
       <c r="E36" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="F36" s="40" t="s">
+      <c r="F36" s="41" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37" s="63"/>
-      <c r="B37" s="62"/>
-      <c r="C37" s="62"/>
-      <c r="D37" s="62"/>
+      <c r="A37" s="44"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
       <c r="E37" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="F37" s="41"/>
+      <c r="F37" s="42"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38" s="63"/>
-      <c r="B38" s="62"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="62"/>
+      <c r="A38" s="44"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
       <c r="E38" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="F38" s="53"/>
+      <c r="F38" s="43"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39" s="63"/>
-      <c r="B39" s="62"/>
-      <c r="C39" s="62"/>
-      <c r="D39" s="62"/>
+      <c r="A39" s="44"/>
+      <c r="B39" s="45"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="45"/>
       <c r="E39" s="24" t="s">
         <v>81</v>
       </c>
       <c r="F39" s="24"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" s="63"/>
-      <c r="B40" s="62"/>
-      <c r="C40" s="62"/>
-      <c r="D40" s="62"/>
+      <c r="A40" s="44"/>
+      <c r="B40" s="45"/>
+      <c r="C40" s="45"/>
+      <c r="D40" s="45"/>
       <c r="E40" s="24" t="s">
         <v>82</v>
       </c>
       <c r="F40" s="24"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" s="63"/>
-      <c r="B41" s="62"/>
-      <c r="C41" s="62"/>
-      <c r="D41" s="62"/>
+      <c r="A41" s="44"/>
+      <c r="B41" s="45"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="45"/>
       <c r="E41" s="24" t="s">
         <v>83</v>
       </c>
       <c r="F41" s="24"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42" s="63"/>
-      <c r="B42" s="62"/>
-      <c r="C42" s="62"/>
-      <c r="D42" s="62"/>
+      <c r="A42" s="44"/>
+      <c r="B42" s="45"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="45"/>
       <c r="E42" s="24" t="s">
         <v>85</v>
       </c>
@@ -1739,16 +1867,16 @@
       <c r="F55" s="7"/>
     </row>
     <row r="56" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="57">
+      <c r="A56" s="49">
         <v>12</v>
       </c>
-      <c r="B56" s="54" t="s">
+      <c r="B56" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C56" s="54" t="s">
+      <c r="C56" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="D56" s="54" t="s">
+      <c r="D56" s="46" t="s">
         <v>44</v>
       </c>
       <c r="E56" s="17" t="s">
@@ -1757,30 +1885,30 @@
       <c r="F56" s="36"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A57" s="58"/>
-      <c r="B57" s="55"/>
-      <c r="C57" s="55"/>
-      <c r="D57" s="55"/>
+      <c r="A57" s="50"/>
+      <c r="B57" s="47"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
       <c r="E57" s="17" t="s">
         <v>42</v>
       </c>
       <c r="F57" s="36"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A58" s="58"/>
-      <c r="B58" s="55"/>
-      <c r="C58" s="55"/>
-      <c r="D58" s="55"/>
+      <c r="A58" s="50"/>
+      <c r="B58" s="47"/>
+      <c r="C58" s="47"/>
+      <c r="D58" s="47"/>
       <c r="E58" s="17" t="s">
         <v>37</v>
       </c>
       <c r="F58" s="36"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A59" s="59"/>
-      <c r="B59" s="56"/>
-      <c r="C59" s="56"/>
-      <c r="D59" s="56"/>
+      <c r="A59" s="51"/>
+      <c r="B59" s="48"/>
+      <c r="C59" s="48"/>
+      <c r="D59" s="48"/>
       <c r="E59" s="17" t="s">
         <v>38</v>
       </c>
@@ -1803,40 +1931,40 @@
       <c r="F70" s="7"/>
     </row>
     <row r="71" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A71" s="46">
+      <c r="A71" s="54">
         <v>10</v>
       </c>
-      <c r="B71" s="49" t="s">
+      <c r="B71" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="C71" s="49" t="s">
+      <c r="C71" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="D71" s="49" t="s">
+      <c r="D71" s="57" t="s">
         <v>33</v>
       </c>
       <c r="E71" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F71" s="60" t="s">
+      <c r="F71" s="52" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A72" s="47"/>
-      <c r="B72" s="50"/>
-      <c r="C72" s="50"/>
-      <c r="D72" s="50"/>
+      <c r="A72" s="55"/>
+      <c r="B72" s="58"/>
+      <c r="C72" s="58"/>
+      <c r="D72" s="58"/>
       <c r="E72" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="F72" s="61"/>
+      <c r="F72" s="53"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A73" s="48"/>
-      <c r="B73" s="51"/>
-      <c r="C73" s="51"/>
-      <c r="D73" s="51"/>
+      <c r="A73" s="56"/>
+      <c r="B73" s="59"/>
+      <c r="C73" s="59"/>
+      <c r="D73" s="59"/>
       <c r="E73" s="6"/>
       <c r="F73" s="37"/>
     </row>
@@ -1849,16 +1977,16 @@
       <c r="F74" s="7"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A75" s="46">
+      <c r="A75" s="54">
         <v>11</v>
       </c>
-      <c r="B75" s="49" t="s">
+      <c r="B75" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="C75" s="49" t="s">
+      <c r="C75" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="D75" s="49" t="s">
+      <c r="D75" s="57" t="s">
         <v>26</v>
       </c>
       <c r="E75" s="18" t="s">
@@ -1867,20 +1995,20 @@
       <c r="F75" s="37"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A76" s="47"/>
-      <c r="B76" s="50"/>
-      <c r="C76" s="50"/>
-      <c r="D76" s="50"/>
+      <c r="A76" s="55"/>
+      <c r="B76" s="58"/>
+      <c r="C76" s="58"/>
+      <c r="D76" s="58"/>
       <c r="E76" s="18" t="s">
         <v>28</v>
       </c>
       <c r="F76" s="37"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A77" s="48"/>
-      <c r="B77" s="51"/>
-      <c r="C77" s="51"/>
-      <c r="D77" s="51"/>
+      <c r="A77" s="56"/>
+      <c r="B77" s="59"/>
+      <c r="C77" s="59"/>
+      <c r="D77" s="59"/>
       <c r="E77" s="18" t="s">
         <v>29</v>
       </c>
@@ -1894,16 +2022,16 @@
       <c r="E80" s="9"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A81" s="44">
+      <c r="A81" s="62">
         <v>6</v>
       </c>
-      <c r="B81" s="42" t="s">
+      <c r="B81" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C81" s="42" t="s">
+      <c r="C81" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="D81" s="42" t="s">
+      <c r="D81" s="60" t="s">
         <v>19</v>
       </c>
       <c r="E81" s="12" t="s">
@@ -1911,10 +2039,10 @@
       </c>
     </row>
     <row r="82" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A82" s="45"/>
-      <c r="B82" s="43"/>
-      <c r="C82" s="43"/>
-      <c r="D82" s="43"/>
+      <c r="A82" s="63"/>
+      <c r="B82" s="61"/>
+      <c r="C82" s="61"/>
+      <c r="D82" s="61"/>
       <c r="E82" s="12" t="s">
         <v>31</v>
       </c>
@@ -1979,36 +2107,6 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A36:A42"/>
-    <mergeCell ref="B36:B42"/>
-    <mergeCell ref="C36:C42"/>
-    <mergeCell ref="D36:D42"/>
-    <mergeCell ref="F36:F38"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="D56:D59"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="C71:C73"/>
-    <mergeCell ref="D71:D73"/>
-    <mergeCell ref="B21:B27"/>
-    <mergeCell ref="A21:A27"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C21:C27"/>
-    <mergeCell ref="D21:D27"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="D33:D34"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="C2:C7"/>
@@ -2025,6 +2123,36 @@
     <mergeCell ref="B9:B15"/>
     <mergeCell ref="C9:C15"/>
     <mergeCell ref="D9:D15"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C21:C27"/>
+    <mergeCell ref="D21:D27"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="B21:B27"/>
+    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="C71:C73"/>
+    <mergeCell ref="D71:D73"/>
+    <mergeCell ref="C36:C42"/>
+    <mergeCell ref="D36:D42"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A36:A42"/>
+    <mergeCell ref="B36:B42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2035,8 +2163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526350BB-95BB-4BF1-93A5-0B30D123D1AA}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection sqref="A1:F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2071,13 +2199,13 @@
       <c r="A2" s="38">
         <v>1</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="41" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="14" t="s">
@@ -2089,9 +2217,9 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="39"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
       <c r="E3" s="15" t="s">
         <v>67</v>
       </c>
@@ -2101,9 +2229,9 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="39"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
       <c r="E4" s="15" t="s">
         <v>71</v>
       </c>
@@ -2111,9 +2239,9 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="39"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
       <c r="E5" s="15" t="s">
         <v>72</v>
       </c>
@@ -2121,9 +2249,9 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="39"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
       <c r="E6" s="15" t="s">
         <v>73</v>
       </c>
@@ -2131,9 +2259,9 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="39"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
       <c r="E7" s="15" t="s">
         <v>75</v>
       </c>
@@ -2141,9 +2269,9 @@
     </row>
     <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="39"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
       <c r="E8" s="15" t="s">
         <v>68</v>
       </c>
@@ -2151,19 +2279,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="39"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
       <c r="E9" s="15" t="s">
         <v>69</v>
       </c>
       <c r="F9" s="24"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="52"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
       <c r="E10" s="15" t="s">
         <v>14</v>
       </c>
@@ -2181,13 +2309,13 @@
       <c r="A12" s="38">
         <v>2</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="41" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="15" t="s">
@@ -2199,9 +2327,9 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="39"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
       <c r="E13" s="15" t="s">
         <v>112</v>
       </c>
@@ -2209,9 +2337,9 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="39"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
       <c r="E14" s="15" t="s">
         <v>113</v>
       </c>
@@ -2219,19 +2347,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="39"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
       <c r="E15" s="15" t="s">
         <v>114</v>
       </c>
       <c r="F15" s="24"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="52"/>
-      <c r="B16" s="53"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
       <c r="E16" s="11" t="s">
         <v>58</v>
       </c>
@@ -2249,13 +2377,13 @@
       <c r="A18" s="38">
         <v>3</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="41" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="15" t="s">
@@ -2267,9 +2395,9 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="39"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
       <c r="E19" s="15" t="s">
         <v>112</v>
       </c>
@@ -2277,9 +2405,9 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="39"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
       <c r="E20" s="15" t="s">
         <v>116</v>
       </c>
@@ -2287,9 +2415,9 @@
     </row>
     <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="39"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
       <c r="E21" s="15" t="s">
         <v>117</v>
       </c>
@@ -2297,9 +2425,9 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="39"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
       <c r="E22" s="15" t="s">
         <v>119</v>
       </c>
@@ -2307,9 +2435,9 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="39"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
       <c r="E23" s="15" t="s">
         <v>118</v>
       </c>
@@ -2327,13 +2455,13 @@
       <c r="A25" s="38">
         <v>4</v>
       </c>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="41" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="15" t="s">
@@ -2343,9 +2471,9 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="39"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
       <c r="E26" s="15" t="s">
         <v>121</v>
       </c>
@@ -2363,13 +2491,13 @@
       <c r="A28" s="38">
         <v>5</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="40" t="s">
+      <c r="D28" s="41" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="15" t="s">
@@ -2381,9 +2509,9 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="39"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
       <c r="E29" s="15" t="s">
         <v>17</v>
       </c>
@@ -2401,13 +2529,13 @@
       <c r="A31" s="38">
         <v>6</v>
       </c>
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="40" t="s">
+      <c r="C31" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D31" s="40" t="s">
+      <c r="D31" s="41" t="s">
         <v>50</v>
       </c>
       <c r="E31" s="14" t="s">
@@ -2419,9 +2547,9 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="39"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
       <c r="E32" s="15" t="s">
         <v>126</v>
       </c>
@@ -2429,19 +2557,19 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="39"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
       <c r="E33" s="15" t="s">
         <v>124</v>
       </c>
       <c r="F33" s="24"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="52"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
       <c r="E34" s="15" t="s">
         <v>22</v>
       </c>
@@ -2459,13 +2587,13 @@
       <c r="A36" s="38">
         <v>7</v>
       </c>
-      <c r="B36" s="40" t="s">
+      <c r="B36" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="40" t="s">
+      <c r="C36" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="40" t="s">
+      <c r="D36" s="41" t="s">
         <v>24</v>
       </c>
       <c r="E36" s="15" t="s">
@@ -2475,19 +2603,19 @@
     </row>
     <row r="37" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A37" s="39"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
       <c r="E37" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F37" s="24"/>
     </row>
     <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A38" s="52"/>
-      <c r="B38" s="53"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="43"/>
       <c r="E38" s="15" t="s">
         <v>36</v>
       </c>
@@ -2505,13 +2633,13 @@
       <c r="A40" s="38">
         <v>8</v>
       </c>
-      <c r="B40" s="40" t="s">
+      <c r="B40" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="40" t="s">
+      <c r="C40" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="D40" s="40" t="s">
+      <c r="D40" s="41" t="s">
         <v>128</v>
       </c>
       <c r="E40" s="24" t="s">
@@ -2521,58 +2649,54 @@
     </row>
     <row r="41" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A41" s="39"/>
-      <c r="B41" s="41"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="41"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
       <c r="E41" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="F41" s="64"/>
     </row>
     <row r="42" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A42" s="39"/>
-      <c r="B42" s="41"/>
-      <c r="C42" s="41"/>
-      <c r="D42" s="41"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
       <c r="E42" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="F42" s="64"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="39"/>
-      <c r="B43" s="41"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
+      <c r="B43" s="42"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
       <c r="E43" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="F43" s="64"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="39"/>
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="41"/>
-      <c r="E44" s="64" t="s">
+      <c r="B44" s="42"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="F44" s="64"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="39"/>
-      <c r="B45" s="41"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="41"/>
-      <c r="E45" s="65" t="s">
+      <c r="B45" s="42"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="11" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="39"/>
-      <c r="B46" s="41"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="41"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
       <c r="E46" s="24" t="s">
         <v>133</v>
       </c>
@@ -2580,10 +2704,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="39"/>
-      <c r="B47" s="41"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="41"/>
-      <c r="E47" s="66" t="s">
+      <c r="B47" s="42"/>
+      <c r="C47" s="42"/>
+      <c r="D47" s="42"/>
+      <c r="E47" s="14" t="s">
         <v>85</v>
       </c>
       <c r="F47" s="24"/>
@@ -2598,6 +2722,30 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="C2:C10"/>
+    <mergeCell ref="D2:D10"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="A31:A34"/>
     <mergeCell ref="A40:A47"/>
     <mergeCell ref="B40:B47"/>
     <mergeCell ref="C40:C47"/>
@@ -2606,31 +2754,220 @@
     <mergeCell ref="C36:C38"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="C2:C10"/>
-    <mergeCell ref="D2:D10"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="D12:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD0B509-A153-4B31-95B8-BC32DC1B6A3B}">
+  <dimension ref="B2:G31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.06640625" customWidth="1"/>
+    <col min="2" max="2" width="37.46484375" style="64" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.06640625" style="64" customWidth="1"/>
+    <col min="4" max="4" width="41.73046875" style="66" customWidth="1"/>
+    <col min="5" max="5" width="9.06640625" style="64"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B2" s="65" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="65"/>
+      <c r="D2" s="67" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B3" s="64" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" s="66" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B4" s="64" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B5" s="64" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="66" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B6" s="64" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="66" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B8" s="66" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="66" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B9" s="64" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" s="66" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B10" s="64" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B11" s="64" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B14" s="65" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" s="66" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B15" s="64" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" s="66" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B16" s="64" t="s">
+        <v>161</v>
+      </c>
+      <c r="D16" s="66" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B17" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" s="66" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B18" s="64" t="s">
+        <v>163</v>
+      </c>
+      <c r="D18" s="66" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B19" s="64" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B21" s="66" t="s">
+        <v>165</v>
+      </c>
+      <c r="D21" s="66" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="64" t="s">
+        <v>151</v>
+      </c>
+      <c r="D22" s="66" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B23" s="64" t="s">
+        <v>152</v>
+      </c>
+      <c r="D23" s="68" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B24" s="64" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" s="66" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B25" s="64" t="s">
+        <v>154</v>
+      </c>
+      <c r="D25" s="66" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B26" s="64" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B27" s="64" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B28" s="64" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B29" s="64" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B30" s="64" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B31" s="64" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Improved UML and created UML table
</commit_message>
<xml_diff>
--- a/User Stories/NataliaUserStories.xlsx
+++ b/User Stories/NataliaUserStories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Palej\Desktop\Software Design with AI for Cloud\Year_3\agile-labs3\Newsagent-Project\User Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75044E9D-91BE-48A2-8F11-04D16429B5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A7AEE6-62C3-4B6B-95A6-DAF763ED861B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminUserStories" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="180">
   <si>
     <t>As an admin</t>
   </si>
@@ -566,6 +566,18 @@
   </si>
   <si>
     <t>User and Customer standalone</t>
+  </si>
+  <si>
+    <t>+createNewCustomer(customerID: int, firstName: String, lastName: String, custAddress: String, phoneNo: String)</t>
+  </si>
+  <si>
+    <t>+updateCustomer (customerID: int, firstName: String, lastName: String, custAddress: String, phoneNo: String)</t>
+  </si>
+  <si>
+    <t>+readCustomer() : void</t>
+  </si>
+  <si>
+    <t>+printCustomer() : void</t>
   </si>
 </sst>
 </file>
@@ -762,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -878,24 +890,72 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -908,59 +968,29 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1284,7 +1314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB095BD-E922-497D-B7ED-398078A18E3D}">
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1317,16 +1347,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="43">
+      <c r="A2" s="41">
         <v>1</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="44" t="s">
         <v>40</v>
       </c>
       <c r="E2" s="15" t="s">
@@ -1337,10 +1367,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="44"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
       <c r="E3" s="15" t="s">
         <v>54</v>
       </c>
@@ -1349,40 +1379,40 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="44"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
       <c r="E4" s="15" t="s">
         <v>56</v>
       </c>
       <c r="F4" s="24"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="44"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
       <c r="E5" s="15" t="s">
         <v>57</v>
       </c>
       <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="44"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
+      <c r="A6" s="42"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
       <c r="E6" s="15" t="s">
         <v>46</v>
       </c>
       <c r="F6" s="24"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="44"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
+      <c r="A7" s="42"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
       <c r="E7" s="15" t="s">
         <v>38</v>
       </c>
@@ -1397,16 +1427,16 @@
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="43">
+      <c r="A9" s="41">
         <v>2</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="44" t="s">
         <v>91</v>
       </c>
       <c r="E9" s="14" t="s">
@@ -1417,60 +1447,60 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="44"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
       <c r="E10" s="15" t="s">
         <v>97</v>
       </c>
       <c r="F10" s="24"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="44"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
       <c r="E11" s="15" t="s">
         <v>100</v>
       </c>
       <c r="F11" s="24"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="44"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
       <c r="E12" s="15" t="s">
         <v>98</v>
       </c>
       <c r="F12" s="24"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="44"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
       <c r="E13" s="15" t="s">
         <v>99</v>
       </c>
       <c r="F13" s="24"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="44"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
       <c r="E14" s="15" t="s">
         <v>93</v>
       </c>
       <c r="F14" s="24"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="57"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
       <c r="E15" s="15" t="s">
         <v>14</v>
       </c>
@@ -1485,16 +1515,16 @@
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" s="43">
+      <c r="A17" s="41">
         <v>3</v>
       </c>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="45" t="s">
+      <c r="D17" s="44" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="15" t="s">
@@ -1505,20 +1535,20 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="44"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
       <c r="E18" s="15" t="s">
         <v>101</v>
       </c>
       <c r="F18" s="24"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="57"/>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
       <c r="E19" s="11" t="s">
         <v>58</v>
       </c>
@@ -1533,16 +1563,16 @@
       <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="43">
+      <c r="A21" s="41">
         <v>4</v>
       </c>
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="45" t="s">
+      <c r="C21" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="45" t="s">
+      <c r="D21" s="44" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="15" t="s">
@@ -1553,60 +1583,60 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" s="44"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
       <c r="E22" s="15" t="s">
         <v>106</v>
       </c>
       <c r="F22" s="24"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="44"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="15" t="s">
         <v>107</v>
       </c>
       <c r="F23" s="24"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" s="44"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
+      <c r="A24" s="42"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
       <c r="E24" s="15" t="s">
         <v>108</v>
       </c>
       <c r="F24" s="24"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="44"/>
-      <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
+      <c r="A25" s="42"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
       <c r="E25" s="15" t="s">
         <v>102</v>
       </c>
       <c r="F25" s="24"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="44"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
+      <c r="A26" s="42"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
       <c r="E26" s="15" t="s">
         <v>103</v>
       </c>
       <c r="F26" s="24"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" s="57"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
+      <c r="A27" s="43"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
       <c r="E27" s="15" t="s">
         <v>11</v>
       </c>
@@ -1621,16 +1651,16 @@
       <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="43">
+      <c r="A29" s="41">
         <v>5</v>
       </c>
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="45" t="s">
+      <c r="C29" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="45" t="s">
+      <c r="D29" s="44" t="s">
         <v>92</v>
       </c>
       <c r="E29" s="15" t="s">
@@ -1639,20 +1669,20 @@
       <c r="F29" s="24"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" s="44"/>
-      <c r="B30" s="46"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
       <c r="E30" s="15" t="s">
         <v>104</v>
       </c>
       <c r="F30" s="24"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31" s="57"/>
-      <c r="B31" s="58"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="58"/>
+      <c r="A31" s="43"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
       <c r="E31" s="15" t="s">
         <v>105</v>
       </c>
@@ -1667,16 +1697,16 @@
       <c r="F32" s="7"/>
     </row>
     <row r="33" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A33" s="43">
+      <c r="A33" s="41">
         <v>6</v>
       </c>
-      <c r="B33" s="45" t="s">
+      <c r="B33" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="45" t="s">
+      <c r="C33" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="45" t="s">
+      <c r="D33" s="44" t="s">
         <v>16</v>
       </c>
       <c r="E33" s="15" t="s">
@@ -1687,10 +1717,10 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="57"/>
-      <c r="B34" s="58"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
+      <c r="A34" s="43"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
       <c r="E34" s="15" t="s">
         <v>110</v>
       </c>
@@ -1705,80 +1735,80 @@
       <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="68">
+      <c r="A36" s="47">
         <v>7</v>
       </c>
-      <c r="B36" s="64" t="s">
+      <c r="B36" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="64" t="s">
+      <c r="C36" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="D36" s="64" t="s">
+      <c r="D36" s="48" t="s">
         <v>78</v>
       </c>
       <c r="E36" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="F36" s="45" t="s">
+      <c r="F36" s="44" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37" s="68"/>
-      <c r="B37" s="64"/>
-      <c r="C37" s="64"/>
-      <c r="D37" s="64"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
       <c r="E37" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="F37" s="46"/>
+      <c r="F37" s="45"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38" s="68"/>
-      <c r="B38" s="64"/>
-      <c r="C38" s="64"/>
-      <c r="D38" s="64"/>
+      <c r="A38" s="47"/>
+      <c r="B38" s="48"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="48"/>
       <c r="E38" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="F38" s="58"/>
+      <c r="F38" s="46"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39" s="68"/>
-      <c r="B39" s="64"/>
-      <c r="C39" s="64"/>
-      <c r="D39" s="64"/>
+      <c r="A39" s="47"/>
+      <c r="B39" s="48"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="48"/>
       <c r="E39" s="24" t="s">
         <v>81</v>
       </c>
       <c r="F39" s="24"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" s="68"/>
-      <c r="B40" s="64"/>
-      <c r="C40" s="64"/>
-      <c r="D40" s="64"/>
+      <c r="A40" s="47"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="48"/>
+      <c r="D40" s="48"/>
       <c r="E40" s="24" t="s">
         <v>82</v>
       </c>
       <c r="F40" s="24"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" s="68"/>
-      <c r="B41" s="64"/>
-      <c r="C41" s="64"/>
-      <c r="D41" s="64"/>
+      <c r="A41" s="47"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="48"/>
       <c r="E41" s="24" t="s">
         <v>83</v>
       </c>
       <c r="F41" s="24"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42" s="68"/>
-      <c r="B42" s="64"/>
-      <c r="C42" s="64"/>
-      <c r="D42" s="64"/>
+      <c r="A42" s="47"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="48"/>
       <c r="E42" s="24" t="s">
         <v>85</v>
       </c>
@@ -1867,16 +1897,16 @@
       <c r="F55" s="7"/>
     </row>
     <row r="56" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="59">
+      <c r="A56" s="52">
         <v>12</v>
       </c>
-      <c r="B56" s="65" t="s">
+      <c r="B56" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C56" s="65" t="s">
+      <c r="C56" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="D56" s="65" t="s">
+      <c r="D56" s="49" t="s">
         <v>44</v>
       </c>
       <c r="E56" s="17" t="s">
@@ -1885,30 +1915,30 @@
       <c r="F56" s="36"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A57" s="60"/>
-      <c r="B57" s="66"/>
-      <c r="C57" s="66"/>
-      <c r="D57" s="66"/>
+      <c r="A57" s="53"/>
+      <c r="B57" s="50"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="50"/>
       <c r="E57" s="17" t="s">
         <v>42</v>
       </c>
       <c r="F57" s="36"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A58" s="60"/>
-      <c r="B58" s="66"/>
-      <c r="C58" s="66"/>
-      <c r="D58" s="66"/>
+      <c r="A58" s="53"/>
+      <c r="B58" s="50"/>
+      <c r="C58" s="50"/>
+      <c r="D58" s="50"/>
       <c r="E58" s="17" t="s">
         <v>37</v>
       </c>
       <c r="F58" s="36"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A59" s="61"/>
-      <c r="B59" s="67"/>
-      <c r="C59" s="67"/>
-      <c r="D59" s="67"/>
+      <c r="A59" s="54"/>
+      <c r="B59" s="51"/>
+      <c r="C59" s="51"/>
+      <c r="D59" s="51"/>
       <c r="E59" s="17" t="s">
         <v>38</v>
       </c>
@@ -1931,40 +1961,40 @@
       <c r="F70" s="7"/>
     </row>
     <row r="71" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A71" s="51">
+      <c r="A71" s="57">
         <v>10</v>
       </c>
-      <c r="B71" s="54" t="s">
+      <c r="B71" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="C71" s="54" t="s">
+      <c r="C71" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="D71" s="54" t="s">
+      <c r="D71" s="60" t="s">
         <v>33</v>
       </c>
       <c r="E71" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F71" s="62" t="s">
+      <c r="F71" s="55" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A72" s="52"/>
-      <c r="B72" s="55"/>
-      <c r="C72" s="55"/>
-      <c r="D72" s="55"/>
+      <c r="A72" s="58"/>
+      <c r="B72" s="61"/>
+      <c r="C72" s="61"/>
+      <c r="D72" s="61"/>
       <c r="E72" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="F72" s="63"/>
+      <c r="F72" s="56"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A73" s="53"/>
-      <c r="B73" s="56"/>
-      <c r="C73" s="56"/>
-      <c r="D73" s="56"/>
+      <c r="A73" s="59"/>
+      <c r="B73" s="62"/>
+      <c r="C73" s="62"/>
+      <c r="D73" s="62"/>
       <c r="E73" s="6"/>
       <c r="F73" s="37"/>
     </row>
@@ -1977,16 +2007,16 @@
       <c r="F74" s="7"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A75" s="51">
+      <c r="A75" s="57">
         <v>11</v>
       </c>
-      <c r="B75" s="54" t="s">
+      <c r="B75" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="C75" s="54" t="s">
+      <c r="C75" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="D75" s="54" t="s">
+      <c r="D75" s="60" t="s">
         <v>26</v>
       </c>
       <c r="E75" s="18" t="s">
@@ -1995,20 +2025,20 @@
       <c r="F75" s="37"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A76" s="52"/>
-      <c r="B76" s="55"/>
-      <c r="C76" s="55"/>
-      <c r="D76" s="55"/>
+      <c r="A76" s="58"/>
+      <c r="B76" s="61"/>
+      <c r="C76" s="61"/>
+      <c r="D76" s="61"/>
       <c r="E76" s="18" t="s">
         <v>28</v>
       </c>
       <c r="F76" s="37"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A77" s="53"/>
-      <c r="B77" s="56"/>
-      <c r="C77" s="56"/>
-      <c r="D77" s="56"/>
+      <c r="A77" s="59"/>
+      <c r="B77" s="62"/>
+      <c r="C77" s="62"/>
+      <c r="D77" s="62"/>
       <c r="E77" s="18" t="s">
         <v>29</v>
       </c>
@@ -2022,16 +2052,16 @@
       <c r="E80" s="9"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A81" s="49">
+      <c r="A81" s="65">
         <v>6</v>
       </c>
-      <c r="B81" s="47" t="s">
+      <c r="B81" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C81" s="47" t="s">
+      <c r="C81" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="D81" s="47" t="s">
+      <c r="D81" s="63" t="s">
         <v>19</v>
       </c>
       <c r="E81" s="12" t="s">
@@ -2039,10 +2069,10 @@
       </c>
     </row>
     <row r="82" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A82" s="50"/>
-      <c r="B82" s="48"/>
-      <c r="C82" s="48"/>
-      <c r="D82" s="48"/>
+      <c r="A82" s="66"/>
+      <c r="B82" s="64"/>
+      <c r="C82" s="64"/>
+      <c r="D82" s="64"/>
       <c r="E82" s="12" t="s">
         <v>31</v>
       </c>
@@ -2107,36 +2137,6 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A36:A42"/>
-    <mergeCell ref="B36:B42"/>
-    <mergeCell ref="C36:C42"/>
-    <mergeCell ref="D36:D42"/>
-    <mergeCell ref="F36:F38"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="D56:D59"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="C71:C73"/>
-    <mergeCell ref="D71:D73"/>
-    <mergeCell ref="B21:B27"/>
-    <mergeCell ref="A21:A27"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C21:C27"/>
-    <mergeCell ref="D21:D27"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="D33:D34"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="C2:C7"/>
@@ -2153,6 +2153,36 @@
     <mergeCell ref="B9:B15"/>
     <mergeCell ref="C9:C15"/>
     <mergeCell ref="D9:D15"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C21:C27"/>
+    <mergeCell ref="D21:D27"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="B21:B27"/>
+    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="C71:C73"/>
+    <mergeCell ref="D71:D73"/>
+    <mergeCell ref="C36:C42"/>
+    <mergeCell ref="D36:D42"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A36:A42"/>
+    <mergeCell ref="B36:B42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2164,7 +2194,7 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40:C47"/>
+      <selection activeCell="C36" sqref="C36:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2196,16 +2226,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="43">
+      <c r="A2" s="41">
         <v>1</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="44" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="14" t="s">
@@ -2216,10 +2246,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="44"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
       <c r="E3" s="15" t="s">
         <v>67</v>
       </c>
@@ -2228,70 +2258,70 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="44"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
       <c r="E4" s="15" t="s">
         <v>71</v>
       </c>
       <c r="F4" s="24"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="44"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
       <c r="E5" s="15" t="s">
         <v>72</v>
       </c>
       <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="44"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
+      <c r="A6" s="42"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
       <c r="E6" s="15" t="s">
         <v>73</v>
       </c>
       <c r="F6" s="24"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="44"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
+      <c r="A7" s="42"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
       <c r="E7" s="15" t="s">
         <v>75</v>
       </c>
       <c r="F7" s="24"/>
     </row>
     <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="44"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
+      <c r="A8" s="42"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
       <c r="E8" s="15" t="s">
         <v>68</v>
       </c>
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="44"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
       <c r="E9" s="15" t="s">
         <v>69</v>
       </c>
       <c r="F9" s="24"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="57"/>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
       <c r="E10" s="15" t="s">
         <v>14</v>
       </c>
@@ -2306,16 +2336,16 @@
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="43">
+      <c r="A12" s="41">
         <v>2</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="44" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="15" t="s">
@@ -2326,40 +2356,40 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="44"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
       <c r="E13" s="15" t="s">
         <v>112</v>
       </c>
       <c r="F13" s="24"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="44"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
       <c r="E14" s="15" t="s">
         <v>113</v>
       </c>
       <c r="F14" s="24"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="44"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
       <c r="E15" s="15" t="s">
         <v>114</v>
       </c>
       <c r="F15" s="24"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="57"/>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
       <c r="E16" s="11" t="s">
         <v>58</v>
       </c>
@@ -2374,16 +2404,16 @@
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="43">
+      <c r="A18" s="41">
         <v>3</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="45" t="s">
+      <c r="D18" s="44" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="15" t="s">
@@ -2394,50 +2424,50 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="44"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
       <c r="E19" s="15" t="s">
         <v>112</v>
       </c>
       <c r="F19" s="24"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" s="44"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
       <c r="E20" s="15" t="s">
         <v>116</v>
       </c>
       <c r="F20" s="24"/>
     </row>
     <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="44"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
+      <c r="A21" s="42"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
       <c r="E21" s="15" t="s">
         <v>117</v>
       </c>
       <c r="F21" s="24"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" s="44"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
       <c r="E22" s="15" t="s">
         <v>119</v>
       </c>
       <c r="F22" s="24"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="44"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="15" t="s">
         <v>118</v>
       </c>
@@ -2452,16 +2482,16 @@
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A25" s="43">
+      <c r="A25" s="41">
         <v>4</v>
       </c>
-      <c r="B25" s="45" t="s">
+      <c r="B25" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="45" t="s">
+      <c r="C25" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="D25" s="45" t="s">
+      <c r="D25" s="44" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="15" t="s">
@@ -2470,10 +2500,10 @@
       <c r="F25" s="24"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="44"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
+      <c r="A26" s="42"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
       <c r="E26" s="15" t="s">
         <v>121</v>
       </c>
@@ -2488,16 +2518,16 @@
       <c r="F27" s="7"/>
     </row>
     <row r="28" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A28" s="43">
+      <c r="A28" s="41">
         <v>5</v>
       </c>
-      <c r="B28" s="45" t="s">
+      <c r="B28" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="45" t="s">
+      <c r="C28" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="45" t="s">
+      <c r="D28" s="44" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="15" t="s">
@@ -2508,10 +2538,10 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="44"/>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
+      <c r="A29" s="42"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
       <c r="E29" s="15" t="s">
         <v>17</v>
       </c>
@@ -2526,16 +2556,16 @@
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="43">
+      <c r="A31" s="41">
         <v>6</v>
       </c>
-      <c r="B31" s="45" t="s">
+      <c r="B31" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="45" t="s">
+      <c r="C31" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="D31" s="45" t="s">
+      <c r="D31" s="44" t="s">
         <v>50</v>
       </c>
       <c r="E31" s="14" t="s">
@@ -2546,30 +2576,30 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32" s="44"/>
-      <c r="B32" s="46"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
+      <c r="A32" s="42"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
       <c r="E32" s="15" t="s">
         <v>126</v>
       </c>
       <c r="F32" s="24"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33" s="44"/>
-      <c r="B33" s="46"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="46"/>
+      <c r="A33" s="42"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
       <c r="E33" s="15" t="s">
         <v>124</v>
       </c>
       <c r="F33" s="24"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="57"/>
-      <c r="B34" s="58"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
+      <c r="A34" s="43"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
       <c r="E34" s="15" t="s">
         <v>22</v>
       </c>
@@ -2584,16 +2614,16 @@
       <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A36" s="43">
+      <c r="A36" s="41">
         <v>7</v>
       </c>
-      <c r="B36" s="45" t="s">
+      <c r="B36" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="45" t="s">
+      <c r="C36" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="45" t="s">
+      <c r="D36" s="44" t="s">
         <v>24</v>
       </c>
       <c r="E36" s="15" t="s">
@@ -2602,20 +2632,20 @@
       <c r="F36" s="24"/>
     </row>
     <row r="37" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A37" s="44"/>
-      <c r="B37" s="46"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
       <c r="E37" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F37" s="24"/>
     </row>
     <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A38" s="57"/>
-      <c r="B38" s="58"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
+      <c r="A38" s="43"/>
+      <c r="B38" s="46"/>
+      <c r="C38" s="46"/>
+      <c r="D38" s="46"/>
       <c r="E38" s="15" t="s">
         <v>36</v>
       </c>
@@ -2630,16 +2660,16 @@
       <c r="F39" s="7"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" s="43">
+      <c r="A40" s="41">
         <v>8</v>
       </c>
-      <c r="B40" s="45" t="s">
+      <c r="B40" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="45" t="s">
+      <c r="C40" s="44" t="s">
         <v>127</v>
       </c>
-      <c r="D40" s="45" t="s">
+      <c r="D40" s="44" t="s">
         <v>128</v>
       </c>
       <c r="E40" s="24" t="s">
@@ -2648,65 +2678,70 @@
       <c r="F40" s="24"/>
     </row>
     <row r="41" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A41" s="44"/>
-      <c r="B41" s="46"/>
-      <c r="C41" s="46"/>
-      <c r="D41" s="46"/>
+      <c r="A41" s="42"/>
+      <c r="B41" s="45"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="45"/>
       <c r="E41" s="24" t="s">
         <v>130</v>
       </c>
+      <c r="F41" s="24"/>
     </row>
     <row r="42" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A42" s="44"/>
-      <c r="B42" s="46"/>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
+      <c r="A42" s="42"/>
+      <c r="B42" s="45"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="45"/>
       <c r="E42" s="24" t="s">
         <v>131</v>
       </c>
+      <c r="F42" s="24"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43" s="44"/>
-      <c r="B43" s="46"/>
-      <c r="C43" s="46"/>
-      <c r="D43" s="46"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="45"/>
+      <c r="C43" s="45"/>
+      <c r="D43" s="45"/>
       <c r="E43" s="24" t="s">
         <v>132</v>
       </c>
+      <c r="F43" s="24"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44" s="44"/>
-      <c r="B44" s="46"/>
-      <c r="C44" s="46"/>
-      <c r="D44" s="46"/>
-      <c r="E44" s="11" t="s">
+      <c r="A44" s="42"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="24" t="s">
         <v>134</v>
       </c>
+      <c r="F44" s="24"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A45" s="44"/>
-      <c r="B45" s="46"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="11" t="s">
+      <c r="A45" s="42"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="24" t="s">
         <v>135</v>
       </c>
+      <c r="F45" s="24"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46" s="44"/>
-      <c r="B46" s="46"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
+      <c r="A46" s="42"/>
+      <c r="B46" s="45"/>
+      <c r="C46" s="45"/>
+      <c r="D46" s="45"/>
       <c r="E46" s="24" t="s">
         <v>133</v>
       </c>
       <c r="F46" s="24"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47" s="44"/>
-      <c r="B47" s="46"/>
-      <c r="C47" s="46"/>
-      <c r="D47" s="46"/>
+      <c r="A47" s="42"/>
+      <c r="B47" s="45"/>
+      <c r="C47" s="45"/>
+      <c r="D47" s="45"/>
       <c r="E47" s="14" t="s">
         <v>85</v>
       </c>
@@ -2722,6 +2757,30 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="C2:C10"/>
+    <mergeCell ref="D2:D10"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="A31:A34"/>
     <mergeCell ref="A40:A47"/>
     <mergeCell ref="B40:B47"/>
     <mergeCell ref="C40:C47"/>
@@ -2730,30 +2789,6 @@
     <mergeCell ref="C36:C38"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="C2:C10"/>
-    <mergeCell ref="D2:D10"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="D12:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2761,10 +2796,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD0B509-A153-4B31-95B8-BC32DC1B6A3B}">
-  <dimension ref="B2:G31"/>
+  <dimension ref="B2:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2773,197 +2808,197 @@
     <col min="2" max="2" width="37.46484375" style="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.06640625" style="38" customWidth="1"/>
     <col min="4" max="4" width="41.73046875" style="40" customWidth="1"/>
-    <col min="5" max="5" width="9.06640625" style="38"/>
+    <col min="5" max="5" width="3.796875" style="38" customWidth="1"/>
+    <col min="6" max="6" width="37.9296875" customWidth="1"/>
+    <col min="7" max="7" width="3.59765625" customWidth="1"/>
+    <col min="8" max="8" width="40.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B2" s="39" t="s">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B2" s="74" t="s">
         <v>137</v>
       </c>
       <c r="C2" s="39"/>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="75" t="s">
         <v>138</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="74" t="s">
+        <v>148</v>
+      </c>
+      <c r="H2" s="76" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B3" s="38" t="s">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B3" s="73" t="s">
         <v>143</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="67" t="s">
         <v>143</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F3" s="73" t="s">
+        <v>160</v>
+      </c>
+      <c r="H3" s="67" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B4" s="38" t="s">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B4" s="71" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="68" t="s">
         <v>145</v>
       </c>
-      <c r="G4" t="s">
+      <c r="F4" s="71" t="s">
+        <v>161</v>
+      </c>
+      <c r="H4" s="68" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B5" s="38" t="s">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B5" s="71" t="s">
         <v>144</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="68" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B6" s="38" t="s">
+      <c r="F5" s="71" t="s">
+        <v>162</v>
+      </c>
+      <c r="H5" s="68" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B6" s="71" t="s">
         <v>146</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="68" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B8" s="40" t="s">
+      <c r="F6" s="71" t="s">
+        <v>163</v>
+      </c>
+      <c r="H6" s="68" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B7" s="71"/>
+      <c r="D7" s="70"/>
+      <c r="F7" s="72" t="s">
+        <v>164</v>
+      </c>
+      <c r="H7" s="70"/>
+    </row>
+    <row r="8" spans="2:17" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B8" s="67" t="s">
         <v>149</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="68" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B9" s="38" t="s">
+      <c r="F8" s="68" t="s">
+        <v>165</v>
+      </c>
+      <c r="H8" s="68" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B9" s="68" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" s="70" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9" s="71" t="s">
+        <v>151</v>
+      </c>
+      <c r="H9" s="68" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B10" s="68" t="s">
+        <v>177</v>
+      </c>
+      <c r="F10" s="71" t="s">
+        <v>152</v>
+      </c>
+      <c r="H10" s="69" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B11" s="71" t="s">
         <v>139</v>
       </c>
-      <c r="D9" s="40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B10" s="38" t="s">
+      <c r="F11" s="71" t="s">
+        <v>153</v>
+      </c>
+      <c r="H11" s="68" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B12" s="71" t="s">
+        <v>178</v>
+      </c>
+      <c r="F12" s="71" t="s">
+        <v>154</v>
+      </c>
+      <c r="H12" s="70" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B13" s="71" t="s">
+        <v>179</v>
+      </c>
+      <c r="F13" s="71" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B14" s="71" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B11" s="38" t="s">
+      <c r="F14" s="71" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B15" s="72" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B14" s="39" t="s">
-        <v>148</v>
-      </c>
-      <c r="D14" s="40" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B15" s="38" t="s">
-        <v>160</v>
-      </c>
-      <c r="D15" s="40" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B16" s="38" t="s">
-        <v>161</v>
-      </c>
-      <c r="D16" s="40" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B17" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="D17" s="40" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B18" s="38" t="s">
-        <v>163</v>
-      </c>
-      <c r="D18" s="40" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B19" s="38" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B21" s="40" t="s">
-        <v>165</v>
-      </c>
-      <c r="D21" s="40" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B22" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="D22" s="40" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B23" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="D23" s="42" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B24" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="D24" s="40" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B25" s="38" t="s">
-        <v>154</v>
-      </c>
-      <c r="D25" s="40" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B26" s="38" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B27" s="38" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B28" s="38" t="s">
+      <c r="F15" s="71" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B29" s="38" t="s">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="F16" s="71" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B30" s="38" t="s">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F17" s="71" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B31" s="38" t="s">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F18" s="72" t="s">
         <v>166</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated TeamPlan, Justification and UserStory for Newsagent
</commit_message>
<xml_diff>
--- a/User Stories/NataliaUserStories.xlsx
+++ b/User Stories/NataliaUserStories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Palej\Desktop\Software Design with AI for Cloud\Year_3\agile-labs3\Newsagent-Project\User Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A7AEE6-62C3-4B6B-95A6-DAF763ED861B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CDBAF4-A486-4E85-B632-0D6733ADC24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminUserStories" sheetId="1" r:id="rId1"/>
@@ -421,9 +421,6 @@
     <t>Verify accStatus is successfully changed to "Annual Leave"</t>
   </si>
   <si>
-    <t>I want to generate delivery doc</t>
-  </si>
-  <si>
     <t>so that my drivers can work</t>
   </si>
   <si>
@@ -578,6 +575,9 @@
   </si>
   <si>
     <t>+printCustomer() : void</t>
+  </si>
+  <si>
+    <t>I want to generate delivery docket report</t>
   </si>
 </sst>
 </file>
@@ -890,84 +890,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -991,6 +913,84 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1314,7 +1314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB095BD-E922-497D-B7ED-398078A18E3D}">
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1347,16 +1347,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="41">
+      <c r="A2" s="51">
         <v>1</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="53" t="s">
         <v>40</v>
       </c>
       <c r="E2" s="15" t="s">
@@ -1367,10 +1367,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="42"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
       <c r="E3" s="15" t="s">
         <v>54</v>
       </c>
@@ -1379,40 +1379,40 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="42"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
       <c r="E4" s="15" t="s">
         <v>56</v>
       </c>
       <c r="F4" s="24"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="42"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
       <c r="E5" s="15" t="s">
         <v>57</v>
       </c>
       <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="42"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
       <c r="E6" s="15" t="s">
         <v>46</v>
       </c>
       <c r="F6" s="24"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="42"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
       <c r="E7" s="15" t="s">
         <v>38</v>
       </c>
@@ -1427,16 +1427,16 @@
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="41">
+      <c r="A9" s="51">
         <v>2</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="53" t="s">
         <v>91</v>
       </c>
       <c r="E9" s="14" t="s">
@@ -1447,60 +1447,60 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="42"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
       <c r="E10" s="15" t="s">
         <v>97</v>
       </c>
       <c r="F10" s="24"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="42"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
       <c r="E11" s="15" t="s">
         <v>100</v>
       </c>
       <c r="F11" s="24"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="42"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
+      <c r="A12" s="52"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
       <c r="E12" s="15" t="s">
         <v>98</v>
       </c>
       <c r="F12" s="24"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="42"/>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
+      <c r="A13" s="52"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
       <c r="E13" s="15" t="s">
         <v>99</v>
       </c>
       <c r="F13" s="24"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="42"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
+      <c r="A14" s="52"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
       <c r="E14" s="15" t="s">
         <v>93</v>
       </c>
       <c r="F14" s="24"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="43"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
+      <c r="A15" s="65"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
       <c r="E15" s="15" t="s">
         <v>14</v>
       </c>
@@ -1515,16 +1515,16 @@
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" s="41">
+      <c r="A17" s="51">
         <v>3</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="D17" s="53" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="15" t="s">
@@ -1535,20 +1535,20 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="42"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
+      <c r="A18" s="52"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="15" t="s">
         <v>101</v>
       </c>
       <c r="F18" s="24"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="43"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
+      <c r="A19" s="65"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
       <c r="E19" s="11" t="s">
         <v>58</v>
       </c>
@@ -1563,16 +1563,16 @@
       <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="41">
+      <c r="A21" s="51">
         <v>4</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="44" t="s">
+      <c r="C21" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="44" t="s">
+      <c r="D21" s="53" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="15" t="s">
@@ -1583,60 +1583,60 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" s="42"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
+      <c r="A22" s="52"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
       <c r="E22" s="15" t="s">
         <v>106</v>
       </c>
       <c r="F22" s="24"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="42"/>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
+      <c r="A23" s="52"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
       <c r="E23" s="15" t="s">
         <v>107</v>
       </c>
       <c r="F23" s="24"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" s="42"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
+      <c r="A24" s="52"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
       <c r="E24" s="15" t="s">
         <v>108</v>
       </c>
       <c r="F24" s="24"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="42"/>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
+      <c r="A25" s="52"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
       <c r="E25" s="15" t="s">
         <v>102</v>
       </c>
       <c r="F25" s="24"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="42"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
+      <c r="A26" s="52"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
       <c r="E26" s="15" t="s">
         <v>103</v>
       </c>
       <c r="F26" s="24"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" s="43"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
+      <c r="A27" s="65"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="66"/>
       <c r="E27" s="15" t="s">
         <v>11</v>
       </c>
@@ -1651,16 +1651,16 @@
       <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="41">
+      <c r="A29" s="51">
         <v>5</v>
       </c>
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="44" t="s">
+      <c r="C29" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="44" t="s">
+      <c r="D29" s="53" t="s">
         <v>92</v>
       </c>
       <c r="E29" s="15" t="s">
@@ -1669,20 +1669,20 @@
       <c r="F29" s="24"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" s="42"/>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
+      <c r="A30" s="52"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
       <c r="E30" s="15" t="s">
         <v>104</v>
       </c>
       <c r="F30" s="24"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31" s="43"/>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
+      <c r="A31" s="65"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
       <c r="E31" s="15" t="s">
         <v>105</v>
       </c>
@@ -1697,16 +1697,16 @@
       <c r="F32" s="7"/>
     </row>
     <row r="33" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A33" s="41">
+      <c r="A33" s="51">
         <v>6</v>
       </c>
-      <c r="B33" s="44" t="s">
+      <c r="B33" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="44" t="s">
+      <c r="C33" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="44" t="s">
+      <c r="D33" s="53" t="s">
         <v>16</v>
       </c>
       <c r="E33" s="15" t="s">
@@ -1717,10 +1717,10 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="43"/>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
+      <c r="A34" s="65"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
       <c r="E34" s="15" t="s">
         <v>110</v>
       </c>
@@ -1735,80 +1735,80 @@
       <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="47">
+      <c r="A36" s="76">
         <v>7</v>
       </c>
-      <c r="B36" s="48" t="s">
+      <c r="B36" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="48" t="s">
+      <c r="C36" s="72" t="s">
         <v>77</v>
       </c>
-      <c r="D36" s="48" t="s">
+      <c r="D36" s="72" t="s">
         <v>78</v>
       </c>
       <c r="E36" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="F36" s="44" t="s">
-        <v>136</v>
+      <c r="F36" s="53" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37" s="47"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
+      <c r="A37" s="76"/>
+      <c r="B37" s="72"/>
+      <c r="C37" s="72"/>
+      <c r="D37" s="72"/>
       <c r="E37" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="F37" s="45"/>
+      <c r="F37" s="54"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38" s="47"/>
-      <c r="B38" s="48"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="48"/>
+      <c r="A38" s="76"/>
+      <c r="B38" s="72"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="72"/>
       <c r="E38" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="F38" s="46"/>
+      <c r="F38" s="66"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39" s="47"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
+      <c r="A39" s="76"/>
+      <c r="B39" s="72"/>
+      <c r="C39" s="72"/>
+      <c r="D39" s="72"/>
       <c r="E39" s="24" t="s">
         <v>81</v>
       </c>
       <c r="F39" s="24"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" s="47"/>
-      <c r="B40" s="48"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="48"/>
+      <c r="A40" s="76"/>
+      <c r="B40" s="72"/>
+      <c r="C40" s="72"/>
+      <c r="D40" s="72"/>
       <c r="E40" s="24" t="s">
         <v>82</v>
       </c>
       <c r="F40" s="24"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" s="47"/>
-      <c r="B41" s="48"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
+      <c r="A41" s="76"/>
+      <c r="B41" s="72"/>
+      <c r="C41" s="72"/>
+      <c r="D41" s="72"/>
       <c r="E41" s="24" t="s">
         <v>83</v>
       </c>
       <c r="F41" s="24"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42" s="47"/>
-      <c r="B42" s="48"/>
-      <c r="C42" s="48"/>
-      <c r="D42" s="48"/>
+      <c r="A42" s="76"/>
+      <c r="B42" s="72"/>
+      <c r="C42" s="72"/>
+      <c r="D42" s="72"/>
       <c r="E42" s="24" t="s">
         <v>85</v>
       </c>
@@ -1897,16 +1897,16 @@
       <c r="F55" s="7"/>
     </row>
     <row r="56" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="52">
+      <c r="A56" s="67">
         <v>12</v>
       </c>
-      <c r="B56" s="49" t="s">
+      <c r="B56" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C56" s="49" t="s">
+      <c r="C56" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="D56" s="49" t="s">
+      <c r="D56" s="73" t="s">
         <v>44</v>
       </c>
       <c r="E56" s="17" t="s">
@@ -1915,30 +1915,30 @@
       <c r="F56" s="36"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A57" s="53"/>
-      <c r="B57" s="50"/>
-      <c r="C57" s="50"/>
-      <c r="D57" s="50"/>
+      <c r="A57" s="68"/>
+      <c r="B57" s="74"/>
+      <c r="C57" s="74"/>
+      <c r="D57" s="74"/>
       <c r="E57" s="17" t="s">
         <v>42</v>
       </c>
       <c r="F57" s="36"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A58" s="53"/>
-      <c r="B58" s="50"/>
-      <c r="C58" s="50"/>
-      <c r="D58" s="50"/>
+      <c r="A58" s="68"/>
+      <c r="B58" s="74"/>
+      <c r="C58" s="74"/>
+      <c r="D58" s="74"/>
       <c r="E58" s="17" t="s">
         <v>37</v>
       </c>
       <c r="F58" s="36"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A59" s="54"/>
-      <c r="B59" s="51"/>
-      <c r="C59" s="51"/>
-      <c r="D59" s="51"/>
+      <c r="A59" s="69"/>
+      <c r="B59" s="75"/>
+      <c r="C59" s="75"/>
+      <c r="D59" s="75"/>
       <c r="E59" s="17" t="s">
         <v>38</v>
       </c>
@@ -1961,40 +1961,40 @@
       <c r="F70" s="7"/>
     </row>
     <row r="71" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A71" s="57">
+      <c r="A71" s="59">
         <v>10</v>
       </c>
-      <c r="B71" s="60" t="s">
+      <c r="B71" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="C71" s="60" t="s">
+      <c r="C71" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="D71" s="60" t="s">
+      <c r="D71" s="62" t="s">
         <v>33</v>
       </c>
       <c r="E71" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F71" s="55" t="s">
+      <c r="F71" s="70" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A72" s="58"/>
-      <c r="B72" s="61"/>
-      <c r="C72" s="61"/>
-      <c r="D72" s="61"/>
+      <c r="A72" s="60"/>
+      <c r="B72" s="63"/>
+      <c r="C72" s="63"/>
+      <c r="D72" s="63"/>
       <c r="E72" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="F72" s="56"/>
+      <c r="F72" s="71"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A73" s="59"/>
-      <c r="B73" s="62"/>
-      <c r="C73" s="62"/>
-      <c r="D73" s="62"/>
+      <c r="A73" s="61"/>
+      <c r="B73" s="64"/>
+      <c r="C73" s="64"/>
+      <c r="D73" s="64"/>
       <c r="E73" s="6"/>
       <c r="F73" s="37"/>
     </row>
@@ -2007,16 +2007,16 @@
       <c r="F74" s="7"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A75" s="57">
+      <c r="A75" s="59">
         <v>11</v>
       </c>
-      <c r="B75" s="60" t="s">
+      <c r="B75" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="C75" s="60" t="s">
+      <c r="C75" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="D75" s="60" t="s">
+      <c r="D75" s="62" t="s">
         <v>26</v>
       </c>
       <c r="E75" s="18" t="s">
@@ -2025,20 +2025,20 @@
       <c r="F75" s="37"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A76" s="58"/>
-      <c r="B76" s="61"/>
-      <c r="C76" s="61"/>
-      <c r="D76" s="61"/>
+      <c r="A76" s="60"/>
+      <c r="B76" s="63"/>
+      <c r="C76" s="63"/>
+      <c r="D76" s="63"/>
       <c r="E76" s="18" t="s">
         <v>28</v>
       </c>
       <c r="F76" s="37"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A77" s="59"/>
-      <c r="B77" s="62"/>
-      <c r="C77" s="62"/>
-      <c r="D77" s="62"/>
+      <c r="A77" s="61"/>
+      <c r="B77" s="64"/>
+      <c r="C77" s="64"/>
+      <c r="D77" s="64"/>
       <c r="E77" s="18" t="s">
         <v>29</v>
       </c>
@@ -2052,16 +2052,16 @@
       <c r="E80" s="9"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A81" s="65">
+      <c r="A81" s="57">
         <v>6</v>
       </c>
-      <c r="B81" s="63" t="s">
+      <c r="B81" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C81" s="63" t="s">
+      <c r="C81" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="D81" s="63" t="s">
+      <c r="D81" s="55" t="s">
         <v>19</v>
       </c>
       <c r="E81" s="12" t="s">
@@ -2069,10 +2069,10 @@
       </c>
     </row>
     <row r="82" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A82" s="66"/>
-      <c r="B82" s="64"/>
-      <c r="C82" s="64"/>
-      <c r="D82" s="64"/>
+      <c r="A82" s="58"/>
+      <c r="B82" s="56"/>
+      <c r="C82" s="56"/>
+      <c r="D82" s="56"/>
       <c r="E82" s="12" t="s">
         <v>31</v>
       </c>
@@ -2137,6 +2137,36 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A36:A42"/>
+    <mergeCell ref="B36:B42"/>
+    <mergeCell ref="C36:C42"/>
+    <mergeCell ref="D36:D42"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="C71:C73"/>
+    <mergeCell ref="D71:D73"/>
+    <mergeCell ref="B21:B27"/>
+    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C21:C27"/>
+    <mergeCell ref="D21:D27"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D33:D34"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="C2:C7"/>
@@ -2153,36 +2183,6 @@
     <mergeCell ref="B9:B15"/>
     <mergeCell ref="C9:C15"/>
     <mergeCell ref="D9:D15"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C21:C27"/>
-    <mergeCell ref="D21:D27"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="B21:B27"/>
-    <mergeCell ref="A21:A27"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="C71:C73"/>
-    <mergeCell ref="D71:D73"/>
-    <mergeCell ref="C36:C42"/>
-    <mergeCell ref="D36:D42"/>
-    <mergeCell ref="F36:F38"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="D56:D59"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A36:A42"/>
-    <mergeCell ref="B36:B42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2193,8 +2193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526350BB-95BB-4BF1-93A5-0B30D123D1AA}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36:C38"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2226,16 +2226,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="41">
+      <c r="A2" s="51">
         <v>1</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="53" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="14" t="s">
@@ -2246,10 +2246,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="42"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
       <c r="E3" s="15" t="s">
         <v>67</v>
       </c>
@@ -2258,70 +2258,70 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="42"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
       <c r="E4" s="15" t="s">
         <v>71</v>
       </c>
       <c r="F4" s="24"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="42"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
       <c r="E5" s="15" t="s">
         <v>72</v>
       </c>
       <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="42"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
       <c r="E6" s="15" t="s">
         <v>73</v>
       </c>
       <c r="F6" s="24"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="42"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
       <c r="E7" s="15" t="s">
         <v>75</v>
       </c>
       <c r="F7" s="24"/>
     </row>
     <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="42"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
       <c r="E8" s="15" t="s">
         <v>68</v>
       </c>
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="42"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
       <c r="E9" s="15" t="s">
         <v>69</v>
       </c>
       <c r="F9" s="24"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="43"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
       <c r="E10" s="15" t="s">
         <v>14</v>
       </c>
@@ -2336,16 +2336,16 @@
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="41">
+      <c r="A12" s="51">
         <v>2</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="53" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="15" t="s">
@@ -2356,40 +2356,40 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="42"/>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
+      <c r="A13" s="52"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
       <c r="E13" s="15" t="s">
         <v>112</v>
       </c>
       <c r="F13" s="24"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="42"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
+      <c r="A14" s="52"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
       <c r="E14" s="15" t="s">
         <v>113</v>
       </c>
       <c r="F14" s="24"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="42"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
       <c r="E15" s="15" t="s">
         <v>114</v>
       </c>
       <c r="F15" s="24"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="43"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
+      <c r="A16" s="65"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
       <c r="E16" s="11" t="s">
         <v>58</v>
       </c>
@@ -2404,16 +2404,16 @@
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="41">
+      <c r="A18" s="51">
         <v>3</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="53" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="15" t="s">
@@ -2424,50 +2424,50 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="42"/>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
+      <c r="A19" s="52"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
       <c r="E19" s="15" t="s">
         <v>112</v>
       </c>
       <c r="F19" s="24"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" s="42"/>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
+      <c r="A20" s="52"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
       <c r="E20" s="15" t="s">
         <v>116</v>
       </c>
       <c r="F20" s="24"/>
     </row>
     <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="42"/>
-      <c r="B21" s="45"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
+      <c r="A21" s="52"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
       <c r="E21" s="15" t="s">
         <v>117</v>
       </c>
       <c r="F21" s="24"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" s="42"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
+      <c r="A22" s="52"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
       <c r="E22" s="15" t="s">
         <v>119</v>
       </c>
       <c r="F22" s="24"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="42"/>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
+      <c r="A23" s="52"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
       <c r="E23" s="15" t="s">
         <v>118</v>
       </c>
@@ -2482,16 +2482,16 @@
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A25" s="41">
+      <c r="A25" s="51">
         <v>4</v>
       </c>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="44" t="s">
+      <c r="C25" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="D25" s="44" t="s">
+      <c r="D25" s="53" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="15" t="s">
@@ -2500,10 +2500,10 @@
       <c r="F25" s="24"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="42"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
+      <c r="A26" s="52"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
       <c r="E26" s="15" t="s">
         <v>121</v>
       </c>
@@ -2518,16 +2518,16 @@
       <c r="F27" s="7"/>
     </row>
     <row r="28" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A28" s="41">
+      <c r="A28" s="51">
         <v>5</v>
       </c>
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="44" t="s">
+      <c r="C28" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="44" t="s">
+      <c r="D28" s="53" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="15" t="s">
@@ -2538,10 +2538,10 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="42"/>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
+      <c r="A29" s="52"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
       <c r="E29" s="15" t="s">
         <v>17</v>
       </c>
@@ -2556,16 +2556,16 @@
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="41">
+      <c r="A31" s="51">
         <v>6</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="44" t="s">
+      <c r="C31" s="53" t="s">
         <v>123</v>
       </c>
-      <c r="D31" s="44" t="s">
+      <c r="D31" s="53" t="s">
         <v>50</v>
       </c>
       <c r="E31" s="14" t="s">
@@ -2576,30 +2576,30 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32" s="42"/>
-      <c r="B32" s="45"/>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
+      <c r="A32" s="52"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
       <c r="E32" s="15" t="s">
         <v>126</v>
       </c>
       <c r="F32" s="24"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33" s="42"/>
-      <c r="B33" s="45"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
+      <c r="A33" s="52"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
       <c r="E33" s="15" t="s">
         <v>124</v>
       </c>
       <c r="F33" s="24"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="43"/>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
+      <c r="A34" s="65"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
       <c r="E34" s="15" t="s">
         <v>22</v>
       </c>
@@ -2614,16 +2614,16 @@
       <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A36" s="41">
+      <c r="A36" s="51">
         <v>7</v>
       </c>
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="44" t="s">
+      <c r="C36" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="44" t="s">
+      <c r="D36" s="53" t="s">
         <v>24</v>
       </c>
       <c r="E36" s="15" t="s">
@@ -2632,20 +2632,20 @@
       <c r="F36" s="24"/>
     </row>
     <row r="37" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A37" s="42"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
+      <c r="A37" s="52"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
       <c r="E37" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F37" s="24"/>
     </row>
     <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A38" s="43"/>
-      <c r="B38" s="46"/>
-      <c r="C38" s="46"/>
-      <c r="D38" s="46"/>
+      <c r="A38" s="65"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="66"/>
       <c r="E38" s="15" t="s">
         <v>36</v>
       </c>
@@ -2660,88 +2660,88 @@
       <c r="F39" s="7"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" s="41">
+      <c r="A40" s="51">
         <v>8</v>
       </c>
-      <c r="B40" s="44" t="s">
+      <c r="B40" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="44" t="s">
+      <c r="C40" s="53" t="s">
+        <v>179</v>
+      </c>
+      <c r="D40" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="D40" s="44" t="s">
+      <c r="E40" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="E40" s="24" t="s">
+      <c r="F40" s="24"/>
+    </row>
+    <row r="41" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A41" s="52"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="F40" s="24"/>
-    </row>
-    <row r="41" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A41" s="42"/>
-      <c r="B41" s="45"/>
-      <c r="C41" s="45"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="24" t="s">
+      <c r="F41" s="24"/>
+    </row>
+    <row r="42" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A42" s="52"/>
+      <c r="B42" s="54"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="F41" s="24"/>
-    </row>
-    <row r="42" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A42" s="42"/>
-      <c r="B42" s="45"/>
-      <c r="C42" s="45"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="24" t="s">
+      <c r="F42" s="24"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" s="52"/>
+      <c r="B43" s="54"/>
+      <c r="C43" s="54"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="F42" s="24"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43" s="42"/>
-      <c r="B43" s="45"/>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="24" t="s">
+      <c r="F43" s="24"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" s="52"/>
+      <c r="B44" s="54"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="F44" s="24"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" s="52"/>
+      <c r="B45" s="54"/>
+      <c r="C45" s="54"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="F45" s="24"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46" s="52"/>
+      <c r="B46" s="54"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="F43" s="24"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44" s="42"/>
-      <c r="B44" s="45"/>
-      <c r="C44" s="45"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="F44" s="24"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A45" s="42"/>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="F45" s="24"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46" s="42"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="24" t="s">
-        <v>133</v>
-      </c>
       <c r="F46" s="24"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47" s="42"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
+      <c r="A47" s="52"/>
+      <c r="B47" s="54"/>
+      <c r="C47" s="54"/>
+      <c r="D47" s="54"/>
       <c r="E47" s="14" t="s">
         <v>85</v>
       </c>
@@ -2757,6 +2757,30 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A40:A47"/>
+    <mergeCell ref="B40:B47"/>
+    <mergeCell ref="C40:C47"/>
+    <mergeCell ref="D40:D47"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="B2:B10"/>
     <mergeCell ref="C2:C10"/>
@@ -2765,30 +2789,6 @@
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
     <mergeCell ref="D12:D16"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A40:A47"/>
-    <mergeCell ref="B40:B47"/>
-    <mergeCell ref="C40:C47"/>
-    <mergeCell ref="D40:D47"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="A36:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2815,191 +2815,191 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="39"/>
+      <c r="D2" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="75" t="s">
+      <c r="F2" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="H2" s="50" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B3" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>159</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B4" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B5" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="45" t="s">
+        <v>161</v>
+      </c>
+      <c r="H5" s="42" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B6" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>162</v>
+      </c>
+      <c r="H6" s="42" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B7" s="45"/>
+      <c r="D7" s="44"/>
+      <c r="F7" s="46" t="s">
+        <v>163</v>
+      </c>
+      <c r="H7" s="44"/>
+    </row>
+    <row r="8" spans="2:17" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B8" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="H8" s="42" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B9" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="F9" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="H9" s="42" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B10" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="F10" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="H10" s="43" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B11" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="F2" s="74" t="s">
-        <v>148</v>
-      </c>
-      <c r="H2" s="76" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B3" s="73" t="s">
-        <v>143</v>
-      </c>
-      <c r="D3" s="67" t="s">
-        <v>143</v>
-      </c>
-      <c r="F3" s="73" t="s">
-        <v>160</v>
-      </c>
-      <c r="H3" s="67" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B4" s="71" t="s">
-        <v>145</v>
-      </c>
-      <c r="D4" s="68" t="s">
-        <v>145</v>
-      </c>
-      <c r="F4" s="71" t="s">
-        <v>161</v>
-      </c>
-      <c r="H4" s="68" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B5" s="71" t="s">
-        <v>144</v>
-      </c>
-      <c r="D5" s="68" t="s">
-        <v>144</v>
-      </c>
-      <c r="F5" s="71" t="s">
-        <v>162</v>
-      </c>
-      <c r="H5" s="68" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B6" s="71" t="s">
-        <v>146</v>
-      </c>
-      <c r="D6" s="68" t="s">
-        <v>147</v>
-      </c>
-      <c r="F6" s="71" t="s">
-        <v>163</v>
-      </c>
-      <c r="H6" s="68" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B7" s="71"/>
-      <c r="D7" s="70"/>
-      <c r="F7" s="72" t="s">
-        <v>164</v>
-      </c>
-      <c r="H7" s="70"/>
-    </row>
-    <row r="8" spans="2:17" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B8" s="67" t="s">
-        <v>149</v>
-      </c>
-      <c r="D8" s="68" t="s">
-        <v>150</v>
-      </c>
-      <c r="F8" s="68" t="s">
+      <c r="F11" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="H11" s="42" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B12" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="H12" s="44" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B13" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="F13" s="45" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B14" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="F14" s="45" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B15" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="F16" s="45" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F17" s="45" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F18" s="46" t="s">
         <v>165</v>
-      </c>
-      <c r="H8" s="68" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B9" s="68" t="s">
-        <v>176</v>
-      </c>
-      <c r="D9" s="70" t="s">
-        <v>142</v>
-      </c>
-      <c r="F9" s="71" t="s">
-        <v>151</v>
-      </c>
-      <c r="H9" s="68" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B10" s="68" t="s">
-        <v>177</v>
-      </c>
-      <c r="F10" s="71" t="s">
-        <v>152</v>
-      </c>
-      <c r="H10" s="69" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B11" s="71" t="s">
-        <v>139</v>
-      </c>
-      <c r="F11" s="71" t="s">
-        <v>153</v>
-      </c>
-      <c r="H11" s="68" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B12" s="71" t="s">
-        <v>178</v>
-      </c>
-      <c r="F12" s="71" t="s">
-        <v>154</v>
-      </c>
-      <c r="H12" s="70" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B13" s="71" t="s">
-        <v>179</v>
-      </c>
-      <c r="F13" s="71" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B14" s="71" t="s">
-        <v>140</v>
-      </c>
-      <c r="F14" s="71" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B15" s="72" t="s">
-        <v>141</v>
-      </c>
-      <c r="F15" s="71" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="F16" s="71" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.45">
-      <c r="F17" s="71" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.45">
-      <c r="F18" s="72" t="s">
-        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Designed Newsagent JUnit Tests
</commit_message>
<xml_diff>
--- a/User Stories/NataliaUserStories.xlsx
+++ b/User Stories/NataliaUserStories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Palej\Desktop\Software Design with AI for Cloud\Year_3\agile-labs3\Newsagent-Project\User Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A7AEE6-62C3-4B6B-95A6-DAF763ED861B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4E2BC4-4AF2-4134-9E8D-DD0781572B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
+    <workbookView xWindow="17330" yWindow="750" windowWidth="19650" windowHeight="18430" activeTab="1" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminUserStories" sheetId="1" r:id="rId1"/>
@@ -265,9 +265,6 @@
     <t>Phone number format 0 11 222 333 (total of 10 digits)</t>
   </si>
   <si>
-    <t>Verify valid phoneNo &lt;= 13 digits</t>
-  </si>
-  <si>
     <t xml:space="preserve">Handle spaces on phoneNo and if cust enters +353 </t>
   </si>
   <si>
@@ -307,9 +304,6 @@
     <t xml:space="preserve">I want to delete customer account </t>
   </si>
   <si>
-    <t>I want to read customer account</t>
-  </si>
-  <si>
     <t>I want to print customer account</t>
   </si>
   <si>
@@ -578,6 +572,12 @@
   </si>
   <si>
     <t>+printCustomer() : void</t>
+  </si>
+  <si>
+    <t>Verify valid phoneNo &lt;= 13 characters</t>
+  </si>
+  <si>
+    <t>I want to read customer account details</t>
   </si>
 </sst>
 </file>
@@ -774,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -889,84 +889,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -991,6 +913,87 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1314,21 +1317,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB095BD-E922-497D-B7ED-398078A18E3D}">
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.9296875" style="27" customWidth="1"/>
-    <col min="2" max="2" width="13.06640625" customWidth="1"/>
-    <col min="3" max="3" width="28.46484375" customWidth="1"/>
-    <col min="4" max="4" width="35.19921875" customWidth="1"/>
-    <col min="5" max="5" width="57.86328125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="39.46484375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="2.90625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" customWidth="1"/>
+    <col min="4" max="4" width="35.1796875" customWidth="1"/>
+    <col min="5" max="5" width="57.81640625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="39.453125" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="25"/>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1346,17 +1349,17 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="41">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="51">
         <v>1</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="53" t="s">
         <v>40</v>
       </c>
       <c r="E2" s="15" t="s">
@@ -1366,11 +1369,11 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="42"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="52"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
       <c r="E3" s="15" t="s">
         <v>54</v>
       </c>
@@ -1378,47 +1381,47 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="42"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="52"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
       <c r="E4" s="15" t="s">
         <v>56</v>
       </c>
       <c r="F4" s="24"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="42"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="52"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
       <c r="E5" s="15" t="s">
         <v>57</v>
       </c>
       <c r="F5" s="24"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="42"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="52"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
       <c r="E6" s="15" t="s">
         <v>46</v>
       </c>
       <c r="F6" s="24"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="42"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="52"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
       <c r="E7" s="15" t="s">
         <v>38</v>
       </c>
       <c r="F7" s="24"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="28"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1426,87 +1429,87 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="41">
+    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="51">
         <v>2</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="44" t="s">
-        <v>91</v>
+      <c r="D9" s="53" t="s">
+        <v>89</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>47</v>
       </c>
       <c r="F9" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="52"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" s="24"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="52"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="24"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="52"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="15" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="42"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="15" t="s">
+      <c r="F12" s="24"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="52"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="F10" s="24"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="42"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" s="24"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="42"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="F12" s="24"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="42"/>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="15" t="s">
-        <v>99</v>
-      </c>
       <c r="F13" s="24"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="42"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="52"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
       <c r="E14" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F14" s="24"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="43"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="65"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
       <c r="E15" s="15" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="24"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="26"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1514,47 +1517,47 @@
       <c r="E16" s="16"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" s="41">
+    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="51">
         <v>3</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="D17" s="53" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F17" s="24" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="42"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="52"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F18" s="24"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="43"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="65"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
       <c r="E19" s="11" t="s">
         <v>58</v>
       </c>
       <c r="F19" s="24"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="26"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1562,87 +1565,87 @@
       <c r="E20" s="16"/>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="41">
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="51">
         <v>4</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="44" t="s">
+      <c r="C21" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="44" t="s">
+      <c r="D21" s="53" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>47</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" s="42"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="52"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
       <c r="E22" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F22" s="24"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="52"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" s="24"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="52"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="F22" s="24"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="42"/>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="F23" s="24"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" s="42"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="15" t="s">
-        <v>108</v>
-      </c>
       <c r="F24" s="24"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="42"/>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="52"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
       <c r="E25" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F25" s="24"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="42"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="52"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
       <c r="E26" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F26" s="24"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" s="43"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="65"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="66"/>
       <c r="E27" s="15" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="24"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="26"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -1650,45 +1653,45 @@
       <c r="E28" s="16"/>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="41">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="51">
         <v>5</v>
       </c>
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="44" t="s">
+      <c r="C29" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="44" t="s">
-        <v>92</v>
+      <c r="D29" s="53" t="s">
+        <v>90</v>
       </c>
       <c r="E29" s="15" t="s">
         <v>47</v>
       </c>
       <c r="F29" s="24"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" s="42"/>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="52"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
       <c r="E30" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F30" s="24"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31" s="43"/>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="65"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
       <c r="E31" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F31" s="24"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="26"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -1696,37 +1699,37 @@
       <c r="E32" s="16"/>
       <c r="F32" s="7"/>
     </row>
-    <row r="33" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A33" s="41">
+    <row r="33" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" s="51">
         <v>6</v>
       </c>
-      <c r="B33" s="44" t="s">
+      <c r="B33" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="44" t="s">
+      <c r="C33" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="44" t="s">
+      <c r="D33" s="53" t="s">
         <v>16</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F33" s="24" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="43"/>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="65"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
       <c r="E34" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F34" s="24"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="29"/>
       <c r="B35" s="20"/>
       <c r="C35" s="20"/>
@@ -1734,87 +1737,87 @@
       <c r="E35" s="21"/>
       <c r="F35" s="7"/>
     </row>
-    <row r="36" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="47">
+    <row r="36" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="76">
         <v>7</v>
       </c>
-      <c r="B36" s="48" t="s">
+      <c r="B36" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="48" t="s">
+      <c r="C36" s="72" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="72" t="s">
         <v>77</v>
       </c>
-      <c r="D36" s="48" t="s">
+      <c r="E36" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F36" s="53" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="76"/>
+      <c r="B37" s="72"/>
+      <c r="C37" s="72"/>
+      <c r="D37" s="72"/>
+      <c r="E37" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="E36" s="24" t="s">
+      <c r="F37" s="54"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="76"/>
+      <c r="B38" s="72"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="72"/>
+      <c r="E38" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F38" s="66"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="76"/>
+      <c r="B39" s="72"/>
+      <c r="C39" s="72"/>
+      <c r="D39" s="72"/>
+      <c r="E39" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F39" s="24"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="76"/>
+      <c r="B40" s="72"/>
+      <c r="C40" s="72"/>
+      <c r="D40" s="72"/>
+      <c r="E40" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" s="24"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="76"/>
+      <c r="B41" s="72"/>
+      <c r="C41" s="72"/>
+      <c r="D41" s="72"/>
+      <c r="E41" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="F41" s="24"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="76"/>
+      <c r="B42" s="72"/>
+      <c r="C42" s="72"/>
+      <c r="D42" s="72"/>
+      <c r="E42" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="F36" s="44" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37" s="47"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
-      <c r="E37" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="F37" s="45"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38" s="47"/>
-      <c r="B38" s="48"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="48"/>
-      <c r="E38" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F38" s="46"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39" s="47"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="F39" s="24"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" s="47"/>
-      <c r="B40" s="48"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="48"/>
-      <c r="E40" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="F40" s="24"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" s="47"/>
-      <c r="B41" s="48"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F41" s="24"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42" s="47"/>
-      <c r="B42" s="48"/>
-      <c r="C42" s="48"/>
-      <c r="D42" s="48"/>
-      <c r="E42" s="24" t="s">
-        <v>85</v>
-      </c>
       <c r="F42" s="24"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="30"/>
       <c r="B43" s="22"/>
       <c r="C43" s="22"/>
@@ -1822,73 +1825,73 @@
       <c r="E43" s="23"/>
       <c r="F43" s="7"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="31"/>
       <c r="B44" s="19"/>
       <c r="C44" s="19"/>
       <c r="D44" s="19"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="31"/>
       <c r="B45" s="19"/>
       <c r="C45" s="19"/>
       <c r="D45" s="19"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="31"/>
       <c r="B46" s="19"/>
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="31"/>
       <c r="B47" s="19"/>
       <c r="C47" s="19"/>
       <c r="D47" s="19"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="31"/>
       <c r="B48" s="19"/>
       <c r="C48" s="19"/>
       <c r="D48" s="19"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="31"/>
       <c r="B49" s="19"/>
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="31"/>
       <c r="B50" s="19"/>
       <c r="C50" s="19"/>
       <c r="D50" s="19"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="31"/>
       <c r="B51" s="19"/>
       <c r="C51" s="19"/>
       <c r="D51" s="19"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="31"/>
       <c r="B52" s="19"/>
       <c r="C52" s="19"/>
       <c r="D52" s="19"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="31"/>
       <c r="B53" s="19"/>
       <c r="C53" s="19"/>
       <c r="D53" s="19"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="31"/>
       <c r="B54" s="19"/>
       <c r="C54" s="19"/>
       <c r="D54" s="19"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="28"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1896,17 +1899,17 @@
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
     </row>
-    <row r="56" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="52">
+    <row r="56" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="67">
         <v>12</v>
       </c>
-      <c r="B56" s="49" t="s">
+      <c r="B56" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C56" s="49" t="s">
+      <c r="C56" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="D56" s="49" t="s">
+      <c r="D56" s="73" t="s">
         <v>44</v>
       </c>
       <c r="E56" s="17" t="s">
@@ -1914,37 +1917,37 @@
       </c>
       <c r="F56" s="36"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A57" s="53"/>
-      <c r="B57" s="50"/>
-      <c r="C57" s="50"/>
-      <c r="D57" s="50"/>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" s="68"/>
+      <c r="B57" s="74"/>
+      <c r="C57" s="74"/>
+      <c r="D57" s="74"/>
       <c r="E57" s="17" t="s">
         <v>42</v>
       </c>
       <c r="F57" s="36"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A58" s="53"/>
-      <c r="B58" s="50"/>
-      <c r="C58" s="50"/>
-      <c r="D58" s="50"/>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" s="68"/>
+      <c r="B58" s="74"/>
+      <c r="C58" s="74"/>
+      <c r="D58" s="74"/>
       <c r="E58" s="17" t="s">
         <v>37</v>
       </c>
       <c r="F58" s="36"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A59" s="54"/>
-      <c r="B59" s="51"/>
-      <c r="C59" s="51"/>
-      <c r="D59" s="51"/>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" s="69"/>
+      <c r="B59" s="75"/>
+      <c r="C59" s="75"/>
+      <c r="D59" s="75"/>
       <c r="E59" s="17" t="s">
         <v>38</v>
       </c>
       <c r="F59" s="36"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="32"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
@@ -1952,7 +1955,7 @@
       <c r="E60" s="16"/>
       <c r="F60" s="7"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="26"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
@@ -1960,45 +1963,45 @@
       <c r="E70" s="16"/>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A71" s="57">
+    <row r="71" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A71" s="59">
         <v>10</v>
       </c>
-      <c r="B71" s="60" t="s">
+      <c r="B71" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="C71" s="60" t="s">
+      <c r="C71" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="D71" s="60" t="s">
+      <c r="D71" s="62" t="s">
         <v>33</v>
       </c>
       <c r="E71" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F71" s="55" t="s">
+      <c r="F71" s="70" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A72" s="58"/>
-      <c r="B72" s="61"/>
-      <c r="C72" s="61"/>
-      <c r="D72" s="61"/>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72" s="60"/>
+      <c r="B72" s="63"/>
+      <c r="C72" s="63"/>
+      <c r="D72" s="63"/>
       <c r="E72" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="F72" s="56"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A73" s="59"/>
-      <c r="B73" s="62"/>
-      <c r="C73" s="62"/>
-      <c r="D73" s="62"/>
+      <c r="F72" s="71"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A73" s="61"/>
+      <c r="B73" s="64"/>
+      <c r="C73" s="64"/>
+      <c r="D73" s="64"/>
       <c r="E73" s="6"/>
       <c r="F73" s="37"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="26"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
@@ -2006,17 +2009,17 @@
       <c r="E74" s="16"/>
       <c r="F74" s="7"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A75" s="57">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A75" s="59">
         <v>11</v>
       </c>
-      <c r="B75" s="60" t="s">
+      <c r="B75" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="C75" s="60" t="s">
+      <c r="C75" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="D75" s="60" t="s">
+      <c r="D75" s="62" t="s">
         <v>26</v>
       </c>
       <c r="E75" s="18" t="s">
@@ -2024,67 +2027,67 @@
       </c>
       <c r="F75" s="37"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A76" s="58"/>
-      <c r="B76" s="61"/>
-      <c r="C76" s="61"/>
-      <c r="D76" s="61"/>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A76" s="60"/>
+      <c r="B76" s="63"/>
+      <c r="C76" s="63"/>
+      <c r="D76" s="63"/>
       <c r="E76" s="18" t="s">
         <v>28</v>
       </c>
       <c r="F76" s="37"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A77" s="59"/>
-      <c r="B77" s="62"/>
-      <c r="C77" s="62"/>
-      <c r="D77" s="62"/>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A77" s="61"/>
+      <c r="B77" s="64"/>
+      <c r="C77" s="64"/>
+      <c r="D77" s="64"/>
       <c r="E77" s="18" t="s">
         <v>29</v>
       </c>
       <c r="F77" s="37"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="26"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="9"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A81" s="65">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" s="57">
         <v>6</v>
       </c>
-      <c r="B81" s="63" t="s">
+      <c r="B81" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C81" s="63" t="s">
+      <c r="C81" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="D81" s="63" t="s">
+      <c r="D81" s="55" t="s">
         <v>19</v>
       </c>
       <c r="E81" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A82" s="66"/>
-      <c r="B82" s="64"/>
-      <c r="C82" s="64"/>
-      <c r="D82" s="64"/>
+    <row r="82" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A82" s="58"/>
+      <c r="B82" s="56"/>
+      <c r="C82" s="56"/>
+      <c r="D82" s="56"/>
       <c r="E82" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="26"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="9"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="33">
         <v>7</v>
       </c>
@@ -2101,7 +2104,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="34"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -2110,7 +2113,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="34"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -2119,7 +2122,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="35"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
@@ -2128,7 +2131,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="26"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2137,6 +2140,36 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A36:A42"/>
+    <mergeCell ref="B36:B42"/>
+    <mergeCell ref="C36:C42"/>
+    <mergeCell ref="D36:D42"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="C71:C73"/>
+    <mergeCell ref="D71:D73"/>
+    <mergeCell ref="B21:B27"/>
+    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C21:C27"/>
+    <mergeCell ref="D21:D27"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D33:D34"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="C2:C7"/>
@@ -2153,36 +2186,6 @@
     <mergeCell ref="B9:B15"/>
     <mergeCell ref="C9:C15"/>
     <mergeCell ref="D9:D15"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C21:C27"/>
-    <mergeCell ref="D21:D27"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="B21:B27"/>
-    <mergeCell ref="A21:A27"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="C71:C73"/>
-    <mergeCell ref="D71:D73"/>
-    <mergeCell ref="C36:C42"/>
-    <mergeCell ref="D36:D42"/>
-    <mergeCell ref="F36:F38"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="D56:D59"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A36:A42"/>
-    <mergeCell ref="B36:B42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2193,21 +2196,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526350BB-95BB-4BF1-93A5-0B30D123D1AA}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36:C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.9296875" style="27" customWidth="1"/>
-    <col min="2" max="2" width="23.46484375" customWidth="1"/>
-    <col min="3" max="3" width="27.86328125" customWidth="1"/>
+    <col min="1" max="1" width="2.90625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" customWidth="1"/>
+    <col min="3" max="3" width="27.81640625" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="52.59765625" customWidth="1"/>
-    <col min="6" max="6" width="44.19921875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.6328125" customWidth="1"/>
+    <col min="6" max="6" width="44.1796875" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="25"/>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -2225,17 +2228,17 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="41">
+    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="51">
         <v>1</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="44" t="s">
+      <c r="C2" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="53" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="14" t="s">
@@ -2245,89 +2248,89 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="42"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="15" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="52"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="77" t="s">
         <v>67</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="42"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="52"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="77" t="s">
         <v>71</v>
       </c>
       <c r="F4" s="24"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="42"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="15" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="52"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="77" t="s">
         <v>72</v>
       </c>
       <c r="F5" s="24"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="42"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="15" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="52"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="77" t="s">
         <v>73</v>
       </c>
       <c r="F6" s="24"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="42"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="15" t="s">
-        <v>75</v>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="52"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="77" t="s">
+        <v>178</v>
       </c>
       <c r="F7" s="24"/>
     </row>
-    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="42"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="15" t="s">
+    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="52"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="77" t="s">
         <v>68</v>
       </c>
       <c r="F8" s="24"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="42"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="15" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="52"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="77" t="s">
         <v>69</v>
       </c>
       <c r="F9" s="24"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="43"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="15" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="65"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="77" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="24"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="26"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -2335,67 +2338,67 @@
       <c r="E11" s="16"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="41">
+    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="51">
         <v>2</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="D12" s="44" t="s">
+      <c r="C12" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="53" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F12" s="24" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="42"/>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="52"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
       <c r="E13" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="F13" s="24"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="52"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="F14" s="24"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="52"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="F13" s="24"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="42"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="F14" s="24"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="42"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="15" t="s">
-        <v>114</v>
-      </c>
       <c r="F15" s="24"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="43"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="65"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
       <c r="E16" s="11" t="s">
         <v>58</v>
       </c>
       <c r="F16" s="24"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="26"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -2403,77 +2406,77 @@
       <c r="E17" s="16"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="41">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="51">
         <v>3</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" s="44" t="s">
+      <c r="C18" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="53" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="42"/>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="52"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
       <c r="E19" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F19" s="24"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" s="42"/>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
+    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="52"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
       <c r="E20" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="24"/>
+    </row>
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="52"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="24"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="52"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" s="24"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="52"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="F20" s="24"/>
-    </row>
-    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="42"/>
-      <c r="B21" s="45"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="F21" s="24"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" s="42"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="F22" s="24"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="42"/>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="15" t="s">
-        <v>118</v>
-      </c>
       <c r="F23" s="24"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="26"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -2481,35 +2484,35 @@
       <c r="E24" s="16"/>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A25" s="41">
+    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="51">
         <v>4</v>
       </c>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25" s="44" t="s">
+      <c r="C25" s="53" t="s">
+        <v>179</v>
+      </c>
+      <c r="D25" s="53" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F25" s="24"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="42"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="52"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
       <c r="E26" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F26" s="24"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="26"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -2517,37 +2520,37 @@
       <c r="E27" s="16"/>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A28" s="41">
+    <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="51">
         <v>5</v>
       </c>
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="44" t="s">
+      <c r="C28" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="53" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F28" s="24" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="42"/>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="52"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
       <c r="E29" s="15" t="s">
         <v>17</v>
       </c>
       <c r="F29" s="24"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="26"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -2555,57 +2558,57 @@
       <c r="E30" s="16"/>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="41">
+    <row r="31" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="51">
         <v>6</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="D31" s="44" t="s">
+      <c r="C31" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="53" t="s">
         <v>50</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>47</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32" s="42"/>
-      <c r="B32" s="45"/>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="52"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
       <c r="E32" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F32" s="24"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33" s="42"/>
-      <c r="B33" s="45"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="52"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
       <c r="E33" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F33" s="24"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="43"/>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="65"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
       <c r="E34" s="15" t="s">
         <v>22</v>
       </c>
       <c r="F34" s="24"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="26"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -2613,17 +2616,17 @@
       <c r="E35" s="16"/>
       <c r="F35" s="7"/>
     </row>
-    <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A36" s="41">
+    <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="51">
         <v>7</v>
       </c>
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="44" t="s">
+      <c r="C36" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="44" t="s">
+      <c r="D36" s="53" t="s">
         <v>24</v>
       </c>
       <c r="E36" s="15" t="s">
@@ -2631,27 +2634,27 @@
       </c>
       <c r="F36" s="24"/>
     </row>
-    <row r="37" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A37" s="42"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
+    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" s="52"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
       <c r="E37" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F37" s="24"/>
     </row>
-    <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A38" s="43"/>
-      <c r="B38" s="46"/>
-      <c r="C38" s="46"/>
-      <c r="D38" s="46"/>
+    <row r="38" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="65"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="66"/>
       <c r="E38" s="15" t="s">
         <v>36</v>
       </c>
       <c r="F38" s="24"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="26"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -2659,95 +2662,95 @@
       <c r="E39" s="16"/>
       <c r="F39" s="7"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" s="41">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="51">
         <v>8</v>
       </c>
-      <c r="B40" s="44" t="s">
+      <c r="B40" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="44" t="s">
+      <c r="C40" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="D40" s="53" t="s">
+        <v>126</v>
+      </c>
+      <c r="E40" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="D40" s="44" t="s">
+      <c r="F40" s="24"/>
+    </row>
+    <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="52"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="E40" s="24" t="s">
+      <c r="F41" s="24"/>
+    </row>
+    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="52"/>
+      <c r="B42" s="54"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="F40" s="24"/>
-    </row>
-    <row r="41" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A41" s="42"/>
-      <c r="B41" s="45"/>
-      <c r="C41" s="45"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="24" t="s">
+      <c r="F42" s="24"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="52"/>
+      <c r="B43" s="54"/>
+      <c r="C43" s="54"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="F41" s="24"/>
-    </row>
-    <row r="42" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A42" s="42"/>
-      <c r="B42" s="45"/>
-      <c r="C42" s="45"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="24" t="s">
+      <c r="F43" s="24"/>
+    </row>
+    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="52"/>
+      <c r="B44" s="54"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F44" s="24"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="52"/>
+      <c r="B45" s="54"/>
+      <c r="C45" s="54"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="F45" s="24"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="52"/>
+      <c r="B46" s="54"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="F42" s="24"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43" s="42"/>
-      <c r="B43" s="45"/>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F43" s="24"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44" s="42"/>
-      <c r="B44" s="45"/>
-      <c r="C44" s="45"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="F44" s="24"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A45" s="42"/>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="F45" s="24"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46" s="42"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="24" t="s">
-        <v>133</v>
-      </c>
       <c r="F46" s="24"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47" s="42"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" s="52"/>
+      <c r="B47" s="54"/>
+      <c r="C47" s="54"/>
+      <c r="D47" s="54"/>
       <c r="E47" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F47" s="24"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="26"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -2757,6 +2760,30 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A40:A47"/>
+    <mergeCell ref="B40:B47"/>
+    <mergeCell ref="C40:C47"/>
+    <mergeCell ref="D40:D47"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="B2:B10"/>
     <mergeCell ref="C2:C10"/>
@@ -2765,30 +2792,6 @@
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
     <mergeCell ref="D12:D16"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A40:A47"/>
-    <mergeCell ref="B40:B47"/>
-    <mergeCell ref="C40:C47"/>
-    <mergeCell ref="D40:D47"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="A36:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2802,204 +2805,204 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.06640625" customWidth="1"/>
-    <col min="2" max="2" width="37.46484375" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.06640625" style="38" customWidth="1"/>
-    <col min="4" max="4" width="41.73046875" style="40" customWidth="1"/>
-    <col min="5" max="5" width="3.796875" style="38" customWidth="1"/>
-    <col min="6" max="6" width="37.9296875" customWidth="1"/>
-    <col min="7" max="7" width="3.59765625" customWidth="1"/>
-    <col min="8" max="8" width="40.59765625" customWidth="1"/>
+    <col min="1" max="1" width="2.08984375" customWidth="1"/>
+    <col min="2" max="2" width="37.453125" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.08984375" style="38" customWidth="1"/>
+    <col min="4" max="4" width="41.7265625" style="40" customWidth="1"/>
+    <col min="5" max="5" width="3.81640625" style="38" customWidth="1"/>
+    <col min="6" max="6" width="37.90625" customWidth="1"/>
+    <col min="7" max="7" width="3.6328125" customWidth="1"/>
+    <col min="8" max="8" width="40.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B2" s="74" t="s">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B2" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="39"/>
+      <c r="D2" s="49" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="H2" s="50" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B3" s="47" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B4" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="F4" s="45" t="s">
+        <v>159</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B5" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="F5" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="H5" s="42" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B6" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>161</v>
+      </c>
+      <c r="H6" s="42" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B7" s="45"/>
+      <c r="D7" s="44"/>
+      <c r="F7" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="H7" s="44"/>
+    </row>
+    <row r="8" spans="2:17" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="41" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>163</v>
+      </c>
+      <c r="H8" s="42" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="F9" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="H9" s="42" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="F10" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="H10" s="43" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B11" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="75" t="s">
+      <c r="F11" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="H11" s="42" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B12" s="45" t="s">
+        <v>176</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="H12" s="44" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B13" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="F13" s="45" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B14" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="F2" s="74" t="s">
-        <v>148</v>
-      </c>
-      <c r="H2" s="76" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B3" s="73" t="s">
-        <v>143</v>
-      </c>
-      <c r="D3" s="67" t="s">
-        <v>143</v>
-      </c>
-      <c r="F3" s="73" t="s">
-        <v>160</v>
-      </c>
-      <c r="H3" s="67" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B4" s="71" t="s">
-        <v>145</v>
-      </c>
-      <c r="D4" s="68" t="s">
-        <v>145</v>
-      </c>
-      <c r="F4" s="71" t="s">
-        <v>161</v>
-      </c>
-      <c r="H4" s="68" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B5" s="71" t="s">
-        <v>144</v>
-      </c>
-      <c r="D5" s="68" t="s">
-        <v>144</v>
-      </c>
-      <c r="F5" s="71" t="s">
-        <v>162</v>
-      </c>
-      <c r="H5" s="68" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B6" s="71" t="s">
-        <v>146</v>
-      </c>
-      <c r="D6" s="68" t="s">
-        <v>147</v>
-      </c>
-      <c r="F6" s="71" t="s">
-        <v>163</v>
-      </c>
-      <c r="H6" s="68" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B7" s="71"/>
-      <c r="D7" s="70"/>
-      <c r="F7" s="72" t="s">
+      <c r="F14" s="45" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B15" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="F16" s="45" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F17" s="45" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F18" s="46" t="s">
         <v>164</v>
-      </c>
-      <c r="H7" s="70"/>
-    </row>
-    <row r="8" spans="2:17" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B8" s="67" t="s">
-        <v>149</v>
-      </c>
-      <c r="D8" s="68" t="s">
-        <v>150</v>
-      </c>
-      <c r="F8" s="68" t="s">
-        <v>165</v>
-      </c>
-      <c r="H8" s="68" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B9" s="68" t="s">
-        <v>176</v>
-      </c>
-      <c r="D9" s="70" t="s">
-        <v>142</v>
-      </c>
-      <c r="F9" s="71" t="s">
-        <v>151</v>
-      </c>
-      <c r="H9" s="68" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B10" s="68" t="s">
-        <v>177</v>
-      </c>
-      <c r="F10" s="71" t="s">
-        <v>152</v>
-      </c>
-      <c r="H10" s="69" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B11" s="71" t="s">
-        <v>139</v>
-      </c>
-      <c r="F11" s="71" t="s">
-        <v>153</v>
-      </c>
-      <c r="H11" s="68" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B12" s="71" t="s">
-        <v>178</v>
-      </c>
-      <c r="F12" s="71" t="s">
-        <v>154</v>
-      </c>
-      <c r="H12" s="70" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B13" s="71" t="s">
-        <v>179</v>
-      </c>
-      <c r="F13" s="71" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B14" s="71" t="s">
-        <v>140</v>
-      </c>
-      <c r="F14" s="71" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B15" s="72" t="s">
-        <v>141</v>
-      </c>
-      <c r="F15" s="71" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="F16" s="71" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.45">
-      <c r="F17" s="71" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.45">
-      <c r="F18" s="72" t="s">
-        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished JUnit Tests for Cust,Admin,Newsagent
</commit_message>
<xml_diff>
--- a/User Stories/NataliaUserStories.xlsx
+++ b/User Stories/NataliaUserStories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Palej\Desktop\Software Design with AI for Cloud\Year_3\agile-labs3\Newsagent-Project\User Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C68B71C-CBB1-497C-88E9-DAC19F67A41B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C589FF87-38F8-4E12-A7C2-07724521BB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="184">
   <si>
     <t>As an admin</t>
   </si>
@@ -266,9 +266,6 @@
   </si>
   <si>
     <t>Verify if no role specified, user cannot print/generateInvoice()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify admin can revoke/change role </t>
   </si>
   <si>
     <t>Verify system checks if role = Driver or role = Newsagent</t>
@@ -894,6 +891,66 @@
     <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -901,73 +958,13 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1289,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB095BD-E922-497D-B7ED-398078A18E3D}">
-  <dimension ref="A1:F83"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1327,13 +1324,13 @@
       <c r="A2" s="47">
         <v>1</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="50" t="s">
-        <v>173</v>
-      </c>
-      <c r="D2" s="50" t="s">
+      <c r="C2" s="49" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" s="49" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="15" t="s">
@@ -1345,9 +1342,9 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="48"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
       <c r="E3" s="15" t="s">
         <v>47</v>
       </c>
@@ -1357,9 +1354,9 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="48"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
       <c r="E4" s="15" t="s">
         <v>49</v>
       </c>
@@ -1367,9 +1364,9 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="48"/>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
       <c r="E5" s="15" t="s">
         <v>50</v>
       </c>
@@ -1377,29 +1374,29 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="48"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
       <c r="E6" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="48"/>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
       <c r="E7" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="48"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
       <c r="E8" s="15" t="s">
         <v>37</v>
       </c>
@@ -1417,77 +1414,77 @@
       <c r="A10" s="47">
         <v>2</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="50" t="s">
-        <v>84</v>
+      <c r="D10" s="49" t="s">
+        <v>83</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="48"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
       <c r="E11" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="48"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
       <c r="E12" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="48"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
       <c r="E13" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="48"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
       <c r="E14" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="48"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
       <c r="E15" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="49"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
       <c r="E16" s="15" t="s">
         <v>14</v>
       </c>
@@ -1505,17 +1502,17 @@
       <c r="A18" s="47">
         <v>3</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="50" t="s">
+      <c r="D18" s="49" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F18" s="21" t="s">
         <v>52</v>
@@ -1523,19 +1520,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="48"/>
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
       <c r="E19" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" s="49"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
       <c r="E20" s="11" t="s">
         <v>51</v>
       </c>
@@ -1553,77 +1550,77 @@
       <c r="A22" s="47">
         <v>4</v>
       </c>
-      <c r="B22" s="50" t="s">
+      <c r="B22" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="50" t="s">
+      <c r="C22" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="50" t="s">
+      <c r="D22" s="49" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>40</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="48"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
       <c r="E23" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F23" s="21"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="48"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
       <c r="E24" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F24" s="21"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="48"/>
-      <c r="B25" s="51"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
       <c r="E25" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F25" s="21"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="48"/>
-      <c r="B26" s="51"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
       <c r="E26" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F26" s="21"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="48"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
       <c r="E27" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F27" s="21"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" s="49"/>
-      <c r="B28" s="52"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="52"/>
+      <c r="A28" s="61"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
       <c r="E28" s="15" t="s">
         <v>11</v>
       </c>
@@ -1641,14 +1638,14 @@
       <c r="A30" s="47">
         <v>5</v>
       </c>
-      <c r="B30" s="50" t="s">
+      <c r="B30" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="50" t="s">
+      <c r="C30" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="50" t="s">
-        <v>85</v>
+      <c r="D30" s="49" t="s">
+        <v>84</v>
       </c>
       <c r="E30" s="15" t="s">
         <v>40</v>
@@ -1657,21 +1654,21 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="48"/>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
       <c r="E31" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F31" s="21"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" s="61"/>
+      <c r="B32" s="62"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="F31" s="21"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32" s="49"/>
-      <c r="B32" s="52"/>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="15" t="s">
-        <v>98</v>
       </c>
       <c r="F32" s="21"/>
     </row>
@@ -1687,29 +1684,29 @@
       <c r="A34" s="47">
         <v>6</v>
       </c>
-      <c r="B34" s="50" t="s">
+      <c r="B34" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="50" t="s">
+      <c r="C34" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="50" t="s">
+      <c r="D34" s="49" t="s">
         <v>16</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35" s="49"/>
-      <c r="B35" s="52"/>
-      <c r="C35" s="52"/>
-      <c r="D35" s="52"/>
+      <c r="A35" s="61"/>
+      <c r="B35" s="62"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
       <c r="E35" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F35" s="21"/>
     </row>
@@ -1722,240 +1719,240 @@
       <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="53">
+      <c r="A37" s="66">
         <v>7</v>
       </c>
-      <c r="B37" s="54" t="s">
+      <c r="B37" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="54" t="s">
+      <c r="C37" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="54" t="s">
+      <c r="D37" s="65" t="s">
         <v>71</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="F37" s="50" t="s">
-        <v>128</v>
+        <v>76</v>
+      </c>
+      <c r="F37" s="49" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38" s="53"/>
-      <c r="B38" s="54"/>
-      <c r="C38" s="54"/>
-      <c r="D38" s="54"/>
+      <c r="A38" s="66"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
       <c r="E38" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F38" s="51"/>
+      <c r="F38" s="50"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39" s="53"/>
-      <c r="B39" s="54"/>
-      <c r="C39" s="54"/>
-      <c r="D39" s="54"/>
+      <c r="A39" s="66"/>
+      <c r="B39" s="65"/>
+      <c r="C39" s="65"/>
+      <c r="D39" s="65"/>
       <c r="E39" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="F39" s="52"/>
+      <c r="F39" s="62"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" s="53"/>
-      <c r="B40" s="54"/>
-      <c r="C40" s="54"/>
-      <c r="D40" s="54"/>
+      <c r="A40" s="66"/>
+      <c r="B40" s="65"/>
+      <c r="C40" s="65"/>
+      <c r="D40" s="65"/>
       <c r="E40" s="21" t="s">
         <v>74</v>
       </c>
       <c r="F40" s="21"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" s="53"/>
-      <c r="B41" s="54"/>
-      <c r="C41" s="54"/>
-      <c r="D41" s="54"/>
+      <c r="A41" s="66"/>
+      <c r="B41" s="65"/>
+      <c r="C41" s="65"/>
+      <c r="D41" s="65"/>
       <c r="E41" s="21" t="s">
         <v>75</v>
       </c>
       <c r="F41" s="21"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42" s="53"/>
-      <c r="B42" s="54"/>
-      <c r="C42" s="54"/>
-      <c r="D42" s="54"/>
+      <c r="A42" s="66"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="65"/>
       <c r="E42" s="21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F42" s="21"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43" s="53"/>
-      <c r="B43" s="54"/>
-      <c r="C43" s="54"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="F43" s="21"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44" s="27"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="67"/>
-      <c r="D44" s="67"/>
-      <c r="E44" s="68"/>
-      <c r="F44" s="7"/>
-    </row>
-    <row r="45" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A45" s="46">
+      <c r="A43" s="27"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="45"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="67">
         <v>8</v>
       </c>
-      <c r="B45" s="45" t="s">
+      <c r="B44" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C45" s="45" t="s">
+      <c r="C44" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="D44" s="49" t="s">
         <v>175</v>
       </c>
-      <c r="D45" s="45" t="s">
-        <v>176</v>
-      </c>
+      <c r="E44" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F44" s="21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" s="68"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
       <c r="E45" s="21" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F45" s="21" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46" s="46"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
+      <c r="A46" s="68"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="50"/>
       <c r="E46" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F46" s="21" t="s">
-        <v>180</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F46" s="21"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47" s="46"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
+      <c r="A47" s="68"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
       <c r="E47" s="21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F47" s="21"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A48" s="46"/>
-      <c r="B48" s="45"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
+      <c r="A48" s="68"/>
+      <c r="B48" s="50"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
       <c r="E48" s="21" t="s">
-        <v>50</v>
+        <v>176</v>
       </c>
       <c r="F48" s="21"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A49" s="46"/>
-      <c r="B49" s="45"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
+      <c r="A49" s="68"/>
+      <c r="B49" s="50"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="50"/>
       <c r="E49" s="21" t="s">
         <v>177</v>
       </c>
       <c r="F49" s="21"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A50" s="46"/>
-      <c r="B50" s="45"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
+      <c r="A50" s="69"/>
+      <c r="B50" s="62"/>
+      <c r="C50" s="62"/>
+      <c r="D50" s="62"/>
       <c r="E50" s="21" t="s">
-        <v>178</v>
+        <v>37</v>
       </c>
       <c r="F50" s="21"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A51" s="46"/>
-      <c r="B51" s="45"/>
+      <c r="A51" s="27"/>
+      <c r="B51" s="20"/>
       <c r="C51" s="45"/>
       <c r="D51" s="45"/>
-      <c r="E51" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="F51" s="21"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A52" s="27"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="67"/>
-      <c r="D52" s="67"/>
-      <c r="E52" s="68"/>
-      <c r="F52" s="7"/>
+      <c r="A52" s="67">
+        <v>9</v>
+      </c>
+      <c r="B52" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="49" t="s">
+        <v>182</v>
+      </c>
+      <c r="D52" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A53" s="46">
-        <v>9</v>
-      </c>
-      <c r="B53" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="C53" s="45" t="s">
-        <v>183</v>
-      </c>
-      <c r="D53" s="45" t="s">
-        <v>184</v>
-      </c>
+      <c r="A53" s="68"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="50"/>
       <c r="E53" s="21" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F53" s="21" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A54" s="46"/>
-      <c r="B54" s="45"/>
-      <c r="C54" s="45"/>
-      <c r="D54" s="45"/>
+      <c r="A54" s="68"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="50"/>
       <c r="E54" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F54" s="21" t="s">
-        <v>182</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F54" s="21"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A55" s="46"/>
-      <c r="B55" s="45"/>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
+      <c r="A55" s="68"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="50"/>
       <c r="E55" s="21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F55" s="21"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A56" s="69"/>
-      <c r="B56" s="45"/>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45"/>
+      <c r="A56" s="68"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="50"/>
       <c r="E56" s="21" t="s">
-        <v>50</v>
+        <v>176</v>
       </c>
       <c r="F56" s="21"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A57" s="69"/>
-      <c r="B57" s="45"/>
-      <c r="C57" s="45"/>
-      <c r="D57" s="45"/>
+      <c r="A57" s="68"/>
+      <c r="B57" s="50"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="50"/>
       <c r="E57" s="21" t="s">
         <v>177</v>
       </c>
@@ -1963,179 +1960,178 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="69"/>
-      <c r="B58" s="45"/>
-      <c r="C58" s="45"/>
-      <c r="D58" s="45"/>
+      <c r="B58" s="62"/>
+      <c r="C58" s="62"/>
+      <c r="D58" s="62"/>
       <c r="E58" s="21" t="s">
-        <v>178</v>
+        <v>37</v>
       </c>
       <c r="F58" s="21"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A59" s="69"/>
-      <c r="B59" s="45"/>
+      <c r="A59" s="27"/>
+      <c r="B59" s="20"/>
       <c r="C59" s="45"/>
       <c r="D59" s="45"/>
-      <c r="E59" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="F59" s="21"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A60" s="27"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="67"/>
-      <c r="D60" s="67"/>
-      <c r="E60" s="68"/>
-      <c r="F60" s="7"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A65" s="23"/>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="7"/>
-    </row>
-    <row r="66" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A66" s="57">
+      <c r="E59" s="46"/>
+      <c r="F59" s="7"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64" s="23"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="7"/>
+    </row>
+    <row r="65" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A65" s="55">
         <v>10</v>
       </c>
-      <c r="B66" s="60" t="s">
+      <c r="B65" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="C66" s="60" t="s">
+      <c r="C65" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="D66" s="60" t="s">
+      <c r="D65" s="58" t="s">
         <v>33</v>
       </c>
+      <c r="E65" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F65" s="63" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A66" s="56"/>
+      <c r="B66" s="59"/>
+      <c r="C66" s="59"/>
+      <c r="D66" s="59"/>
       <c r="E66" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F66" s="55" t="s">
-        <v>58</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="F66" s="64"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A67" s="58"/>
-      <c r="B67" s="61"/>
-      <c r="C67" s="61"/>
-      <c r="D67" s="61"/>
-      <c r="E67" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F67" s="56"/>
+      <c r="A67" s="57"/>
+      <c r="B67" s="60"/>
+      <c r="C67" s="60"/>
+      <c r="D67" s="60"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="31"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A68" s="59"/>
-      <c r="B68" s="62"/>
-      <c r="C68" s="62"/>
-      <c r="D68" s="62"/>
-      <c r="E68" s="6"/>
-      <c r="F68" s="31"/>
+      <c r="A68" s="23"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="7"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A69" s="23"/>
-      <c r="B69" s="8"/>
-      <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="16"/>
-      <c r="F69" s="7"/>
+      <c r="A69" s="55">
+        <v>11</v>
+      </c>
+      <c r="B69" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="C69" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="D69" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="E69" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F69" s="31"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A70" s="57">
-        <v>11</v>
-      </c>
-      <c r="B70" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="C70" s="60" t="s">
-        <v>42</v>
-      </c>
-      <c r="D70" s="60" t="s">
-        <v>26</v>
-      </c>
+      <c r="A70" s="56"/>
+      <c r="B70" s="59"/>
+      <c r="C70" s="59"/>
+      <c r="D70" s="59"/>
       <c r="E70" s="17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F70" s="31"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A71" s="58"/>
-      <c r="B71" s="61"/>
-      <c r="C71" s="61"/>
-      <c r="D71" s="61"/>
+      <c r="A71" s="57"/>
+      <c r="B71" s="60"/>
+      <c r="C71" s="60"/>
+      <c r="D71" s="60"/>
       <c r="E71" s="17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F71" s="31"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A72" s="59"/>
-      <c r="B72" s="62"/>
-      <c r="C72" s="62"/>
-      <c r="D72" s="62"/>
-      <c r="E72" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F72" s="31"/>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A74" s="23"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="9"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A75" s="23"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="9"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A76" s="65">
+      <c r="A75" s="53">
         <v>6</v>
       </c>
-      <c r="B76" s="63" t="s">
+      <c r="B75" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C76" s="63" t="s">
+      <c r="C75" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="D76" s="63" t="s">
+      <c r="D75" s="51" t="s">
         <v>19</v>
       </c>
+      <c r="E75" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A76" s="54"/>
+      <c r="B76" s="52"/>
+      <c r="C76" s="52"/>
+      <c r="D76" s="52"/>
       <c r="E76" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A77" s="66"/>
-      <c r="B77" s="64"/>
-      <c r="C77" s="64"/>
-      <c r="D77" s="64"/>
-      <c r="E77" s="12" t="s">
         <v>31</v>
       </c>
     </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A77" s="23"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="9"/>
+    </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A78" s="23"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="9"/>
+      <c r="A78" s="28">
+        <v>7</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E78" s="13" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A79" s="28">
-        <v>7</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="A79" s="29"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
       <c r="E79" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.45">
@@ -2144,78 +2140,77 @@
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
       <c r="E80" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A81" s="29"/>
-      <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
+      <c r="A81" s="30"/>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
       <c r="E81" s="13" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A82" s="30"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
-      <c r="E82" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A83" s="23"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="9"/>
+      <c r="A82" s="23"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="C2:C8"/>
-    <mergeCell ref="D2:D8"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="C70:C72"/>
-    <mergeCell ref="D70:D72"/>
-    <mergeCell ref="A10:A16"/>
-    <mergeCell ref="B10:B16"/>
-    <mergeCell ref="C10:C16"/>
-    <mergeCell ref="D10:D16"/>
+  <mergeCells count="50">
+    <mergeCell ref="C44:C50"/>
+    <mergeCell ref="B44:B50"/>
+    <mergeCell ref="D44:D50"/>
+    <mergeCell ref="A44:A50"/>
+    <mergeCell ref="A52:A58"/>
+    <mergeCell ref="B52:B58"/>
+    <mergeCell ref="C52:C58"/>
+    <mergeCell ref="D52:D58"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="D37:D42"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="B37:B42"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="D65:D67"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A18:A20"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="C30:C32"/>
     <mergeCell ref="C22:C28"/>
     <mergeCell ref="D22:D28"/>
     <mergeCell ref="D30:D32"/>
     <mergeCell ref="D34:D35"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="C66:C68"/>
-    <mergeCell ref="D66:D68"/>
-    <mergeCell ref="C37:C43"/>
-    <mergeCell ref="D37:D43"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A37:A43"/>
-    <mergeCell ref="B37:B43"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="C69:C71"/>
+    <mergeCell ref="D69:D71"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="B10:B16"/>
+    <mergeCell ref="C10:C16"/>
+    <mergeCell ref="D10:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2262,13 +2257,13 @@
       <c r="A2" s="47">
         <v>1</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="50" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="50" t="s">
+      <c r="C2" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="49" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="14" t="s">
@@ -2280,9 +2275,9 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="48"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
       <c r="E3" s="15" t="s">
         <v>60</v>
       </c>
@@ -2292,9 +2287,9 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="48"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
       <c r="E4" s="15" t="s">
         <v>64</v>
       </c>
@@ -2302,9 +2297,9 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="48"/>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
       <c r="E5" s="15" t="s">
         <v>65</v>
       </c>
@@ -2312,9 +2307,9 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="48"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
       <c r="E6" s="15" t="s">
         <v>66</v>
       </c>
@@ -2322,9 +2317,9 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="48"/>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
       <c r="E7" s="15" t="s">
         <v>68</v>
       </c>
@@ -2332,9 +2327,9 @@
     </row>
     <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="48"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
       <c r="E8" s="15" t="s">
         <v>61</v>
       </c>
@@ -2342,19 +2337,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="48"/>
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
       <c r="E9" s="15" t="s">
         <v>62</v>
       </c>
       <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="49"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
+      <c r="A10" s="61"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
       <c r="E10" s="15" t="s">
         <v>14</v>
       </c>
@@ -2372,17 +2367,17 @@
       <c r="A12" s="47">
         <v>2</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="50" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="50" t="s">
+      <c r="C12" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="49" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F12" s="21" t="s">
         <v>52</v>
@@ -2390,39 +2385,39 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="48"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
       <c r="E13" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="48"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
       <c r="E14" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="48"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
       <c r="E15" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="49"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
       <c r="E16" s="11" t="s">
         <v>51</v>
       </c>
@@ -2440,17 +2435,17 @@
       <c r="A18" s="47">
         <v>3</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="50" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" s="50" t="s">
+      <c r="C18" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="49" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F18" s="21" t="s">
         <v>53</v>
@@ -2458,51 +2453,51 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="48"/>
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
       <c r="E19" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="48"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
       <c r="E20" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F20" s="21"/>
     </row>
     <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="48"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
       <c r="E21" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F21" s="21"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="48"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
       <c r="E22" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F22" s="21"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="48"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
       <c r="E23" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F23" s="21"/>
     </row>
@@ -2518,27 +2513,27 @@
       <c r="A25" s="47">
         <v>4</v>
       </c>
-      <c r="B25" s="50" t="s">
+      <c r="B25" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="50" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="50" t="s">
+      <c r="C25" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="49" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F25" s="21"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="48"/>
-      <c r="B26" s="51"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
       <c r="E26" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F26" s="21"/>
     </row>
@@ -2554,17 +2549,17 @@
       <c r="A28" s="47">
         <v>5</v>
       </c>
-      <c r="B28" s="50" t="s">
+      <c r="B28" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="50" t="s">
-        <v>83</v>
-      </c>
-      <c r="D28" s="50" t="s">
+      <c r="C28" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="49" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>59</v>
@@ -2572,9 +2567,9 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="48"/>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
       <c r="E29" s="15" t="s">
         <v>17</v>
       </c>
@@ -2592,47 +2587,47 @@
       <c r="A31" s="47">
         <v>6</v>
       </c>
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="50" t="s">
-        <v>116</v>
-      </c>
-      <c r="D31" s="50" t="s">
+      <c r="C31" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="D31" s="49" t="s">
         <v>43</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>40</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="48"/>
-      <c r="B32" s="51"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
       <c r="E32" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F32" s="21"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="48"/>
-      <c r="B33" s="51"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
       <c r="E33" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F33" s="21"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="49"/>
-      <c r="B34" s="52"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="52"/>
+      <c r="A34" s="61"/>
+      <c r="B34" s="62"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
       <c r="E34" s="15" t="s">
         <v>22</v>
       </c>
@@ -2650,13 +2645,13 @@
       <c r="A36" s="47">
         <v>7</v>
       </c>
-      <c r="B36" s="50" t="s">
+      <c r="B36" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="50" t="s">
+      <c r="C36" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="50" t="s">
+      <c r="D36" s="49" t="s">
         <v>24</v>
       </c>
       <c r="E36" s="15" t="s">
@@ -2666,19 +2661,19 @@
     </row>
     <row r="37" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A37" s="48"/>
-      <c r="B37" s="51"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="51"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="50"/>
       <c r="E37" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F37" s="21"/>
     </row>
     <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A38" s="49"/>
-      <c r="B38" s="52"/>
-      <c r="C38" s="52"/>
-      <c r="D38" s="52"/>
+      <c r="A38" s="61"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
       <c r="E38" s="15" t="s">
         <v>36</v>
       </c>
@@ -2696,87 +2691,87 @@
       <c r="A40" s="47">
         <v>8</v>
       </c>
-      <c r="B40" s="50" t="s">
+      <c r="B40" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="50" t="s">
-        <v>172</v>
-      </c>
-      <c r="D40" s="50" t="s">
+      <c r="C40" s="49" t="s">
+        <v>171</v>
+      </c>
+      <c r="D40" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="E40" s="21" t="s">
         <v>120</v>
-      </c>
-      <c r="E40" s="21" t="s">
-        <v>121</v>
       </c>
       <c r="F40" s="21"/>
     </row>
     <row r="41" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A41" s="48"/>
-      <c r="B41" s="51"/>
-      <c r="C41" s="51"/>
-      <c r="D41" s="51"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
       <c r="E41" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F41" s="21"/>
     </row>
     <row r="42" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A42" s="48"/>
-      <c r="B42" s="51"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
       <c r="E42" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F42" s="21"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="48"/>
-      <c r="B43" s="51"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="51"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="50"/>
       <c r="E43" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F43" s="21"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="48"/>
-      <c r="B44" s="51"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="51"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
       <c r="E44" s="21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F44" s="21"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="48"/>
-      <c r="B45" s="51"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
       <c r="E45" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F45" s="21"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="48"/>
-      <c r="B46" s="51"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="50"/>
       <c r="E46" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F46" s="21"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="48"/>
-      <c r="B47" s="51"/>
-      <c r="C47" s="51"/>
-      <c r="D47" s="51"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
       <c r="E47" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F47" s="21"/>
     </row>
@@ -2790,6 +2785,30 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A40:A47"/>
+    <mergeCell ref="B40:B47"/>
+    <mergeCell ref="C40:C47"/>
+    <mergeCell ref="D40:D47"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="B2:B10"/>
     <mergeCell ref="C2:C10"/>
@@ -2798,30 +2817,6 @@
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
     <mergeCell ref="D12:D16"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A40:A47"/>
-    <mergeCell ref="B40:B47"/>
-    <mergeCell ref="C40:C47"/>
-    <mergeCell ref="D40:D47"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="A36:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2849,190 +2844,190 @@
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B2" s="42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C2" s="33"/>
       <c r="D2" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F2" s="42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H2" s="44" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B3" s="41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B4" s="39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F4" s="39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B5" s="39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F5" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H5" s="36" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B6" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="D6" s="36" t="s">
-        <v>139</v>
-      </c>
       <c r="F6" s="39" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B7" s="39"/>
       <c r="D7" s="38"/>
       <c r="F7" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H7" s="38"/>
     </row>
     <row r="8" spans="2:17" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B8" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="D8" s="36" t="s">
-        <v>142</v>
-      </c>
       <c r="F8" s="36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H8" s="36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="2:17" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B9" s="36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F9" s="39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H9" s="36" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="2:17" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B10" s="36" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F10" s="39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B11" s="39" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F11" s="39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H11" s="36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B12" s="39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F12" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H12" s="38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B13" s="39" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F13" s="39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B14" s="39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F14" s="39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B15" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F15" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.45">
       <c r="F16" s="39" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.45">
       <c r="F17" s="39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.45">
       <c r="F18" s="40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created getters/setters for Customer, fixed UMLs
</commit_message>
<xml_diff>
--- a/User Stories/NataliaUserStories.xlsx
+++ b/User Stories/NataliaUserStories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Palej\Desktop\Software Design with AI for Cloud\Year_3\agile-labs3\Newsagent-Project\User Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C589FF87-38F8-4E12-A7C2-07724521BB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6C0429-C16D-4062-836C-AD5D61D5175F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminUserStories" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="185">
   <si>
     <t>As an admin</t>
   </si>
@@ -439,9 +439,6 @@
     <t>+generateDeliveryDoc() : void</t>
   </si>
   <si>
-    <t>+givePermission() : void</t>
-  </si>
-  <si>
     <t>- username : String</t>
   </si>
   <si>
@@ -523,15 +520,6 @@
     <t>+ updateUserAccount(username: String, password: String, role: String): void</t>
   </si>
   <si>
-    <t>+ deleteUserAccount(username: String): void</t>
-  </si>
-  <si>
-    <t>+ readUserAccount(username: String): void</t>
-  </si>
-  <si>
-    <t>+ printUserAccount(username: String): void</t>
-  </si>
-  <si>
     <t>Admin extends User</t>
   </si>
   <si>
@@ -590,6 +578,21 @@
   </si>
   <si>
     <t>so that I can log in with driver permissions</t>
+  </si>
+  <si>
+    <t>+User: (username: String, password: String, role: String, userDatabase: Database)</t>
+  </si>
+  <si>
+    <t>+ printUserAccount(): void</t>
+  </si>
+  <si>
+    <t>+ givePermission() : void</t>
+  </si>
+  <si>
+    <t>+ readUserAccount(): void</t>
+  </si>
+  <si>
+    <t>+ deleteUserAccount(): void</t>
   </si>
 </sst>
 </file>
@@ -898,15 +901,60 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -920,51 +968,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1288,21 +1291,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB095BD-E922-497D-B7ED-398078A18E3D}">
   <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.9296875" style="24" customWidth="1"/>
-    <col min="2" max="2" width="13.06640625" customWidth="1"/>
-    <col min="3" max="3" width="28.46484375" customWidth="1"/>
-    <col min="4" max="4" width="35.19921875" customWidth="1"/>
-    <col min="5" max="5" width="57.86328125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="39.46484375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="2.90625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" customWidth="1"/>
+    <col min="4" max="4" width="35.1796875" customWidth="1"/>
+    <col min="5" max="5" width="57.81640625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="39.453125" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="22"/>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1320,17 +1323,17 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="47">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="54">
         <v>1</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49" t="s">
-        <v>172</v>
-      </c>
-      <c r="D2" s="49" t="s">
+      <c r="C2" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="47" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="15" t="s">
@@ -1340,11 +1343,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="48"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="55"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
       <c r="E3" s="15" t="s">
         <v>47</v>
       </c>
@@ -1352,57 +1355,57 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="48"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="55"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
       <c r="E4" s="15" t="s">
         <v>49</v>
       </c>
       <c r="F4" s="21"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="48"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="55"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
       <c r="E5" s="15" t="s">
         <v>50</v>
       </c>
       <c r="F5" s="21"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="48"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="55"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
       <c r="E6" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="55"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="48"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="15" t="s">
-        <v>177</v>
-      </c>
       <c r="F7" s="21"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="48"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="55"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
       <c r="E8" s="15" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="21"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="25"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1410,17 +1413,17 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="47">
+    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="54">
         <v>2</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="49" t="s">
+      <c r="D10" s="47" t="s">
         <v>83</v>
       </c>
       <c r="E10" s="14" t="s">
@@ -1430,67 +1433,67 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="48"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="55"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
       <c r="E11" s="15" t="s">
         <v>89</v>
       </c>
       <c r="F11" s="21"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="48"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="55"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
       <c r="E12" s="15" t="s">
         <v>92</v>
       </c>
       <c r="F12" s="21"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="48"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="55"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
       <c r="E13" s="15" t="s">
         <v>90</v>
       </c>
       <c r="F13" s="21"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="48"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="55"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
       <c r="E14" s="15" t="s">
         <v>91</v>
       </c>
       <c r="F14" s="21"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="48"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="55"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
       <c r="E15" s="15" t="s">
         <v>85</v>
       </c>
       <c r="F15" s="21"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="61"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="56"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
       <c r="E16" s="15" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="21"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="23"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1498,17 +1501,17 @@
       <c r="E17" s="16"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="47">
+    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="54">
         <v>3</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="49" t="s">
+      <c r="D18" s="47" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="15" t="s">
@@ -1518,27 +1521,27 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="48"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="55"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="15" t="s">
         <v>93</v>
       </c>
       <c r="F19" s="21"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" s="61"/>
-      <c r="B20" s="62"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="56"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
       <c r="E20" s="11" t="s">
         <v>51</v>
       </c>
       <c r="F20" s="21"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="23"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1546,17 +1549,17 @@
       <c r="E21" s="16"/>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A22" s="47">
+    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="54">
         <v>4</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="49" t="s">
+      <c r="C22" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="49" t="s">
+      <c r="D22" s="47" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="15" t="s">
@@ -1566,67 +1569,67 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="48"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="55"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
       <c r="E23" s="15" t="s">
         <v>98</v>
       </c>
       <c r="F23" s="21"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" s="48"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="55"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
       <c r="E24" s="15" t="s">
         <v>99</v>
       </c>
       <c r="F24" s="21"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="48"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="55"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="15" t="s">
         <v>100</v>
       </c>
       <c r="F25" s="21"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="48"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="55"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
       <c r="E26" s="15" t="s">
         <v>94</v>
       </c>
       <c r="F26" s="21"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" s="48"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="55"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
       <c r="E27" s="15" t="s">
         <v>95</v>
       </c>
       <c r="F27" s="21"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" s="61"/>
-      <c r="B28" s="62"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="62"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="56"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
       <c r="E28" s="15" t="s">
         <v>11</v>
       </c>
       <c r="F28" s="21"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="23"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -1634,17 +1637,17 @@
       <c r="E29" s="16"/>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" s="47">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="54">
         <v>5</v>
       </c>
-      <c r="B30" s="49" t="s">
+      <c r="B30" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="49" t="s">
+      <c r="C30" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="49" t="s">
+      <c r="D30" s="47" t="s">
         <v>84</v>
       </c>
       <c r="E30" s="15" t="s">
@@ -1652,27 +1655,27 @@
       </c>
       <c r="F30" s="21"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31" s="48"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="55"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
       <c r="E31" s="15" t="s">
         <v>96</v>
       </c>
       <c r="F31" s="21"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32" s="61"/>
-      <c r="B32" s="62"/>
-      <c r="C32" s="62"/>
-      <c r="D32" s="62"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="56"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
       <c r="E32" s="15" t="s">
         <v>97</v>
       </c>
       <c r="F32" s="21"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="23"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -1680,17 +1683,17 @@
       <c r="E33" s="16"/>
       <c r="F33" s="7"/>
     </row>
-    <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A34" s="47">
+    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="54">
         <v>6</v>
       </c>
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="49" t="s">
+      <c r="C34" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="49" t="s">
+      <c r="D34" s="47" t="s">
         <v>16</v>
       </c>
       <c r="E34" s="15" t="s">
@@ -1700,17 +1703,17 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35" s="61"/>
-      <c r="B35" s="62"/>
-      <c r="C35" s="62"/>
-      <c r="D35" s="62"/>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="56"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
       <c r="E35" s="15" t="s">
         <v>102</v>
       </c>
       <c r="F35" s="21"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="26"/>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
@@ -1718,77 +1721,77 @@
       <c r="E36" s="19"/>
       <c r="F36" s="7"/>
     </row>
-    <row r="37" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="66">
+    <row r="37" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="57">
         <v>7</v>
       </c>
-      <c r="B37" s="65" t="s">
+      <c r="B37" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="65" t="s">
+      <c r="C37" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="65" t="s">
+      <c r="D37" s="53" t="s">
         <v>71</v>
       </c>
       <c r="E37" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="F37" s="49" t="s">
+      <c r="F37" s="47" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38" s="66"/>
-      <c r="B38" s="65"/>
-      <c r="C38" s="65"/>
-      <c r="D38" s="65"/>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="57"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
       <c r="E38" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F38" s="50"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39" s="66"/>
-      <c r="B39" s="65"/>
-      <c r="C39" s="65"/>
-      <c r="D39" s="65"/>
+      <c r="F38" s="48"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="57"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
       <c r="E39" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="F39" s="62"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" s="66"/>
-      <c r="B40" s="65"/>
-      <c r="C40" s="65"/>
-      <c r="D40" s="65"/>
+      <c r="F39" s="49"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="57"/>
+      <c r="B40" s="53"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="53"/>
       <c r="E40" s="21" t="s">
         <v>74</v>
       </c>
       <c r="F40" s="21"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" s="66"/>
-      <c r="B41" s="65"/>
-      <c r="C41" s="65"/>
-      <c r="D41" s="65"/>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="57"/>
+      <c r="B41" s="53"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="53"/>
       <c r="E41" s="21" t="s">
         <v>75</v>
       </c>
       <c r="F41" s="21"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42" s="66"/>
-      <c r="B42" s="65"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="57"/>
+      <c r="B42" s="53"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="53"/>
       <c r="E42" s="21" t="s">
         <v>77</v>
       </c>
       <c r="F42" s="21"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="27"/>
       <c r="B43" s="20"/>
       <c r="C43" s="45"/>
@@ -1796,89 +1799,89 @@
       <c r="E43" s="46"/>
       <c r="F43" s="7"/>
     </row>
-    <row r="44" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="67">
+    <row r="44" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="50">
         <v>8</v>
       </c>
-      <c r="B44" s="49" t="s">
+      <c r="B44" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="49" t="s">
-        <v>174</v>
-      </c>
-      <c r="D44" s="49" t="s">
-        <v>175</v>
+      <c r="C44" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="D44" s="47" t="s">
+        <v>171</v>
       </c>
       <c r="E44" s="21" t="s">
         <v>39</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A45" s="68"/>
-      <c r="B45" s="50"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="50"/>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="51"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="48"/>
+      <c r="D45" s="48"/>
       <c r="E45" s="21" t="s">
         <v>47</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46" s="68"/>
-      <c r="B46" s="50"/>
-      <c r="C46" s="50"/>
-      <c r="D46" s="50"/>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="51"/>
+      <c r="B46" s="48"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="48"/>
       <c r="E46" s="21" t="s">
         <v>49</v>
       </c>
       <c r="F46" s="21"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47" s="68"/>
-      <c r="B47" s="50"/>
-      <c r="C47" s="50"/>
-      <c r="D47" s="50"/>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" s="51"/>
+      <c r="B47" s="48"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="48"/>
       <c r="E47" s="21" t="s">
         <v>50</v>
       </c>
       <c r="F47" s="21"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A48" s="68"/>
-      <c r="B48" s="50"/>
-      <c r="C48" s="50"/>
-      <c r="D48" s="50"/>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" s="51"/>
+      <c r="B48" s="48"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="48"/>
       <c r="E48" s="21" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F48" s="21"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A49" s="68"/>
-      <c r="B49" s="50"/>
-      <c r="C49" s="50"/>
-      <c r="D49" s="50"/>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" s="51"/>
+      <c r="B49" s="48"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="48"/>
       <c r="E49" s="21" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F49" s="21"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A50" s="69"/>
-      <c r="B50" s="62"/>
-      <c r="C50" s="62"/>
-      <c r="D50" s="62"/>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" s="52"/>
+      <c r="B50" s="49"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="49"/>
       <c r="E50" s="21" t="s">
         <v>37</v>
       </c>
       <c r="F50" s="21"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="27"/>
       <c r="B51" s="20"/>
       <c r="C51" s="45"/>
@@ -1886,89 +1889,89 @@
       <c r="E51" s="46"/>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A52" s="67">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" s="50">
         <v>9</v>
       </c>
-      <c r="B52" s="49" t="s">
+      <c r="B52" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C52" s="49" t="s">
-        <v>182</v>
-      </c>
-      <c r="D52" s="49" t="s">
-        <v>183</v>
+      <c r="C52" s="47" t="s">
+        <v>178</v>
+      </c>
+      <c r="D52" s="47" t="s">
+        <v>179</v>
       </c>
       <c r="E52" s="21" t="s">
         <v>39</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A53" s="68"/>
-      <c r="B53" s="50"/>
-      <c r="C53" s="50"/>
-      <c r="D53" s="50"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" s="51"/>
+      <c r="B53" s="48"/>
+      <c r="C53" s="48"/>
+      <c r="D53" s="48"/>
       <c r="E53" s="21" t="s">
         <v>47</v>
       </c>
       <c r="F53" s="21" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A54" s="68"/>
-      <c r="B54" s="50"/>
-      <c r="C54" s="50"/>
-      <c r="D54" s="50"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" s="51"/>
+      <c r="B54" s="48"/>
+      <c r="C54" s="48"/>
+      <c r="D54" s="48"/>
       <c r="E54" s="21" t="s">
         <v>49</v>
       </c>
       <c r="F54" s="21"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A55" s="68"/>
-      <c r="B55" s="50"/>
-      <c r="C55" s="50"/>
-      <c r="D55" s="50"/>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" s="51"/>
+      <c r="B55" s="48"/>
+      <c r="C55" s="48"/>
+      <c r="D55" s="48"/>
       <c r="E55" s="21" t="s">
         <v>50</v>
       </c>
       <c r="F55" s="21"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A56" s="68"/>
-      <c r="B56" s="50"/>
-      <c r="C56" s="50"/>
-      <c r="D56" s="50"/>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" s="51"/>
+      <c r="B56" s="48"/>
+      <c r="C56" s="48"/>
+      <c r="D56" s="48"/>
       <c r="E56" s="21" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F56" s="21"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A57" s="68"/>
-      <c r="B57" s="50"/>
-      <c r="C57" s="50"/>
-      <c r="D57" s="50"/>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" s="51"/>
+      <c r="B57" s="48"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="48"/>
       <c r="E57" s="21" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F57" s="21"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A58" s="69"/>
-      <c r="B58" s="62"/>
-      <c r="C58" s="62"/>
-      <c r="D58" s="62"/>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" s="52"/>
+      <c r="B58" s="49"/>
+      <c r="C58" s="49"/>
+      <c r="D58" s="49"/>
       <c r="E58" s="21" t="s">
         <v>37</v>
       </c>
       <c r="F58" s="21"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="27"/>
       <c r="B59" s="20"/>
       <c r="C59" s="45"/>
@@ -1976,7 +1979,7 @@
       <c r="E59" s="46"/>
       <c r="F59" s="7"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="23"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
@@ -1984,45 +1987,45 @@
       <c r="E64" s="16"/>
       <c r="F64" s="7"/>
     </row>
-    <row r="65" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A65" s="55">
+    <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A65" s="60">
         <v>10</v>
       </c>
-      <c r="B65" s="58" t="s">
+      <c r="B65" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="C65" s="58" t="s">
+      <c r="C65" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="D65" s="58" t="s">
+      <c r="D65" s="63" t="s">
         <v>33</v>
       </c>
       <c r="E65" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F65" s="63" t="s">
+      <c r="F65" s="58" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A66" s="56"/>
-      <c r="B66" s="59"/>
-      <c r="C66" s="59"/>
-      <c r="D66" s="59"/>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66" s="61"/>
+      <c r="B66" s="64"/>
+      <c r="C66" s="64"/>
+      <c r="D66" s="64"/>
       <c r="E66" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="F66" s="64"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A67" s="57"/>
-      <c r="B67" s="60"/>
-      <c r="C67" s="60"/>
-      <c r="D67" s="60"/>
+      <c r="F66" s="59"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67" s="62"/>
+      <c r="B67" s="65"/>
+      <c r="C67" s="65"/>
+      <c r="D67" s="65"/>
       <c r="E67" s="6"/>
       <c r="F67" s="31"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="23"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
@@ -2030,17 +2033,17 @@
       <c r="E68" s="16"/>
       <c r="F68" s="7"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A69" s="55">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69" s="60">
         <v>11</v>
       </c>
-      <c r="B69" s="58" t="s">
+      <c r="B69" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="C69" s="58" t="s">
+      <c r="C69" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="D69" s="58" t="s">
+      <c r="D69" s="63" t="s">
         <v>26</v>
       </c>
       <c r="E69" s="17" t="s">
@@ -2048,67 +2051,67 @@
       </c>
       <c r="F69" s="31"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A70" s="56"/>
-      <c r="B70" s="59"/>
-      <c r="C70" s="59"/>
-      <c r="D70" s="59"/>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70" s="61"/>
+      <c r="B70" s="64"/>
+      <c r="C70" s="64"/>
+      <c r="D70" s="64"/>
       <c r="E70" s="17" t="s">
         <v>28</v>
       </c>
       <c r="F70" s="31"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A71" s="57"/>
-      <c r="B71" s="60"/>
-      <c r="C71" s="60"/>
-      <c r="D71" s="60"/>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71" s="62"/>
+      <c r="B71" s="65"/>
+      <c r="C71" s="65"/>
+      <c r="D71" s="65"/>
       <c r="E71" s="17" t="s">
         <v>29</v>
       </c>
       <c r="F71" s="31"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="23"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="9"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A75" s="53">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A75" s="68">
         <v>6</v>
       </c>
-      <c r="B75" s="51" t="s">
+      <c r="B75" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="C75" s="51" t="s">
+      <c r="C75" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="D75" s="51" t="s">
+      <c r="D75" s="66" t="s">
         <v>19</v>
       </c>
       <c r="E75" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A76" s="54"/>
-      <c r="B76" s="52"/>
-      <c r="C76" s="52"/>
-      <c r="D76" s="52"/>
+    <row r="76" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A76" s="69"/>
+      <c r="B76" s="67"/>
+      <c r="C76" s="67"/>
+      <c r="D76" s="67"/>
       <c r="E76" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="23"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="9"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="28">
         <v>7</v>
       </c>
@@ -2125,7 +2128,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="29"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -2134,7 +2137,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="29"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -2143,7 +2146,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="30"/>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
@@ -2152,7 +2155,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="23"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2161,40 +2164,6 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="C44:C50"/>
-    <mergeCell ref="B44:B50"/>
-    <mergeCell ref="D44:D50"/>
-    <mergeCell ref="A44:A50"/>
-    <mergeCell ref="A52:A58"/>
-    <mergeCell ref="B52:B58"/>
-    <mergeCell ref="C52:C58"/>
-    <mergeCell ref="D52:D58"/>
-    <mergeCell ref="C37:C42"/>
-    <mergeCell ref="D37:D42"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="B37:B42"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="D65:D67"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="C22:C28"/>
-    <mergeCell ref="D22:D28"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="D34:D35"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="B2:B8"/>
     <mergeCell ref="C2:C8"/>
@@ -2211,6 +2180,40 @@
     <mergeCell ref="B10:B16"/>
     <mergeCell ref="C10:C16"/>
     <mergeCell ref="D10:D16"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C22:C28"/>
+    <mergeCell ref="D22:D28"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="D65:D67"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="D37:D42"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="B37:B42"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="C44:C50"/>
+    <mergeCell ref="B44:B50"/>
+    <mergeCell ref="D44:D50"/>
+    <mergeCell ref="A44:A50"/>
+    <mergeCell ref="A52:A58"/>
+    <mergeCell ref="B52:B58"/>
+    <mergeCell ref="C52:C58"/>
+    <mergeCell ref="D52:D58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2221,21 +2224,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526350BB-95BB-4BF1-93A5-0B30D123D1AA}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.9296875" style="24" customWidth="1"/>
-    <col min="2" max="2" width="23.46484375" customWidth="1"/>
-    <col min="3" max="3" width="27.86328125" customWidth="1"/>
+    <col min="1" max="1" width="2.90625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" customWidth="1"/>
+    <col min="3" max="3" width="27.81640625" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="52.59765625" customWidth="1"/>
-    <col min="6" max="6" width="44.19921875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.6328125" customWidth="1"/>
+    <col min="6" max="6" width="44.1796875" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="22"/>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -2253,17 +2256,17 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="47">
+    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="54">
         <v>1</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="47" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="14" t="s">
@@ -2273,11 +2276,11 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="48"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="55"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
       <c r="E3" s="15" t="s">
         <v>60</v>
       </c>
@@ -2285,77 +2288,77 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="48"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="55"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
       <c r="E4" s="15" t="s">
         <v>64</v>
       </c>
       <c r="F4" s="21"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="48"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="55"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
       <c r="E5" s="15" t="s">
         <v>65</v>
       </c>
       <c r="F5" s="21"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="48"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="55"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
       <c r="E6" s="15" t="s">
         <v>66</v>
       </c>
       <c r="F6" s="21"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="48"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="55"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
       <c r="E7" s="15" t="s">
         <v>68</v>
       </c>
       <c r="F7" s="21"/>
     </row>
-    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="48"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
+    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="55"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
       <c r="E8" s="15" t="s">
         <v>61</v>
       </c>
       <c r="F8" s="21"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="48"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="55"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
       <c r="E9" s="15" t="s">
         <v>62</v>
       </c>
       <c r="F9" s="21"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="61"/>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="56"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
       <c r="E10" s="15" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="21"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="23"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -2363,17 +2366,17 @@
       <c r="E11" s="16"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="47">
+    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="54">
         <v>2</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="D12" s="47" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="15" t="s">
@@ -2383,47 +2386,47 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="48"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="55"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
       <c r="E13" s="15" t="s">
         <v>104</v>
       </c>
       <c r="F13" s="21"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="48"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="55"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
       <c r="E14" s="15" t="s">
         <v>105</v>
       </c>
       <c r="F14" s="21"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="48"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="55"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
       <c r="E15" s="15" t="s">
         <v>106</v>
       </c>
       <c r="F15" s="21"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="61"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="56"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
       <c r="E16" s="11" t="s">
         <v>51</v>
       </c>
       <c r="F16" s="21"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="23"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -2431,17 +2434,17 @@
       <c r="E17" s="16"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="47">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="54">
         <v>3</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="49" t="s">
+      <c r="D18" s="47" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="15" t="s">
@@ -2451,57 +2454,57 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="48"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="55"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="15" t="s">
         <v>104</v>
       </c>
       <c r="F19" s="21"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" s="48"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
+    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="55"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="15" t="s">
         <v>108</v>
       </c>
       <c r="F20" s="21"/>
     </row>
-    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="48"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="55"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
       <c r="E21" s="15" t="s">
         <v>109</v>
       </c>
       <c r="F21" s="21"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" s="48"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="55"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
       <c r="E22" s="15" t="s">
         <v>111</v>
       </c>
       <c r="F22" s="21"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="48"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="55"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
       <c r="E23" s="15" t="s">
         <v>110</v>
       </c>
       <c r="F23" s="21"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="23"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -2509,17 +2512,17 @@
       <c r="E24" s="16"/>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A25" s="47">
+    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="54">
         <v>4</v>
       </c>
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="49" t="s">
+      <c r="C25" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="D25" s="49" t="s">
+      <c r="D25" s="47" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="15" t="s">
@@ -2527,17 +2530,17 @@
       </c>
       <c r="F25" s="21"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="48"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="55"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
       <c r="E26" s="15" t="s">
         <v>113</v>
       </c>
       <c r="F26" s="21"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="23"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -2545,17 +2548,17 @@
       <c r="E27" s="16"/>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A28" s="47">
+    <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="54">
         <v>5</v>
       </c>
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="49" t="s">
+      <c r="C28" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="D28" s="49" t="s">
+      <c r="D28" s="47" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="15" t="s">
@@ -2565,17 +2568,17 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="48"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="55"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="48"/>
       <c r="E29" s="15" t="s">
         <v>17</v>
       </c>
       <c r="F29" s="21"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="23"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -2583,17 +2586,17 @@
       <c r="E30" s="16"/>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="47">
+    <row r="31" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="54">
         <v>6</v>
       </c>
-      <c r="B31" s="49" t="s">
+      <c r="B31" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="49" t="s">
+      <c r="C31" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="D31" s="49" t="s">
+      <c r="D31" s="47" t="s">
         <v>43</v>
       </c>
       <c r="E31" s="14" t="s">
@@ -2603,37 +2606,37 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32" s="48"/>
-      <c r="B32" s="50"/>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="55"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
       <c r="E32" s="15" t="s">
         <v>118</v>
       </c>
       <c r="F32" s="21"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33" s="48"/>
-      <c r="B33" s="50"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="50"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="55"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
       <c r="E33" s="15" t="s">
         <v>116</v>
       </c>
       <c r="F33" s="21"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="61"/>
-      <c r="B34" s="62"/>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="56"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
       <c r="E34" s="15" t="s">
         <v>22</v>
       </c>
       <c r="F34" s="21"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="23"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -2641,17 +2644,17 @@
       <c r="E35" s="16"/>
       <c r="F35" s="7"/>
     </row>
-    <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A36" s="47">
+    <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="54">
         <v>7</v>
       </c>
-      <c r="B36" s="49" t="s">
+      <c r="B36" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="49" t="s">
+      <c r="C36" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="49" t="s">
+      <c r="D36" s="47" t="s">
         <v>24</v>
       </c>
       <c r="E36" s="15" t="s">
@@ -2659,27 +2662,27 @@
       </c>
       <c r="F36" s="21"/>
     </row>
-    <row r="37" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A37" s="48"/>
-      <c r="B37" s="50"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
+    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" s="55"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
       <c r="E37" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F37" s="21"/>
     </row>
-    <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A38" s="61"/>
-      <c r="B38" s="62"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="62"/>
+    <row r="38" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="56"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
       <c r="E38" s="15" t="s">
         <v>36</v>
       </c>
       <c r="F38" s="21"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="23"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -2687,17 +2690,17 @@
       <c r="E39" s="16"/>
       <c r="F39" s="7"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" s="47">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="54">
         <v>8</v>
       </c>
-      <c r="B40" s="49" t="s">
+      <c r="B40" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="49" t="s">
-        <v>171</v>
-      </c>
-      <c r="D40" s="49" t="s">
+      <c r="C40" s="47" t="s">
+        <v>167</v>
+      </c>
+      <c r="D40" s="47" t="s">
         <v>119</v>
       </c>
       <c r="E40" s="21" t="s">
@@ -2705,77 +2708,77 @@
       </c>
       <c r="F40" s="21"/>
     </row>
-    <row r="41" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A41" s="48"/>
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
+    <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="55"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="48"/>
       <c r="E41" s="21" t="s">
         <v>121</v>
       </c>
       <c r="F41" s="21"/>
     </row>
-    <row r="42" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A42" s="48"/>
-      <c r="B42" s="50"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="50"/>
+    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="55"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="48"/>
       <c r="E42" s="21" t="s">
         <v>122</v>
       </c>
       <c r="F42" s="21"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43" s="48"/>
-      <c r="B43" s="50"/>
-      <c r="C43" s="50"/>
-      <c r="D43" s="50"/>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="55"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="48"/>
       <c r="E43" s="21" t="s">
         <v>123</v>
       </c>
       <c r="F43" s="21"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44" s="48"/>
-      <c r="B44" s="50"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="50"/>
+    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="55"/>
+      <c r="B44" s="48"/>
+      <c r="C44" s="48"/>
+      <c r="D44" s="48"/>
       <c r="E44" s="21" t="s">
         <v>125</v>
       </c>
       <c r="F44" s="21"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A45" s="48"/>
-      <c r="B45" s="50"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="50"/>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="55"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="48"/>
+      <c r="D45" s="48"/>
       <c r="E45" s="21" t="s">
         <v>126</v>
       </c>
       <c r="F45" s="21"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46" s="48"/>
-      <c r="B46" s="50"/>
-      <c r="C46" s="50"/>
-      <c r="D46" s="50"/>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="55"/>
+      <c r="B46" s="48"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="48"/>
       <c r="E46" s="21" t="s">
         <v>124</v>
       </c>
       <c r="F46" s="21"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47" s="48"/>
-      <c r="B47" s="50"/>
-      <c r="C47" s="50"/>
-      <c r="D47" s="50"/>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" s="55"/>
+      <c r="B47" s="48"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="48"/>
       <c r="E47" s="14" t="s">
         <v>77</v>
       </c>
       <c r="F47" s="21"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="23"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -2785,6 +2788,30 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="C2:C10"/>
+    <mergeCell ref="D2:D10"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="A31:A34"/>
     <mergeCell ref="A40:A47"/>
     <mergeCell ref="B40:B47"/>
     <mergeCell ref="C40:C47"/>
@@ -2793,30 +2820,6 @@
     <mergeCell ref="C36:C38"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="C2:C10"/>
-    <mergeCell ref="D2:D10"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="D12:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2824,25 +2827,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD0B509-A153-4B31-95B8-BC32DC1B6A3B}">
-  <dimension ref="B2:Q18"/>
+  <dimension ref="B2:J18"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.06640625" customWidth="1"/>
-    <col min="2" max="2" width="37.46484375" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.06640625" style="32" customWidth="1"/>
-    <col min="4" max="4" width="41.73046875" style="34" customWidth="1"/>
-    <col min="5" max="5" width="3.796875" style="32" customWidth="1"/>
-    <col min="6" max="6" width="37.9296875" customWidth="1"/>
-    <col min="7" max="7" width="3.59765625" customWidth="1"/>
-    <col min="8" max="8" width="40.59765625" customWidth="1"/>
+    <col min="1" max="1" width="2.08984375" customWidth="1"/>
+    <col min="2" max="2" width="37.453125" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.08984375" style="32" customWidth="1"/>
+    <col min="4" max="4" width="41.7265625" style="34" customWidth="1"/>
+    <col min="5" max="5" width="3.81640625" style="32" customWidth="1"/>
+    <col min="6" max="6" width="37.90625" customWidth="1"/>
+    <col min="7" max="7" width="3.6328125" customWidth="1"/>
+    <col min="8" max="8" width="40.6328125" customWidth="1"/>
+    <col min="9" max="9" width="3.26953125" customWidth="1"/>
+    <col min="10" max="10" width="26.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="42" t="s">
         <v>128</v>
       </c>
@@ -2851,183 +2856,187 @@
         <v>129</v>
       </c>
       <c r="F2" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="J2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>150</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="J3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="J4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="39"/>
+      <c r="D7" s="36"/>
+      <c r="F7" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="H7" s="38"/>
+    </row>
+    <row r="8" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="D8" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="H8" s="35" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="D9" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="F9" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="36" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B3" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="D3" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="F3" s="41" t="s">
-        <v>151</v>
-      </c>
-      <c r="H3" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B4" s="39" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="F4" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="H4" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B5" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="F5" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="H5" s="36" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B6" s="39" t="s">
-        <v>137</v>
-      </c>
-      <c r="D6" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="F6" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="H6" s="36" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B7" s="39"/>
-      <c r="D7" s="38"/>
-      <c r="F7" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="H7" s="38"/>
-    </row>
-    <row r="8" spans="2:17" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B8" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>141</v>
-      </c>
-      <c r="F8" s="36" t="s">
-        <v>156</v>
-      </c>
-      <c r="H8" s="36" t="s">
+      <c r="D10" s="36" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="9" spans="2:17" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B9" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="D9" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="F9" s="39" t="s">
+      <c r="F10" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="H9" s="36" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B10" s="36" t="s">
-        <v>168</v>
-      </c>
-      <c r="F10" s="39" t="s">
-        <v>143</v>
-      </c>
-      <c r="H10" s="37" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="H10" s="38"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="39" t="s">
         <v>130</v>
       </c>
+      <c r="D11" s="37" t="s">
+        <v>184</v>
+      </c>
       <c r="F11" s="39" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="F12" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="H11" s="36" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B12" s="39" t="s">
-        <v>169</v>
-      </c>
-      <c r="F12" s="39" t="s">
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="F13" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="H12" s="38" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B13" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="F13" s="39" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="39" t="s">
         <v>131</v>
       </c>
       <c r="F14" s="39" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.45">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="40" t="s">
         <v>132</v>
       </c>
       <c r="F15" s="39" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="F16" s="39" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="F16" s="39" t="s">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F17" s="39" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.45">
-      <c r="F17" s="39" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F18" s="40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Designed DB UML and Tests
</commit_message>
<xml_diff>
--- a/User Stories/NataliaUserStories.xlsx
+++ b/User Stories/NataliaUserStories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cad1acabf18afac6/Desktop/Software Design with AI for Cloud/Year_3/agile-labs3/Newsagent-Project/User Stories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="444" documentId="13_ncr:1_{7B2E17FA-F2A9-4DCC-A803-850E080333ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57F8BC66-1230-49D3-A591-B6675BDD9146}"/>
+  <xr:revisionPtr revIDLastSave="560" documentId="13_ncr:1_{7B2E17FA-F2A9-4DCC-A803-850E080333ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{706D3FA1-34FF-4746-B170-F0F00F53DEBA}"/>
   <bookViews>
-    <workbookView xWindow="10820" yWindow="500" windowWidth="27590" windowHeight="19310" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
+    <workbookView xWindow="9960" yWindow="2470" windowWidth="24720" windowHeight="15640" activeTab="3" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminUserStories" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="255">
   <si>
     <t>As an admin</t>
   </si>
@@ -771,6 +771,39 @@
   </si>
   <si>
     <t>DELETE FROM newsagentDetails WHERE newsagentID="2";</t>
+  </si>
+  <si>
+    <t>DatabaseConnector</t>
+  </si>
+  <si>
+    <t>- DB_DRIVER : String final</t>
+  </si>
+  <si>
+    <t>- JDBC_URL : String final</t>
+  </si>
+  <si>
+    <t>- USERNAME : String final</t>
+  </si>
+  <si>
+    <t>- PASSWORD : String final</t>
+  </si>
+  <si>
+    <t>+ getConnection() : static</t>
+  </si>
+  <si>
+    <t>Test connectivity with newsagentdb database</t>
+  </si>
+  <si>
+    <t>3 Lidia Dadal</t>
+  </si>
+  <si>
+    <t>4 Lola Maltese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Adrian Kochatek </t>
+  </si>
+  <si>
+    <t>ResultSet resultSet = query.executeQuery("Select * from customerDetails");</t>
   </si>
 </sst>
 </file>
@@ -853,7 +886,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -946,11 +979,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1078,15 +1142,69 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1096,90 +1214,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3004,7 +3071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB095BD-E922-497D-B7ED-398078A18E3D}">
   <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C69" sqref="C69:C71"/>
     </sheetView>
   </sheetViews>
@@ -3037,16 +3104,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="54">
+      <c r="A2" s="50">
         <v>1</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="52" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="15" t="s">
@@ -3057,10 +3124,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="55"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
       <c r="E3" s="15" t="s">
         <v>47</v>
       </c>
@@ -3069,50 +3136,50 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="55"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
       <c r="E4" s="15" t="s">
         <v>49</v>
       </c>
       <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="55"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
+      <c r="A5" s="51"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
       <c r="E5" s="15" t="s">
         <v>50</v>
       </c>
       <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="55"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
+      <c r="A6" s="51"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
       <c r="E6" s="15" t="s">
         <v>168</v>
       </c>
       <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="55"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
+      <c r="A7" s="51"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
       <c r="E7" s="15" t="s">
         <v>172</v>
       </c>
       <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="55"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
       <c r="E8" s="15" t="s">
         <v>37</v>
       </c>
@@ -3127,16 +3194,16 @@
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="54">
+      <c r="A10" s="50">
         <v>2</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="47" t="s">
+      <c r="D10" s="52" t="s">
         <v>82</v>
       </c>
       <c r="E10" s="14" t="s">
@@ -3147,60 +3214,60 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="55"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
+      <c r="A11" s="51"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
       <c r="E11" s="15" t="s">
         <v>88</v>
       </c>
       <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="55"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
+      <c r="A12" s="51"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
       <c r="E12" s="15" t="s">
         <v>91</v>
       </c>
       <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="55"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
+      <c r="A13" s="51"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
       <c r="E13" s="15" t="s">
         <v>89</v>
       </c>
       <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="55"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
       <c r="E14" s="15" t="s">
         <v>90</v>
       </c>
       <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="55"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
+      <c r="A15" s="51"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
       <c r="E15" s="15" t="s">
         <v>84</v>
       </c>
       <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="56"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
+      <c r="A16" s="64"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
       <c r="E16" s="15" t="s">
         <v>14</v>
       </c>
@@ -3215,16 +3282,16 @@
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="54">
+      <c r="A18" s="50">
         <v>3</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="47" t="s">
+      <c r="D18" s="52" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="15" t="s">
@@ -3235,20 +3302,20 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="55"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
+      <c r="A19" s="51"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
       <c r="E19" s="15" t="s">
         <v>92</v>
       </c>
       <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="56"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
+      <c r="A20" s="64"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
       <c r="E20" s="11" t="s">
         <v>51</v>
       </c>
@@ -3263,16 +3330,16 @@
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="54">
+      <c r="A22" s="50">
         <v>4</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="47" t="s">
+      <c r="C22" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="47" t="s">
+      <c r="D22" s="52" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="15" t="s">
@@ -3283,60 +3350,60 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="55"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
+      <c r="A23" s="51"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
       <c r="E23" s="15" t="s">
         <v>97</v>
       </c>
       <c r="F23" s="21"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="55"/>
-      <c r="B24" s="48"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
+      <c r="A24" s="51"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
       <c r="E24" s="15" t="s">
         <v>98</v>
       </c>
       <c r="F24" s="21"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="55"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
+      <c r="A25" s="51"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
       <c r="E25" s="15" t="s">
         <v>99</v>
       </c>
       <c r="F25" s="21"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="55"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
+      <c r="A26" s="51"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
       <c r="E26" s="15" t="s">
         <v>93</v>
       </c>
       <c r="F26" s="21"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="55"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
+      <c r="A27" s="51"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
       <c r="E27" s="15" t="s">
         <v>94</v>
       </c>
       <c r="F27" s="21"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="56"/>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
+      <c r="A28" s="64"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
       <c r="E28" s="15" t="s">
         <v>11</v>
       </c>
@@ -3351,16 +3418,16 @@
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="54">
+      <c r="A30" s="50">
         <v>5</v>
       </c>
-      <c r="B30" s="47" t="s">
+      <c r="B30" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="47" t="s">
+      <c r="C30" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="47" t="s">
+      <c r="D30" s="52" t="s">
         <v>83</v>
       </c>
       <c r="E30" s="15" t="s">
@@ -3369,20 +3436,20 @@
       <c r="F30" s="21"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="55"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
+      <c r="A31" s="51"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
       <c r="E31" s="15" t="s">
         <v>95</v>
       </c>
       <c r="F31" s="21"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="56"/>
-      <c r="B32" s="49"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
+      <c r="A32" s="64"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
       <c r="E32" s="15" t="s">
         <v>96</v>
       </c>
@@ -3397,16 +3464,16 @@
       <c r="F33" s="7"/>
     </row>
     <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="54">
+      <c r="A34" s="50">
         <v>6</v>
       </c>
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="47" t="s">
+      <c r="C34" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="47" t="s">
+      <c r="D34" s="52" t="s">
         <v>16</v>
       </c>
       <c r="E34" s="15" t="s">
@@ -3417,10 +3484,10 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="56"/>
-      <c r="B35" s="49"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
+      <c r="A35" s="64"/>
+      <c r="B35" s="65"/>
+      <c r="C35" s="65"/>
+      <c r="D35" s="65"/>
       <c r="E35" s="15" t="s">
         <v>101</v>
       </c>
@@ -3435,70 +3502,70 @@
       <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="57">
+      <c r="A37" s="69">
         <v>7</v>
       </c>
-      <c r="B37" s="53" t="s">
+      <c r="B37" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="53" t="s">
+      <c r="C37" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="53" t="s">
+      <c r="D37" s="68" t="s">
         <v>70</v>
       </c>
       <c r="E37" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="F37" s="47" t="s">
+      <c r="F37" s="52" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="57"/>
-      <c r="B38" s="53"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
+      <c r="A38" s="69"/>
+      <c r="B38" s="68"/>
+      <c r="C38" s="68"/>
+      <c r="D38" s="68"/>
       <c r="E38" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="F38" s="48"/>
+      <c r="F38" s="53"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="57"/>
-      <c r="B39" s="53"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
+      <c r="A39" s="69"/>
+      <c r="B39" s="68"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="68"/>
       <c r="E39" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F39" s="49"/>
+      <c r="F39" s="65"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="57"/>
-      <c r="B40" s="53"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="53"/>
+      <c r="A40" s="69"/>
+      <c r="B40" s="68"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="68"/>
       <c r="E40" s="21" t="s">
         <v>73</v>
       </c>
       <c r="F40" s="21"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="57"/>
-      <c r="B41" s="53"/>
-      <c r="C41" s="53"/>
-      <c r="D41" s="53"/>
+      <c r="A41" s="69"/>
+      <c r="B41" s="68"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="68"/>
       <c r="E41" s="21" t="s">
         <v>74</v>
       </c>
       <c r="F41" s="21"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="57"/>
-      <c r="B42" s="53"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="53"/>
+      <c r="A42" s="69"/>
+      <c r="B42" s="68"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="68"/>
       <c r="E42" s="21" t="s">
         <v>76</v>
       </c>
@@ -3513,16 +3580,16 @@
       <c r="F43" s="7"/>
     </row>
     <row r="44" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="50">
+      <c r="A44" s="70">
         <v>8</v>
       </c>
-      <c r="B44" s="47" t="s">
+      <c r="B44" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="47" t="s">
+      <c r="C44" s="52" t="s">
         <v>169</v>
       </c>
-      <c r="D44" s="47" t="s">
+      <c r="D44" s="52" t="s">
         <v>170</v>
       </c>
       <c r="E44" s="21" t="s">
@@ -3533,10 +3600,10 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="51"/>
-      <c r="B45" s="48"/>
-      <c r="C45" s="48"/>
-      <c r="D45" s="48"/>
+      <c r="A45" s="71"/>
+      <c r="B45" s="53"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
       <c r="E45" s="21" t="s">
         <v>47</v>
       </c>
@@ -3545,50 +3612,50 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="51"/>
-      <c r="B46" s="48"/>
-      <c r="C46" s="48"/>
-      <c r="D46" s="48"/>
+      <c r="A46" s="71"/>
+      <c r="B46" s="53"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="53"/>
       <c r="E46" s="21" t="s">
         <v>49</v>
       </c>
       <c r="F46" s="21"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="51"/>
-      <c r="B47" s="48"/>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
+      <c r="A47" s="71"/>
+      <c r="B47" s="53"/>
+      <c r="C47" s="53"/>
+      <c r="D47" s="53"/>
       <c r="E47" s="21" t="s">
         <v>50</v>
       </c>
       <c r="F47" s="21"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" s="51"/>
-      <c r="B48" s="48"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
+      <c r="A48" s="71"/>
+      <c r="B48" s="53"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="53"/>
       <c r="E48" s="21" t="s">
         <v>171</v>
       </c>
       <c r="F48" s="21"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="51"/>
-      <c r="B49" s="48"/>
-      <c r="C49" s="48"/>
-      <c r="D49" s="48"/>
+      <c r="A49" s="71"/>
+      <c r="B49" s="53"/>
+      <c r="C49" s="53"/>
+      <c r="D49" s="53"/>
       <c r="E49" s="21" t="s">
         <v>172</v>
       </c>
       <c r="F49" s="21"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="52"/>
-      <c r="B50" s="49"/>
-      <c r="C50" s="49"/>
-      <c r="D50" s="49"/>
+      <c r="A50" s="72"/>
+      <c r="B50" s="65"/>
+      <c r="C50" s="65"/>
+      <c r="D50" s="65"/>
       <c r="E50" s="21" t="s">
         <v>37</v>
       </c>
@@ -3603,16 +3670,16 @@
       <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="50">
+      <c r="A52" s="70">
         <v>9</v>
       </c>
-      <c r="B52" s="47" t="s">
+      <c r="B52" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C52" s="47" t="s">
+      <c r="C52" s="52" t="s">
         <v>177</v>
       </c>
-      <c r="D52" s="47" t="s">
+      <c r="D52" s="52" t="s">
         <v>178</v>
       </c>
       <c r="E52" s="21" t="s">
@@ -3623,10 +3690,10 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="51"/>
-      <c r="B53" s="48"/>
-      <c r="C53" s="48"/>
-      <c r="D53" s="48"/>
+      <c r="A53" s="71"/>
+      <c r="B53" s="53"/>
+      <c r="C53" s="53"/>
+      <c r="D53" s="53"/>
       <c r="E53" s="21" t="s">
         <v>47</v>
       </c>
@@ -3635,50 +3702,50 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="51"/>
-      <c r="B54" s="48"/>
-      <c r="C54" s="48"/>
-      <c r="D54" s="48"/>
+      <c r="A54" s="71"/>
+      <c r="B54" s="53"/>
+      <c r="C54" s="53"/>
+      <c r="D54" s="53"/>
       <c r="E54" s="21" t="s">
         <v>49</v>
       </c>
       <c r="F54" s="21"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" s="51"/>
-      <c r="B55" s="48"/>
-      <c r="C55" s="48"/>
-      <c r="D55" s="48"/>
+      <c r="A55" s="71"/>
+      <c r="B55" s="53"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="53"/>
       <c r="E55" s="21" t="s">
         <v>50</v>
       </c>
       <c r="F55" s="21"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="51"/>
-      <c r="B56" s="48"/>
-      <c r="C56" s="48"/>
-      <c r="D56" s="48"/>
+      <c r="A56" s="71"/>
+      <c r="B56" s="53"/>
+      <c r="C56" s="53"/>
+      <c r="D56" s="53"/>
       <c r="E56" s="21" t="s">
         <v>171</v>
       </c>
       <c r="F56" s="21"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A57" s="51"/>
-      <c r="B57" s="48"/>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
+      <c r="A57" s="71"/>
+      <c r="B57" s="53"/>
+      <c r="C57" s="53"/>
+      <c r="D57" s="53"/>
       <c r="E57" s="21" t="s">
         <v>172</v>
       </c>
       <c r="F57" s="21"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="52"/>
-      <c r="B58" s="49"/>
-      <c r="C58" s="49"/>
-      <c r="D58" s="49"/>
+      <c r="A58" s="72"/>
+      <c r="B58" s="65"/>
+      <c r="C58" s="65"/>
+      <c r="D58" s="65"/>
       <c r="E58" s="21" t="s">
         <v>37</v>
       </c>
@@ -3701,40 +3768,40 @@
       <c r="F64" s="7"/>
     </row>
     <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="60">
+      <c r="A65" s="58">
         <v>10</v>
       </c>
-      <c r="B65" s="63" t="s">
+      <c r="B65" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="C65" s="63" t="s">
+      <c r="C65" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="D65" s="63" t="s">
+      <c r="D65" s="61" t="s">
         <v>33</v>
       </c>
       <c r="E65" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F65" s="58" t="s">
+      <c r="F65" s="66" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66" s="61"/>
-      <c r="B66" s="64"/>
-      <c r="C66" s="64"/>
-      <c r="D66" s="64"/>
+      <c r="A66" s="59"/>
+      <c r="B66" s="62"/>
+      <c r="C66" s="62"/>
+      <c r="D66" s="62"/>
       <c r="E66" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="F66" s="59"/>
+      <c r="F66" s="67"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" s="62"/>
-      <c r="B67" s="65"/>
-      <c r="C67" s="65"/>
-      <c r="D67" s="65"/>
+      <c r="A67" s="60"/>
+      <c r="B67" s="63"/>
+      <c r="C67" s="63"/>
+      <c r="D67" s="63"/>
       <c r="E67" s="6"/>
       <c r="F67" s="31"/>
     </row>
@@ -3747,16 +3814,16 @@
       <c r="F68" s="7"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="60">
+      <c r="A69" s="58">
         <v>11</v>
       </c>
-      <c r="B69" s="63" t="s">
+      <c r="B69" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="C69" s="63" t="s">
+      <c r="C69" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="D69" s="63" t="s">
+      <c r="D69" s="61" t="s">
         <v>26</v>
       </c>
       <c r="E69" s="17" t="s">
@@ -3765,20 +3832,20 @@
       <c r="F69" s="31"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="61"/>
-      <c r="B70" s="64"/>
-      <c r="C70" s="64"/>
-      <c r="D70" s="64"/>
+      <c r="A70" s="59"/>
+      <c r="B70" s="62"/>
+      <c r="C70" s="62"/>
+      <c r="D70" s="62"/>
       <c r="E70" s="17" t="s">
         <v>28</v>
       </c>
       <c r="F70" s="31"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" s="62"/>
-      <c r="B71" s="65"/>
-      <c r="C71" s="65"/>
-      <c r="D71" s="65"/>
+      <c r="A71" s="60"/>
+      <c r="B71" s="63"/>
+      <c r="C71" s="63"/>
+      <c r="D71" s="63"/>
       <c r="E71" s="17" t="s">
         <v>29</v>
       </c>
@@ -3792,16 +3859,16 @@
       <c r="E74" s="9"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="68">
+      <c r="A75" s="56">
         <v>6</v>
       </c>
-      <c r="B75" s="66" t="s">
+      <c r="B75" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C75" s="66" t="s">
+      <c r="C75" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="D75" s="66" t="s">
+      <c r="D75" s="54" t="s">
         <v>19</v>
       </c>
       <c r="E75" s="12" t="s">
@@ -3809,10 +3876,10 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A76" s="69"/>
-      <c r="B76" s="67"/>
-      <c r="C76" s="67"/>
-      <c r="D76" s="67"/>
+      <c r="A76" s="57"/>
+      <c r="B76" s="55"/>
+      <c r="C76" s="55"/>
+      <c r="D76" s="55"/>
       <c r="E76" s="12" t="s">
         <v>31</v>
       </c>
@@ -3877,6 +3944,40 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="C44:C50"/>
+    <mergeCell ref="B44:B50"/>
+    <mergeCell ref="D44:D50"/>
+    <mergeCell ref="A44:A50"/>
+    <mergeCell ref="A52:A58"/>
+    <mergeCell ref="B52:B58"/>
+    <mergeCell ref="C52:C58"/>
+    <mergeCell ref="D52:D58"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="D37:D42"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="B37:B42"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="D65:D67"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C22:C28"/>
+    <mergeCell ref="D22:D28"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="B2:B8"/>
     <mergeCell ref="C2:C8"/>
@@ -3893,40 +3994,6 @@
     <mergeCell ref="B10:B16"/>
     <mergeCell ref="C10:C16"/>
     <mergeCell ref="D10:D16"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C22:C28"/>
-    <mergeCell ref="D22:D28"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="D65:D67"/>
-    <mergeCell ref="C37:C42"/>
-    <mergeCell ref="D37:D42"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="B37:B42"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="C44:C50"/>
-    <mergeCell ref="B44:B50"/>
-    <mergeCell ref="D44:D50"/>
-    <mergeCell ref="A44:A50"/>
-    <mergeCell ref="A52:A58"/>
-    <mergeCell ref="B52:B58"/>
-    <mergeCell ref="C52:C58"/>
-    <mergeCell ref="D52:D58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3970,16 +4037,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="54">
+      <c r="A2" s="50">
         <v>1</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="52" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="14" t="s">
@@ -3990,10 +4057,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="55"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
       <c r="E3" s="15" t="s">
         <v>60</v>
       </c>
@@ -4002,70 +4069,70 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="55"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
       <c r="E4" s="15" t="s">
         <v>64</v>
       </c>
       <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="55"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
+      <c r="A5" s="51"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
       <c r="E5" s="15" t="s">
         <v>65</v>
       </c>
       <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="55"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
+      <c r="A6" s="51"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
       <c r="E6" s="15" t="s">
         <v>184</v>
       </c>
       <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="55"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
+      <c r="A7" s="51"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
       <c r="E7" s="15" t="s">
         <v>67</v>
       </c>
       <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="55"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
       <c r="E8" s="15" t="s">
         <v>61</v>
       </c>
       <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="55"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
       <c r="E9" s="15" t="s">
         <v>62</v>
       </c>
       <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="56"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
       <c r="E10" s="15" t="s">
         <v>14</v>
       </c>
@@ -4080,16 +4147,16 @@
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="54">
+      <c r="A12" s="50">
         <v>2</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="52" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="15" t="s">
@@ -4100,40 +4167,40 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="55"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
+      <c r="A13" s="51"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
       <c r="E13" s="15" t="s">
         <v>103</v>
       </c>
       <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="55"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
       <c r="E14" s="15" t="s">
         <v>104</v>
       </c>
       <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="55"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
+      <c r="A15" s="51"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
       <c r="E15" s="15" t="s">
         <v>105</v>
       </c>
       <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="56"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
+      <c r="A16" s="64"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
       <c r="E16" s="11" t="s">
         <v>51</v>
       </c>
@@ -4148,16 +4215,16 @@
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="54">
+      <c r="A18" s="50">
         <v>3</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="47" t="s">
+      <c r="D18" s="52" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="15" t="s">
@@ -4168,50 +4235,50 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="55"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
+      <c r="A19" s="51"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
       <c r="E19" s="15" t="s">
         <v>103</v>
       </c>
       <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="55"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
+      <c r="A20" s="51"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
       <c r="E20" s="15" t="s">
         <v>107</v>
       </c>
       <c r="F20" s="21"/>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="55"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
+      <c r="A21" s="51"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
       <c r="E21" s="15" t="s">
         <v>108</v>
       </c>
       <c r="F21" s="21"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="55"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
+      <c r="A22" s="51"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
       <c r="E22" s="15" t="s">
         <v>110</v>
       </c>
       <c r="F22" s="21"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="55"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
+      <c r="A23" s="51"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
       <c r="E23" s="15" t="s">
         <v>109</v>
       </c>
@@ -4226,16 +4293,16 @@
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="54">
+      <c r="A25" s="50">
         <v>4</v>
       </c>
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="47" t="s">
+      <c r="C25" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="47" t="s">
+      <c r="D25" s="52" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="15" t="s">
@@ -4244,10 +4311,10 @@
       <c r="F25" s="21"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="55"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
+      <c r="A26" s="51"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
       <c r="E26" s="15" t="s">
         <v>112</v>
       </c>
@@ -4262,16 +4329,16 @@
       <c r="F27" s="7"/>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="54">
+      <c r="A28" s="50">
         <v>5</v>
       </c>
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="47" t="s">
+      <c r="C28" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="D28" s="47" t="s">
+      <c r="D28" s="52" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="15" t="s">
@@ -4282,10 +4349,10 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="55"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
+      <c r="A29" s="51"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
       <c r="E29" s="15" t="s">
         <v>17</v>
       </c>
@@ -4300,16 +4367,16 @@
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="54">
+      <c r="A31" s="50">
         <v>6</v>
       </c>
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="47" t="s">
+      <c r="C31" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="D31" s="47" t="s">
+      <c r="D31" s="52" t="s">
         <v>43</v>
       </c>
       <c r="E31" s="14" t="s">
@@ -4320,30 +4387,30 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="55"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
+      <c r="A32" s="51"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
       <c r="E32" s="15" t="s">
         <v>117</v>
       </c>
       <c r="F32" s="21"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="55"/>
-      <c r="B33" s="48"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
+      <c r="A33" s="51"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
       <c r="E33" s="15" t="s">
         <v>115</v>
       </c>
       <c r="F33" s="21"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="56"/>
-      <c r="B34" s="49"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="49"/>
+      <c r="A34" s="64"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="65"/>
       <c r="E34" s="15" t="s">
         <v>22</v>
       </c>
@@ -4358,16 +4425,16 @@
       <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="54">
+      <c r="A36" s="50">
         <v>7</v>
       </c>
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="47" t="s">
+      <c r="D36" s="52" t="s">
         <v>24</v>
       </c>
       <c r="E36" s="15" t="s">
@@ -4376,20 +4443,20 @@
       <c r="F36" s="21"/>
     </row>
     <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="55"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
+      <c r="A37" s="51"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
       <c r="E37" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F37" s="21"/>
     </row>
     <row r="38" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="56"/>
-      <c r="B38" s="49"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="49"/>
+      <c r="A38" s="64"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
       <c r="E38" s="15" t="s">
         <v>36</v>
       </c>
@@ -4404,16 +4471,16 @@
       <c r="F39" s="7"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="54">
+      <c r="A40" s="50">
         <v>8</v>
       </c>
-      <c r="B40" s="47" t="s">
+      <c r="B40" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="47" t="s">
+      <c r="C40" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="D40" s="47" t="s">
+      <c r="D40" s="52" t="s">
         <v>118</v>
       </c>
       <c r="E40" s="21" t="s">
@@ -4422,70 +4489,70 @@
       <c r="F40" s="21"/>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="55"/>
-      <c r="B41" s="48"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
+      <c r="A41" s="51"/>
+      <c r="B41" s="53"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="53"/>
       <c r="E41" s="21" t="s">
         <v>120</v>
       </c>
       <c r="F41" s="21"/>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="55"/>
-      <c r="B42" s="48"/>
-      <c r="C42" s="48"/>
-      <c r="D42" s="48"/>
+      <c r="A42" s="51"/>
+      <c r="B42" s="53"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="53"/>
       <c r="E42" s="21" t="s">
         <v>121</v>
       </c>
       <c r="F42" s="21"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="55"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="48"/>
-      <c r="D43" s="48"/>
+      <c r="A43" s="51"/>
+      <c r="B43" s="53"/>
+      <c r="C43" s="53"/>
+      <c r="D43" s="53"/>
       <c r="E43" s="21" t="s">
         <v>122</v>
       </c>
       <c r="F43" s="21"/>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="55"/>
-      <c r="B44" s="48"/>
-      <c r="C44" s="48"/>
-      <c r="D44" s="48"/>
+      <c r="A44" s="51"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
       <c r="E44" s="21" t="s">
         <v>124</v>
       </c>
       <c r="F44" s="21"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="55"/>
-      <c r="B45" s="48"/>
-      <c r="C45" s="48"/>
-      <c r="D45" s="48"/>
+      <c r="A45" s="51"/>
+      <c r="B45" s="53"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
       <c r="E45" s="21" t="s">
         <v>125</v>
       </c>
       <c r="F45" s="21"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="55"/>
-      <c r="B46" s="48"/>
-      <c r="C46" s="48"/>
-      <c r="D46" s="48"/>
+      <c r="A46" s="51"/>
+      <c r="B46" s="53"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="53"/>
       <c r="E46" s="21" t="s">
         <v>123</v>
       </c>
       <c r="F46" s="21"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="55"/>
-      <c r="B47" s="48"/>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
+      <c r="A47" s="51"/>
+      <c r="B47" s="53"/>
+      <c r="C47" s="53"/>
+      <c r="D47" s="53"/>
       <c r="E47" s="14" t="s">
         <v>76</v>
       </c>
@@ -4501,6 +4568,30 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A40:A47"/>
+    <mergeCell ref="B40:B47"/>
+    <mergeCell ref="C40:C47"/>
+    <mergeCell ref="D40:D47"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="B2:B10"/>
     <mergeCell ref="C2:C10"/>
@@ -4509,30 +4600,6 @@
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
     <mergeCell ref="D12:D16"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A40:A47"/>
-    <mergeCell ref="B40:B47"/>
-    <mergeCell ref="C40:C47"/>
-    <mergeCell ref="D40:D47"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="A36:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4540,10 +4607,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD0B509-A153-4B31-95B8-BC32DC1B6A3B}">
-  <dimension ref="B2:J18"/>
+  <dimension ref="B2:J26"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4742,14 +4809,47 @@
         <v>147</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="F17" s="39" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="F18" s="40" t="s">
         <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B20" s="42" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B21" s="41" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B22" s="39" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B23" s="39" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B24" s="39" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B25" s="40"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B26" s="74" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -4759,989 +4859,975 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A678BF3-4A56-4A1E-B2DF-017A74834050}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.26953125" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="78"/>
+    <col min="1" max="1" width="1.26953125" style="84" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="92"/>
     <col min="3" max="3" width="73" customWidth="1"/>
-    <col min="4" max="4" width="3.36328125" customWidth="1"/>
+    <col min="4" max="4" width="1.54296875" style="84" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="92"/>
     <col min="6" max="6" width="58.453125" customWidth="1"/>
-    <col min="7" max="7" width="3.36328125" customWidth="1"/>
+    <col min="7" max="7" width="1.453125" style="82" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="92"/>
     <col min="9" max="9" width="63.36328125" customWidth="1"/>
     <col min="10" max="10" width="2.1796875" customWidth="1"/>
+    <col min="11" max="11" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="49.54296875" customWidth="1"/>
+    <col min="13" max="13" width="2.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="83"/>
-      <c r="B1" s="72" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="81"/>
+      <c r="B1" s="73" t="s">
         <v>190</v>
       </c>
-      <c r="C1" s="72"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="72" t="s">
+      <c r="C1" s="73"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="73" t="s">
         <v>191</v>
       </c>
-      <c r="F1" s="72"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="72" t="s">
+      <c r="F1" s="73"/>
+      <c r="H1" s="73" t="s">
         <v>192</v>
       </c>
-      <c r="I1" s="72"/>
-      <c r="J1" s="83"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="83"/>
-      <c r="B2" s="76"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="83"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="83"/>
-      <c r="B3" s="75" t="s">
+      <c r="I1" s="73"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="73" t="s">
+        <v>192</v>
+      </c>
+      <c r="L1" s="73"/>
+      <c r="M1" s="81"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="81"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="47"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="47"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="81"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="81"/>
+      <c r="B3" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="48" t="s">
         <v>186</v>
       </c>
-      <c r="D3" s="79"/>
-      <c r="E3" s="73" t="s">
+      <c r="D3" s="86"/>
+      <c r="E3" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="F3" s="73" t="s">
+      <c r="F3" s="48" t="s">
         <v>186</v>
       </c>
-      <c r="G3" s="79"/>
-      <c r="H3" s="73" t="s">
+      <c r="H3" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="I3" s="73" t="s">
+      <c r="I3" s="48" t="s">
         <v>186</v>
       </c>
-      <c r="J3" s="83"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="83"/>
-      <c r="B4" s="75" t="s">
+      <c r="J3" s="81"/>
+      <c r="K3" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="L3" s="75" t="s">
+        <v>186</v>
+      </c>
+      <c r="M3" s="81"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="81"/>
+      <c r="B4" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="48" t="s">
         <v>202</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="73" t="s">
+      <c r="D4" s="87"/>
+      <c r="E4" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="F4" s="73" t="s">
+      <c r="F4" s="48" t="s">
         <v>203</v>
       </c>
-      <c r="G4" s="80"/>
-      <c r="H4" s="73" t="s">
+      <c r="H4" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="I4" s="73" t="s">
+      <c r="I4" s="48" t="s">
         <v>204</v>
       </c>
-      <c r="J4" s="83"/>
-    </row>
-    <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="83"/>
-      <c r="B5" s="75" t="s">
+      <c r="J4" s="81"/>
+      <c r="K4" s="48" t="s">
+        <v>187</v>
+      </c>
+      <c r="L4" s="75" t="s">
+        <v>250</v>
+      </c>
+      <c r="M4" s="81"/>
+    </row>
+    <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="81"/>
+      <c r="B5" s="89" t="s">
         <v>188</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="D5" s="80"/>
-      <c r="E5" s="73" t="s">
+      <c r="D5" s="87"/>
+      <c r="E5" s="89" t="s">
         <v>188</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="G5" s="80"/>
-      <c r="H5" s="73" t="s">
+      <c r="H5" s="89" t="s">
         <v>188</v>
       </c>
       <c r="I5" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="J5" s="83"/>
-    </row>
-    <row r="6" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="83"/>
-      <c r="B6" s="75" t="s">
+      <c r="J5" s="81"/>
+      <c r="K5" s="77" t="s">
+        <v>188</v>
+      </c>
+      <c r="L5" s="76" t="s">
+        <v>254</v>
+      </c>
+      <c r="M5" s="81"/>
+    </row>
+    <row r="6" spans="1:13" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="81"/>
+      <c r="B6" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="73" t="s">
+      <c r="C6" s="48"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="F6" s="73"/>
-      <c r="G6" s="81"/>
-      <c r="H6" s="73" t="s">
+      <c r="F6" s="48"/>
+      <c r="H6" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="I6" s="73"/>
-      <c r="J6" s="83"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="83"/>
-      <c r="B7" s="77"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="83"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="83"/>
-      <c r="B8" s="75" t="s">
+      <c r="I6" s="48"/>
+      <c r="J6" s="81"/>
+      <c r="K6" s="70" t="s">
+        <v>189</v>
+      </c>
+      <c r="L6" s="78" t="s">
+        <v>253</v>
+      </c>
+      <c r="M6" s="81"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="81"/>
+      <c r="B7" s="90"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="49"/>
+      <c r="H7" s="90"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="71"/>
+      <c r="L7" s="79" t="s">
+        <v>251</v>
+      </c>
+      <c r="M7" s="81"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="81"/>
+      <c r="B8" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="48" t="s">
         <v>193</v>
       </c>
-      <c r="D8" s="79"/>
-      <c r="E8" s="73" t="s">
+      <c r="D8" s="86"/>
+      <c r="E8" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="F8" s="73" t="s">
+      <c r="F8" s="48" t="s">
         <v>193</v>
       </c>
-      <c r="G8" s="79"/>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="I8" s="73" t="s">
+      <c r="I8" s="48" t="s">
         <v>193</v>
       </c>
-      <c r="J8" s="83"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="83"/>
-      <c r="B9" s="75" t="s">
+      <c r="J8" s="81"/>
+      <c r="K8" s="72"/>
+      <c r="L8" s="80" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="81"/>
+      <c r="B9" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="C9" s="73" t="s">
+      <c r="C9" s="48" t="s">
         <v>202</v>
       </c>
-      <c r="D9" s="80"/>
-      <c r="E9" s="73" t="s">
+      <c r="D9" s="87"/>
+      <c r="E9" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="F9" s="73" t="s">
+      <c r="F9" s="48" t="s">
         <v>203</v>
       </c>
-      <c r="G9" s="80"/>
-      <c r="H9" s="73" t="s">
+      <c r="H9" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="I9" s="73" t="s">
+      <c r="I9" s="48" t="s">
         <v>224</v>
       </c>
-      <c r="J9" s="83"/>
-    </row>
-    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="83"/>
-      <c r="B10" s="75" t="s">
+      <c r="J9" s="81"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+    </row>
+    <row r="10" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="81"/>
+      <c r="B10" s="89" t="s">
         <v>188</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="D10" s="80"/>
-      <c r="E10" s="73" t="s">
+      <c r="D10" s="87"/>
+      <c r="E10" s="89" t="s">
         <v>188</v>
       </c>
       <c r="F10" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="G10" s="80"/>
-      <c r="H10" s="73" t="s">
+      <c r="H10" s="89" t="s">
         <v>188</v>
       </c>
       <c r="I10" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="J10" s="83"/>
-    </row>
-    <row r="11" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="83"/>
-      <c r="B11" s="75" t="s">
+      <c r="J10" s="81"/>
+    </row>
+    <row r="11" spans="1:13" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="81"/>
+      <c r="B11" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="73" t="s">
+      <c r="C11" s="48"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="F11" s="73"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="73" t="s">
+      <c r="F11" s="48"/>
+      <c r="H11" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="I11" s="73"/>
-      <c r="J11" s="83"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="83"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="83"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="83"/>
-      <c r="B13" s="75" t="s">
+      <c r="I11" s="48"/>
+      <c r="J11" s="81"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="81"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="49"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="81"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="81"/>
+      <c r="B13" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="73" t="s">
+      <c r="C13" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="D13" s="79"/>
-      <c r="E13" s="73" t="s">
+      <c r="D13" s="86"/>
+      <c r="E13" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="F13" s="73" t="s">
+      <c r="F13" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="G13" s="79"/>
-      <c r="H13" s="73" t="s">
+      <c r="H13" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="I13" s="73" t="s">
+      <c r="I13" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="J13" s="83"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="83"/>
-      <c r="B14" s="75" t="s">
+      <c r="J13" s="81"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="81"/>
+      <c r="B14" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="C14" s="73" t="s">
+      <c r="C14" s="48" t="s">
         <v>202</v>
       </c>
-      <c r="D14" s="80"/>
-      <c r="E14" s="73" t="s">
+      <c r="D14" s="87"/>
+      <c r="E14" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="F14" s="73"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="73" t="s">
+      <c r="F14" s="48"/>
+      <c r="H14" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="I14" s="73"/>
-      <c r="J14" s="83"/>
-    </row>
-    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="83"/>
-      <c r="B15" s="75" t="s">
+      <c r="I14" s="48"/>
+      <c r="J14" s="81"/>
+    </row>
+    <row r="15" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="81"/>
+      <c r="B15" s="89" t="s">
         <v>188</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="D15" s="80"/>
-      <c r="E15" s="73" t="s">
+      <c r="D15" s="87"/>
+      <c r="E15" s="89" t="s">
         <v>188</v>
       </c>
       <c r="F15" s="21"/>
-      <c r="G15" s="80"/>
-      <c r="H15" s="73" t="s">
+      <c r="H15" s="89" t="s">
         <v>188</v>
       </c>
       <c r="I15" s="21"/>
-      <c r="J15" s="83"/>
-    </row>
-    <row r="16" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="83"/>
-      <c r="B16" s="75" t="s">
+      <c r="J15" s="81"/>
+    </row>
+    <row r="16" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="81"/>
+      <c r="B16" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="C16" s="73"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="73" t="s">
+      <c r="C16" s="48"/>
+      <c r="D16" s="88"/>
+      <c r="E16" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="F16" s="73"/>
-      <c r="G16" s="81"/>
-      <c r="H16" s="73" t="s">
+      <c r="F16" s="48"/>
+      <c r="H16" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="I16" s="73"/>
-      <c r="J16" s="83"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="81"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="83"/>
-      <c r="B17" s="77"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="83"/>
+      <c r="A17" s="81"/>
+      <c r="B17" s="90"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="49"/>
+      <c r="H17" s="90"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="81"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="83"/>
-      <c r="B18" s="75" t="s">
+      <c r="A18" s="81"/>
+      <c r="B18" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="C18" s="73" t="s">
+      <c r="C18" s="48" t="s">
         <v>195</v>
       </c>
-      <c r="D18" s="79"/>
-      <c r="E18" s="73" t="s">
+      <c r="D18" s="86"/>
+      <c r="E18" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="F18" s="73" t="s">
+      <c r="F18" s="48" t="s">
         <v>195</v>
       </c>
-      <c r="G18" s="79"/>
-      <c r="H18" s="73" t="s">
+      <c r="H18" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="I18" s="73" t="s">
+      <c r="I18" s="48" t="s">
         <v>195</v>
       </c>
-      <c r="J18" s="83"/>
+      <c r="J18" s="81"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="83"/>
-      <c r="B19" s="75" t="s">
+      <c r="A19" s="81"/>
+      <c r="B19" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="C19" s="73" t="s">
+      <c r="C19" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="D19" s="80"/>
-      <c r="E19" s="73" t="s">
+      <c r="D19" s="87"/>
+      <c r="E19" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="F19" s="73" t="s">
+      <c r="F19" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="G19" s="80"/>
-      <c r="H19" s="73" t="s">
+      <c r="H19" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="I19" s="73" t="s">
+      <c r="I19" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="J19" s="83"/>
+      <c r="J19" s="81"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="83"/>
-      <c r="B20" s="75" t="s">
+      <c r="A20" s="81"/>
+      <c r="B20" s="89" t="s">
         <v>188</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="D20" s="80"/>
-      <c r="E20" s="73" t="s">
+      <c r="D20" s="87"/>
+      <c r="E20" s="89" t="s">
         <v>188</v>
       </c>
       <c r="F20" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="G20" s="80"/>
-      <c r="H20" s="73" t="s">
+      <c r="H20" s="89" t="s">
         <v>188</v>
       </c>
       <c r="I20" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="J20" s="83"/>
+      <c r="J20" s="81"/>
     </row>
     <row r="21" spans="1:10" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="83"/>
-      <c r="B21" s="75" t="s">
+      <c r="A21" s="81"/>
+      <c r="B21" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="C21" s="73"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="73" t="s">
+      <c r="C21" s="48"/>
+      <c r="D21" s="88"/>
+      <c r="E21" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="F21" s="73"/>
-      <c r="G21" s="81"/>
-      <c r="H21" s="73" t="s">
+      <c r="F21" s="48"/>
+      <c r="H21" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="I21" s="73"/>
-      <c r="J21" s="83"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="81"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="83"/>
-      <c r="B22" s="77"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="83"/>
+      <c r="A22" s="81"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="49"/>
+      <c r="H22" s="90"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="81"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="83"/>
-      <c r="B23" s="75" t="s">
+      <c r="A23" s="81"/>
+      <c r="B23" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="C23" s="73" t="s">
+      <c r="C23" s="48" t="s">
         <v>196</v>
       </c>
-      <c r="D23" s="79"/>
-      <c r="E23" s="73" t="s">
+      <c r="D23" s="86"/>
+      <c r="E23" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="F23" s="73" t="s">
+      <c r="F23" s="48" t="s">
         <v>196</v>
       </c>
-      <c r="G23" s="79"/>
-      <c r="H23" s="73" t="s">
+      <c r="H23" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="I23" s="73" t="s">
+      <c r="I23" s="48" t="s">
         <v>196</v>
       </c>
-      <c r="J23" s="83"/>
+      <c r="J23" s="81"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="83"/>
-      <c r="B24" s="75" t="s">
+      <c r="A24" s="81"/>
+      <c r="B24" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="C24" s="73" t="s">
+      <c r="C24" s="48" t="s">
         <v>214</v>
       </c>
-      <c r="D24" s="80"/>
-      <c r="E24" s="73" t="s">
+      <c r="D24" s="87"/>
+      <c r="E24" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="F24" s="73" t="s">
+      <c r="F24" s="48" t="s">
         <v>234</v>
       </c>
-      <c r="G24" s="80"/>
-      <c r="H24" s="73" t="s">
+      <c r="H24" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="I24" s="73" t="s">
+      <c r="I24" s="48" t="s">
         <v>225</v>
       </c>
-      <c r="J24" s="83"/>
+      <c r="J24" s="81"/>
     </row>
     <row r="25" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="83"/>
-      <c r="B25" s="75" t="s">
+      <c r="A25" s="81"/>
+      <c r="B25" s="89" t="s">
         <v>188</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="D25" s="80"/>
-      <c r="E25" s="73" t="s">
+      <c r="D25" s="87"/>
+      <c r="E25" s="89" t="s">
         <v>188</v>
       </c>
       <c r="F25" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="G25" s="80"/>
-      <c r="H25" s="73" t="s">
+      <c r="H25" s="89" t="s">
         <v>188</v>
       </c>
       <c r="I25" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="J25" s="83"/>
+      <c r="J25" s="81"/>
     </row>
     <row r="26" spans="1:10" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="83"/>
-      <c r="B26" s="75" t="s">
+      <c r="A26" s="81"/>
+      <c r="B26" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="C26" s="73"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="73" t="s">
+      <c r="C26" s="48"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="F26" s="73"/>
-      <c r="G26" s="81"/>
-      <c r="H26" s="73" t="s">
+      <c r="F26" s="48"/>
+      <c r="H26" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="I26" s="73"/>
-      <c r="J26" s="83"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="81"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="83"/>
-      <c r="B27" s="77"/>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="74"/>
-      <c r="I27" s="74"/>
-      <c r="J27" s="83"/>
+      <c r="A27" s="81"/>
+      <c r="B27" s="90"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="49"/>
+      <c r="H27" s="90"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="81"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="83"/>
-      <c r="B28" s="75" t="s">
+      <c r="A28" s="81"/>
+      <c r="B28" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="C28" s="73" t="s">
+      <c r="C28" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="D28" s="79"/>
-      <c r="E28" s="73" t="s">
+      <c r="D28" s="86"/>
+      <c r="E28" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="F28" s="73" t="s">
+      <c r="F28" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="G28" s="79"/>
-      <c r="H28" s="73" t="s">
+      <c r="H28" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="I28" s="73" t="s">
+      <c r="I28" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="J28" s="83"/>
+      <c r="J28" s="81"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="83"/>
-      <c r="B29" s="75" t="s">
+      <c r="A29" s="81"/>
+      <c r="B29" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="C29" s="73" t="s">
+      <c r="C29" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="D29" s="80"/>
-      <c r="E29" s="73" t="s">
+      <c r="D29" s="87"/>
+      <c r="E29" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="F29" s="73" t="s">
+      <c r="F29" s="48" t="s">
         <v>236</v>
       </c>
-      <c r="G29" s="80"/>
-      <c r="H29" s="73" t="s">
+      <c r="H29" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="I29" s="73" t="s">
+      <c r="I29" s="48" t="s">
         <v>227</v>
       </c>
-      <c r="J29" s="83"/>
+      <c r="J29" s="81"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="83"/>
-      <c r="B30" s="75" t="s">
+      <c r="A30" s="81"/>
+      <c r="B30" s="89" t="s">
         <v>188</v>
       </c>
       <c r="C30" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="D30" s="80"/>
-      <c r="E30" s="73" t="s">
+      <c r="D30" s="87"/>
+      <c r="E30" s="89" t="s">
         <v>188</v>
       </c>
-      <c r="F30" s="73" t="s">
+      <c r="F30" s="48" t="s">
         <v>237</v>
       </c>
-      <c r="G30" s="80"/>
-      <c r="H30" s="73" t="s">
+      <c r="H30" s="89" t="s">
         <v>188</v>
       </c>
-      <c r="I30" s="73" t="s">
+      <c r="I30" s="48" t="s">
         <v>228</v>
       </c>
-      <c r="J30" s="83"/>
+      <c r="J30" s="81"/>
     </row>
     <row r="31" spans="1:10" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="83"/>
-      <c r="B31" s="75" t="s">
+      <c r="A31" s="81"/>
+      <c r="B31" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="C31" s="73"/>
-      <c r="D31" s="81"/>
-      <c r="E31" s="73" t="s">
+      <c r="C31" s="48"/>
+      <c r="D31" s="88"/>
+      <c r="E31" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="F31" s="73"/>
-      <c r="G31" s="81"/>
-      <c r="H31" s="73" t="s">
+      <c r="F31" s="48"/>
+      <c r="H31" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="I31" s="73"/>
-      <c r="J31" s="83"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="81"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" s="83"/>
-      <c r="B32" s="77"/>
-      <c r="C32" s="74"/>
-      <c r="D32" s="74"/>
-      <c r="E32" s="74"/>
-      <c r="F32" s="74"/>
-      <c r="G32" s="74"/>
-      <c r="H32" s="74"/>
-      <c r="I32" s="74"/>
-      <c r="J32" s="83"/>
+      <c r="A32" s="81"/>
+      <c r="B32" s="90"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="49"/>
+      <c r="H32" s="90"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="81"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="83"/>
-      <c r="B33" s="75" t="s">
+      <c r="A33" s="81"/>
+      <c r="B33" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="C33" s="73" t="s">
+      <c r="C33" s="48" t="s">
         <v>196</v>
       </c>
-      <c r="D33" s="79"/>
-      <c r="E33" s="73" t="s">
+      <c r="D33" s="86"/>
+      <c r="E33" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="F33" s="73" t="s">
+      <c r="F33" s="48" t="s">
         <v>196</v>
       </c>
-      <c r="G33" s="79"/>
-      <c r="H33" s="73" t="s">
+      <c r="H33" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="I33" s="73" t="s">
+      <c r="I33" s="48" t="s">
         <v>196</v>
       </c>
-      <c r="J33" s="83"/>
+      <c r="J33" s="81"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="83"/>
-      <c r="B34" s="75" t="s">
+      <c r="A34" s="81"/>
+      <c r="B34" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="C34" s="73" t="s">
+      <c r="C34" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="D34" s="80"/>
-      <c r="E34" s="73" t="s">
+      <c r="D34" s="87"/>
+      <c r="E34" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="F34" s="73" t="s">
+      <c r="F34" s="48" t="s">
         <v>200</v>
       </c>
-      <c r="G34" s="80"/>
-      <c r="H34" s="73" t="s">
+      <c r="H34" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="I34" s="73" t="s">
+      <c r="I34" s="48" t="s">
         <v>201</v>
       </c>
-      <c r="J34" s="83"/>
+      <c r="J34" s="81"/>
     </row>
     <row r="35" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="83"/>
-      <c r="B35" s="75" t="s">
+      <c r="A35" s="81"/>
+      <c r="B35" s="89" t="s">
         <v>188</v>
       </c>
       <c r="C35" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="D35" s="80"/>
-      <c r="E35" s="73" t="s">
+      <c r="D35" s="87"/>
+      <c r="E35" s="89" t="s">
         <v>188</v>
       </c>
       <c r="F35" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="G35" s="80"/>
-      <c r="H35" s="73" t="s">
+      <c r="H35" s="89" t="s">
         <v>188</v>
       </c>
       <c r="I35" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="J35" s="83"/>
+      <c r="J35" s="81"/>
     </row>
     <row r="36" spans="1:10" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="83"/>
-      <c r="B36" s="75" t="s">
+      <c r="A36" s="81"/>
+      <c r="B36" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="C36" s="73"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="73" t="s">
+      <c r="C36" s="48"/>
+      <c r="D36" s="88"/>
+      <c r="E36" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="F36" s="73"/>
-      <c r="G36" s="81"/>
-      <c r="H36" s="73" t="s">
+      <c r="F36" s="48"/>
+      <c r="H36" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="I36" s="73"/>
-      <c r="J36" s="83"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="81"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A37" s="83"/>
-      <c r="B37" s="77"/>
-      <c r="C37" s="74"/>
-      <c r="D37" s="82"/>
-      <c r="E37" s="74"/>
-      <c r="F37" s="74"/>
-      <c r="G37" s="74"/>
-      <c r="H37" s="74"/>
-      <c r="I37" s="74"/>
-      <c r="J37" s="83"/>
+      <c r="A37" s="81"/>
+      <c r="B37" s="90"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="85"/>
+      <c r="E37" s="90"/>
+      <c r="F37" s="49"/>
+      <c r="H37" s="90"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="81"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="83"/>
-      <c r="B38" s="75" t="s">
+      <c r="A38" s="81"/>
+      <c r="B38" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="C38" s="73" t="s">
+      <c r="C38" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="D38" s="79"/>
-      <c r="E38" s="73" t="s">
+      <c r="D38" s="86"/>
+      <c r="E38" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="F38" s="73" t="s">
+      <c r="F38" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="G38" s="79"/>
-      <c r="H38" s="73" t="s">
+      <c r="H38" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="I38" s="73" t="s">
+      <c r="I38" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="J38" s="83"/>
+      <c r="J38" s="81"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" s="83"/>
-      <c r="B39" s="75" t="s">
+      <c r="A39" s="81"/>
+      <c r="B39" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="C39" s="73" t="s">
+      <c r="C39" s="48" t="s">
         <v>199</v>
       </c>
-      <c r="D39" s="80"/>
-      <c r="E39" s="73" t="s">
+      <c r="D39" s="87"/>
+      <c r="E39" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="F39" s="73" t="s">
+      <c r="F39" s="48" t="s">
         <v>239</v>
       </c>
-      <c r="G39" s="80"/>
-      <c r="H39" s="73" t="s">
+      <c r="H39" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="I39" s="73" t="s">
+      <c r="I39" s="48" t="s">
         <v>230</v>
       </c>
-      <c r="J39" s="83"/>
+      <c r="J39" s="81"/>
     </row>
     <row r="40" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="83"/>
-      <c r="B40" s="75" t="s">
+      <c r="A40" s="81"/>
+      <c r="B40" s="89" t="s">
         <v>188</v>
       </c>
       <c r="C40" s="21" t="s">
         <v>219</v>
       </c>
-      <c r="D40" s="80"/>
-      <c r="E40" s="73" t="s">
+      <c r="D40" s="87"/>
+      <c r="E40" s="89" t="s">
         <v>188</v>
       </c>
       <c r="F40" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="G40" s="80"/>
-      <c r="H40" s="73" t="s">
+      <c r="H40" s="89" t="s">
         <v>188</v>
       </c>
       <c r="I40" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="J40" s="83"/>
+      <c r="J40" s="81"/>
     </row>
     <row r="41" spans="1:10" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="83"/>
-      <c r="B41" s="75" t="s">
+      <c r="A41" s="81"/>
+      <c r="B41" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="C41" s="73"/>
-      <c r="D41" s="81"/>
-      <c r="E41" s="73" t="s">
+      <c r="C41" s="48"/>
+      <c r="D41" s="88"/>
+      <c r="E41" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="F41" s="73"/>
-      <c r="G41" s="81"/>
-      <c r="H41" s="73" t="s">
+      <c r="F41" s="48"/>
+      <c r="H41" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="I41" s="73"/>
-      <c r="J41" s="83"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="81"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A42" s="83"/>
-      <c r="B42" s="77"/>
-      <c r="C42" s="74"/>
-      <c r="D42" s="74"/>
-      <c r="E42" s="74"/>
-      <c r="F42" s="74"/>
-      <c r="G42" s="74"/>
-      <c r="H42" s="74"/>
-      <c r="I42" s="74"/>
-      <c r="J42" s="83"/>
+      <c r="A42" s="81"/>
+      <c r="B42" s="90"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="75"/>
+      <c r="E42" s="90"/>
+      <c r="F42" s="49"/>
+      <c r="H42" s="90"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="81"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A43" s="83"/>
-      <c r="B43" s="75" t="s">
+      <c r="A43" s="81"/>
+      <c r="B43" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="C43" s="73" t="s">
+      <c r="C43" s="48" t="s">
         <v>198</v>
       </c>
-      <c r="D43" s="79"/>
-      <c r="E43" s="75" t="s">
+      <c r="D43" s="86"/>
+      <c r="E43" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="F43" s="73" t="s">
+      <c r="F43" s="48" t="s">
         <v>198</v>
       </c>
-      <c r="G43" s="79"/>
-      <c r="H43" s="75" t="s">
+      <c r="H43" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="I43" s="73" t="s">
+      <c r="I43" s="48" t="s">
         <v>198</v>
       </c>
-      <c r="J43" s="83"/>
+      <c r="J43" s="81"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A44" s="83"/>
-      <c r="B44" s="75" t="s">
+      <c r="A44" s="81"/>
+      <c r="B44" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="C44" s="73" t="s">
+      <c r="C44" s="48" t="s">
         <v>220</v>
       </c>
-      <c r="D44" s="80"/>
-      <c r="E44" s="75" t="s">
+      <c r="D44" s="87"/>
+      <c r="E44" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="F44" s="73" t="s">
+      <c r="F44" s="48" t="s">
         <v>241</v>
       </c>
-      <c r="G44" s="80"/>
-      <c r="H44" s="75" t="s">
+      <c r="H44" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="I44" s="73" t="s">
+      <c r="I44" s="48" t="s">
         <v>221</v>
       </c>
-      <c r="J44" s="83"/>
+      <c r="J44" s="81"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A45" s="83"/>
-      <c r="B45" s="75" t="s">
+      <c r="A45" s="81"/>
+      <c r="B45" s="89" t="s">
         <v>188</v>
       </c>
       <c r="C45" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="D45" s="80"/>
-      <c r="E45" s="75" t="s">
+      <c r="D45" s="87"/>
+      <c r="E45" s="89" t="s">
         <v>188</v>
       </c>
       <c r="F45" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="G45" s="80"/>
-      <c r="H45" s="75" t="s">
+      <c r="H45" s="89" t="s">
         <v>188</v>
       </c>
       <c r="I45" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="J45" s="83"/>
+      <c r="J45" s="81"/>
     </row>
     <row r="46" spans="1:10" ht="88" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="83"/>
-      <c r="B46" s="75" t="s">
+      <c r="A46" s="81"/>
+      <c r="B46" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="C46" s="73"/>
-      <c r="D46" s="81"/>
-      <c r="E46" s="75" t="s">
+      <c r="C46" s="48"/>
+      <c r="D46" s="88"/>
+      <c r="E46" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="F46" s="73"/>
-      <c r="G46" s="81"/>
-      <c r="H46" s="75" t="s">
+      <c r="F46" s="48"/>
+      <c r="H46" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="I46" s="73"/>
-      <c r="J46" s="83"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="81"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A47" s="83"/>
-      <c r="B47" s="77"/>
-      <c r="C47" s="74"/>
-      <c r="D47" s="74"/>
-      <c r="E47" s="77"/>
-      <c r="F47" s="74"/>
-      <c r="G47" s="74"/>
-      <c r="H47" s="77"/>
-      <c r="I47" s="74"/>
-      <c r="J47" s="83"/>
+      <c r="A47" s="81"/>
+      <c r="B47" s="90"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="75"/>
+      <c r="E47" s="90"/>
+      <c r="F47" s="49"/>
+      <c r="H47" s="90"/>
+      <c r="I47" s="49"/>
+      <c r="J47" s="81"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="D43:D46"/>
-    <mergeCell ref="A1:A47"/>
-    <mergeCell ref="J1:J47"/>
-    <mergeCell ref="G28:G31"/>
-    <mergeCell ref="G33:G36"/>
-    <mergeCell ref="G38:G41"/>
-    <mergeCell ref="G43:G46"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="G3:G6"/>
-    <mergeCell ref="G8:G11"/>
-    <mergeCell ref="G13:G16"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="G23:G26"/>
+  <mergeCells count="5">
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="K6:K8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="D33:D36"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="D8:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Updated UML to match the methods names, marked User/Admin/Customer done
</commit_message>
<xml_diff>
--- a/User Stories/NataliaUserStories.xlsx
+++ b/User Stories/NataliaUserStories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cad1acabf18afac6/Desktop/Software Design with AI for Cloud/Year_3/agile-labs3/Newsagent-Project/User Stories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="444" documentId="13_ncr:1_{7B2E17FA-F2A9-4DCC-A803-850E080333ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57F8BC66-1230-49D3-A591-B6675BDD9146}"/>
+  <xr:revisionPtr revIDLastSave="539" documentId="13_ncr:1_{7B2E17FA-F2A9-4DCC-A803-850E080333ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0D8BE94-FE48-44AC-9C91-AB97ABC9B086}"/>
   <bookViews>
-    <workbookView xWindow="10820" yWindow="500" windowWidth="27590" windowHeight="19310" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
+    <workbookView xWindow="15530" yWindow="2750" windowWidth="22160" windowHeight="16250" activeTab="2" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminUserStories" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="252">
   <si>
     <t>As an admin</t>
   </si>
@@ -428,15 +428,9 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>+deactivateCustomer() : void</t>
-  </si>
-  <si>
     <t>+generateInvoice() : void</t>
   </si>
   <si>
-    <t>+generateDeliveryDoc() : void</t>
-  </si>
-  <si>
     <t>- username : String</t>
   </si>
   <si>
@@ -458,9 +452,6 @@
     <t>+Newsagent : (username: String, password: String, role: String, customerDatabase: Database)</t>
   </si>
   <si>
-    <t>+Admin : (uesrname: String, password: String, role: String, userDatabase: Database)</t>
-  </si>
-  <si>
     <t>+getCustID() : void</t>
   </si>
   <si>
@@ -497,15 +488,9 @@
     <t>- lastName : String</t>
   </si>
   <si>
-    <t>- custAddress : String</t>
-  </si>
-  <si>
     <t>- phoneNo : String</t>
   </si>
   <si>
-    <t>+Customer(custID: int, firstName: String, lastName: String, custAddress: String, phoneNo: String)</t>
-  </si>
-  <si>
     <t>+setPhoneNo() : String</t>
   </si>
   <si>
@@ -515,30 +500,6 @@
     <t>+ createUserAccount(username: String, password: String, role: String): void</t>
   </si>
   <si>
-    <t>+ updateUserAccount(username: String, password: String, role: String): void</t>
-  </si>
-  <si>
-    <t>Admin extends User</t>
-  </si>
-  <si>
-    <t>Newsagent extends User</t>
-  </si>
-  <si>
-    <t>User and Customer standalone</t>
-  </si>
-  <si>
-    <t>+createNewCustomer(customerID: int, firstName: String, lastName: String, custAddress: String, phoneNo: String)</t>
-  </si>
-  <si>
-    <t>+updateCustomer (customerID: int, firstName: String, lastName: String, custAddress: String, phoneNo: String)</t>
-  </si>
-  <si>
-    <t>+readCustomer() : void</t>
-  </si>
-  <si>
-    <t>+printCustomer() : void</t>
-  </si>
-  <si>
     <t>I want to generate delivery docket report</t>
   </si>
   <si>
@@ -581,18 +542,6 @@
     <t>+User: (username: String, password: String, role: String, userDatabase: Database)</t>
   </si>
   <si>
-    <t>+ printUserAccount(): void</t>
-  </si>
-  <si>
-    <t>+ givePermission() : void</t>
-  </si>
-  <si>
-    <t>+ readUserAccount(): void</t>
-  </si>
-  <si>
-    <t>+ deleteUserAccount(): void</t>
-  </si>
-  <si>
     <t>Verify valid 0 &lt; custAddress &lt;= 20 characters</t>
   </si>
   <si>
@@ -771,13 +720,88 @@
   </si>
   <si>
     <t>DELETE FROM newsagentDetails WHERE newsagentID="2";</t>
+  </si>
+  <si>
+    <t>- address : String</t>
+  </si>
+  <si>
+    <t>+Customer(firstName: String, lastName: String, custAddress: String, phoneNo: String)</t>
+  </si>
+  <si>
+    <t>+Customer()</t>
+  </si>
+  <si>
+    <t>+getCustomerDetails(int id) : String</t>
+  </si>
+  <si>
+    <t>+getAllCustomerDetails() : String</t>
+  </si>
+  <si>
+    <t>+getCustomerOrder(int id) : String</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>+Admin()</t>
+  </si>
+  <si>
+    <t>+Newsagent()</t>
+  </si>
+  <si>
+    <t>+User()</t>
+  </si>
+  <si>
+    <t>+getUsername() : void</t>
+  </si>
+  <si>
+    <t>+getPassword() : void</t>
+  </si>
+  <si>
+    <t>+getRole() : void</t>
+  </si>
+  <si>
+    <t>+setUsername() : String</t>
+  </si>
+  <si>
+    <t>+setPassword() : String</t>
+  </si>
+  <si>
+    <t>+serRole() : String</t>
+  </si>
+  <si>
+    <t>+ updateUser(int id): void</t>
+  </si>
+  <si>
+    <t>+updateCustomer (int id)</t>
+  </si>
+  <si>
+    <t>+generateDeliveryReport() : void</t>
+  </si>
+  <si>
+    <t>+createCustomer(firstName: String, lastName: String, address: String, phoneNo: String)</t>
+  </si>
+  <si>
+    <t>+ getUser(int id): void</t>
+  </si>
+  <si>
+    <t>+ deleteUser(int id): void</t>
+  </si>
+  <si>
+    <t>+Admin : (username: String, password: String, role: String, userDatabase: Database)</t>
+  </si>
+  <si>
+    <t>+getCustomer(int id) : void</t>
+  </si>
+  <si>
+    <t>+deactivateCustomer(int id) : void</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -814,8 +838,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -849,6 +881,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -950,7 +988,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1052,9 +1090,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1078,80 +1113,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1166,6 +1129,78 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1175,11 +1210,21 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3004,7 +3049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB095BD-E922-497D-B7ED-398078A18E3D}">
   <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C69" sqref="C69:C71"/>
     </sheetView>
   </sheetViews>
@@ -3037,16 +3082,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="54">
+      <c r="A2" s="55">
         <v>1</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="47" t="s">
-        <v>167</v>
-      </c>
-      <c r="D2" s="47" t="s">
+      <c r="C2" s="57" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="57" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="15" t="s">
@@ -3057,10 +3102,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="55"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
+      <c r="A3" s="56"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
       <c r="E3" s="15" t="s">
         <v>47</v>
       </c>
@@ -3069,50 +3114,50 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="55"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
+      <c r="A4" s="56"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
       <c r="E4" s="15" t="s">
         <v>49</v>
       </c>
       <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="55"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="15" t="s">
         <v>50</v>
       </c>
       <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="55"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
+      <c r="A6" s="56"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
       <c r="E6" s="15" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="55"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
+      <c r="A7" s="56"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
       <c r="E7" s="15" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="55"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
+      <c r="A8" s="56"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
       <c r="E8" s="15" t="s">
         <v>37</v>
       </c>
@@ -3127,16 +3172,16 @@
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="54">
+      <c r="A10" s="55">
         <v>2</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="47" t="s">
+      <c r="D10" s="57" t="s">
         <v>82</v>
       </c>
       <c r="E10" s="14" t="s">
@@ -3147,60 +3192,60 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="55"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
+      <c r="A11" s="56"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
       <c r="E11" s="15" t="s">
         <v>88</v>
       </c>
       <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="55"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
+      <c r="A12" s="56"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
       <c r="E12" s="15" t="s">
         <v>91</v>
       </c>
       <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="55"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
+      <c r="A13" s="56"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
       <c r="E13" s="15" t="s">
         <v>89</v>
       </c>
       <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="55"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
+      <c r="A14" s="56"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
       <c r="E14" s="15" t="s">
         <v>90</v>
       </c>
       <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="55"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
+      <c r="A15" s="56"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
       <c r="E15" s="15" t="s">
         <v>84</v>
       </c>
       <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="56"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
+      <c r="A16" s="69"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
       <c r="E16" s="15" t="s">
         <v>14</v>
       </c>
@@ -3215,16 +3260,16 @@
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="54">
+      <c r="A18" s="55">
         <v>3</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="47" t="s">
+      <c r="D18" s="57" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="15" t="s">
@@ -3235,20 +3280,20 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="55"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
       <c r="E19" s="15" t="s">
         <v>92</v>
       </c>
       <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="56"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
+      <c r="A20" s="69"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
       <c r="E20" s="11" t="s">
         <v>51</v>
       </c>
@@ -3263,16 +3308,16 @@
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="54">
+      <c r="A22" s="55">
         <v>4</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="47" t="s">
+      <c r="C22" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="47" t="s">
+      <c r="D22" s="57" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="15" t="s">
@@ -3283,60 +3328,60 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="55"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
+      <c r="A23" s="56"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
       <c r="E23" s="15" t="s">
         <v>97</v>
       </c>
       <c r="F23" s="21"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="55"/>
-      <c r="B24" s="48"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
+      <c r="A24" s="56"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
       <c r="E24" s="15" t="s">
         <v>98</v>
       </c>
       <c r="F24" s="21"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="55"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
+      <c r="A25" s="56"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
       <c r="E25" s="15" t="s">
         <v>99</v>
       </c>
       <c r="F25" s="21"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="55"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
+      <c r="A26" s="56"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
       <c r="E26" s="15" t="s">
         <v>93</v>
       </c>
       <c r="F26" s="21"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="55"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
+      <c r="A27" s="56"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58"/>
       <c r="E27" s="15" t="s">
         <v>94</v>
       </c>
       <c r="F27" s="21"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="56"/>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
+      <c r="A28" s="69"/>
+      <c r="B28" s="70"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="70"/>
       <c r="E28" s="15" t="s">
         <v>11</v>
       </c>
@@ -3351,16 +3396,16 @@
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="54">
+      <c r="A30" s="55">
         <v>5</v>
       </c>
-      <c r="B30" s="47" t="s">
+      <c r="B30" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="47" t="s">
+      <c r="C30" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="47" t="s">
+      <c r="D30" s="57" t="s">
         <v>83</v>
       </c>
       <c r="E30" s="15" t="s">
@@ -3369,20 +3414,20 @@
       <c r="F30" s="21"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="55"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
+      <c r="A31" s="56"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="58"/>
       <c r="E31" s="15" t="s">
         <v>95</v>
       </c>
       <c r="F31" s="21"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="56"/>
-      <c r="B32" s="49"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
+      <c r="A32" s="69"/>
+      <c r="B32" s="70"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="70"/>
       <c r="E32" s="15" t="s">
         <v>96</v>
       </c>
@@ -3397,16 +3442,16 @@
       <c r="F33" s="7"/>
     </row>
     <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="54">
+      <c r="A34" s="55">
         <v>6</v>
       </c>
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="47" t="s">
+      <c r="C34" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="47" t="s">
+      <c r="D34" s="57" t="s">
         <v>16</v>
       </c>
       <c r="E34" s="15" t="s">
@@ -3417,10 +3462,10 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="56"/>
-      <c r="B35" s="49"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
+      <c r="A35" s="69"/>
+      <c r="B35" s="70"/>
+      <c r="C35" s="70"/>
+      <c r="D35" s="70"/>
       <c r="E35" s="15" t="s">
         <v>101</v>
       </c>
@@ -3435,70 +3480,70 @@
       <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="57">
+      <c r="A37" s="74">
         <v>7</v>
       </c>
-      <c r="B37" s="53" t="s">
+      <c r="B37" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="53" t="s">
+      <c r="C37" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="53" t="s">
+      <c r="D37" s="73" t="s">
         <v>70</v>
       </c>
       <c r="E37" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="F37" s="47" t="s">
+      <c r="F37" s="57" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="57"/>
-      <c r="B38" s="53"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
+      <c r="A38" s="74"/>
+      <c r="B38" s="73"/>
+      <c r="C38" s="73"/>
+      <c r="D38" s="73"/>
       <c r="E38" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="F38" s="48"/>
+      <c r="F38" s="58"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="57"/>
-      <c r="B39" s="53"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
+      <c r="A39" s="74"/>
+      <c r="B39" s="73"/>
+      <c r="C39" s="73"/>
+      <c r="D39" s="73"/>
       <c r="E39" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F39" s="49"/>
+      <c r="F39" s="70"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="57"/>
-      <c r="B40" s="53"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="53"/>
+      <c r="A40" s="74"/>
+      <c r="B40" s="73"/>
+      <c r="C40" s="73"/>
+      <c r="D40" s="73"/>
       <c r="E40" s="21" t="s">
         <v>73</v>
       </c>
       <c r="F40" s="21"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="57"/>
-      <c r="B41" s="53"/>
-      <c r="C41" s="53"/>
-      <c r="D41" s="53"/>
+      <c r="A41" s="74"/>
+      <c r="B41" s="73"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="73"/>
       <c r="E41" s="21" t="s">
         <v>74</v>
       </c>
       <c r="F41" s="21"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="57"/>
-      <c r="B42" s="53"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="53"/>
+      <c r="A42" s="74"/>
+      <c r="B42" s="73"/>
+      <c r="C42" s="73"/>
+      <c r="D42" s="73"/>
       <c r="E42" s="21" t="s">
         <v>76</v>
       </c>
@@ -3507,88 +3552,88 @@
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="27"/>
       <c r="B43" s="20"/>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="46"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="45"/>
       <c r="F43" s="7"/>
     </row>
     <row r="44" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="50">
+      <c r="A44" s="75">
         <v>8</v>
       </c>
-      <c r="B44" s="47" t="s">
+      <c r="B44" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="47" t="s">
-        <v>169</v>
-      </c>
-      <c r="D44" s="47" t="s">
-        <v>170</v>
+      <c r="C44" s="57" t="s">
+        <v>156</v>
+      </c>
+      <c r="D44" s="57" t="s">
+        <v>157</v>
       </c>
       <c r="E44" s="21" t="s">
         <v>39</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="51"/>
-      <c r="B45" s="48"/>
-      <c r="C45" s="48"/>
-      <c r="D45" s="48"/>
+      <c r="A45" s="76"/>
+      <c r="B45" s="58"/>
+      <c r="C45" s="58"/>
+      <c r="D45" s="58"/>
       <c r="E45" s="21" t="s">
         <v>47</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="51"/>
-      <c r="B46" s="48"/>
-      <c r="C46" s="48"/>
-      <c r="D46" s="48"/>
+      <c r="A46" s="76"/>
+      <c r="B46" s="58"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="58"/>
       <c r="E46" s="21" t="s">
         <v>49</v>
       </c>
       <c r="F46" s="21"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="51"/>
-      <c r="B47" s="48"/>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
+      <c r="A47" s="76"/>
+      <c r="B47" s="58"/>
+      <c r="C47" s="58"/>
+      <c r="D47" s="58"/>
       <c r="E47" s="21" t="s">
         <v>50</v>
       </c>
       <c r="F47" s="21"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" s="51"/>
-      <c r="B48" s="48"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
+      <c r="A48" s="76"/>
+      <c r="B48" s="58"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="58"/>
       <c r="E48" s="21" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="F48" s="21"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="51"/>
-      <c r="B49" s="48"/>
-      <c r="C49" s="48"/>
-      <c r="D49" s="48"/>
+      <c r="A49" s="76"/>
+      <c r="B49" s="58"/>
+      <c r="C49" s="58"/>
+      <c r="D49" s="58"/>
       <c r="E49" s="21" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="F49" s="21"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="52"/>
-      <c r="B50" s="49"/>
-      <c r="C50" s="49"/>
-      <c r="D50" s="49"/>
+      <c r="A50" s="77"/>
+      <c r="B50" s="70"/>
+      <c r="C50" s="70"/>
+      <c r="D50" s="70"/>
       <c r="E50" s="21" t="s">
         <v>37</v>
       </c>
@@ -3597,88 +3642,88 @@
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="27"/>
       <c r="B51" s="20"/>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="46"/>
+      <c r="C51" s="44"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="45"/>
       <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="50">
+      <c r="A52" s="75">
         <v>9</v>
       </c>
-      <c r="B52" s="47" t="s">
+      <c r="B52" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C52" s="47" t="s">
-        <v>177</v>
-      </c>
-      <c r="D52" s="47" t="s">
-        <v>178</v>
+      <c r="C52" s="57" t="s">
+        <v>164</v>
+      </c>
+      <c r="D52" s="57" t="s">
+        <v>165</v>
       </c>
       <c r="E52" s="21" t="s">
         <v>39</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="51"/>
-      <c r="B53" s="48"/>
-      <c r="C53" s="48"/>
-      <c r="D53" s="48"/>
+      <c r="A53" s="76"/>
+      <c r="B53" s="58"/>
+      <c r="C53" s="58"/>
+      <c r="D53" s="58"/>
       <c r="E53" s="21" t="s">
         <v>47</v>
       </c>
       <c r="F53" s="21" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="51"/>
-      <c r="B54" s="48"/>
-      <c r="C54" s="48"/>
-      <c r="D54" s="48"/>
+      <c r="A54" s="76"/>
+      <c r="B54" s="58"/>
+      <c r="C54" s="58"/>
+      <c r="D54" s="58"/>
       <c r="E54" s="21" t="s">
         <v>49</v>
       </c>
       <c r="F54" s="21"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" s="51"/>
-      <c r="B55" s="48"/>
-      <c r="C55" s="48"/>
-      <c r="D55" s="48"/>
+      <c r="A55" s="76"/>
+      <c r="B55" s="58"/>
+      <c r="C55" s="58"/>
+      <c r="D55" s="58"/>
       <c r="E55" s="21" t="s">
         <v>50</v>
       </c>
       <c r="F55" s="21"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="51"/>
-      <c r="B56" s="48"/>
-      <c r="C56" s="48"/>
-      <c r="D56" s="48"/>
+      <c r="A56" s="76"/>
+      <c r="B56" s="58"/>
+      <c r="C56" s="58"/>
+      <c r="D56" s="58"/>
       <c r="E56" s="21" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="F56" s="21"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A57" s="51"/>
-      <c r="B57" s="48"/>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
+      <c r="A57" s="76"/>
+      <c r="B57" s="58"/>
+      <c r="C57" s="58"/>
+      <c r="D57" s="58"/>
       <c r="E57" s="21" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="F57" s="21"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="52"/>
-      <c r="B58" s="49"/>
-      <c r="C58" s="49"/>
-      <c r="D58" s="49"/>
+      <c r="A58" s="77"/>
+      <c r="B58" s="70"/>
+      <c r="C58" s="70"/>
+      <c r="D58" s="70"/>
       <c r="E58" s="21" t="s">
         <v>37</v>
       </c>
@@ -3687,9 +3732,9 @@
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="27"/>
       <c r="B59" s="20"/>
-      <c r="C59" s="45"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="46"/>
+      <c r="C59" s="44"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="45"/>
       <c r="F59" s="7"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
@@ -3701,40 +3746,40 @@
       <c r="F64" s="7"/>
     </row>
     <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="60">
+      <c r="A65" s="63">
         <v>10</v>
       </c>
-      <c r="B65" s="63" t="s">
+      <c r="B65" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="C65" s="63" t="s">
+      <c r="C65" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="D65" s="63" t="s">
+      <c r="D65" s="66" t="s">
         <v>33</v>
       </c>
       <c r="E65" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F65" s="58" t="s">
+      <c r="F65" s="71" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66" s="61"/>
-      <c r="B66" s="64"/>
-      <c r="C66" s="64"/>
-      <c r="D66" s="64"/>
+      <c r="A66" s="64"/>
+      <c r="B66" s="67"/>
+      <c r="C66" s="67"/>
+      <c r="D66" s="67"/>
       <c r="E66" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="F66" s="59"/>
+      <c r="F66" s="72"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" s="62"/>
-      <c r="B67" s="65"/>
-      <c r="C67" s="65"/>
-      <c r="D67" s="65"/>
+      <c r="A67" s="65"/>
+      <c r="B67" s="68"/>
+      <c r="C67" s="68"/>
+      <c r="D67" s="68"/>
       <c r="E67" s="6"/>
       <c r="F67" s="31"/>
     </row>
@@ -3747,16 +3792,16 @@
       <c r="F68" s="7"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="60">
+      <c r="A69" s="63">
         <v>11</v>
       </c>
-      <c r="B69" s="63" t="s">
+      <c r="B69" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="C69" s="63" t="s">
+      <c r="C69" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="D69" s="63" t="s">
+      <c r="D69" s="66" t="s">
         <v>26</v>
       </c>
       <c r="E69" s="17" t="s">
@@ -3765,20 +3810,20 @@
       <c r="F69" s="31"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="61"/>
-      <c r="B70" s="64"/>
-      <c r="C70" s="64"/>
-      <c r="D70" s="64"/>
+      <c r="A70" s="64"/>
+      <c r="B70" s="67"/>
+      <c r="C70" s="67"/>
+      <c r="D70" s="67"/>
       <c r="E70" s="17" t="s">
         <v>28</v>
       </c>
       <c r="F70" s="31"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" s="62"/>
-      <c r="B71" s="65"/>
-      <c r="C71" s="65"/>
-      <c r="D71" s="65"/>
+      <c r="A71" s="65"/>
+      <c r="B71" s="68"/>
+      <c r="C71" s="68"/>
+      <c r="D71" s="68"/>
       <c r="E71" s="17" t="s">
         <v>29</v>
       </c>
@@ -3792,16 +3837,16 @@
       <c r="E74" s="9"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="68">
+      <c r="A75" s="61">
         <v>6</v>
       </c>
-      <c r="B75" s="66" t="s">
+      <c r="B75" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C75" s="66" t="s">
+      <c r="C75" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="D75" s="66" t="s">
+      <c r="D75" s="59" t="s">
         <v>19</v>
       </c>
       <c r="E75" s="12" t="s">
@@ -3809,10 +3854,10 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A76" s="69"/>
-      <c r="B76" s="67"/>
-      <c r="C76" s="67"/>
-      <c r="D76" s="67"/>
+      <c r="A76" s="62"/>
+      <c r="B76" s="60"/>
+      <c r="C76" s="60"/>
+      <c r="D76" s="60"/>
       <c r="E76" s="12" t="s">
         <v>31</v>
       </c>
@@ -3877,6 +3922,40 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="C44:C50"/>
+    <mergeCell ref="B44:B50"/>
+    <mergeCell ref="D44:D50"/>
+    <mergeCell ref="A44:A50"/>
+    <mergeCell ref="A52:A58"/>
+    <mergeCell ref="B52:B58"/>
+    <mergeCell ref="C52:C58"/>
+    <mergeCell ref="D52:D58"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="D37:D42"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="B37:B42"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="D65:D67"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C22:C28"/>
+    <mergeCell ref="D22:D28"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="B2:B8"/>
     <mergeCell ref="C2:C8"/>
@@ -3893,40 +3972,6 @@
     <mergeCell ref="B10:B16"/>
     <mergeCell ref="C10:C16"/>
     <mergeCell ref="D10:D16"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C22:C28"/>
-    <mergeCell ref="D22:D28"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="D65:D67"/>
-    <mergeCell ref="C37:C42"/>
-    <mergeCell ref="D37:D42"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="B37:B42"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="C44:C50"/>
-    <mergeCell ref="B44:B50"/>
-    <mergeCell ref="D44:D50"/>
-    <mergeCell ref="A44:A50"/>
-    <mergeCell ref="A52:A58"/>
-    <mergeCell ref="B52:B58"/>
-    <mergeCell ref="C52:C58"/>
-    <mergeCell ref="D52:D58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3970,16 +4015,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="54">
+      <c r="A2" s="55">
         <v>1</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="57" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="14" t="s">
@@ -3990,10 +4035,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="55"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
+      <c r="A3" s="56"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
       <c r="E3" s="15" t="s">
         <v>60</v>
       </c>
@@ -4002,70 +4047,70 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="55"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
+      <c r="A4" s="56"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
       <c r="E4" s="15" t="s">
         <v>64</v>
       </c>
       <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="55"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="15" t="s">
         <v>65</v>
       </c>
       <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="55"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
+      <c r="A6" s="56"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
       <c r="E6" s="15" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="55"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
+      <c r="A7" s="56"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
       <c r="E7" s="15" t="s">
         <v>67</v>
       </c>
       <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="55"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
+      <c r="A8" s="56"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
       <c r="E8" s="15" t="s">
         <v>61</v>
       </c>
       <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="55"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
+      <c r="A9" s="56"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
       <c r="E9" s="15" t="s">
         <v>62</v>
       </c>
       <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="56"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
+      <c r="A10" s="69"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
       <c r="E10" s="15" t="s">
         <v>14</v>
       </c>
@@ -4080,16 +4125,16 @@
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="54">
+      <c r="A12" s="55">
         <v>2</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="57" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="15" t="s">
@@ -4100,40 +4145,40 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="55"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
+      <c r="A13" s="56"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
       <c r="E13" s="15" t="s">
         <v>103</v>
       </c>
       <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="55"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
+      <c r="A14" s="56"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
       <c r="E14" s="15" t="s">
         <v>104</v>
       </c>
       <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="55"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
+      <c r="A15" s="56"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
       <c r="E15" s="15" t="s">
         <v>105</v>
       </c>
       <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="56"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
+      <c r="A16" s="69"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
       <c r="E16" s="11" t="s">
         <v>51</v>
       </c>
@@ -4148,16 +4193,16 @@
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="54">
+      <c r="A18" s="55">
         <v>3</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="47" t="s">
+      <c r="D18" s="57" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="15" t="s">
@@ -4168,50 +4213,50 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="55"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
       <c r="E19" s="15" t="s">
         <v>103</v>
       </c>
       <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="55"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
       <c r="E20" s="15" t="s">
         <v>107</v>
       </c>
       <c r="F20" s="21"/>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="55"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
+      <c r="A21" s="56"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="58"/>
       <c r="E21" s="15" t="s">
         <v>108</v>
       </c>
       <c r="F21" s="21"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="55"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
+      <c r="A22" s="56"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
       <c r="E22" s="15" t="s">
         <v>110</v>
       </c>
       <c r="F22" s="21"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="55"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
+      <c r="A23" s="56"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
       <c r="E23" s="15" t="s">
         <v>109</v>
       </c>
@@ -4226,16 +4271,16 @@
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="54">
+      <c r="A25" s="55">
         <v>4</v>
       </c>
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="47" t="s">
+      <c r="C25" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="47" t="s">
+      <c r="D25" s="57" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="15" t="s">
@@ -4244,10 +4289,10 @@
       <c r="F25" s="21"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="55"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
+      <c r="A26" s="56"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
       <c r="E26" s="15" t="s">
         <v>112</v>
       </c>
@@ -4262,16 +4307,16 @@
       <c r="F27" s="7"/>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="54">
+      <c r="A28" s="55">
         <v>5</v>
       </c>
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="47" t="s">
+      <c r="C28" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="D28" s="47" t="s">
+      <c r="D28" s="57" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="15" t="s">
@@ -4282,10 +4327,10 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="55"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
+      <c r="A29" s="56"/>
+      <c r="B29" s="58"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="58"/>
       <c r="E29" s="15" t="s">
         <v>17</v>
       </c>
@@ -4300,16 +4345,16 @@
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="54">
+      <c r="A31" s="55">
         <v>6</v>
       </c>
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="47" t="s">
+      <c r="C31" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="D31" s="47" t="s">
+      <c r="D31" s="57" t="s">
         <v>43</v>
       </c>
       <c r="E31" s="14" t="s">
@@ -4320,30 +4365,30 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="55"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
+      <c r="A32" s="56"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="58"/>
       <c r="E32" s="15" t="s">
         <v>117</v>
       </c>
       <c r="F32" s="21"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="55"/>
-      <c r="B33" s="48"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
+      <c r="A33" s="56"/>
+      <c r="B33" s="58"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="58"/>
       <c r="E33" s="15" t="s">
         <v>115</v>
       </c>
       <c r="F33" s="21"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="56"/>
-      <c r="B34" s="49"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="49"/>
+      <c r="A34" s="69"/>
+      <c r="B34" s="70"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
       <c r="E34" s="15" t="s">
         <v>22</v>
       </c>
@@ -4358,16 +4403,16 @@
       <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="54">
+      <c r="A36" s="55">
         <v>7</v>
       </c>
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="47" t="s">
+      <c r="D36" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E36" s="15" t="s">
@@ -4376,20 +4421,20 @@
       <c r="F36" s="21"/>
     </row>
     <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="55"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
+      <c r="A37" s="56"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="58"/>
       <c r="E37" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F37" s="21"/>
     </row>
     <row r="38" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="56"/>
-      <c r="B38" s="49"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="49"/>
+      <c r="A38" s="69"/>
+      <c r="B38" s="70"/>
+      <c r="C38" s="70"/>
+      <c r="D38" s="70"/>
       <c r="E38" s="15" t="s">
         <v>36</v>
       </c>
@@ -4404,16 +4449,16 @@
       <c r="F39" s="7"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="54">
+      <c r="A40" s="55">
         <v>8</v>
       </c>
-      <c r="B40" s="47" t="s">
+      <c r="B40" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="47" t="s">
-        <v>166</v>
-      </c>
-      <c r="D40" s="47" t="s">
+      <c r="C40" s="57" t="s">
+        <v>153</v>
+      </c>
+      <c r="D40" s="57" t="s">
         <v>118</v>
       </c>
       <c r="E40" s="21" t="s">
@@ -4422,70 +4467,70 @@
       <c r="F40" s="21"/>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="55"/>
-      <c r="B41" s="48"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
+      <c r="A41" s="56"/>
+      <c r="B41" s="58"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="58"/>
       <c r="E41" s="21" t="s">
         <v>120</v>
       </c>
       <c r="F41" s="21"/>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="55"/>
-      <c r="B42" s="48"/>
-      <c r="C42" s="48"/>
-      <c r="D42" s="48"/>
+      <c r="A42" s="56"/>
+      <c r="B42" s="58"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="58"/>
       <c r="E42" s="21" t="s">
         <v>121</v>
       </c>
       <c r="F42" s="21"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="55"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="48"/>
-      <c r="D43" s="48"/>
+      <c r="A43" s="56"/>
+      <c r="B43" s="58"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="58"/>
       <c r="E43" s="21" t="s">
         <v>122</v>
       </c>
       <c r="F43" s="21"/>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="55"/>
-      <c r="B44" s="48"/>
-      <c r="C44" s="48"/>
-      <c r="D44" s="48"/>
+      <c r="A44" s="56"/>
+      <c r="B44" s="58"/>
+      <c r="C44" s="58"/>
+      <c r="D44" s="58"/>
       <c r="E44" s="21" t="s">
         <v>124</v>
       </c>
       <c r="F44" s="21"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="55"/>
-      <c r="B45" s="48"/>
-      <c r="C45" s="48"/>
-      <c r="D45" s="48"/>
+      <c r="A45" s="56"/>
+      <c r="B45" s="58"/>
+      <c r="C45" s="58"/>
+      <c r="D45" s="58"/>
       <c r="E45" s="21" t="s">
         <v>125</v>
       </c>
       <c r="F45" s="21"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="55"/>
-      <c r="B46" s="48"/>
-      <c r="C46" s="48"/>
-      <c r="D46" s="48"/>
+      <c r="A46" s="56"/>
+      <c r="B46" s="58"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="58"/>
       <c r="E46" s="21" t="s">
         <v>123</v>
       </c>
       <c r="F46" s="21"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="55"/>
-      <c r="B47" s="48"/>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
+      <c r="A47" s="56"/>
+      <c r="B47" s="58"/>
+      <c r="C47" s="58"/>
+      <c r="D47" s="58"/>
       <c r="E47" s="14" t="s">
         <v>76</v>
       </c>
@@ -4501,6 +4546,30 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A40:A47"/>
+    <mergeCell ref="B40:B47"/>
+    <mergeCell ref="C40:C47"/>
+    <mergeCell ref="D40:D47"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="B2:B10"/>
     <mergeCell ref="C2:C10"/>
@@ -4509,30 +4578,6 @@
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
     <mergeCell ref="D12:D16"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A40:A47"/>
-    <mergeCell ref="B40:B47"/>
-    <mergeCell ref="C40:C47"/>
-    <mergeCell ref="D40:D47"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="A36:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4540,216 +4585,332 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD0B509-A153-4B31-95B8-BC32DC1B6A3B}">
-  <dimension ref="B2:J18"/>
+  <dimension ref="B2:H25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.08984375" customWidth="1"/>
-    <col min="2" max="2" width="37.453125" style="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.453125" style="32" customWidth="1"/>
     <col min="3" max="3" width="3.08984375" style="32" customWidth="1"/>
     <col min="4" max="4" width="41.7265625" style="34" customWidth="1"/>
     <col min="5" max="5" width="3.81640625" style="32" customWidth="1"/>
-    <col min="6" max="6" width="37.90625" customWidth="1"/>
-    <col min="7" max="7" width="3.6328125" customWidth="1"/>
-    <col min="8" max="8" width="40.6328125" customWidth="1"/>
+    <col min="6" max="6" width="37.90625" style="32" customWidth="1"/>
+    <col min="7" max="7" width="3.6328125" style="32" customWidth="1"/>
+    <col min="8" max="8" width="40.6328125" style="32" customWidth="1"/>
     <col min="9" max="9" width="3.26953125" customWidth="1"/>
     <col min="10" max="10" width="26.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="42" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B2" s="41" t="s">
         <v>127</v>
       </c>
       <c r="C2" s="33"/>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="42" t="s">
         <v>128</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="H2" s="43" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B3" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="39"/>
+      <c r="D7" s="37"/>
+      <c r="F7" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="H7" s="37"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="83" t="s">
+        <v>235</v>
+      </c>
+      <c r="C8" s="83"/>
+      <c r="D8" s="85" t="s">
+        <v>234</v>
+      </c>
+      <c r="E8" s="83"/>
+      <c r="F8" s="40" t="s">
+        <v>229</v>
+      </c>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="85" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="83"/>
+      <c r="D9" s="85" t="s">
+        <v>249</v>
+      </c>
+      <c r="E9" s="83"/>
+      <c r="F9" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="G9" s="83"/>
+      <c r="H9" s="85" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="36" t="s">
+        <v>230</v>
+      </c>
+      <c r="G10" s="83"/>
+      <c r="H10" s="85" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="B11" s="85" t="s">
+        <v>246</v>
+      </c>
+      <c r="C11" s="83"/>
+      <c r="D11" s="85" t="s">
+        <v>152</v>
+      </c>
+      <c r="E11" s="83"/>
+      <c r="F11" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="G11" s="83"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="85" t="s">
+        <v>244</v>
+      </c>
+      <c r="C12" s="83"/>
+      <c r="D12" s="85" t="s">
+        <v>243</v>
+      </c>
+      <c r="E12" s="83"/>
+      <c r="F12" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="G12" s="83"/>
+      <c r="H12" s="83" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="83" t="s">
+        <v>251</v>
+      </c>
+      <c r="C13" s="83"/>
+      <c r="D13" s="86" t="s">
+        <v>248</v>
+      </c>
+      <c r="E13" s="83"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="83"/>
+      <c r="H13" s="83" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="83" t="s">
+        <v>250</v>
+      </c>
+      <c r="C14" s="83"/>
+      <c r="D14" s="85" t="s">
+        <v>247</v>
+      </c>
+      <c r="E14" s="83"/>
+      <c r="F14" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="H2" s="44" t="s">
-        <v>156</v>
-      </c>
-      <c r="J2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="F3" s="41" t="s">
-        <v>149</v>
-      </c>
-      <c r="H3" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="J3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B4" s="39" t="s">
-        <v>134</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="F4" s="39" t="s">
+      <c r="G14" s="83"/>
+      <c r="H14" s="83" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="83" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" s="83"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="G15" s="83"/>
+      <c r="H15" s="83" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="83" t="s">
+        <v>245</v>
+      </c>
+      <c r="C16" s="83"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="G16" s="83"/>
+      <c r="H16" s="83" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C17" s="83"/>
+      <c r="D17" s="84" t="s">
+        <v>233</v>
+      </c>
+      <c r="E17" s="83"/>
+      <c r="F17" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="G17" s="83"/>
+      <c r="H17" s="83" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="83"/>
+      <c r="C18" s="83"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="G18" s="83"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="83"/>
+      <c r="C19" s="83"/>
+      <c r="E19" s="83"/>
+      <c r="F19" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="G19" s="83"/>
+      <c r="H19" s="84" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="83"/>
+      <c r="C20" s="83"/>
+      <c r="E20" s="83"/>
+      <c r="F20" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="G20" s="83"/>
+      <c r="H20" s="83"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B21" s="83"/>
+      <c r="C21" s="83"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="G21" s="83"/>
+      <c r="H21" s="83"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B22" s="83"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="G22" s="83"/>
+      <c r="H22" s="83"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B23" s="83"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="H4" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="J4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B5" s="39" t="s">
-        <v>133</v>
-      </c>
-      <c r="D5" s="36" t="s">
-        <v>133</v>
-      </c>
-      <c r="F5" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="H5" s="36" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="D6" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="F6" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="H6" s="36" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B7" s="39"/>
-      <c r="D7" s="36"/>
-      <c r="F7" s="40" t="s">
-        <v>153</v>
-      </c>
-      <c r="H7" s="38"/>
-    </row>
-    <row r="8" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B8" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="D8" s="35" t="s">
-        <v>139</v>
-      </c>
-      <c r="F8" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="H8" s="35" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B9" s="36" t="s">
-        <v>162</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>157</v>
-      </c>
-      <c r="F9" s="39" t="s">
-        <v>140</v>
-      </c>
-      <c r="H9" s="36" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B10" s="36" t="s">
-        <v>163</v>
-      </c>
-      <c r="D10" s="36" t="s">
-        <v>158</v>
-      </c>
-      <c r="F10" s="39" t="s">
-        <v>141</v>
-      </c>
-      <c r="H10" s="38"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="39" t="s">
-        <v>129</v>
-      </c>
-      <c r="D11" s="37" t="s">
-        <v>183</v>
-      </c>
-      <c r="F11" s="39" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="39" t="s">
-        <v>164</v>
-      </c>
-      <c r="D12" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="F12" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="D13" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="F13" s="39" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="F14" s="39" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="40" t="s">
-        <v>131</v>
-      </c>
-      <c r="F15" s="39" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="F16" s="39" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F17" s="39" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F18" s="40" t="s">
-        <v>155</v>
+      <c r="G23" s="83"/>
+      <c r="H23" s="83"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B24" s="83"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="85"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="83"/>
+      <c r="H24" s="83"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F25" s="84" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -4768,7 +4929,7 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="1.26953125" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="78"/>
+    <col min="2" max="2" width="8.7265625" style="53"/>
     <col min="3" max="3" width="73" customWidth="1"/>
     <col min="4" max="4" width="3.36328125" customWidth="1"/>
     <col min="6" max="6" width="58.453125" customWidth="1"/>
@@ -4778,947 +4939,954 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="83"/>
-      <c r="B1" s="72" t="s">
+      <c r="A1" s="81"/>
+      <c r="B1" s="82" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="82"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="82" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" s="82"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="82" t="s">
+        <v>175</v>
+      </c>
+      <c r="I1" s="82"/>
+      <c r="J1" s="81"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="81"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="81"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="81"/>
+      <c r="B3" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" s="78"/>
+      <c r="E3" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="G3" s="78"/>
+      <c r="H3" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="I3" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="J3" s="81"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="81"/>
+      <c r="B4" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" s="79"/>
+      <c r="E4" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" s="48" t="s">
+        <v>186</v>
+      </c>
+      <c r="G4" s="79"/>
+      <c r="H4" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="I4" s="48" t="s">
+        <v>187</v>
+      </c>
+      <c r="J4" s="81"/>
+    </row>
+    <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="81"/>
+      <c r="B5" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="D5" s="79"/>
+      <c r="E5" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="G5" s="79"/>
+      <c r="H5" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="J5" s="81"/>
+    </row>
+    <row r="6" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="81"/>
+      <c r="B6" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="48"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="F6" s="48"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="I6" s="48"/>
+      <c r="J6" s="81"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="81"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="81"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="81"/>
+      <c r="B8" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" s="78"/>
+      <c r="E8" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="F8" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="G8" s="78"/>
+      <c r="H8" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="I8" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="J8" s="81"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="81"/>
+      <c r="B9" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="D9" s="79"/>
+      <c r="E9" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="F9" s="48" t="s">
+        <v>186</v>
+      </c>
+      <c r="G9" s="79"/>
+      <c r="H9" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="I9" s="48" t="s">
+        <v>207</v>
+      </c>
+      <c r="J9" s="81"/>
+    </row>
+    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="81"/>
+      <c r="B10" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="D10" s="79"/>
+      <c r="E10" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="G10" s="79"/>
+      <c r="H10" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="J10" s="81"/>
+    </row>
+    <row r="11" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="81"/>
+      <c r="B11" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" s="48"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="F11" s="48"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="I11" s="48"/>
+      <c r="J11" s="81"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="81"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="81"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="81"/>
+      <c r="B13" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="D13" s="78"/>
+      <c r="E13" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="G13" s="78"/>
+      <c r="H13" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="I13" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="J13" s="81"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="81"/>
+      <c r="B14" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="D14" s="79"/>
+      <c r="E14" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="F14" s="48"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="I14" s="48"/>
+      <c r="J14" s="81"/>
+    </row>
+    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="81"/>
+      <c r="B15" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="D15" s="79"/>
+      <c r="E15" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="F15" s="21"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="I15" s="21"/>
+      <c r="J15" s="81"/>
+    </row>
+    <row r="16" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="81"/>
+      <c r="B16" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16" s="48"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="F16" s="48"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="I16" s="48"/>
+      <c r="J16" s="81"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="81"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="81"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="81"/>
+      <c r="B18" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" s="48" t="s">
+        <v>178</v>
+      </c>
+      <c r="D18" s="78"/>
+      <c r="E18" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="F18" s="48" t="s">
+        <v>178</v>
+      </c>
+      <c r="G18" s="78"/>
+      <c r="H18" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="I18" s="48" t="s">
+        <v>178</v>
+      </c>
+      <c r="J18" s="81"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="81"/>
+      <c r="B19" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>188</v>
+      </c>
+      <c r="D19" s="79"/>
+      <c r="E19" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="F19" s="48" t="s">
+        <v>188</v>
+      </c>
+      <c r="G19" s="79"/>
+      <c r="H19" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="I19" s="48" t="s">
+        <v>188</v>
+      </c>
+      <c r="J19" s="81"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="81"/>
+      <c r="B20" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="C1" s="72"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="72" t="s">
-        <v>191</v>
-      </c>
-      <c r="F1" s="72"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="72" t="s">
+      <c r="D20" s="79"/>
+      <c r="E20" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="G20" s="79"/>
+      <c r="H20" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="I20" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="I1" s="72"/>
-      <c r="J1" s="83"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="83"/>
-      <c r="B2" s="76"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="83"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="83"/>
-      <c r="B3" s="75" t="s">
-        <v>185</v>
-      </c>
-      <c r="C3" s="73" t="s">
-        <v>186</v>
-      </c>
-      <c r="D3" s="79"/>
-      <c r="E3" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="F3" s="73" t="s">
-        <v>186</v>
-      </c>
-      <c r="G3" s="79"/>
-      <c r="H3" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="I3" s="73" t="s">
-        <v>186</v>
-      </c>
-      <c r="J3" s="83"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="83"/>
-      <c r="B4" s="75" t="s">
-        <v>187</v>
-      </c>
-      <c r="C4" s="73" t="s">
+      <c r="J20" s="81"/>
+    </row>
+    <row r="21" spans="1:10" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="81"/>
+      <c r="B21" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="C21" s="48"/>
+      <c r="D21" s="80"/>
+      <c r="E21" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="F21" s="48"/>
+      <c r="G21" s="80"/>
+      <c r="H21" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="I21" s="48"/>
+      <c r="J21" s="81"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="81"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="81"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="81"/>
+      <c r="B23" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="C23" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="D23" s="78"/>
+      <c r="E23" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="F23" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="G23" s="78"/>
+      <c r="H23" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="I23" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="J23" s="81"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="81"/>
+      <c r="B24" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="C24" s="48" t="s">
+        <v>197</v>
+      </c>
+      <c r="D24" s="79"/>
+      <c r="E24" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="F24" s="48" t="s">
+        <v>217</v>
+      </c>
+      <c r="G24" s="79"/>
+      <c r="H24" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="I24" s="48" t="s">
+        <v>208</v>
+      </c>
+      <c r="J24" s="81"/>
+    </row>
+    <row r="25" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="81"/>
+      <c r="B25" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="D25" s="79"/>
+      <c r="E25" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="G25" s="79"/>
+      <c r="H25" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="I25" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="J25" s="81"/>
+    </row>
+    <row r="26" spans="1:10" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="81"/>
+      <c r="B26" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="C26" s="48"/>
+      <c r="D26" s="80"/>
+      <c r="E26" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="F26" s="48"/>
+      <c r="G26" s="80"/>
+      <c r="H26" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="I26" s="48"/>
+      <c r="J26" s="81"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="81"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="81"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="81"/>
+      <c r="B28" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="C28" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="D28" s="78"/>
+      <c r="E28" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="F28" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="G28" s="78"/>
+      <c r="H28" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="I28" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="J28" s="81"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="81"/>
+      <c r="B29" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="C29" s="48" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" s="79"/>
+      <c r="E29" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="F29" s="48" t="s">
+        <v>219</v>
+      </c>
+      <c r="G29" s="79"/>
+      <c r="H29" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="I29" s="48" t="s">
+        <v>210</v>
+      </c>
+      <c r="J29" s="81"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="81"/>
+      <c r="B30" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="D30" s="79"/>
+      <c r="E30" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="F30" s="48" t="s">
+        <v>220</v>
+      </c>
+      <c r="G30" s="79"/>
+      <c r="H30" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="I30" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="J30" s="81"/>
+    </row>
+    <row r="31" spans="1:10" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="81"/>
+      <c r="B31" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="C31" s="48"/>
+      <c r="D31" s="80"/>
+      <c r="E31" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="F31" s="48"/>
+      <c r="G31" s="80"/>
+      <c r="H31" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="I31" s="48"/>
+      <c r="J31" s="81"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" s="81"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="81"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" s="81"/>
+      <c r="B33" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="C33" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="D33" s="78"/>
+      <c r="E33" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="F33" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="G33" s="78"/>
+      <c r="H33" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="I33" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="J33" s="81"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" s="81"/>
+      <c r="B34" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="C34" s="48" t="s">
+        <v>200</v>
+      </c>
+      <c r="D34" s="79"/>
+      <c r="E34" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="F34" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="G34" s="79"/>
+      <c r="H34" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="I34" s="48" t="s">
+        <v>184</v>
+      </c>
+      <c r="J34" s="81"/>
+    </row>
+    <row r="35" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="81"/>
+      <c r="B35" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="D35" s="79"/>
+      <c r="E35" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="F35" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="G35" s="79"/>
+      <c r="H35" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="I35" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="J35" s="81"/>
+    </row>
+    <row r="36" spans="1:10" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="81"/>
+      <c r="B36" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="C36" s="48"/>
+      <c r="D36" s="80"/>
+      <c r="E36" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="F36" s="48"/>
+      <c r="G36" s="80"/>
+      <c r="H36" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="I36" s="48"/>
+      <c r="J36" s="81"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37" s="81"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="81"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" s="81"/>
+      <c r="B38" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="C38" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="D38" s="78"/>
+      <c r="E38" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="F38" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="G38" s="78"/>
+      <c r="H38" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="I38" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="J38" s="81"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" s="81"/>
+      <c r="B39" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="C39" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="D39" s="79"/>
+      <c r="E39" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="F39" s="48" t="s">
+        <v>222</v>
+      </c>
+      <c r="G39" s="79"/>
+      <c r="H39" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="I39" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="J39" s="81"/>
+    </row>
+    <row r="40" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="81"/>
+      <c r="B40" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="C40" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="73" t="s">
-        <v>187</v>
-      </c>
-      <c r="F4" s="73" t="s">
+      <c r="D40" s="79"/>
+      <c r="E40" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="F40" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="G40" s="79"/>
+      <c r="H40" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="I40" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="J40" s="81"/>
+    </row>
+    <row r="41" spans="1:10" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="81"/>
+      <c r="B41" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="C41" s="48"/>
+      <c r="D41" s="80"/>
+      <c r="E41" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="F41" s="48"/>
+      <c r="G41" s="80"/>
+      <c r="H41" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="I41" s="48"/>
+      <c r="J41" s="81"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42" s="81"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="81"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A43" s="81"/>
+      <c r="B43" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="C43" s="48" t="s">
+        <v>181</v>
+      </c>
+      <c r="D43" s="78"/>
+      <c r="E43" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="F43" s="48" t="s">
+        <v>181</v>
+      </c>
+      <c r="G43" s="78"/>
+      <c r="H43" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="I43" s="48" t="s">
+        <v>181</v>
+      </c>
+      <c r="J43" s="81"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44" s="81"/>
+      <c r="B44" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="C44" s="48" t="s">
         <v>203</v>
       </c>
-      <c r="G4" s="80"/>
-      <c r="H4" s="73" t="s">
-        <v>187</v>
-      </c>
-      <c r="I4" s="73" t="s">
+      <c r="D44" s="79"/>
+      <c r="E44" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="F44" s="48" t="s">
+        <v>224</v>
+      </c>
+      <c r="G44" s="79"/>
+      <c r="H44" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="I44" s="48" t="s">
         <v>204</v>
       </c>
-      <c r="J4" s="83"/>
-    </row>
-    <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="83"/>
-      <c r="B5" s="75" t="s">
-        <v>188</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="D5" s="80"/>
-      <c r="E5" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>232</v>
-      </c>
-      <c r="G5" s="80"/>
-      <c r="H5" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="J5" s="83"/>
-    </row>
-    <row r="6" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="83"/>
-      <c r="B6" s="75" t="s">
-        <v>189</v>
-      </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="F6" s="73"/>
-      <c r="G6" s="81"/>
-      <c r="H6" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="I6" s="73"/>
-      <c r="J6" s="83"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="83"/>
-      <c r="B7" s="77"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="83"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="83"/>
-      <c r="B8" s="75" t="s">
-        <v>185</v>
-      </c>
-      <c r="C8" s="73" t="s">
-        <v>193</v>
-      </c>
-      <c r="D8" s="79"/>
-      <c r="E8" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="F8" s="73" t="s">
-        <v>193</v>
-      </c>
-      <c r="G8" s="79"/>
-      <c r="H8" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="I8" s="73" t="s">
-        <v>193</v>
-      </c>
-      <c r="J8" s="83"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="83"/>
-      <c r="B9" s="75" t="s">
-        <v>187</v>
-      </c>
-      <c r="C9" s="73" t="s">
-        <v>202</v>
-      </c>
-      <c r="D9" s="80"/>
-      <c r="E9" s="73" t="s">
-        <v>187</v>
-      </c>
-      <c r="F9" s="73" t="s">
-        <v>203</v>
-      </c>
-      <c r="G9" s="80"/>
-      <c r="H9" s="73" t="s">
-        <v>187</v>
-      </c>
-      <c r="I9" s="73" t="s">
-        <v>224</v>
-      </c>
-      <c r="J9" s="83"/>
-    </row>
-    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="83"/>
-      <c r="B10" s="75" t="s">
-        <v>188</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="D10" s="80"/>
-      <c r="E10" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="G10" s="80"/>
-      <c r="H10" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="J10" s="83"/>
-    </row>
-    <row r="11" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="83"/>
-      <c r="B11" s="75" t="s">
-        <v>189</v>
-      </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="F11" s="73"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="I11" s="73"/>
-      <c r="J11" s="83"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="83"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="83"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="83"/>
-      <c r="B13" s="75" t="s">
-        <v>185</v>
-      </c>
-      <c r="C13" s="73" t="s">
-        <v>194</v>
-      </c>
-      <c r="D13" s="79"/>
-      <c r="E13" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="F13" s="73" t="s">
-        <v>194</v>
-      </c>
-      <c r="G13" s="79"/>
-      <c r="H13" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="I13" s="73" t="s">
-        <v>194</v>
-      </c>
-      <c r="J13" s="83"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="83"/>
-      <c r="B14" s="75" t="s">
-        <v>187</v>
-      </c>
-      <c r="C14" s="73" t="s">
-        <v>202</v>
-      </c>
-      <c r="D14" s="80"/>
-      <c r="E14" s="73" t="s">
-        <v>187</v>
-      </c>
-      <c r="F14" s="73"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="73" t="s">
-        <v>187</v>
-      </c>
-      <c r="I14" s="73"/>
-      <c r="J14" s="83"/>
-    </row>
-    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="83"/>
-      <c r="B15" s="75" t="s">
-        <v>188</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="D15" s="80"/>
-      <c r="E15" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="80"/>
-      <c r="H15" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="I15" s="21"/>
-      <c r="J15" s="83"/>
-    </row>
-    <row r="16" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="83"/>
-      <c r="B16" s="75" t="s">
-        <v>189</v>
-      </c>
-      <c r="C16" s="73"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="F16" s="73"/>
-      <c r="G16" s="81"/>
-      <c r="H16" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="I16" s="73"/>
-      <c r="J16" s="83"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="83"/>
-      <c r="B17" s="77"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="83"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="83"/>
-      <c r="B18" s="75" t="s">
-        <v>185</v>
-      </c>
-      <c r="C18" s="73" t="s">
-        <v>195</v>
-      </c>
-      <c r="D18" s="79"/>
-      <c r="E18" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="F18" s="73" t="s">
-        <v>195</v>
-      </c>
-      <c r="G18" s="79"/>
-      <c r="H18" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="I18" s="73" t="s">
-        <v>195</v>
-      </c>
-      <c r="J18" s="83"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="83"/>
-      <c r="B19" s="75" t="s">
-        <v>187</v>
-      </c>
-      <c r="C19" s="73" t="s">
+      <c r="J44" s="81"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A45" s="81"/>
+      <c r="B45" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="C45" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="D19" s="80"/>
-      <c r="E19" s="73" t="s">
-        <v>187</v>
-      </c>
-      <c r="F19" s="73" t="s">
-        <v>205</v>
-      </c>
-      <c r="G19" s="80"/>
-      <c r="H19" s="73" t="s">
-        <v>187</v>
-      </c>
-      <c r="I19" s="73" t="s">
-        <v>205</v>
-      </c>
-      <c r="J19" s="83"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="83"/>
-      <c r="B20" s="75" t="s">
-        <v>188</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="D20" s="80"/>
-      <c r="E20" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="G20" s="80"/>
-      <c r="H20" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="I20" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="J20" s="83"/>
-    </row>
-    <row r="21" spans="1:10" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="83"/>
-      <c r="B21" s="75" t="s">
-        <v>189</v>
-      </c>
-      <c r="C21" s="73"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="F21" s="73"/>
-      <c r="G21" s="81"/>
-      <c r="H21" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="I21" s="73"/>
-      <c r="J21" s="83"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="83"/>
-      <c r="B22" s="77"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="83"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="83"/>
-      <c r="B23" s="75" t="s">
-        <v>185</v>
-      </c>
-      <c r="C23" s="73" t="s">
-        <v>196</v>
-      </c>
-      <c r="D23" s="79"/>
-      <c r="E23" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="F23" s="73" t="s">
-        <v>196</v>
-      </c>
-      <c r="G23" s="79"/>
-      <c r="H23" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="I23" s="73" t="s">
-        <v>196</v>
-      </c>
-      <c r="J23" s="83"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="83"/>
-      <c r="B24" s="75" t="s">
-        <v>187</v>
-      </c>
-      <c r="C24" s="73" t="s">
-        <v>214</v>
-      </c>
-      <c r="D24" s="80"/>
-      <c r="E24" s="73" t="s">
-        <v>187</v>
-      </c>
-      <c r="F24" s="73" t="s">
-        <v>234</v>
-      </c>
-      <c r="G24" s="80"/>
-      <c r="H24" s="73" t="s">
-        <v>187</v>
-      </c>
-      <c r="I24" s="73" t="s">
+      <c r="D45" s="79"/>
+      <c r="E45" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="F45" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="J24" s="83"/>
-    </row>
-    <row r="25" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="83"/>
-      <c r="B25" s="75" t="s">
-        <v>188</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>213</v>
-      </c>
-      <c r="D25" s="80"/>
-      <c r="E25" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="G25" s="80"/>
-      <c r="H25" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="I25" s="21" t="s">
+      <c r="G45" s="79"/>
+      <c r="H45" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="I45" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="J25" s="83"/>
-    </row>
-    <row r="26" spans="1:10" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="83"/>
-      <c r="B26" s="75" t="s">
-        <v>189</v>
-      </c>
-      <c r="C26" s="73"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="F26" s="73"/>
-      <c r="G26" s="81"/>
-      <c r="H26" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="I26" s="73"/>
-      <c r="J26" s="83"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="83"/>
-      <c r="B27" s="77"/>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="74"/>
-      <c r="I27" s="74"/>
-      <c r="J27" s="83"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="83"/>
-      <c r="B28" s="75" t="s">
-        <v>185</v>
-      </c>
-      <c r="C28" s="73" t="s">
-        <v>197</v>
-      </c>
-      <c r="D28" s="79"/>
-      <c r="E28" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="F28" s="73" t="s">
-        <v>197</v>
-      </c>
-      <c r="G28" s="79"/>
-      <c r="H28" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="I28" s="73" t="s">
-        <v>197</v>
-      </c>
-      <c r="J28" s="83"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="83"/>
-      <c r="B29" s="75" t="s">
-        <v>187</v>
-      </c>
-      <c r="C29" s="73" t="s">
-        <v>215</v>
-      </c>
-      <c r="D29" s="80"/>
-      <c r="E29" s="73" t="s">
-        <v>187</v>
-      </c>
-      <c r="F29" s="73" t="s">
-        <v>236</v>
-      </c>
-      <c r="G29" s="80"/>
-      <c r="H29" s="73" t="s">
-        <v>187</v>
-      </c>
-      <c r="I29" s="73" t="s">
-        <v>227</v>
-      </c>
-      <c r="J29" s="83"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="83"/>
-      <c r="B30" s="75" t="s">
-        <v>188</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="D30" s="80"/>
-      <c r="E30" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="F30" s="73" t="s">
-        <v>237</v>
-      </c>
-      <c r="G30" s="80"/>
-      <c r="H30" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="I30" s="73" t="s">
-        <v>228</v>
-      </c>
-      <c r="J30" s="83"/>
-    </row>
-    <row r="31" spans="1:10" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="83"/>
-      <c r="B31" s="75" t="s">
-        <v>189</v>
-      </c>
-      <c r="C31" s="73"/>
-      <c r="D31" s="81"/>
-      <c r="E31" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="F31" s="73"/>
-      <c r="G31" s="81"/>
-      <c r="H31" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="I31" s="73"/>
-      <c r="J31" s="83"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" s="83"/>
-      <c r="B32" s="77"/>
-      <c r="C32" s="74"/>
-      <c r="D32" s="74"/>
-      <c r="E32" s="74"/>
-      <c r="F32" s="74"/>
-      <c r="G32" s="74"/>
-      <c r="H32" s="74"/>
-      <c r="I32" s="74"/>
-      <c r="J32" s="83"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="83"/>
-      <c r="B33" s="75" t="s">
-        <v>185</v>
-      </c>
-      <c r="C33" s="73" t="s">
-        <v>196</v>
-      </c>
-      <c r="D33" s="79"/>
-      <c r="E33" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="F33" s="73" t="s">
-        <v>196</v>
-      </c>
-      <c r="G33" s="79"/>
-      <c r="H33" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="I33" s="73" t="s">
-        <v>196</v>
-      </c>
-      <c r="J33" s="83"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="83"/>
-      <c r="B34" s="75" t="s">
-        <v>187</v>
-      </c>
-      <c r="C34" s="73" t="s">
-        <v>217</v>
-      </c>
-      <c r="D34" s="80"/>
-      <c r="E34" s="73" t="s">
-        <v>187</v>
-      </c>
-      <c r="F34" s="73" t="s">
-        <v>200</v>
-      </c>
-      <c r="G34" s="80"/>
-      <c r="H34" s="73" t="s">
-        <v>187</v>
-      </c>
-      <c r="I34" s="73" t="s">
-        <v>201</v>
-      </c>
-      <c r="J34" s="83"/>
-    </row>
-    <row r="35" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="83"/>
-      <c r="B35" s="75" t="s">
-        <v>188</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="D35" s="80"/>
-      <c r="E35" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="F35" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="G35" s="80"/>
-      <c r="H35" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="I35" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="J35" s="83"/>
-    </row>
-    <row r="36" spans="1:10" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="83"/>
-      <c r="B36" s="75" t="s">
-        <v>189</v>
-      </c>
-      <c r="C36" s="73"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="F36" s="73"/>
-      <c r="G36" s="81"/>
-      <c r="H36" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="I36" s="73"/>
-      <c r="J36" s="83"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A37" s="83"/>
-      <c r="B37" s="77"/>
-      <c r="C37" s="74"/>
-      <c r="D37" s="82"/>
-      <c r="E37" s="74"/>
-      <c r="F37" s="74"/>
-      <c r="G37" s="74"/>
-      <c r="H37" s="74"/>
-      <c r="I37" s="74"/>
-      <c r="J37" s="83"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="83"/>
-      <c r="B38" s="75" t="s">
-        <v>185</v>
-      </c>
-      <c r="C38" s="73" t="s">
-        <v>197</v>
-      </c>
-      <c r="D38" s="79"/>
-      <c r="E38" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="F38" s="73" t="s">
-        <v>197</v>
-      </c>
-      <c r="G38" s="79"/>
-      <c r="H38" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="I38" s="73" t="s">
-        <v>197</v>
-      </c>
-      <c r="J38" s="83"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" s="83"/>
-      <c r="B39" s="75" t="s">
-        <v>187</v>
-      </c>
-      <c r="C39" s="73" t="s">
-        <v>199</v>
-      </c>
-      <c r="D39" s="80"/>
-      <c r="E39" s="73" t="s">
-        <v>187</v>
-      </c>
-      <c r="F39" s="73" t="s">
-        <v>239</v>
-      </c>
-      <c r="G39" s="80"/>
-      <c r="H39" s="73" t="s">
-        <v>187</v>
-      </c>
-      <c r="I39" s="73" t="s">
-        <v>230</v>
-      </c>
-      <c r="J39" s="83"/>
-    </row>
-    <row r="40" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="83"/>
-      <c r="B40" s="75" t="s">
-        <v>188</v>
-      </c>
-      <c r="C40" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="D40" s="80"/>
-      <c r="E40" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="F40" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="G40" s="80"/>
-      <c r="H40" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="I40" s="21" t="s">
-        <v>231</v>
-      </c>
-      <c r="J40" s="83"/>
-    </row>
-    <row r="41" spans="1:10" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="83"/>
-      <c r="B41" s="75" t="s">
-        <v>189</v>
-      </c>
-      <c r="C41" s="73"/>
-      <c r="D41" s="81"/>
-      <c r="E41" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="F41" s="73"/>
-      <c r="G41" s="81"/>
-      <c r="H41" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="I41" s="73"/>
-      <c r="J41" s="83"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A42" s="83"/>
-      <c r="B42" s="77"/>
-      <c r="C42" s="74"/>
-      <c r="D42" s="74"/>
-      <c r="E42" s="74"/>
-      <c r="F42" s="74"/>
-      <c r="G42" s="74"/>
-      <c r="H42" s="74"/>
-      <c r="I42" s="74"/>
-      <c r="J42" s="83"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A43" s="83"/>
-      <c r="B43" s="75" t="s">
-        <v>185</v>
-      </c>
-      <c r="C43" s="73" t="s">
-        <v>198</v>
-      </c>
-      <c r="D43" s="79"/>
-      <c r="E43" s="75" t="s">
-        <v>185</v>
-      </c>
-      <c r="F43" s="73" t="s">
-        <v>198</v>
-      </c>
-      <c r="G43" s="79"/>
-      <c r="H43" s="75" t="s">
-        <v>185</v>
-      </c>
-      <c r="I43" s="73" t="s">
-        <v>198</v>
-      </c>
-      <c r="J43" s="83"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A44" s="83"/>
-      <c r="B44" s="75" t="s">
-        <v>187</v>
-      </c>
-      <c r="C44" s="73" t="s">
-        <v>220</v>
-      </c>
-      <c r="D44" s="80"/>
-      <c r="E44" s="75" t="s">
-        <v>187</v>
-      </c>
-      <c r="F44" s="73" t="s">
-        <v>241</v>
-      </c>
-      <c r="G44" s="80"/>
-      <c r="H44" s="75" t="s">
-        <v>187</v>
-      </c>
-      <c r="I44" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="J44" s="83"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A45" s="83"/>
-      <c r="B45" s="75" t="s">
-        <v>188</v>
-      </c>
-      <c r="C45" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="D45" s="80"/>
-      <c r="E45" s="75" t="s">
-        <v>188</v>
-      </c>
-      <c r="F45" s="21" t="s">
-        <v>242</v>
-      </c>
-      <c r="G45" s="80"/>
-      <c r="H45" s="75" t="s">
-        <v>188</v>
-      </c>
-      <c r="I45" s="21" t="s">
-        <v>243</v>
-      </c>
-      <c r="J45" s="83"/>
+      <c r="J45" s="81"/>
     </row>
     <row r="46" spans="1:10" ht="88" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="83"/>
-      <c r="B46" s="75" t="s">
-        <v>189</v>
-      </c>
-      <c r="C46" s="73"/>
-      <c r="D46" s="81"/>
-      <c r="E46" s="75" t="s">
-        <v>189</v>
-      </c>
-      <c r="F46" s="73"/>
-      <c r="G46" s="81"/>
-      <c r="H46" s="75" t="s">
-        <v>189</v>
-      </c>
-      <c r="I46" s="73"/>
-      <c r="J46" s="83"/>
+      <c r="A46" s="81"/>
+      <c r="B46" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="C46" s="48"/>
+      <c r="D46" s="80"/>
+      <c r="E46" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="F46" s="48"/>
+      <c r="G46" s="80"/>
+      <c r="H46" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="I46" s="48"/>
+      <c r="J46" s="81"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A47" s="83"/>
-      <c r="B47" s="77"/>
-      <c r="C47" s="74"/>
-      <c r="D47" s="74"/>
-      <c r="E47" s="77"/>
-      <c r="F47" s="74"/>
-      <c r="G47" s="74"/>
-      <c r="H47" s="77"/>
-      <c r="I47" s="74"/>
-      <c r="J47" s="83"/>
+      <c r="A47" s="81"/>
+      <c r="B47" s="52"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="49"/>
+      <c r="E47" s="52"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="49"/>
+      <c r="H47" s="52"/>
+      <c r="I47" s="49"/>
+      <c r="J47" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="D33:D36"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="D18:D21"/>
     <mergeCell ref="D43:D46"/>
     <mergeCell ref="A1:A47"/>
     <mergeCell ref="J1:J47"/>
@@ -5735,13 +5903,6 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="D33:D36"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="D8:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added comments, updated variables visibility and getCustomer method
</commit_message>
<xml_diff>
--- a/User Stories/NataliaUserStories.xlsx
+++ b/User Stories/NataliaUserStories.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cad1acabf18afac6/Desktop/Software Design with AI for Cloud/Year_3/agile-labs3/Newsagent-Project/User Stories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="539" documentId="13_ncr:1_{7B2E17FA-F2A9-4DCC-A803-850E080333ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0D8BE94-FE48-44AC-9C91-AB97ABC9B086}"/>
+  <xr:revisionPtr revIDLastSave="717" documentId="13_ncr:1_{7B2E17FA-F2A9-4DCC-A803-850E080333ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD2F20F0-CCF2-4241-AD8F-603297AE5673}"/>
   <bookViews>
-    <workbookView xWindow="15530" yWindow="2750" windowWidth="22160" windowHeight="16250" activeTab="2" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
+    <workbookView xWindow="21160" yWindow="2750" windowWidth="16530" windowHeight="16250" activeTab="1" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminUserStories" sheetId="1" r:id="rId1"/>
     <sheet name="NewsagentUserStories" sheetId="2" r:id="rId2"/>
     <sheet name="UMLs" sheetId="3" r:id="rId3"/>
-    <sheet name="MySQL Tests" sheetId="4" r:id="rId4"/>
+    <sheet name="JUnit" sheetId="5" r:id="rId4"/>
+    <sheet name="MySQL Tests" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="266">
   <si>
     <t>As an admin</t>
   </si>
@@ -242,9 +243,6 @@
     <t>Phone number format 0 11 222 333 (total of 10 digits)</t>
   </si>
   <si>
-    <t>Verify valid phoneNo &lt;= 13 digits</t>
-  </si>
-  <si>
     <t xml:space="preserve">Handle spaces on phoneNo and if cust enters +353 </t>
   </si>
   <si>
@@ -440,18 +438,9 @@
     <t>- password : String</t>
   </si>
   <si>
-    <t>- customerDatabase: Database</t>
-  </si>
-  <si>
-    <t>- userDatabase : Database</t>
-  </si>
-  <si>
     <t>Customer</t>
   </si>
   <si>
-    <t>+Newsagent : (username: String, password: String, role: String, customerDatabase: Database)</t>
-  </si>
-  <si>
     <t>+getCustID() : void</t>
   </si>
   <si>
@@ -539,9 +528,6 @@
     <t>so that I can log in with driver permissions</t>
   </si>
   <si>
-    <t>+User: (username: String, password: String, role: String, userDatabase: Database)</t>
-  </si>
-  <si>
     <t>Verify valid 0 &lt; custAddress &lt;= 20 characters</t>
   </si>
   <si>
@@ -731,12 +717,6 @@
     <t>+Customer()</t>
   </si>
   <si>
-    <t>+getCustomerDetails(int id) : String</t>
-  </si>
-  <si>
-    <t>+getAllCustomerDetails() : String</t>
-  </si>
-  <si>
     <t>+getCustomerOrder(int id) : String</t>
   </si>
   <si>
@@ -788,20 +768,83 @@
     <t>+ deleteUser(int id): void</t>
   </si>
   <si>
-    <t>+Admin : (username: String, password: String, role: String, userDatabase: Database)</t>
-  </si>
-  <si>
-    <t>+getCustomer(int id) : void</t>
-  </si>
-  <si>
     <t>+deactivateCustomer(int id) : void</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>- DB_DRIVER : String</t>
+  </si>
+  <si>
+    <t>- JDBC_URL : String</t>
+  </si>
+  <si>
+    <t>- USERNAME : String</t>
+  </si>
+  <si>
+    <t>- PASSWORD : String</t>
+  </si>
+  <si>
+    <t>+ Connection getConnection()</t>
+  </si>
+  <si>
+    <t>- newsagentID : int</t>
+  </si>
+  <si>
+    <t>- adminID : int</t>
+  </si>
+  <si>
+    <t>- userID : int</t>
+  </si>
+  <si>
+    <t>+Newsagent : (username: String, password: String, role: String)</t>
+  </si>
+  <si>
+    <t>+Admin : (username: String, password: String, role: String)</t>
+  </si>
+  <si>
+    <t>+User: (username: String, password: String, role: String)</t>
+  </si>
+  <si>
+    <t>+getAllUsers() : void</t>
+  </si>
+  <si>
+    <t>+ isValidUsername(String username) : boolean</t>
+  </si>
+  <si>
+    <t>+isValidPassword(String password) : boolean</t>
+  </si>
+  <si>
+    <t>+isValidRole(String role) : boolean</t>
+  </si>
+  <si>
+    <t>+isValidUpdate(String updateColumn, String newValue) : boolean</t>
+  </si>
+  <si>
+    <t>+isValidAddress(String address) : boolean</t>
+  </si>
+  <si>
+    <t>+isValidPhoneNo(String phoneNo) : boolean</t>
+  </si>
+  <si>
+    <t>+getCustomer(int id) : String</t>
+  </si>
+  <si>
+    <t>+getAllCustomers() : String</t>
+  </si>
+  <si>
+    <t>+isValidName(String firstName) : boolean</t>
+  </si>
+  <si>
+    <t>Verify valid 10 digits &lt; phoneNo &lt;= 12 digits</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -842,6 +885,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -988,7 +1038,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1132,16 +1182,64 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1156,51 +1254,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1216,15 +1269,24 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1250,6 +1312,187 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>37354</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>74706</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2779060</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>155841</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44D60117-9839-A68D-6CE1-7C2F4067F98A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3227295" y="4549588"/>
+          <a:ext cx="2741706" cy="3442900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>22411</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>171823</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2578803</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEC1F80D-A7CF-5CC0-DCCA-84A9C8DC111F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6394823" y="5386294"/>
+          <a:ext cx="2556392" cy="2741706"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>89648</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>119529</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2807403</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>127001</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62AED55F-78CF-AA51-96CE-F2A708311613}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9360648" y="4213411"/>
+          <a:ext cx="2717755" cy="2995707"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>119530</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2196353</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>66756</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{304D75E9-E105-B890-9399-EDF4D68BA8DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12363824" y="2906059"/>
+          <a:ext cx="2173941" cy="2188402"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2750,6 +2993,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3082,16 +3329,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="55">
+      <c r="A2" s="63">
         <v>1</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="57" t="s">
-        <v>154</v>
-      </c>
-      <c r="D2" s="57" t="s">
+      <c r="C2" s="56" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="56" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="15" t="s">
@@ -3102,10 +3349,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="56"/>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
       <c r="E3" s="15" t="s">
         <v>47</v>
       </c>
@@ -3114,50 +3361,50 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="56"/>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
+      <c r="A4" s="64"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="15" t="s">
         <v>49</v>
       </c>
       <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="56"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
+      <c r="A5" s="64"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="15" t="s">
         <v>50</v>
       </c>
       <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="56"/>
-      <c r="B6" s="58"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
+      <c r="A6" s="64"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
       <c r="E6" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="64"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="56"/>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="15" t="s">
-        <v>159</v>
-      </c>
       <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="56"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
       <c r="E8" s="15" t="s">
         <v>37</v>
       </c>
@@ -3172,80 +3419,80 @@
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="55">
+      <c r="A10" s="63">
         <v>2</v>
       </c>
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="57" t="s">
-        <v>82</v>
+      <c r="D10" s="56" t="s">
+        <v>81</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="64"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="15" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="56"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="15" t="s">
+      <c r="F11" s="21"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="64"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="21"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="64"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="F11" s="21"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="56"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="21"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="56"/>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="15" t="s">
+      <c r="F13" s="21"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="64"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="21"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="56"/>
-      <c r="B14" s="58"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="15" t="s">
-        <v>90</v>
-      </c>
       <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="56"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
+      <c r="A15" s="64"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
       <c r="E15" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="69"/>
-      <c r="B16" s="70"/>
-      <c r="C16" s="70"/>
-      <c r="D16" s="70"/>
+      <c r="A16" s="65"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
       <c r="E16" s="15" t="s">
         <v>14</v>
       </c>
@@ -3260,40 +3507,40 @@
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="55">
+      <c r="A18" s="63">
         <v>3</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="57" t="s">
+      <c r="C18" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="57" t="s">
+      <c r="D18" s="56" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F18" s="21" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="56"/>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
+      <c r="A19" s="64"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
       <c r="E19" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="69"/>
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
+      <c r="A20" s="65"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
       <c r="E20" s="11" t="s">
         <v>51</v>
       </c>
@@ -3308,80 +3555,80 @@
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="55">
+      <c r="A22" s="63">
         <v>4</v>
       </c>
-      <c r="B22" s="57" t="s">
+      <c r="B22" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="57" t="s">
+      <c r="C22" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="57" t="s">
+      <c r="D22" s="56" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>40</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="56"/>
-      <c r="B23" s="58"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="58"/>
+      <c r="A23" s="64"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
       <c r="E23" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" s="21"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="64"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="F23" s="21"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="56"/>
-      <c r="B24" s="58"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="15" t="s">
+      <c r="F24" s="21"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="64"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="F24" s="21"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="56"/>
-      <c r="B25" s="58"/>
-      <c r="C25" s="58"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="15" t="s">
-        <v>99</v>
-      </c>
       <c r="F25" s="21"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="56"/>
-      <c r="B26" s="58"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
+      <c r="A26" s="64"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
       <c r="E26" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" s="21"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="64"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="F26" s="21"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="56"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="15" t="s">
-        <v>94</v>
-      </c>
       <c r="F27" s="21"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="69"/>
-      <c r="B28" s="70"/>
-      <c r="C28" s="70"/>
-      <c r="D28" s="70"/>
+      <c r="A28" s="65"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="58"/>
       <c r="E28" s="15" t="s">
         <v>11</v>
       </c>
@@ -3396,17 +3643,17 @@
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="55">
+      <c r="A30" s="63">
         <v>5</v>
       </c>
-      <c r="B30" s="57" t="s">
+      <c r="B30" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="57" t="s">
+      <c r="C30" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="57" t="s">
-        <v>83</v>
+      <c r="D30" s="56" t="s">
+        <v>82</v>
       </c>
       <c r="E30" s="15" t="s">
         <v>40</v>
@@ -3414,22 +3661,22 @@
       <c r="F30" s="21"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="56"/>
-      <c r="B31" s="58"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="58"/>
+      <c r="A31" s="64"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
       <c r="E31" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" s="21"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="65"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="15" t="s">
         <v>95</v>
-      </c>
-      <c r="F31" s="21"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="69"/>
-      <c r="B32" s="70"/>
-      <c r="C32" s="70"/>
-      <c r="D32" s="70"/>
-      <c r="E32" s="15" t="s">
-        <v>96</v>
       </c>
       <c r="F32" s="21"/>
     </row>
@@ -3442,32 +3689,32 @@
       <c r="F33" s="7"/>
     </row>
     <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="55">
+      <c r="A34" s="63">
         <v>6</v>
       </c>
-      <c r="B34" s="57" t="s">
+      <c r="B34" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="57" t="s">
+      <c r="C34" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="57" t="s">
+      <c r="D34" s="56" t="s">
         <v>16</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="69"/>
-      <c r="B35" s="70"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="70"/>
+      <c r="A35" s="65"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="58"/>
       <c r="E35" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F35" s="21"/>
     </row>
@@ -3480,72 +3727,72 @@
       <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="74">
+      <c r="A37" s="66">
         <v>7</v>
       </c>
-      <c r="B37" s="73" t="s">
+      <c r="B37" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="73" t="s">
+      <c r="C37" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="73" t="s">
+      <c r="E37" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F37" s="56" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="66"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="E37" s="21" t="s">
+      <c r="F38" s="57"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="66"/>
+      <c r="B39" s="62"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" s="58"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="66"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="62"/>
+      <c r="E40" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F40" s="21"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="66"/>
+      <c r="B41" s="62"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41" s="21"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="66"/>
+      <c r="B42" s="62"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="21" t="s">
         <v>75</v>
-      </c>
-      <c r="F37" s="57" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="74"/>
-      <c r="B38" s="73"/>
-      <c r="C38" s="73"/>
-      <c r="D38" s="73"/>
-      <c r="E38" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="F38" s="58"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="74"/>
-      <c r="B39" s="73"/>
-      <c r="C39" s="73"/>
-      <c r="D39" s="73"/>
-      <c r="E39" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F39" s="70"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="74"/>
-      <c r="B40" s="73"/>
-      <c r="C40" s="73"/>
-      <c r="D40" s="73"/>
-      <c r="E40" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="F40" s="21"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="74"/>
-      <c r="B41" s="73"/>
-      <c r="C41" s="73"/>
-      <c r="D41" s="73"/>
-      <c r="E41" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="F41" s="21"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="74"/>
-      <c r="B42" s="73"/>
-      <c r="C42" s="73"/>
-      <c r="D42" s="73"/>
-      <c r="E42" s="21" t="s">
-        <v>76</v>
       </c>
       <c r="F42" s="21"/>
     </row>
@@ -3558,82 +3805,82 @@
       <c r="F43" s="7"/>
     </row>
     <row r="44" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="75">
+      <c r="A44" s="59">
         <v>8</v>
       </c>
-      <c r="B44" s="57" t="s">
+      <c r="B44" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="57" t="s">
-        <v>156</v>
-      </c>
-      <c r="D44" s="57" t="s">
-        <v>157</v>
+      <c r="C44" s="56" t="s">
+        <v>152</v>
+      </c>
+      <c r="D44" s="56" t="s">
+        <v>153</v>
       </c>
       <c r="E44" s="21" t="s">
         <v>39</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="76"/>
-      <c r="B45" s="58"/>
-      <c r="C45" s="58"/>
-      <c r="D45" s="58"/>
+      <c r="A45" s="60"/>
+      <c r="B45" s="57"/>
+      <c r="C45" s="57"/>
+      <c r="D45" s="57"/>
       <c r="E45" s="21" t="s">
         <v>47</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="76"/>
-      <c r="B46" s="58"/>
-      <c r="C46" s="58"/>
-      <c r="D46" s="58"/>
+      <c r="A46" s="60"/>
+      <c r="B46" s="57"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
       <c r="E46" s="21" t="s">
         <v>49</v>
       </c>
       <c r="F46" s="21"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="76"/>
-      <c r="B47" s="58"/>
-      <c r="C47" s="58"/>
-      <c r="D47" s="58"/>
+      <c r="A47" s="60"/>
+      <c r="B47" s="57"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
       <c r="E47" s="21" t="s">
         <v>50</v>
       </c>
       <c r="F47" s="21"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" s="76"/>
-      <c r="B48" s="58"/>
-      <c r="C48" s="58"/>
-      <c r="D48" s="58"/>
+      <c r="A48" s="60"/>
+      <c r="B48" s="57"/>
+      <c r="C48" s="57"/>
+      <c r="D48" s="57"/>
       <c r="E48" s="21" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F48" s="21"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="76"/>
-      <c r="B49" s="58"/>
-      <c r="C49" s="58"/>
-      <c r="D49" s="58"/>
+      <c r="A49" s="60"/>
+      <c r="B49" s="57"/>
+      <c r="C49" s="57"/>
+      <c r="D49" s="57"/>
       <c r="E49" s="21" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F49" s="21"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="77"/>
-      <c r="B50" s="70"/>
-      <c r="C50" s="70"/>
-      <c r="D50" s="70"/>
+      <c r="A50" s="61"/>
+      <c r="B50" s="58"/>
+      <c r="C50" s="58"/>
+      <c r="D50" s="58"/>
       <c r="E50" s="21" t="s">
         <v>37</v>
       </c>
@@ -3648,82 +3895,82 @@
       <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="75">
+      <c r="A52" s="59">
         <v>9</v>
       </c>
-      <c r="B52" s="57" t="s">
+      <c r="B52" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C52" s="57" t="s">
-        <v>164</v>
-      </c>
-      <c r="D52" s="57" t="s">
-        <v>165</v>
+      <c r="C52" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="D52" s="56" t="s">
+        <v>161</v>
       </c>
       <c r="E52" s="21" t="s">
         <v>39</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="76"/>
-      <c r="B53" s="58"/>
-      <c r="C53" s="58"/>
-      <c r="D53" s="58"/>
+      <c r="A53" s="60"/>
+      <c r="B53" s="57"/>
+      <c r="C53" s="57"/>
+      <c r="D53" s="57"/>
       <c r="E53" s="21" t="s">
         <v>47</v>
       </c>
       <c r="F53" s="21" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="76"/>
-      <c r="B54" s="58"/>
-      <c r="C54" s="58"/>
-      <c r="D54" s="58"/>
+      <c r="A54" s="60"/>
+      <c r="B54" s="57"/>
+      <c r="C54" s="57"/>
+      <c r="D54" s="57"/>
       <c r="E54" s="21" t="s">
         <v>49</v>
       </c>
       <c r="F54" s="21"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" s="76"/>
-      <c r="B55" s="58"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="58"/>
+      <c r="A55" s="60"/>
+      <c r="B55" s="57"/>
+      <c r="C55" s="57"/>
+      <c r="D55" s="57"/>
       <c r="E55" s="21" t="s">
         <v>50</v>
       </c>
       <c r="F55" s="21"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="76"/>
-      <c r="B56" s="58"/>
-      <c r="C56" s="58"/>
-      <c r="D56" s="58"/>
+      <c r="A56" s="60"/>
+      <c r="B56" s="57"/>
+      <c r="C56" s="57"/>
+      <c r="D56" s="57"/>
       <c r="E56" s="21" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F56" s="21"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A57" s="76"/>
-      <c r="B57" s="58"/>
-      <c r="C57" s="58"/>
-      <c r="D57" s="58"/>
+      <c r="A57" s="60"/>
+      <c r="B57" s="57"/>
+      <c r="C57" s="57"/>
+      <c r="D57" s="57"/>
       <c r="E57" s="21" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F57" s="21"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="77"/>
-      <c r="B58" s="70"/>
-      <c r="C58" s="70"/>
-      <c r="D58" s="70"/>
+      <c r="A58" s="61"/>
+      <c r="B58" s="58"/>
+      <c r="C58" s="58"/>
+      <c r="D58" s="58"/>
       <c r="E58" s="21" t="s">
         <v>37</v>
       </c>
@@ -3746,40 +3993,40 @@
       <c r="F64" s="7"/>
     </row>
     <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="63">
+      <c r="A65" s="69">
         <v>10</v>
       </c>
-      <c r="B65" s="66" t="s">
+      <c r="B65" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="C65" s="66" t="s">
+      <c r="C65" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="D65" s="66" t="s">
+      <c r="D65" s="72" t="s">
         <v>33</v>
       </c>
       <c r="E65" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F65" s="71" t="s">
+      <c r="F65" s="67" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66" s="64"/>
-      <c r="B66" s="67"/>
-      <c r="C66" s="67"/>
-      <c r="D66" s="67"/>
+      <c r="A66" s="70"/>
+      <c r="B66" s="73"/>
+      <c r="C66" s="73"/>
+      <c r="D66" s="73"/>
       <c r="E66" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="F66" s="72"/>
+      <c r="F66" s="68"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" s="65"/>
-      <c r="B67" s="68"/>
-      <c r="C67" s="68"/>
-      <c r="D67" s="68"/>
+      <c r="A67" s="71"/>
+      <c r="B67" s="74"/>
+      <c r="C67" s="74"/>
+      <c r="D67" s="74"/>
       <c r="E67" s="6"/>
       <c r="F67" s="31"/>
     </row>
@@ -3792,16 +4039,16 @@
       <c r="F68" s="7"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="63">
+      <c r="A69" s="69">
         <v>11</v>
       </c>
-      <c r="B69" s="66" t="s">
+      <c r="B69" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="C69" s="66" t="s">
+      <c r="C69" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="D69" s="66" t="s">
+      <c r="D69" s="72" t="s">
         <v>26</v>
       </c>
       <c r="E69" s="17" t="s">
@@ -3810,20 +4057,20 @@
       <c r="F69" s="31"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="64"/>
-      <c r="B70" s="67"/>
-      <c r="C70" s="67"/>
-      <c r="D70" s="67"/>
+      <c r="A70" s="70"/>
+      <c r="B70" s="73"/>
+      <c r="C70" s="73"/>
+      <c r="D70" s="73"/>
       <c r="E70" s="17" t="s">
         <v>28</v>
       </c>
       <c r="F70" s="31"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" s="65"/>
-      <c r="B71" s="68"/>
-      <c r="C71" s="68"/>
-      <c r="D71" s="68"/>
+      <c r="A71" s="71"/>
+      <c r="B71" s="74"/>
+      <c r="C71" s="74"/>
+      <c r="D71" s="74"/>
       <c r="E71" s="17" t="s">
         <v>29</v>
       </c>
@@ -3837,16 +4084,16 @@
       <c r="E74" s="9"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="61">
+      <c r="A75" s="77">
         <v>6</v>
       </c>
-      <c r="B75" s="59" t="s">
+      <c r="B75" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="C75" s="59" t="s">
+      <c r="C75" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="D75" s="59" t="s">
+      <c r="D75" s="75" t="s">
         <v>19</v>
       </c>
       <c r="E75" s="12" t="s">
@@ -3854,10 +4101,10 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A76" s="62"/>
-      <c r="B76" s="60"/>
-      <c r="C76" s="60"/>
-      <c r="D76" s="60"/>
+      <c r="A76" s="78"/>
+      <c r="B76" s="76"/>
+      <c r="C76" s="76"/>
+      <c r="D76" s="76"/>
       <c r="E76" s="12" t="s">
         <v>31</v>
       </c>
@@ -3922,40 +4169,6 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="C44:C50"/>
-    <mergeCell ref="B44:B50"/>
-    <mergeCell ref="D44:D50"/>
-    <mergeCell ref="A44:A50"/>
-    <mergeCell ref="A52:A58"/>
-    <mergeCell ref="B52:B58"/>
-    <mergeCell ref="C52:C58"/>
-    <mergeCell ref="D52:D58"/>
-    <mergeCell ref="C37:C42"/>
-    <mergeCell ref="D37:D42"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="B37:B42"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="D65:D67"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C22:C28"/>
-    <mergeCell ref="D22:D28"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="B2:B8"/>
     <mergeCell ref="C2:C8"/>
@@ -3972,6 +4185,40 @@
     <mergeCell ref="B10:B16"/>
     <mergeCell ref="C10:C16"/>
     <mergeCell ref="D10:D16"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C22:C28"/>
+    <mergeCell ref="D22:D28"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="D65:D67"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="D37:D42"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="B37:B42"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="C44:C50"/>
+    <mergeCell ref="B44:B50"/>
+    <mergeCell ref="D44:D50"/>
+    <mergeCell ref="A44:A50"/>
+    <mergeCell ref="A52:A58"/>
+    <mergeCell ref="B52:B58"/>
+    <mergeCell ref="C52:C58"/>
+    <mergeCell ref="D52:D58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3982,8 +4229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526350BB-95BB-4BF1-93A5-0B30D123D1AA}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4015,16 +4262,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="55">
+      <c r="A2" s="63">
         <v>1</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="57" t="s">
+      <c r="C2" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="56" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="14" t="s">
@@ -4035,82 +4282,82 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="56"/>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
       <c r="E3" s="15" t="s">
         <v>60</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="56"/>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
+      <c r="A4" s="64"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="15" t="s">
         <v>64</v>
       </c>
       <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="56"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
+      <c r="A5" s="64"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="15" t="s">
         <v>65</v>
       </c>
       <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="56"/>
-      <c r="B6" s="58"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
+      <c r="A6" s="64"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
       <c r="E6" s="15" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="56"/>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
       <c r="E7" s="15" t="s">
-        <v>67</v>
+        <v>265</v>
       </c>
       <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="56"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
       <c r="E8" s="15" t="s">
         <v>61</v>
       </c>
       <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="56"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
       <c r="E9" s="15" t="s">
         <v>62</v>
       </c>
       <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="69"/>
-      <c r="B10" s="70"/>
-      <c r="C10" s="70"/>
-      <c r="D10" s="70"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
       <c r="E10" s="15" t="s">
         <v>14</v>
       </c>
@@ -4125,60 +4372,60 @@
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="55">
+      <c r="A12" s="63">
         <v>2</v>
       </c>
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" s="57" t="s">
+      <c r="C12" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="56" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F12" s="21" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="56"/>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
+      <c r="A13" s="64"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
       <c r="E13" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" s="21"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="64"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="F13" s="21"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="56"/>
-      <c r="B14" s="58"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="15" t="s">
+      <c r="F14" s="21"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="64"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="F14" s="21"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="56"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="15" t="s">
-        <v>105</v>
-      </c>
       <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="69"/>
-      <c r="B16" s="70"/>
-      <c r="C16" s="70"/>
-      <c r="D16" s="70"/>
+      <c r="A16" s="65"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
       <c r="E16" s="11" t="s">
         <v>51</v>
       </c>
@@ -4193,72 +4440,72 @@
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="55">
+      <c r="A18" s="63">
         <v>3</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="57" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="57" t="s">
+      <c r="C18" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="56" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F18" s="21" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="56"/>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
+      <c r="A19" s="64"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
       <c r="E19" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="56"/>
-      <c r="B20" s="58"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
+      <c r="A20" s="64"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
       <c r="E20" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="21"/>
+    </row>
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="64"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="F20" s="21"/>
-    </row>
-    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="56"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="15" t="s">
+      <c r="F21" s="21"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="64"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" s="21"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="64"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="15" t="s">
         <v>108</v>
-      </c>
-      <c r="F21" s="21"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="56"/>
-      <c r="B22" s="58"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="F22" s="21"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="56"/>
-      <c r="B23" s="58"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="15" t="s">
-        <v>109</v>
       </c>
       <c r="F23" s="21"/>
     </row>
@@ -4271,30 +4518,30 @@
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="55">
+      <c r="A25" s="63">
         <v>4</v>
       </c>
-      <c r="B25" s="57" t="s">
+      <c r="B25" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="57" t="s">
-        <v>80</v>
-      </c>
-      <c r="D25" s="57" t="s">
+      <c r="C25" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="56" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="F25" s="21"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="64"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="15" t="s">
         <v>111</v>
-      </c>
-      <c r="F25" s="21"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="56"/>
-      <c r="B26" s="58"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="15" t="s">
-        <v>112</v>
       </c>
       <c r="F26" s="21"/>
     </row>
@@ -4307,30 +4554,30 @@
       <c r="F27" s="7"/>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="55">
+      <c r="A28" s="63">
         <v>5</v>
       </c>
-      <c r="B28" s="57" t="s">
+      <c r="B28" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="57" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="57" t="s">
+      <c r="C28" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="56" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="56"/>
-      <c r="B29" s="58"/>
-      <c r="C29" s="58"/>
-      <c r="D29" s="58"/>
+      <c r="A29" s="64"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
       <c r="E29" s="15" t="s">
         <v>17</v>
       </c>
@@ -4345,50 +4592,50 @@
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="55">
+      <c r="A31" s="63">
         <v>6</v>
       </c>
-      <c r="B31" s="57" t="s">
+      <c r="B31" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="57" t="s">
-        <v>114</v>
-      </c>
-      <c r="D31" s="57" t="s">
+      <c r="C31" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="D31" s="56" t="s">
         <v>43</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>40</v>
       </c>
       <c r="F31" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="64"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="15" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="56"/>
-      <c r="B32" s="58"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="15" t="s">
-        <v>117</v>
-      </c>
       <c r="F32" s="21"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="56"/>
-      <c r="B33" s="58"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="58"/>
+      <c r="A33" s="64"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="57"/>
       <c r="E33" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F33" s="21"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="69"/>
-      <c r="B34" s="70"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="70"/>
+      <c r="A34" s="65"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="58"/>
       <c r="E34" s="15" t="s">
         <v>22</v>
       </c>
@@ -4403,16 +4650,16 @@
       <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="55">
+      <c r="A36" s="63">
         <v>7</v>
       </c>
-      <c r="B36" s="57" t="s">
+      <c r="B36" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="57" t="s">
+      <c r="C36" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="57" t="s">
+      <c r="D36" s="56" t="s">
         <v>24</v>
       </c>
       <c r="E36" s="15" t="s">
@@ -4421,20 +4668,20 @@
       <c r="F36" s="21"/>
     </row>
     <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="56"/>
-      <c r="B37" s="58"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="58"/>
+      <c r="A37" s="64"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
       <c r="E37" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F37" s="21"/>
     </row>
     <row r="38" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="69"/>
-      <c r="B38" s="70"/>
-      <c r="C38" s="70"/>
-      <c r="D38" s="70"/>
+      <c r="A38" s="65"/>
+      <c r="B38" s="58"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="58"/>
       <c r="E38" s="15" t="s">
         <v>36</v>
       </c>
@@ -4449,90 +4696,90 @@
       <c r="F39" s="7"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="55">
+      <c r="A40" s="63">
         <v>8</v>
       </c>
-      <c r="B40" s="57" t="s">
+      <c r="B40" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="57" t="s">
-        <v>153</v>
-      </c>
-      <c r="D40" s="57" t="s">
+      <c r="C40" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="D40" s="56" t="s">
+        <v>117</v>
+      </c>
+      <c r="E40" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="E40" s="21" t="s">
+      <c r="F40" s="21"/>
+    </row>
+    <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="64"/>
+      <c r="B41" s="57"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="F40" s="21"/>
-    </row>
-    <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="56"/>
-      <c r="B41" s="58"/>
-      <c r="C41" s="58"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="21" t="s">
+      <c r="F41" s="21"/>
+    </row>
+    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="64"/>
+      <c r="B42" s="57"/>
+      <c r="C42" s="57"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="F41" s="21"/>
-    </row>
-    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="56"/>
-      <c r="B42" s="58"/>
-      <c r="C42" s="58"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="21" t="s">
+      <c r="F42" s="21"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="64"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="57"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="F42" s="21"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="56"/>
-      <c r="B43" s="58"/>
-      <c r="C43" s="58"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="21" t="s">
+      <c r="F43" s="21"/>
+    </row>
+    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="64"/>
+      <c r="B44" s="57"/>
+      <c r="C44" s="57"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="F44" s="21"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="64"/>
+      <c r="B45" s="57"/>
+      <c r="C45" s="57"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="F45" s="21"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="64"/>
+      <c r="B46" s="57"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="F43" s="21"/>
-    </row>
-    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="56"/>
-      <c r="B44" s="58"/>
-      <c r="C44" s="58"/>
-      <c r="D44" s="58"/>
-      <c r="E44" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="F44" s="21"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="56"/>
-      <c r="B45" s="58"/>
-      <c r="C45" s="58"/>
-      <c r="D45" s="58"/>
-      <c r="E45" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="F45" s="21"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="56"/>
-      <c r="B46" s="58"/>
-      <c r="C46" s="58"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="21" t="s">
-        <v>123</v>
-      </c>
       <c r="F46" s="21"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="56"/>
-      <c r="B47" s="58"/>
-      <c r="C47" s="58"/>
-      <c r="D47" s="58"/>
+      <c r="A47" s="64"/>
+      <c r="B47" s="57"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
       <c r="E47" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F47" s="21"/>
     </row>
@@ -4546,6 +4793,30 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="C2:C10"/>
+    <mergeCell ref="D2:D10"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="A31:A34"/>
     <mergeCell ref="A40:A47"/>
     <mergeCell ref="B40:B47"/>
     <mergeCell ref="C40:C47"/>
@@ -4554,30 +4825,6 @@
     <mergeCell ref="C36:C38"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="C2:C10"/>
-    <mergeCell ref="D2:D10"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="D12:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4585,10 +4832,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD0B509-A153-4B31-95B8-BC32DC1B6A3B}">
-  <dimension ref="B2:H25"/>
+  <dimension ref="B2:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4602,53 +4849,62 @@
     <col min="7" max="7" width="3.6328125" style="32" customWidth="1"/>
     <col min="8" max="8" width="40.6328125" style="32" customWidth="1"/>
     <col min="9" max="9" width="3.26953125" customWidth="1"/>
-    <col min="10" max="10" width="26.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.54296875" style="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C2" s="33"/>
       <c r="D2" s="42" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H2" s="43" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B3" s="40" t="s">
-        <v>130</v>
+        <v>147</v>
+      </c>
+      <c r="J2" s="43" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="35" t="s">
+        <v>249</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>130</v>
+        <v>250</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="H3" s="35" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+        <v>142</v>
+      </c>
+      <c r="H3" s="40" t="s">
+        <v>251</v>
+      </c>
+      <c r="J3" s="35" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="38" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+      <c r="J4" s="36" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="38" t="s">
         <v>131</v>
       </c>
@@ -4656,269 +4912,268 @@
         <v>131</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H5" s="36" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="J5" s="36" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>222</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="J6" s="36" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="39"/>
+      <c r="D7" s="36"/>
+      <c r="F7" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="H7" s="37"/>
+      <c r="J7" s="39"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="32" t="s">
+        <v>228</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>224</v>
+      </c>
+      <c r="H8" s="40" t="s">
+        <v>229</v>
+      </c>
+      <c r="J8" s="40"/>
+    </row>
+    <row r="9" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B9" s="34" t="s">
+        <v>252</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>254</v>
+      </c>
+      <c r="J9" s="39" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D10" s="36"/>
+      <c r="F10" s="36" t="s">
+        <v>262</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="89" t="s">
+        <v>239</v>
+      </c>
+      <c r="D11" s="87" t="s">
+        <v>148</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>263</v>
+      </c>
+      <c r="H11" s="38" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="89"/>
+      <c r="D12" s="87"/>
+      <c r="F12" s="38" t="s">
+        <v>225</v>
+      </c>
+      <c r="H12" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="J12" s="55" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="F13" s="38"/>
+      <c r="H13" s="38" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="D14" s="85" t="s">
+        <v>241</v>
+      </c>
+      <c r="F14" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="H14" s="38" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="86" t="s">
+        <v>242</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>240</v>
+      </c>
+      <c r="F15" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="F6" s="38" t="s">
-        <v>227</v>
-      </c>
-      <c r="H6" s="36" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B7" s="39"/>
-      <c r="D7" s="37"/>
-      <c r="F7" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="H7" s="37"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B8" s="83" t="s">
+      <c r="H15" s="38" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" s="36"/>
+      <c r="F16" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="H16" s="38" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>256</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="H17" s="39" t="s">
         <v>235</v>
       </c>
-      <c r="C8" s="83"/>
-      <c r="D8" s="85" t="s">
-        <v>234</v>
-      </c>
-      <c r="E8" s="83"/>
-      <c r="F8" s="40" t="s">
-        <v>229</v>
-      </c>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B9" s="85" t="s">
-        <v>136</v>
-      </c>
-      <c r="C9" s="83"/>
-      <c r="D9" s="85" t="s">
-        <v>249</v>
-      </c>
-      <c r="E9" s="83"/>
-      <c r="F9" s="36" t="s">
-        <v>228</v>
-      </c>
-      <c r="G9" s="83"/>
-      <c r="H9" s="85" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="C10" s="83"/>
-      <c r="E10" s="83"/>
-      <c r="F10" s="36" t="s">
-        <v>230</v>
-      </c>
-      <c r="G10" s="83"/>
-      <c r="H10" s="85" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="B11" s="85" t="s">
-        <v>246</v>
-      </c>
-      <c r="C11" s="83"/>
-      <c r="D11" s="85" t="s">
-        <v>152</v>
-      </c>
-      <c r="E11" s="83"/>
-      <c r="F11" s="36" t="s">
-        <v>231</v>
-      </c>
-      <c r="G11" s="83"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B12" s="85" t="s">
-        <v>244</v>
-      </c>
-      <c r="C12" s="83"/>
-      <c r="D12" s="85" t="s">
-        <v>243</v>
-      </c>
-      <c r="E12" s="83"/>
-      <c r="F12" s="38" t="s">
-        <v>232</v>
-      </c>
-      <c r="G12" s="83"/>
-      <c r="H12" s="83" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="83" t="s">
-        <v>251</v>
-      </c>
-      <c r="C13" s="83"/>
-      <c r="D13" s="86" t="s">
-        <v>248</v>
-      </c>
-      <c r="E13" s="83"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="83" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B14" s="83" t="s">
-        <v>250</v>
-      </c>
-      <c r="C14" s="83"/>
-      <c r="D14" s="85" t="s">
-        <v>247</v>
-      </c>
-      <c r="E14" s="83"/>
-      <c r="F14" s="38" t="s">
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D18" s="38" t="s">
+        <v>257</v>
+      </c>
+      <c r="F18" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="G14" s="83"/>
-      <c r="H14" s="83" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B15" s="83" t="s">
-        <v>129</v>
-      </c>
-      <c r="C15" s="83"/>
-      <c r="D15" s="85"/>
-      <c r="E15" s="83"/>
-      <c r="F15" s="38" t="s">
+    </row>
+    <row r="19" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="D19" s="38" t="s">
+        <v>258</v>
+      </c>
+      <c r="F19" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="G15" s="83"/>
-      <c r="H15" s="83" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="83" t="s">
-        <v>245</v>
-      </c>
-      <c r="C16" s="83"/>
-      <c r="D16" s="85"/>
-      <c r="E16" s="83"/>
-      <c r="F16" s="38" t="s">
+      <c r="H19" s="55" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="D20" s="87" t="s">
+        <v>259</v>
+      </c>
+      <c r="F20" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="G16" s="83"/>
-      <c r="H16" s="83" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="C17" s="83"/>
-      <c r="D17" s="84" t="s">
-        <v>233</v>
-      </c>
-      <c r="E17" s="83"/>
-      <c r="F17" s="38" t="s">
+    </row>
+    <row r="21" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="D21" s="88"/>
+      <c r="F21" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="G17" s="83"/>
-      <c r="H17" s="83" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B18" s="83"/>
-      <c r="C18" s="83"/>
-      <c r="E18" s="83"/>
-      <c r="F18" s="38" t="s">
+    </row>
+    <row r="22" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="90" t="s">
+        <v>259</v>
+      </c>
+      <c r="D22" s="84"/>
+      <c r="F22" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="G18" s="83"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B19" s="83"/>
-      <c r="C19" s="83"/>
-      <c r="E19" s="83"/>
-      <c r="F19" s="38" t="s">
-        <v>142</v>
-      </c>
-      <c r="G19" s="83"/>
-      <c r="H19" s="84" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B20" s="83"/>
-      <c r="C20" s="83"/>
-      <c r="E20" s="83"/>
-      <c r="F20" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="G20" s="83"/>
-      <c r="H20" s="83"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B21" s="83"/>
-      <c r="C21" s="83"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="38" t="s">
-        <v>144</v>
-      </c>
-      <c r="G21" s="83"/>
-      <c r="H21" s="83"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B22" s="83"/>
-      <c r="C22" s="83"/>
-      <c r="D22" s="85"/>
-      <c r="E22" s="83"/>
-      <c r="F22" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="G22" s="83"/>
-      <c r="H22" s="83"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B23" s="83"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="83"/>
+      <c r="D23" s="55" t="s">
+        <v>226</v>
+      </c>
       <c r="F23" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="G23" s="83"/>
-      <c r="H23" s="83"/>
+        <v>146</v>
+      </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B24" s="83"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="85"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
-      <c r="G24" s="83"/>
-      <c r="H24" s="83"/>
+      <c r="B24" s="90"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="F25" s="84" t="s">
-        <v>233</v>
+      <c r="F25" s="55" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D20:D21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E08554-D8B2-4838-942A-41D15992982E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A678BF3-4A56-4A1E-B2DF-017A74834050}">
   <dimension ref="A1:J47"/>
   <sheetViews>
@@ -4939,25 +5194,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="81"/>
-      <c r="B1" s="82" t="s">
-        <v>173</v>
-      </c>
-      <c r="C1" s="82"/>
+      <c r="A1" s="82"/>
+      <c r="B1" s="83" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="83"/>
       <c r="D1" s="47"/>
-      <c r="E1" s="82" t="s">
-        <v>174</v>
-      </c>
-      <c r="F1" s="82"/>
+      <c r="E1" s="83" t="s">
+        <v>169</v>
+      </c>
+      <c r="F1" s="83"/>
       <c r="G1" s="47"/>
-      <c r="H1" s="82" t="s">
-        <v>175</v>
-      </c>
-      <c r="I1" s="82"/>
-      <c r="J1" s="81"/>
+      <c r="H1" s="83" t="s">
+        <v>170</v>
+      </c>
+      <c r="I1" s="83"/>
+      <c r="J1" s="82"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="81"/>
+      <c r="A2" s="82"/>
       <c r="B2" s="51"/>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
@@ -4966,100 +5221,100 @@
       <c r="G2" s="46"/>
       <c r="H2" s="46"/>
       <c r="I2" s="46"/>
-      <c r="J2" s="81"/>
+      <c r="J2" s="82"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="81"/>
+      <c r="A3" s="82"/>
       <c r="B3" s="50" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>169</v>
-      </c>
-      <c r="D3" s="78"/>
+        <v>164</v>
+      </c>
+      <c r="D3" s="79"/>
       <c r="E3" s="48" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F3" s="48" t="s">
-        <v>169</v>
-      </c>
-      <c r="G3" s="78"/>
+        <v>164</v>
+      </c>
+      <c r="G3" s="79"/>
       <c r="H3" s="48" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="I3" s="48" t="s">
-        <v>169</v>
-      </c>
-      <c r="J3" s="81"/>
+        <v>164</v>
+      </c>
+      <c r="J3" s="82"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="81"/>
+      <c r="A4" s="82"/>
       <c r="B4" s="50" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>185</v>
-      </c>
-      <c r="D4" s="79"/>
+        <v>180</v>
+      </c>
+      <c r="D4" s="80"/>
       <c r="E4" s="48" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F4" s="48" t="s">
-        <v>186</v>
-      </c>
-      <c r="G4" s="79"/>
+        <v>181</v>
+      </c>
+      <c r="G4" s="80"/>
       <c r="H4" s="48" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I4" s="48" t="s">
-        <v>187</v>
-      </c>
-      <c r="J4" s="81"/>
+        <v>182</v>
+      </c>
+      <c r="J4" s="82"/>
     </row>
     <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="81"/>
+      <c r="A5" s="82"/>
       <c r="B5" s="50" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="D5" s="79"/>
+        <v>184</v>
+      </c>
+      <c r="D5" s="80"/>
       <c r="E5" s="48" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="G5" s="79"/>
+        <v>210</v>
+      </c>
+      <c r="G5" s="80"/>
       <c r="H5" s="48" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="J5" s="81"/>
+        <v>201</v>
+      </c>
+      <c r="J5" s="82"/>
     </row>
     <row r="6" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="81"/>
+      <c r="A6" s="82"/>
       <c r="B6" s="50" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C6" s="48"/>
-      <c r="D6" s="80"/>
+      <c r="D6" s="81"/>
       <c r="E6" s="48" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F6" s="48"/>
-      <c r="G6" s="80"/>
+      <c r="G6" s="81"/>
       <c r="H6" s="48" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I6" s="48"/>
-      <c r="J6" s="81"/>
+      <c r="J6" s="82"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="81"/>
+      <c r="A7" s="82"/>
       <c r="B7" s="52"/>
       <c r="C7" s="49"/>
       <c r="D7" s="49"/>
@@ -5068,100 +5323,100 @@
       <c r="G7" s="49"/>
       <c r="H7" s="49"/>
       <c r="I7" s="49"/>
-      <c r="J7" s="81"/>
+      <c r="J7" s="82"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="81"/>
+      <c r="A8" s="82"/>
       <c r="B8" s="50" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>176</v>
-      </c>
-      <c r="D8" s="78"/>
+        <v>171</v>
+      </c>
+      <c r="D8" s="79"/>
       <c r="E8" s="48" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F8" s="48" t="s">
-        <v>176</v>
-      </c>
-      <c r="G8" s="78"/>
+        <v>171</v>
+      </c>
+      <c r="G8" s="79"/>
       <c r="H8" s="48" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="I8" s="48" t="s">
-        <v>176</v>
-      </c>
-      <c r="J8" s="81"/>
+        <v>171</v>
+      </c>
+      <c r="J8" s="82"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="81"/>
+      <c r="A9" s="82"/>
       <c r="B9" s="50" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>185</v>
-      </c>
-      <c r="D9" s="79"/>
+        <v>180</v>
+      </c>
+      <c r="D9" s="80"/>
       <c r="E9" s="48" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F9" s="48" t="s">
+        <v>181</v>
+      </c>
+      <c r="G9" s="80"/>
+      <c r="H9" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="I9" s="48" t="s">
+        <v>202</v>
+      </c>
+      <c r="J9" s="82"/>
+    </row>
+    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="82"/>
+      <c r="B10" s="50" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="D10" s="80"/>
+      <c r="E10" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="G10" s="80"/>
+      <c r="H10" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="I10" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="G9" s="79"/>
-      <c r="H9" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="I9" s="48" t="s">
-        <v>207</v>
-      </c>
-      <c r="J9" s="81"/>
-    </row>
-    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="81"/>
-      <c r="B10" s="50" t="s">
-        <v>171</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="D10" s="79"/>
-      <c r="E10" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="G10" s="79"/>
-      <c r="H10" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="J10" s="81"/>
+      <c r="J10" s="82"/>
     </row>
     <row r="11" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="81"/>
+      <c r="A11" s="82"/>
       <c r="B11" s="50" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C11" s="48"/>
-      <c r="D11" s="80"/>
+      <c r="D11" s="81"/>
       <c r="E11" s="48" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F11" s="48"/>
-      <c r="G11" s="80"/>
+      <c r="G11" s="81"/>
       <c r="H11" s="48" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I11" s="48"/>
-      <c r="J11" s="81"/>
+      <c r="J11" s="82"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="81"/>
+      <c r="A12" s="82"/>
       <c r="B12" s="52"/>
       <c r="C12" s="49"/>
       <c r="D12" s="49"/>
@@ -5170,92 +5425,92 @@
       <c r="G12" s="49"/>
       <c r="H12" s="49"/>
       <c r="I12" s="49"/>
-      <c r="J12" s="81"/>
+      <c r="J12" s="82"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="81"/>
+      <c r="A13" s="82"/>
       <c r="B13" s="50" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>177</v>
-      </c>
-      <c r="D13" s="78"/>
+        <v>172</v>
+      </c>
+      <c r="D13" s="79"/>
       <c r="E13" s="48" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F13" s="48" t="s">
-        <v>177</v>
-      </c>
-      <c r="G13" s="78"/>
+        <v>172</v>
+      </c>
+      <c r="G13" s="79"/>
       <c r="H13" s="48" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="I13" s="48" t="s">
-        <v>177</v>
-      </c>
-      <c r="J13" s="81"/>
+        <v>172</v>
+      </c>
+      <c r="J13" s="82"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="81"/>
+      <c r="A14" s="82"/>
       <c r="B14" s="50" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>185</v>
-      </c>
-      <c r="D14" s="79"/>
+        <v>180</v>
+      </c>
+      <c r="D14" s="80"/>
       <c r="E14" s="48" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F14" s="48"/>
-      <c r="G14" s="79"/>
+      <c r="G14" s="80"/>
       <c r="H14" s="48" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I14" s="48"/>
-      <c r="J14" s="81"/>
+      <c r="J14" s="82"/>
     </row>
     <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="81"/>
+      <c r="A15" s="82"/>
       <c r="B15" s="50" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="D15" s="79"/>
+        <v>190</v>
+      </c>
+      <c r="D15" s="80"/>
       <c r="E15" s="48" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F15" s="21"/>
-      <c r="G15" s="79"/>
+      <c r="G15" s="80"/>
       <c r="H15" s="48" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I15" s="21"/>
-      <c r="J15" s="81"/>
+      <c r="J15" s="82"/>
     </row>
     <row r="16" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="81"/>
+      <c r="A16" s="82"/>
       <c r="B16" s="50" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C16" s="48"/>
-      <c r="D16" s="80"/>
+      <c r="D16" s="81"/>
       <c r="E16" s="48" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F16" s="48"/>
-      <c r="G16" s="80"/>
+      <c r="G16" s="81"/>
       <c r="H16" s="48" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I16" s="48"/>
-      <c r="J16" s="81"/>
+      <c r="J16" s="82"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="81"/>
+      <c r="A17" s="82"/>
       <c r="B17" s="52"/>
       <c r="C17" s="49"/>
       <c r="D17" s="49"/>
@@ -5264,100 +5519,100 @@
       <c r="G17" s="49"/>
       <c r="H17" s="49"/>
       <c r="I17" s="49"/>
-      <c r="J17" s="81"/>
+      <c r="J17" s="82"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="81"/>
+      <c r="A18" s="82"/>
       <c r="B18" s="50" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>178</v>
-      </c>
-      <c r="D18" s="78"/>
+        <v>173</v>
+      </c>
+      <c r="D18" s="79"/>
       <c r="E18" s="48" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F18" s="48" t="s">
-        <v>178</v>
-      </c>
-      <c r="G18" s="78"/>
+        <v>173</v>
+      </c>
+      <c r="G18" s="79"/>
       <c r="H18" s="48" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="I18" s="48" t="s">
-        <v>178</v>
-      </c>
-      <c r="J18" s="81"/>
+        <v>173</v>
+      </c>
+      <c r="J18" s="82"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="81"/>
+      <c r="A19" s="82"/>
       <c r="B19" s="50" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C19" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="D19" s="80"/>
+      <c r="E19" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="F19" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="G19" s="80"/>
+      <c r="H19" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="I19" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="J19" s="82"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="82"/>
+      <c r="B20" s="50" t="s">
+        <v>166</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="D20" s="80"/>
+      <c r="E20" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="F20" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="D19" s="79"/>
-      <c r="E19" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="F19" s="48" t="s">
-        <v>188</v>
-      </c>
-      <c r="G19" s="79"/>
-      <c r="H19" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="I19" s="48" t="s">
-        <v>188</v>
-      </c>
-      <c r="J19" s="81"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="81"/>
-      <c r="B20" s="50" t="s">
-        <v>171</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="D20" s="79"/>
-      <c r="E20" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="G20" s="79"/>
+      <c r="G20" s="80"/>
       <c r="H20" s="48" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I20" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="J20" s="81"/>
+        <v>187</v>
+      </c>
+      <c r="J20" s="82"/>
     </row>
     <row r="21" spans="1:10" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="81"/>
+      <c r="A21" s="82"/>
       <c r="B21" s="50" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C21" s="48"/>
-      <c r="D21" s="80"/>
+      <c r="D21" s="81"/>
       <c r="E21" s="48" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F21" s="48"/>
-      <c r="G21" s="80"/>
+      <c r="G21" s="81"/>
       <c r="H21" s="48" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I21" s="48"/>
-      <c r="J21" s="81"/>
+      <c r="J21" s="82"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="81"/>
+      <c r="A22" s="82"/>
       <c r="B22" s="52"/>
       <c r="C22" s="49"/>
       <c r="D22" s="49"/>
@@ -5366,100 +5621,100 @@
       <c r="G22" s="49"/>
       <c r="H22" s="49"/>
       <c r="I22" s="49"/>
-      <c r="J22" s="81"/>
+      <c r="J22" s="82"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="81"/>
+      <c r="A23" s="82"/>
       <c r="B23" s="50" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>179</v>
-      </c>
-      <c r="D23" s="78"/>
+        <v>174</v>
+      </c>
+      <c r="D23" s="79"/>
       <c r="E23" s="48" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F23" s="48" t="s">
-        <v>179</v>
-      </c>
-      <c r="G23" s="78"/>
+        <v>174</v>
+      </c>
+      <c r="G23" s="79"/>
       <c r="H23" s="48" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="I23" s="48" t="s">
-        <v>179</v>
-      </c>
-      <c r="J23" s="81"/>
+        <v>174</v>
+      </c>
+      <c r="J23" s="82"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="81"/>
+      <c r="A24" s="82"/>
       <c r="B24" s="50" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C24" s="48" t="s">
-        <v>197</v>
-      </c>
-      <c r="D24" s="79"/>
+        <v>192</v>
+      </c>
+      <c r="D24" s="80"/>
       <c r="E24" s="48" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F24" s="48" t="s">
-        <v>217</v>
-      </c>
-      <c r="G24" s="79"/>
+        <v>212</v>
+      </c>
+      <c r="G24" s="80"/>
       <c r="H24" s="48" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I24" s="48" t="s">
-        <v>208</v>
-      </c>
-      <c r="J24" s="81"/>
+        <v>203</v>
+      </c>
+      <c r="J24" s="82"/>
     </row>
     <row r="25" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="81"/>
+      <c r="A25" s="82"/>
       <c r="B25" s="50" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="D25" s="79"/>
+        <v>191</v>
+      </c>
+      <c r="D25" s="80"/>
       <c r="E25" s="48" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="G25" s="79"/>
+        <v>213</v>
+      </c>
+      <c r="G25" s="80"/>
       <c r="H25" s="48" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I25" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="J25" s="81"/>
+        <v>204</v>
+      </c>
+      <c r="J25" s="82"/>
     </row>
     <row r="26" spans="1:10" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="81"/>
+      <c r="A26" s="82"/>
       <c r="B26" s="50" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C26" s="48"/>
-      <c r="D26" s="80"/>
+      <c r="D26" s="81"/>
       <c r="E26" s="48" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F26" s="48"/>
-      <c r="G26" s="80"/>
+      <c r="G26" s="81"/>
       <c r="H26" s="48" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I26" s="48"/>
-      <c r="J26" s="81"/>
+      <c r="J26" s="82"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="81"/>
+      <c r="A27" s="82"/>
       <c r="B27" s="52"/>
       <c r="C27" s="49"/>
       <c r="D27" s="49"/>
@@ -5468,100 +5723,100 @@
       <c r="G27" s="49"/>
       <c r="H27" s="49"/>
       <c r="I27" s="49"/>
-      <c r="J27" s="81"/>
+      <c r="J27" s="82"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="81"/>
+      <c r="A28" s="82"/>
       <c r="B28" s="50" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C28" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="D28" s="78"/>
+        <v>175</v>
+      </c>
+      <c r="D28" s="79"/>
       <c r="E28" s="48" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F28" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="G28" s="78"/>
+        <v>175</v>
+      </c>
+      <c r="G28" s="79"/>
       <c r="H28" s="48" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="I28" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="J28" s="81"/>
+        <v>175</v>
+      </c>
+      <c r="J28" s="82"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="81"/>
+      <c r="A29" s="82"/>
       <c r="B29" s="50" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C29" s="48" t="s">
-        <v>198</v>
-      </c>
-      <c r="D29" s="79"/>
+        <v>193</v>
+      </c>
+      <c r="D29" s="80"/>
       <c r="E29" s="48" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F29" s="48" t="s">
-        <v>219</v>
-      </c>
-      <c r="G29" s="79"/>
+        <v>214</v>
+      </c>
+      <c r="G29" s="80"/>
       <c r="H29" s="48" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I29" s="48" t="s">
-        <v>210</v>
-      </c>
-      <c r="J29" s="81"/>
+        <v>205</v>
+      </c>
+      <c r="J29" s="82"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="81"/>
+      <c r="A30" s="82"/>
       <c r="B30" s="50" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>199</v>
-      </c>
-      <c r="D30" s="79"/>
+        <v>194</v>
+      </c>
+      <c r="D30" s="80"/>
       <c r="E30" s="48" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F30" s="48" t="s">
-        <v>220</v>
-      </c>
-      <c r="G30" s="79"/>
+        <v>215</v>
+      </c>
+      <c r="G30" s="80"/>
       <c r="H30" s="48" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I30" s="48" t="s">
-        <v>211</v>
-      </c>
-      <c r="J30" s="81"/>
+        <v>206</v>
+      </c>
+      <c r="J30" s="82"/>
     </row>
     <row r="31" spans="1:10" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="81"/>
+      <c r="A31" s="82"/>
       <c r="B31" s="50" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C31" s="48"/>
-      <c r="D31" s="80"/>
+      <c r="D31" s="81"/>
       <c r="E31" s="48" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F31" s="48"/>
-      <c r="G31" s="80"/>
+      <c r="G31" s="81"/>
       <c r="H31" s="48" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I31" s="48"/>
-      <c r="J31" s="81"/>
+      <c r="J31" s="82"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" s="81"/>
+      <c r="A32" s="82"/>
       <c r="B32" s="52"/>
       <c r="C32" s="49"/>
       <c r="D32" s="49"/>
@@ -5570,100 +5825,100 @@
       <c r="G32" s="49"/>
       <c r="H32" s="49"/>
       <c r="I32" s="49"/>
-      <c r="J32" s="81"/>
+      <c r="J32" s="82"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="81"/>
+      <c r="A33" s="82"/>
       <c r="B33" s="50" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C33" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="D33" s="79"/>
+      <c r="E33" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="F33" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="G33" s="79"/>
+      <c r="H33" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="I33" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="J33" s="82"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" s="82"/>
+      <c r="B34" s="50" t="s">
+        <v>165</v>
+      </c>
+      <c r="C34" s="48" t="s">
+        <v>195</v>
+      </c>
+      <c r="D34" s="80"/>
+      <c r="E34" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="F34" s="48" t="s">
+        <v>178</v>
+      </c>
+      <c r="G34" s="80"/>
+      <c r="H34" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="I34" s="48" t="s">
         <v>179</v>
       </c>
-      <c r="D33" s="78"/>
-      <c r="E33" s="48" t="s">
-        <v>168</v>
-      </c>
-      <c r="F33" s="48" t="s">
-        <v>179</v>
-      </c>
-      <c r="G33" s="78"/>
-      <c r="H33" s="48" t="s">
-        <v>168</v>
-      </c>
-      <c r="I33" s="48" t="s">
-        <v>179</v>
-      </c>
-      <c r="J33" s="81"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="81"/>
-      <c r="B34" s="50" t="s">
-        <v>170</v>
-      </c>
-      <c r="C34" s="48" t="s">
-        <v>200</v>
-      </c>
-      <c r="D34" s="79"/>
-      <c r="E34" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="F34" s="48" t="s">
-        <v>183</v>
-      </c>
-      <c r="G34" s="79"/>
-      <c r="H34" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="I34" s="48" t="s">
-        <v>184</v>
-      </c>
-      <c r="J34" s="81"/>
+      <c r="J34" s="82"/>
     </row>
     <row r="35" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="81"/>
+      <c r="A35" s="82"/>
       <c r="B35" s="50" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="D35" s="79"/>
+        <v>196</v>
+      </c>
+      <c r="D35" s="80"/>
       <c r="E35" s="48" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="G35" s="79"/>
+        <v>216</v>
+      </c>
+      <c r="G35" s="80"/>
       <c r="H35" s="48" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I35" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="J35" s="81"/>
+        <v>207</v>
+      </c>
+      <c r="J35" s="82"/>
     </row>
     <row r="36" spans="1:10" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="81"/>
+      <c r="A36" s="82"/>
       <c r="B36" s="50" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C36" s="48"/>
-      <c r="D36" s="80"/>
+      <c r="D36" s="81"/>
       <c r="E36" s="48" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F36" s="48"/>
-      <c r="G36" s="80"/>
+      <c r="G36" s="81"/>
       <c r="H36" s="48" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I36" s="48"/>
-      <c r="J36" s="81"/>
+      <c r="J36" s="82"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A37" s="81"/>
+      <c r="A37" s="82"/>
       <c r="B37" s="52"/>
       <c r="C37" s="49"/>
       <c r="D37" s="54"/>
@@ -5672,100 +5927,100 @@
       <c r="G37" s="49"/>
       <c r="H37" s="49"/>
       <c r="I37" s="49"/>
-      <c r="J37" s="81"/>
+      <c r="J37" s="82"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="81"/>
+      <c r="A38" s="82"/>
       <c r="B38" s="50" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C38" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="D38" s="78"/>
+        <v>175</v>
+      </c>
+      <c r="D38" s="79"/>
       <c r="E38" s="48" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F38" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="G38" s="78"/>
+        <v>175</v>
+      </c>
+      <c r="G38" s="79"/>
       <c r="H38" s="48" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="I38" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="J38" s="81"/>
+        <v>175</v>
+      </c>
+      <c r="J38" s="82"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" s="81"/>
+      <c r="A39" s="82"/>
       <c r="B39" s="50" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C39" s="48" t="s">
-        <v>182</v>
-      </c>
-      <c r="D39" s="79"/>
+        <v>177</v>
+      </c>
+      <c r="D39" s="80"/>
       <c r="E39" s="48" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F39" s="48" t="s">
-        <v>222</v>
-      </c>
-      <c r="G39" s="79"/>
+        <v>217</v>
+      </c>
+      <c r="G39" s="80"/>
       <c r="H39" s="48" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I39" s="48" t="s">
-        <v>213</v>
-      </c>
-      <c r="J39" s="81"/>
+        <v>208</v>
+      </c>
+      <c r="J39" s="82"/>
     </row>
     <row r="40" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="81"/>
+      <c r="A40" s="82"/>
       <c r="B40" s="50" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="D40" s="79"/>
+        <v>197</v>
+      </c>
+      <c r="D40" s="80"/>
       <c r="E40" s="48" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="G40" s="79"/>
+        <v>218</v>
+      </c>
+      <c r="G40" s="80"/>
       <c r="H40" s="48" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I40" s="21" t="s">
-        <v>214</v>
-      </c>
-      <c r="J40" s="81"/>
+        <v>209</v>
+      </c>
+      <c r="J40" s="82"/>
     </row>
     <row r="41" spans="1:10" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="81"/>
+      <c r="A41" s="82"/>
       <c r="B41" s="50" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C41" s="48"/>
-      <c r="D41" s="80"/>
+      <c r="D41" s="81"/>
       <c r="E41" s="48" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F41" s="48"/>
-      <c r="G41" s="80"/>
+      <c r="G41" s="81"/>
       <c r="H41" s="48" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I41" s="48"/>
-      <c r="J41" s="81"/>
+      <c r="J41" s="82"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A42" s="81"/>
+      <c r="A42" s="82"/>
       <c r="B42" s="52"/>
       <c r="C42" s="49"/>
       <c r="D42" s="49"/>
@@ -5774,100 +6029,100 @@
       <c r="G42" s="49"/>
       <c r="H42" s="49"/>
       <c r="I42" s="49"/>
-      <c r="J42" s="81"/>
+      <c r="J42" s="82"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A43" s="81"/>
+      <c r="A43" s="82"/>
       <c r="B43" s="50" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C43" s="48" t="s">
-        <v>181</v>
-      </c>
-      <c r="D43" s="78"/>
+        <v>176</v>
+      </c>
+      <c r="D43" s="79"/>
       <c r="E43" s="50" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F43" s="48" t="s">
-        <v>181</v>
-      </c>
-      <c r="G43" s="78"/>
+        <v>176</v>
+      </c>
+      <c r="G43" s="79"/>
       <c r="H43" s="50" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="I43" s="48" t="s">
-        <v>181</v>
-      </c>
-      <c r="J43" s="81"/>
+        <v>176</v>
+      </c>
+      <c r="J43" s="82"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A44" s="81"/>
+      <c r="A44" s="82"/>
       <c r="B44" s="50" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C44" s="48" t="s">
-        <v>203</v>
-      </c>
-      <c r="D44" s="79"/>
+        <v>198</v>
+      </c>
+      <c r="D44" s="80"/>
       <c r="E44" s="50" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F44" s="48" t="s">
-        <v>224</v>
-      </c>
-      <c r="G44" s="79"/>
+        <v>219</v>
+      </c>
+      <c r="G44" s="80"/>
       <c r="H44" s="50" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I44" s="48" t="s">
-        <v>204</v>
-      </c>
-      <c r="J44" s="81"/>
+        <v>199</v>
+      </c>
+      <c r="J44" s="82"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A45" s="81"/>
+      <c r="A45" s="82"/>
       <c r="B45" s="50" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>205</v>
-      </c>
-      <c r="D45" s="79"/>
+        <v>200</v>
+      </c>
+      <c r="D45" s="80"/>
       <c r="E45" s="50" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="G45" s="79"/>
+        <v>220</v>
+      </c>
+      <c r="G45" s="80"/>
       <c r="H45" s="50" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I45" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="J45" s="81"/>
+        <v>221</v>
+      </c>
+      <c r="J45" s="82"/>
     </row>
     <row r="46" spans="1:10" ht="88" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="81"/>
+      <c r="A46" s="82"/>
       <c r="B46" s="50" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C46" s="48"/>
-      <c r="D46" s="80"/>
+      <c r="D46" s="81"/>
       <c r="E46" s="50" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F46" s="48"/>
-      <c r="G46" s="80"/>
+      <c r="G46" s="81"/>
       <c r="H46" s="50" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I46" s="48"/>
-      <c r="J46" s="81"/>
+      <c r="J46" s="82"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A47" s="81"/>
+      <c r="A47" s="82"/>
       <c r="B47" s="52"/>
       <c r="C47" s="49"/>
       <c r="D47" s="49"/>
@@ -5876,17 +6131,10 @@
       <c r="G47" s="49"/>
       <c r="H47" s="52"/>
       <c r="I47" s="49"/>
-      <c r="J47" s="81"/>
+      <c r="J47" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="D33:D36"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="D18:D21"/>
     <mergeCell ref="D43:D46"/>
     <mergeCell ref="A1:A47"/>
     <mergeCell ref="J1:J47"/>
@@ -5903,6 +6151,13 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="D33:D36"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="D18:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Completed 27 tests for Newsagent
</commit_message>
<xml_diff>
--- a/User Stories/NataliaUserStories.xlsx
+++ b/User Stories/NataliaUserStories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cad1acabf18afac6/Desktop/Software Design with AI for Cloud/Year_3/agile-labs3/Newsagent-Project/User Stories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="717" documentId="13_ncr:1_{7B2E17FA-F2A9-4DCC-A803-850E080333ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD2F20F0-CCF2-4241-AD8F-603297AE5673}"/>
+  <xr:revisionPtr revIDLastSave="725" documentId="13_ncr:1_{7B2E17FA-F2A9-4DCC-A803-850E080333ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F5E785B-7E42-4AC8-9638-B6F5BA389E8F}"/>
   <bookViews>
-    <workbookView xWindow="21160" yWindow="2750" windowWidth="16530" windowHeight="16250" activeTab="1" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
+    <workbookView xWindow="14740" yWindow="2750" windowWidth="22950" windowHeight="16250" activeTab="2" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminUserStories" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="267">
   <si>
     <t>As an admin</t>
   </si>
@@ -838,6 +838,9 @@
   </si>
   <si>
     <t>Verify valid 10 digits &lt; phoneNo &lt;= 12 digits</t>
+  </si>
+  <si>
+    <t>+doesCustomerExist(int id) : boolean</t>
   </si>
 </sst>
 </file>
@@ -1038,7 +1041,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1185,15 +1188,70 @@
     <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1203,56 +1261,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1268,25 +1284,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1481,6 +1478,50 @@
         <a:xfrm>
           <a:off x="12363824" y="2906059"/>
           <a:ext cx="2173941" cy="2188402"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>37354</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>82178</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2786530</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>156094</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{152B75F1-05F8-30A3-377D-4F0DA0F3F660}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="186766" y="4743825"/>
+          <a:ext cx="2749176" cy="4182740"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2993,10 +3034,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3329,16 +3366,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="63">
+      <c r="A2" s="58">
         <v>1</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="60" t="s">
         <v>150</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="60" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="15" t="s">
@@ -3349,10 +3386,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="64"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
       <c r="E3" s="15" t="s">
         <v>47</v>
       </c>
@@ -3361,50 +3398,50 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="64"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
       <c r="E4" s="15" t="s">
         <v>49</v>
       </c>
       <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="64"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
       <c r="E5" s="15" t="s">
         <v>50</v>
       </c>
       <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="64"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
       <c r="E6" s="15" t="s">
         <v>151</v>
       </c>
       <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="64"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
+      <c r="A7" s="59"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
       <c r="E7" s="15" t="s">
         <v>155</v>
       </c>
       <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="64"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
+      <c r="A8" s="59"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
       <c r="E8" s="15" t="s">
         <v>37</v>
       </c>
@@ -3419,16 +3456,16 @@
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="63">
+      <c r="A10" s="58">
         <v>2</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="60" t="s">
         <v>81</v>
       </c>
       <c r="E10" s="14" t="s">
@@ -3439,60 +3476,60 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="64"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
+      <c r="A11" s="59"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
       <c r="E11" s="15" t="s">
         <v>87</v>
       </c>
       <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="64"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
+      <c r="A12" s="59"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
       <c r="E12" s="15" t="s">
         <v>90</v>
       </c>
       <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="64"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
+      <c r="A13" s="59"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
       <c r="E13" s="15" t="s">
         <v>88</v>
       </c>
       <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="64"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
+      <c r="A14" s="59"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
       <c r="E14" s="15" t="s">
         <v>89</v>
       </c>
       <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="64"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
+      <c r="A15" s="59"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
       <c r="E15" s="15" t="s">
         <v>83</v>
       </c>
       <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="65"/>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
+      <c r="A16" s="72"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="73"/>
       <c r="E16" s="15" t="s">
         <v>14</v>
       </c>
@@ -3507,16 +3544,16 @@
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="63">
+      <c r="A18" s="58">
         <v>3</v>
       </c>
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="56" t="s">
+      <c r="D18" s="60" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="15" t="s">
@@ -3527,20 +3564,20 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="64"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
+      <c r="A19" s="59"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
       <c r="E19" s="15" t="s">
         <v>91</v>
       </c>
       <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="65"/>
-      <c r="B20" s="58"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
+      <c r="A20" s="72"/>
+      <c r="B20" s="73"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
       <c r="E20" s="11" t="s">
         <v>51</v>
       </c>
@@ -3555,16 +3592,16 @@
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="63">
+      <c r="A22" s="58">
         <v>4</v>
       </c>
-      <c r="B22" s="56" t="s">
+      <c r="B22" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="56" t="s">
+      <c r="C22" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="56" t="s">
+      <c r="D22" s="60" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="15" t="s">
@@ -3575,60 +3612,60 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="64"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
+      <c r="A23" s="59"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
       <c r="E23" s="15" t="s">
         <v>96</v>
       </c>
       <c r="F23" s="21"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="64"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
+      <c r="A24" s="59"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
       <c r="E24" s="15" t="s">
         <v>97</v>
       </c>
       <c r="F24" s="21"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="64"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
+      <c r="A25" s="59"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
       <c r="E25" s="15" t="s">
         <v>98</v>
       </c>
       <c r="F25" s="21"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="64"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
+      <c r="A26" s="59"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
       <c r="E26" s="15" t="s">
         <v>92</v>
       </c>
       <c r="F26" s="21"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="64"/>
-      <c r="B27" s="57"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
+      <c r="A27" s="59"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
       <c r="E27" s="15" t="s">
         <v>93</v>
       </c>
       <c r="F27" s="21"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="65"/>
-      <c r="B28" s="58"/>
-      <c r="C28" s="58"/>
-      <c r="D28" s="58"/>
+      <c r="A28" s="72"/>
+      <c r="B28" s="73"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
       <c r="E28" s="15" t="s">
         <v>11</v>
       </c>
@@ -3643,16 +3680,16 @@
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="63">
+      <c r="A30" s="58">
         <v>5</v>
       </c>
-      <c r="B30" s="56" t="s">
+      <c r="B30" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="56" t="s">
+      <c r="C30" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="56" t="s">
+      <c r="D30" s="60" t="s">
         <v>82</v>
       </c>
       <c r="E30" s="15" t="s">
@@ -3661,20 +3698,20 @@
       <c r="F30" s="21"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="64"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
+      <c r="A31" s="59"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
       <c r="E31" s="15" t="s">
         <v>94</v>
       </c>
       <c r="F31" s="21"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="65"/>
-      <c r="B32" s="58"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="58"/>
+      <c r="A32" s="72"/>
+      <c r="B32" s="73"/>
+      <c r="C32" s="73"/>
+      <c r="D32" s="73"/>
       <c r="E32" s="15" t="s">
         <v>95</v>
       </c>
@@ -3689,16 +3726,16 @@
       <c r="F33" s="7"/>
     </row>
     <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="63">
+      <c r="A34" s="58">
         <v>6</v>
       </c>
-      <c r="B34" s="56" t="s">
+      <c r="B34" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="56" t="s">
+      <c r="C34" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="56" t="s">
+      <c r="D34" s="60" t="s">
         <v>16</v>
       </c>
       <c r="E34" s="15" t="s">
@@ -3709,10 +3746,10 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="65"/>
-      <c r="B35" s="58"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58"/>
+      <c r="A35" s="72"/>
+      <c r="B35" s="73"/>
+      <c r="C35" s="73"/>
+      <c r="D35" s="73"/>
       <c r="E35" s="15" t="s">
         <v>100</v>
       </c>
@@ -3727,70 +3764,70 @@
       <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="66">
+      <c r="A37" s="77">
         <v>7</v>
       </c>
-      <c r="B37" s="62" t="s">
+      <c r="B37" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="62" t="s">
+      <c r="C37" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="D37" s="62" t="s">
+      <c r="D37" s="76" t="s">
         <v>69</v>
       </c>
       <c r="E37" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="F37" s="56" t="s">
+      <c r="F37" s="60" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="66"/>
-      <c r="B38" s="62"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="62"/>
+      <c r="A38" s="77"/>
+      <c r="B38" s="76"/>
+      <c r="C38" s="76"/>
+      <c r="D38" s="76"/>
       <c r="E38" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="F38" s="57"/>
+      <c r="F38" s="61"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="66"/>
-      <c r="B39" s="62"/>
-      <c r="C39" s="62"/>
-      <c r="D39" s="62"/>
+      <c r="A39" s="77"/>
+      <c r="B39" s="76"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="76"/>
       <c r="E39" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="F39" s="58"/>
+      <c r="F39" s="73"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="66"/>
-      <c r="B40" s="62"/>
-      <c r="C40" s="62"/>
-      <c r="D40" s="62"/>
+      <c r="A40" s="77"/>
+      <c r="B40" s="76"/>
+      <c r="C40" s="76"/>
+      <c r="D40" s="76"/>
       <c r="E40" s="21" t="s">
         <v>72</v>
       </c>
       <c r="F40" s="21"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="66"/>
-      <c r="B41" s="62"/>
-      <c r="C41" s="62"/>
-      <c r="D41" s="62"/>
+      <c r="A41" s="77"/>
+      <c r="B41" s="76"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="76"/>
       <c r="E41" s="21" t="s">
         <v>73</v>
       </c>
       <c r="F41" s="21"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="66"/>
-      <c r="B42" s="62"/>
-      <c r="C42" s="62"/>
-      <c r="D42" s="62"/>
+      <c r="A42" s="77"/>
+      <c r="B42" s="76"/>
+      <c r="C42" s="76"/>
+      <c r="D42" s="76"/>
       <c r="E42" s="21" t="s">
         <v>75</v>
       </c>
@@ -3805,16 +3842,16 @@
       <c r="F43" s="7"/>
     </row>
     <row r="44" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="59">
+      <c r="A44" s="78">
         <v>8</v>
       </c>
-      <c r="B44" s="56" t="s">
+      <c r="B44" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="56" t="s">
+      <c r="C44" s="60" t="s">
         <v>152</v>
       </c>
-      <c r="D44" s="56" t="s">
+      <c r="D44" s="60" t="s">
         <v>153</v>
       </c>
       <c r="E44" s="21" t="s">
@@ -3825,10 +3862,10 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="60"/>
-      <c r="B45" s="57"/>
-      <c r="C45" s="57"/>
-      <c r="D45" s="57"/>
+      <c r="A45" s="79"/>
+      <c r="B45" s="61"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="61"/>
       <c r="E45" s="21" t="s">
         <v>47</v>
       </c>
@@ -3837,50 +3874,50 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="60"/>
-      <c r="B46" s="57"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="57"/>
+      <c r="A46" s="79"/>
+      <c r="B46" s="61"/>
+      <c r="C46" s="61"/>
+      <c r="D46" s="61"/>
       <c r="E46" s="21" t="s">
         <v>49</v>
       </c>
       <c r="F46" s="21"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="60"/>
-      <c r="B47" s="57"/>
-      <c r="C47" s="57"/>
-      <c r="D47" s="57"/>
+      <c r="A47" s="79"/>
+      <c r="B47" s="61"/>
+      <c r="C47" s="61"/>
+      <c r="D47" s="61"/>
       <c r="E47" s="21" t="s">
         <v>50</v>
       </c>
       <c r="F47" s="21"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" s="60"/>
-      <c r="B48" s="57"/>
-      <c r="C48" s="57"/>
-      <c r="D48" s="57"/>
+      <c r="A48" s="79"/>
+      <c r="B48" s="61"/>
+      <c r="C48" s="61"/>
+      <c r="D48" s="61"/>
       <c r="E48" s="21" t="s">
         <v>154</v>
       </c>
       <c r="F48" s="21"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="60"/>
-      <c r="B49" s="57"/>
-      <c r="C49" s="57"/>
-      <c r="D49" s="57"/>
+      <c r="A49" s="79"/>
+      <c r="B49" s="61"/>
+      <c r="C49" s="61"/>
+      <c r="D49" s="61"/>
       <c r="E49" s="21" t="s">
         <v>155</v>
       </c>
       <c r="F49" s="21"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="61"/>
-      <c r="B50" s="58"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58"/>
+      <c r="A50" s="80"/>
+      <c r="B50" s="73"/>
+      <c r="C50" s="73"/>
+      <c r="D50" s="73"/>
       <c r="E50" s="21" t="s">
         <v>37</v>
       </c>
@@ -3895,16 +3932,16 @@
       <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="59">
+      <c r="A52" s="78">
         <v>9</v>
       </c>
-      <c r="B52" s="56" t="s">
+      <c r="B52" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C52" s="56" t="s">
+      <c r="C52" s="60" t="s">
         <v>160</v>
       </c>
-      <c r="D52" s="56" t="s">
+      <c r="D52" s="60" t="s">
         <v>161</v>
       </c>
       <c r="E52" s="21" t="s">
@@ -3915,10 +3952,10 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="60"/>
-      <c r="B53" s="57"/>
-      <c r="C53" s="57"/>
-      <c r="D53" s="57"/>
+      <c r="A53" s="79"/>
+      <c r="B53" s="61"/>
+      <c r="C53" s="61"/>
+      <c r="D53" s="61"/>
       <c r="E53" s="21" t="s">
         <v>47</v>
       </c>
@@ -3927,50 +3964,50 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="60"/>
-      <c r="B54" s="57"/>
-      <c r="C54" s="57"/>
-      <c r="D54" s="57"/>
+      <c r="A54" s="79"/>
+      <c r="B54" s="61"/>
+      <c r="C54" s="61"/>
+      <c r="D54" s="61"/>
       <c r="E54" s="21" t="s">
         <v>49</v>
       </c>
       <c r="F54" s="21"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" s="60"/>
-      <c r="B55" s="57"/>
-      <c r="C55" s="57"/>
-      <c r="D55" s="57"/>
+      <c r="A55" s="79"/>
+      <c r="B55" s="61"/>
+      <c r="C55" s="61"/>
+      <c r="D55" s="61"/>
       <c r="E55" s="21" t="s">
         <v>50</v>
       </c>
       <c r="F55" s="21"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="60"/>
-      <c r="B56" s="57"/>
-      <c r="C56" s="57"/>
-      <c r="D56" s="57"/>
+      <c r="A56" s="79"/>
+      <c r="B56" s="61"/>
+      <c r="C56" s="61"/>
+      <c r="D56" s="61"/>
       <c r="E56" s="21" t="s">
         <v>154</v>
       </c>
       <c r="F56" s="21"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A57" s="60"/>
-      <c r="B57" s="57"/>
-      <c r="C57" s="57"/>
-      <c r="D57" s="57"/>
+      <c r="A57" s="79"/>
+      <c r="B57" s="61"/>
+      <c r="C57" s="61"/>
+      <c r="D57" s="61"/>
       <c r="E57" s="21" t="s">
         <v>155</v>
       </c>
       <c r="F57" s="21"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="61"/>
-      <c r="B58" s="58"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="58"/>
+      <c r="A58" s="80"/>
+      <c r="B58" s="73"/>
+      <c r="C58" s="73"/>
+      <c r="D58" s="73"/>
       <c r="E58" s="21" t="s">
         <v>37</v>
       </c>
@@ -3993,40 +4030,40 @@
       <c r="F64" s="7"/>
     </row>
     <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="69">
+      <c r="A65" s="66">
         <v>10</v>
       </c>
-      <c r="B65" s="72" t="s">
+      <c r="B65" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="C65" s="72" t="s">
+      <c r="C65" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="D65" s="72" t="s">
+      <c r="D65" s="69" t="s">
         <v>33</v>
       </c>
       <c r="E65" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F65" s="67" t="s">
+      <c r="F65" s="74" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66" s="70"/>
-      <c r="B66" s="73"/>
-      <c r="C66" s="73"/>
-      <c r="D66" s="73"/>
+      <c r="A66" s="67"/>
+      <c r="B66" s="70"/>
+      <c r="C66" s="70"/>
+      <c r="D66" s="70"/>
       <c r="E66" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="F66" s="68"/>
+      <c r="F66" s="75"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" s="71"/>
-      <c r="B67" s="74"/>
-      <c r="C67" s="74"/>
-      <c r="D67" s="74"/>
+      <c r="A67" s="68"/>
+      <c r="B67" s="71"/>
+      <c r="C67" s="71"/>
+      <c r="D67" s="71"/>
       <c r="E67" s="6"/>
       <c r="F67" s="31"/>
     </row>
@@ -4039,16 +4076,16 @@
       <c r="F68" s="7"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="69">
+      <c r="A69" s="66">
         <v>11</v>
       </c>
-      <c r="B69" s="72" t="s">
+      <c r="B69" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="C69" s="72" t="s">
+      <c r="C69" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="D69" s="72" t="s">
+      <c r="D69" s="69" t="s">
         <v>26</v>
       </c>
       <c r="E69" s="17" t="s">
@@ -4057,20 +4094,20 @@
       <c r="F69" s="31"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="70"/>
-      <c r="B70" s="73"/>
-      <c r="C70" s="73"/>
-      <c r="D70" s="73"/>
+      <c r="A70" s="67"/>
+      <c r="B70" s="70"/>
+      <c r="C70" s="70"/>
+      <c r="D70" s="70"/>
       <c r="E70" s="17" t="s">
         <v>28</v>
       </c>
       <c r="F70" s="31"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" s="71"/>
-      <c r="B71" s="74"/>
-      <c r="C71" s="74"/>
-      <c r="D71" s="74"/>
+      <c r="A71" s="68"/>
+      <c r="B71" s="71"/>
+      <c r="C71" s="71"/>
+      <c r="D71" s="71"/>
       <c r="E71" s="17" t="s">
         <v>29</v>
       </c>
@@ -4084,16 +4121,16 @@
       <c r="E74" s="9"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="77">
+      <c r="A75" s="64">
         <v>6</v>
       </c>
-      <c r="B75" s="75" t="s">
+      <c r="B75" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C75" s="75" t="s">
+      <c r="C75" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="D75" s="75" t="s">
+      <c r="D75" s="62" t="s">
         <v>19</v>
       </c>
       <c r="E75" s="12" t="s">
@@ -4101,10 +4138,10 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A76" s="78"/>
-      <c r="B76" s="76"/>
-      <c r="C76" s="76"/>
-      <c r="D76" s="76"/>
+      <c r="A76" s="65"/>
+      <c r="B76" s="63"/>
+      <c r="C76" s="63"/>
+      <c r="D76" s="63"/>
       <c r="E76" s="12" t="s">
         <v>31</v>
       </c>
@@ -4169,6 +4206,40 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="C44:C50"/>
+    <mergeCell ref="B44:B50"/>
+    <mergeCell ref="D44:D50"/>
+    <mergeCell ref="A44:A50"/>
+    <mergeCell ref="A52:A58"/>
+    <mergeCell ref="B52:B58"/>
+    <mergeCell ref="C52:C58"/>
+    <mergeCell ref="D52:D58"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="D37:D42"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="B37:B42"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="D65:D67"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C22:C28"/>
+    <mergeCell ref="D22:D28"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="B2:B8"/>
     <mergeCell ref="C2:C8"/>
@@ -4185,40 +4256,6 @@
     <mergeCell ref="B10:B16"/>
     <mergeCell ref="C10:C16"/>
     <mergeCell ref="D10:D16"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C22:C28"/>
-    <mergeCell ref="D22:D28"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="D65:D67"/>
-    <mergeCell ref="C37:C42"/>
-    <mergeCell ref="D37:D42"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="B37:B42"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="C44:C50"/>
-    <mergeCell ref="B44:B50"/>
-    <mergeCell ref="D44:D50"/>
-    <mergeCell ref="A44:A50"/>
-    <mergeCell ref="A52:A58"/>
-    <mergeCell ref="B52:B58"/>
-    <mergeCell ref="C52:C58"/>
-    <mergeCell ref="D52:D58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4229,7 +4266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526350BB-95BB-4BF1-93A5-0B30D123D1AA}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -4262,16 +4299,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="63">
+      <c r="A2" s="58">
         <v>1</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="60" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="14" t="s">
@@ -4282,10 +4319,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="64"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
       <c r="E3" s="15" t="s">
         <v>60</v>
       </c>
@@ -4294,70 +4331,70 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="64"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
       <c r="E4" s="15" t="s">
         <v>64</v>
       </c>
       <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="64"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
       <c r="E5" s="15" t="s">
         <v>65</v>
       </c>
       <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="64"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
       <c r="E6" s="15" t="s">
         <v>162</v>
       </c>
       <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="64"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
+      <c r="A7" s="59"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
       <c r="E7" s="15" t="s">
         <v>265</v>
       </c>
       <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="64"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
+      <c r="A8" s="59"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
       <c r="E8" s="15" t="s">
         <v>61</v>
       </c>
       <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="64"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
+      <c r="A9" s="59"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
       <c r="E9" s="15" t="s">
         <v>62</v>
       </c>
       <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="65"/>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
+      <c r="A10" s="72"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
       <c r="E10" s="15" t="s">
         <v>14</v>
       </c>
@@ -4372,16 +4409,16 @@
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="63">
+      <c r="A12" s="58">
         <v>2</v>
       </c>
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="56" t="s">
+      <c r="C12" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="60" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="15" t="s">
@@ -4392,40 +4429,40 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="64"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
+      <c r="A13" s="59"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
       <c r="E13" s="15" t="s">
         <v>102</v>
       </c>
       <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="64"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
+      <c r="A14" s="59"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
       <c r="E14" s="15" t="s">
         <v>103</v>
       </c>
       <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="64"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
+      <c r="A15" s="59"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
       <c r="E15" s="15" t="s">
         <v>104</v>
       </c>
       <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="65"/>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
+      <c r="A16" s="72"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="73"/>
       <c r="E16" s="11" t="s">
         <v>51</v>
       </c>
@@ -4440,16 +4477,16 @@
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="63">
+      <c r="A18" s="58">
         <v>3</v>
       </c>
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="56" t="s">
+      <c r="D18" s="60" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="15" t="s">
@@ -4460,50 +4497,50 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="64"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
+      <c r="A19" s="59"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
       <c r="E19" s="15" t="s">
         <v>102</v>
       </c>
       <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="64"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
+      <c r="A20" s="59"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
       <c r="E20" s="15" t="s">
         <v>106</v>
       </c>
       <c r="F20" s="21"/>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="64"/>
-      <c r="B21" s="57"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
+      <c r="A21" s="59"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
       <c r="E21" s="15" t="s">
         <v>107</v>
       </c>
       <c r="F21" s="21"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="64"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
+      <c r="A22" s="59"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
       <c r="E22" s="15" t="s">
         <v>109</v>
       </c>
       <c r="F22" s="21"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="64"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
+      <c r="A23" s="59"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
       <c r="E23" s="15" t="s">
         <v>108</v>
       </c>
@@ -4518,16 +4555,16 @@
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="63">
+      <c r="A25" s="58">
         <v>4</v>
       </c>
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="56" t="s">
+      <c r="C25" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="56" t="s">
+      <c r="D25" s="60" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="15" t="s">
@@ -4536,10 +4573,10 @@
       <c r="F25" s="21"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="64"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
+      <c r="A26" s="59"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
       <c r="E26" s="15" t="s">
         <v>111</v>
       </c>
@@ -4554,16 +4591,16 @@
       <c r="F27" s="7"/>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="63">
+      <c r="A28" s="58">
         <v>5</v>
       </c>
-      <c r="B28" s="56" t="s">
+      <c r="B28" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="56" t="s">
+      <c r="C28" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="56" t="s">
+      <c r="D28" s="60" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="15" t="s">
@@ -4574,10 +4611,10 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="64"/>
-      <c r="B29" s="57"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
+      <c r="A29" s="59"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="61"/>
+      <c r="D29" s="61"/>
       <c r="E29" s="15" t="s">
         <v>17</v>
       </c>
@@ -4592,16 +4629,16 @@
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="63">
+      <c r="A31" s="58">
         <v>6</v>
       </c>
-      <c r="B31" s="56" t="s">
+      <c r="B31" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="56" t="s">
+      <c r="C31" s="60" t="s">
         <v>113</v>
       </c>
-      <c r="D31" s="56" t="s">
+      <c r="D31" s="60" t="s">
         <v>43</v>
       </c>
       <c r="E31" s="14" t="s">
@@ -4612,30 +4649,30 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="64"/>
-      <c r="B32" s="57"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="57"/>
+      <c r="A32" s="59"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
       <c r="E32" s="15" t="s">
         <v>116</v>
       </c>
       <c r="F32" s="21"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="64"/>
-      <c r="B33" s="57"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="57"/>
+      <c r="A33" s="59"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="61"/>
       <c r="E33" s="15" t="s">
         <v>114</v>
       </c>
       <c r="F33" s="21"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="65"/>
-      <c r="B34" s="58"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
+      <c r="A34" s="72"/>
+      <c r="B34" s="73"/>
+      <c r="C34" s="73"/>
+      <c r="D34" s="73"/>
       <c r="E34" s="15" t="s">
         <v>22</v>
       </c>
@@ -4650,16 +4687,16 @@
       <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="63">
+      <c r="A36" s="58">
         <v>7</v>
       </c>
-      <c r="B36" s="56" t="s">
+      <c r="B36" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="56" t="s">
+      <c r="C36" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="56" t="s">
+      <c r="D36" s="60" t="s">
         <v>24</v>
       </c>
       <c r="E36" s="15" t="s">
@@ -4668,20 +4705,20 @@
       <c r="F36" s="21"/>
     </row>
     <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="64"/>
-      <c r="B37" s="57"/>
-      <c r="C37" s="57"/>
-      <c r="D37" s="57"/>
+      <c r="A37" s="59"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="61"/>
       <c r="E37" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F37" s="21"/>
     </row>
     <row r="38" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="65"/>
-      <c r="B38" s="58"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
+      <c r="A38" s="72"/>
+      <c r="B38" s="73"/>
+      <c r="C38" s="73"/>
+      <c r="D38" s="73"/>
       <c r="E38" s="15" t="s">
         <v>36</v>
       </c>
@@ -4696,16 +4733,16 @@
       <c r="F39" s="7"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="63">
+      <c r="A40" s="58">
         <v>8</v>
       </c>
-      <c r="B40" s="56" t="s">
+      <c r="B40" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="56" t="s">
+      <c r="C40" s="60" t="s">
         <v>149</v>
       </c>
-      <c r="D40" s="56" t="s">
+      <c r="D40" s="60" t="s">
         <v>117</v>
       </c>
       <c r="E40" s="21" t="s">
@@ -4714,70 +4751,70 @@
       <c r="F40" s="21"/>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="64"/>
-      <c r="B41" s="57"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="57"/>
+      <c r="A41" s="59"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
       <c r="E41" s="21" t="s">
         <v>119</v>
       </c>
       <c r="F41" s="21"/>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="64"/>
-      <c r="B42" s="57"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="57"/>
+      <c r="A42" s="59"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="61"/>
       <c r="E42" s="21" t="s">
         <v>120</v>
       </c>
       <c r="F42" s="21"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="64"/>
-      <c r="B43" s="57"/>
-      <c r="C43" s="57"/>
-      <c r="D43" s="57"/>
+      <c r="A43" s="59"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="61"/>
+      <c r="D43" s="61"/>
       <c r="E43" s="21" t="s">
         <v>121</v>
       </c>
       <c r="F43" s="21"/>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="64"/>
-      <c r="B44" s="57"/>
-      <c r="C44" s="57"/>
-      <c r="D44" s="57"/>
+      <c r="A44" s="59"/>
+      <c r="B44" s="61"/>
+      <c r="C44" s="61"/>
+      <c r="D44" s="61"/>
       <c r="E44" s="21" t="s">
         <v>123</v>
       </c>
       <c r="F44" s="21"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="64"/>
-      <c r="B45" s="57"/>
-      <c r="C45" s="57"/>
-      <c r="D45" s="57"/>
+      <c r="A45" s="59"/>
+      <c r="B45" s="61"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="61"/>
       <c r="E45" s="21" t="s">
         <v>124</v>
       </c>
       <c r="F45" s="21"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="64"/>
-      <c r="B46" s="57"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="57"/>
+      <c r="A46" s="59"/>
+      <c r="B46" s="61"/>
+      <c r="C46" s="61"/>
+      <c r="D46" s="61"/>
       <c r="E46" s="21" t="s">
         <v>122</v>
       </c>
       <c r="F46" s="21"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="64"/>
-      <c r="B47" s="57"/>
-      <c r="C47" s="57"/>
-      <c r="D47" s="57"/>
+      <c r="A47" s="59"/>
+      <c r="B47" s="61"/>
+      <c r="C47" s="61"/>
+      <c r="D47" s="61"/>
       <c r="E47" s="14" t="s">
         <v>75</v>
       </c>
@@ -4793,6 +4830,30 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A40:A47"/>
+    <mergeCell ref="B40:B47"/>
+    <mergeCell ref="C40:C47"/>
+    <mergeCell ref="D40:D47"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="B2:B10"/>
     <mergeCell ref="C2:C10"/>
@@ -4801,30 +4862,6 @@
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
     <mergeCell ref="D12:D16"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A40:A47"/>
-    <mergeCell ref="B40:B47"/>
-    <mergeCell ref="C40:C47"/>
-    <mergeCell ref="D40:D47"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="A36:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4834,8 +4871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD0B509-A153-4B31-95B8-BC32DC1B6A3B}">
   <dimension ref="B2:J25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4989,10 +5026,10 @@
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="89" t="s">
+      <c r="B11" s="81" t="s">
         <v>239</v>
       </c>
-      <c r="D11" s="87" t="s">
+      <c r="D11" s="82" t="s">
         <v>148</v>
       </c>
       <c r="F11" s="36" t="s">
@@ -5003,8 +5040,8 @@
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="89"/>
-      <c r="D12" s="87"/>
+      <c r="B12" s="81"/>
+      <c r="D12" s="82"/>
       <c r="F12" s="38" t="s">
         <v>225</v>
       </c>
@@ -5031,7 +5068,7 @@
       <c r="B14" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="D14" s="85" t="s">
+      <c r="D14" s="56" t="s">
         <v>241</v>
       </c>
       <c r="F14" s="38" t="s">
@@ -5042,7 +5079,7 @@
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="86" t="s">
+      <c r="B15" s="57" t="s">
         <v>242</v>
       </c>
       <c r="D15" s="36" t="s">
@@ -5107,7 +5144,7 @@
       <c r="B20" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="D20" s="87" t="s">
+      <c r="D20" s="82" t="s">
         <v>259</v>
       </c>
       <c r="F20" s="38" t="s">
@@ -5118,21 +5155,21 @@
       <c r="B21" s="32" t="s">
         <v>261</v>
       </c>
-      <c r="D21" s="88"/>
+      <c r="D21" s="83"/>
       <c r="F21" s="38" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="90" t="s">
+      <c r="B22" s="81" t="s">
         <v>259</v>
       </c>
-      <c r="D22" s="84"/>
       <c r="F22" s="38" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B23" s="81"/>
       <c r="D23" s="55" t="s">
         <v>226</v>
       </c>
@@ -5141,7 +5178,9 @@
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B24" s="90"/>
+      <c r="B24" s="32" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="F25" s="55" t="s">
@@ -5149,10 +5188,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B22:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5194,25 +5234,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="82"/>
-      <c r="B1" s="83" t="s">
+      <c r="A1" s="87"/>
+      <c r="B1" s="88" t="s">
         <v>168</v>
       </c>
-      <c r="C1" s="83"/>
+      <c r="C1" s="88"/>
       <c r="D1" s="47"/>
-      <c r="E1" s="83" t="s">
+      <c r="E1" s="88" t="s">
         <v>169</v>
       </c>
-      <c r="F1" s="83"/>
+      <c r="F1" s="88"/>
       <c r="G1" s="47"/>
-      <c r="H1" s="83" t="s">
+      <c r="H1" s="88" t="s">
         <v>170</v>
       </c>
-      <c r="I1" s="83"/>
-      <c r="J1" s="82"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="87"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="82"/>
+      <c r="A2" s="87"/>
       <c r="B2" s="51"/>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
@@ -5221,100 +5261,100 @@
       <c r="G2" s="46"/>
       <c r="H2" s="46"/>
       <c r="I2" s="46"/>
-      <c r="J2" s="82"/>
+      <c r="J2" s="87"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="82"/>
+      <c r="A3" s="87"/>
       <c r="B3" s="50" t="s">
         <v>163</v>
       </c>
       <c r="C3" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="D3" s="79"/>
+      <c r="D3" s="84"/>
       <c r="E3" s="48" t="s">
         <v>163</v>
       </c>
       <c r="F3" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="G3" s="79"/>
+      <c r="G3" s="84"/>
       <c r="H3" s="48" t="s">
         <v>163</v>
       </c>
       <c r="I3" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="J3" s="82"/>
+      <c r="J3" s="87"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="82"/>
+      <c r="A4" s="87"/>
       <c r="B4" s="50" t="s">
         <v>165</v>
       </c>
       <c r="C4" s="48" t="s">
         <v>180</v>
       </c>
-      <c r="D4" s="80"/>
+      <c r="D4" s="85"/>
       <c r="E4" s="48" t="s">
         <v>165</v>
       </c>
       <c r="F4" s="48" t="s">
         <v>181</v>
       </c>
-      <c r="G4" s="80"/>
+      <c r="G4" s="85"/>
       <c r="H4" s="48" t="s">
         <v>165</v>
       </c>
       <c r="I4" s="48" t="s">
         <v>182</v>
       </c>
-      <c r="J4" s="82"/>
+      <c r="J4" s="87"/>
     </row>
     <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="82"/>
+      <c r="A5" s="87"/>
       <c r="B5" s="50" t="s">
         <v>166</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="D5" s="80"/>
+      <c r="D5" s="85"/>
       <c r="E5" s="48" t="s">
         <v>166</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="G5" s="80"/>
+      <c r="G5" s="85"/>
       <c r="H5" s="48" t="s">
         <v>166</v>
       </c>
       <c r="I5" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="J5" s="82"/>
+      <c r="J5" s="87"/>
     </row>
     <row r="6" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="82"/>
+      <c r="A6" s="87"/>
       <c r="B6" s="50" t="s">
         <v>167</v>
       </c>
       <c r="C6" s="48"/>
-      <c r="D6" s="81"/>
+      <c r="D6" s="86"/>
       <c r="E6" s="48" t="s">
         <v>167</v>
       </c>
       <c r="F6" s="48"/>
-      <c r="G6" s="81"/>
+      <c r="G6" s="86"/>
       <c r="H6" s="48" t="s">
         <v>167</v>
       </c>
       <c r="I6" s="48"/>
-      <c r="J6" s="82"/>
+      <c r="J6" s="87"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="82"/>
+      <c r="A7" s="87"/>
       <c r="B7" s="52"/>
       <c r="C7" s="49"/>
       <c r="D7" s="49"/>
@@ -5323,100 +5363,100 @@
       <c r="G7" s="49"/>
       <c r="H7" s="49"/>
       <c r="I7" s="49"/>
-      <c r="J7" s="82"/>
+      <c r="J7" s="87"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="82"/>
+      <c r="A8" s="87"/>
       <c r="B8" s="50" t="s">
         <v>163</v>
       </c>
       <c r="C8" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="D8" s="79"/>
+      <c r="D8" s="84"/>
       <c r="E8" s="48" t="s">
         <v>163</v>
       </c>
       <c r="F8" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="G8" s="79"/>
+      <c r="G8" s="84"/>
       <c r="H8" s="48" t="s">
         <v>163</v>
       </c>
       <c r="I8" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="J8" s="82"/>
+      <c r="J8" s="87"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="82"/>
+      <c r="A9" s="87"/>
       <c r="B9" s="50" t="s">
         <v>165</v>
       </c>
       <c r="C9" s="48" t="s">
         <v>180</v>
       </c>
-      <c r="D9" s="80"/>
+      <c r="D9" s="85"/>
       <c r="E9" s="48" t="s">
         <v>165</v>
       </c>
       <c r="F9" s="48" t="s">
         <v>181</v>
       </c>
-      <c r="G9" s="80"/>
+      <c r="G9" s="85"/>
       <c r="H9" s="48" t="s">
         <v>165</v>
       </c>
       <c r="I9" s="48" t="s">
         <v>202</v>
       </c>
-      <c r="J9" s="82"/>
+      <c r="J9" s="87"/>
     </row>
     <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="82"/>
+      <c r="A10" s="87"/>
       <c r="B10" s="50" t="s">
         <v>166</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="D10" s="80"/>
+      <c r="D10" s="85"/>
       <c r="E10" s="48" t="s">
         <v>166</v>
       </c>
       <c r="F10" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="G10" s="80"/>
+      <c r="G10" s="85"/>
       <c r="H10" s="48" t="s">
         <v>166</v>
       </c>
       <c r="I10" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="J10" s="82"/>
+      <c r="J10" s="87"/>
     </row>
     <row r="11" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="82"/>
+      <c r="A11" s="87"/>
       <c r="B11" s="50" t="s">
         <v>167</v>
       </c>
       <c r="C11" s="48"/>
-      <c r="D11" s="81"/>
+      <c r="D11" s="86"/>
       <c r="E11" s="48" t="s">
         <v>167</v>
       </c>
       <c r="F11" s="48"/>
-      <c r="G11" s="81"/>
+      <c r="G11" s="86"/>
       <c r="H11" s="48" t="s">
         <v>167</v>
       </c>
       <c r="I11" s="48"/>
-      <c r="J11" s="82"/>
+      <c r="J11" s="87"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="82"/>
+      <c r="A12" s="87"/>
       <c r="B12" s="52"/>
       <c r="C12" s="49"/>
       <c r="D12" s="49"/>
@@ -5425,92 +5465,92 @@
       <c r="G12" s="49"/>
       <c r="H12" s="49"/>
       <c r="I12" s="49"/>
-      <c r="J12" s="82"/>
+      <c r="J12" s="87"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="82"/>
+      <c r="A13" s="87"/>
       <c r="B13" s="50" t="s">
         <v>163</v>
       </c>
       <c r="C13" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="D13" s="79"/>
+      <c r="D13" s="84"/>
       <c r="E13" s="48" t="s">
         <v>163</v>
       </c>
       <c r="F13" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="G13" s="79"/>
+      <c r="G13" s="84"/>
       <c r="H13" s="48" t="s">
         <v>163</v>
       </c>
       <c r="I13" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="J13" s="82"/>
+      <c r="J13" s="87"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="82"/>
+      <c r="A14" s="87"/>
       <c r="B14" s="50" t="s">
         <v>165</v>
       </c>
       <c r="C14" s="48" t="s">
         <v>180</v>
       </c>
-      <c r="D14" s="80"/>
+      <c r="D14" s="85"/>
       <c r="E14" s="48" t="s">
         <v>165</v>
       </c>
       <c r="F14" s="48"/>
-      <c r="G14" s="80"/>
+      <c r="G14" s="85"/>
       <c r="H14" s="48" t="s">
         <v>165</v>
       </c>
       <c r="I14" s="48"/>
-      <c r="J14" s="82"/>
+      <c r="J14" s="87"/>
     </row>
     <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="82"/>
+      <c r="A15" s="87"/>
       <c r="B15" s="50" t="s">
         <v>166</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="D15" s="80"/>
+      <c r="D15" s="85"/>
       <c r="E15" s="48" t="s">
         <v>166</v>
       </c>
       <c r="F15" s="21"/>
-      <c r="G15" s="80"/>
+      <c r="G15" s="85"/>
       <c r="H15" s="48" t="s">
         <v>166</v>
       </c>
       <c r="I15" s="21"/>
-      <c r="J15" s="82"/>
+      <c r="J15" s="87"/>
     </row>
     <row r="16" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="82"/>
+      <c r="A16" s="87"/>
       <c r="B16" s="50" t="s">
         <v>167</v>
       </c>
       <c r="C16" s="48"/>
-      <c r="D16" s="81"/>
+      <c r="D16" s="86"/>
       <c r="E16" s="48" t="s">
         <v>167</v>
       </c>
       <c r="F16" s="48"/>
-      <c r="G16" s="81"/>
+      <c r="G16" s="86"/>
       <c r="H16" s="48" t="s">
         <v>167</v>
       </c>
       <c r="I16" s="48"/>
-      <c r="J16" s="82"/>
+      <c r="J16" s="87"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="82"/>
+      <c r="A17" s="87"/>
       <c r="B17" s="52"/>
       <c r="C17" s="49"/>
       <c r="D17" s="49"/>
@@ -5519,100 +5559,100 @@
       <c r="G17" s="49"/>
       <c r="H17" s="49"/>
       <c r="I17" s="49"/>
-      <c r="J17" s="82"/>
+      <c r="J17" s="87"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="82"/>
+      <c r="A18" s="87"/>
       <c r="B18" s="50" t="s">
         <v>163</v>
       </c>
       <c r="C18" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="D18" s="79"/>
+      <c r="D18" s="84"/>
       <c r="E18" s="48" t="s">
         <v>163</v>
       </c>
       <c r="F18" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="G18" s="79"/>
+      <c r="G18" s="84"/>
       <c r="H18" s="48" t="s">
         <v>163</v>
       </c>
       <c r="I18" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="J18" s="82"/>
+      <c r="J18" s="87"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="82"/>
+      <c r="A19" s="87"/>
       <c r="B19" s="50" t="s">
         <v>165</v>
       </c>
       <c r="C19" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="D19" s="80"/>
+      <c r="D19" s="85"/>
       <c r="E19" s="48" t="s">
         <v>165</v>
       </c>
       <c r="F19" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="G19" s="80"/>
+      <c r="G19" s="85"/>
       <c r="H19" s="48" t="s">
         <v>165</v>
       </c>
       <c r="I19" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="J19" s="82"/>
+      <c r="J19" s="87"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="82"/>
+      <c r="A20" s="87"/>
       <c r="B20" s="50" t="s">
         <v>166</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="D20" s="80"/>
+      <c r="D20" s="85"/>
       <c r="E20" s="48" t="s">
         <v>166</v>
       </c>
       <c r="F20" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="G20" s="80"/>
+      <c r="G20" s="85"/>
       <c r="H20" s="48" t="s">
         <v>166</v>
       </c>
       <c r="I20" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="J20" s="82"/>
+      <c r="J20" s="87"/>
     </row>
     <row r="21" spans="1:10" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="82"/>
+      <c r="A21" s="87"/>
       <c r="B21" s="50" t="s">
         <v>167</v>
       </c>
       <c r="C21" s="48"/>
-      <c r="D21" s="81"/>
+      <c r="D21" s="86"/>
       <c r="E21" s="48" t="s">
         <v>167</v>
       </c>
       <c r="F21" s="48"/>
-      <c r="G21" s="81"/>
+      <c r="G21" s="86"/>
       <c r="H21" s="48" t="s">
         <v>167</v>
       </c>
       <c r="I21" s="48"/>
-      <c r="J21" s="82"/>
+      <c r="J21" s="87"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="82"/>
+      <c r="A22" s="87"/>
       <c r="B22" s="52"/>
       <c r="C22" s="49"/>
       <c r="D22" s="49"/>
@@ -5621,100 +5661,100 @@
       <c r="G22" s="49"/>
       <c r="H22" s="49"/>
       <c r="I22" s="49"/>
-      <c r="J22" s="82"/>
+      <c r="J22" s="87"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="82"/>
+      <c r="A23" s="87"/>
       <c r="B23" s="50" t="s">
         <v>163</v>
       </c>
       <c r="C23" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="D23" s="79"/>
+      <c r="D23" s="84"/>
       <c r="E23" s="48" t="s">
         <v>163</v>
       </c>
       <c r="F23" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="G23" s="79"/>
+      <c r="G23" s="84"/>
       <c r="H23" s="48" t="s">
         <v>163</v>
       </c>
       <c r="I23" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="J23" s="82"/>
+      <c r="J23" s="87"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="82"/>
+      <c r="A24" s="87"/>
       <c r="B24" s="50" t="s">
         <v>165</v>
       </c>
       <c r="C24" s="48" t="s">
         <v>192</v>
       </c>
-      <c r="D24" s="80"/>
+      <c r="D24" s="85"/>
       <c r="E24" s="48" t="s">
         <v>165</v>
       </c>
       <c r="F24" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="G24" s="80"/>
+      <c r="G24" s="85"/>
       <c r="H24" s="48" t="s">
         <v>165</v>
       </c>
       <c r="I24" s="48" t="s">
         <v>203</v>
       </c>
-      <c r="J24" s="82"/>
+      <c r="J24" s="87"/>
     </row>
     <row r="25" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="82"/>
+      <c r="A25" s="87"/>
       <c r="B25" s="50" t="s">
         <v>166</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="D25" s="80"/>
+      <c r="D25" s="85"/>
       <c r="E25" s="48" t="s">
         <v>166</v>
       </c>
       <c r="F25" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="G25" s="80"/>
+      <c r="G25" s="85"/>
       <c r="H25" s="48" t="s">
         <v>166</v>
       </c>
       <c r="I25" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="J25" s="82"/>
+      <c r="J25" s="87"/>
     </row>
     <row r="26" spans="1:10" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="82"/>
+      <c r="A26" s="87"/>
       <c r="B26" s="50" t="s">
         <v>167</v>
       </c>
       <c r="C26" s="48"/>
-      <c r="D26" s="81"/>
+      <c r="D26" s="86"/>
       <c r="E26" s="48" t="s">
         <v>167</v>
       </c>
       <c r="F26" s="48"/>
-      <c r="G26" s="81"/>
+      <c r="G26" s="86"/>
       <c r="H26" s="48" t="s">
         <v>167</v>
       </c>
       <c r="I26" s="48"/>
-      <c r="J26" s="82"/>
+      <c r="J26" s="87"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="82"/>
+      <c r="A27" s="87"/>
       <c r="B27" s="52"/>
       <c r="C27" s="49"/>
       <c r="D27" s="49"/>
@@ -5723,100 +5763,100 @@
       <c r="G27" s="49"/>
       <c r="H27" s="49"/>
       <c r="I27" s="49"/>
-      <c r="J27" s="82"/>
+      <c r="J27" s="87"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="82"/>
+      <c r="A28" s="87"/>
       <c r="B28" s="50" t="s">
         <v>163</v>
       </c>
       <c r="C28" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D28" s="79"/>
+      <c r="D28" s="84"/>
       <c r="E28" s="48" t="s">
         <v>163</v>
       </c>
       <c r="F28" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="G28" s="79"/>
+      <c r="G28" s="84"/>
       <c r="H28" s="48" t="s">
         <v>163</v>
       </c>
       <c r="I28" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="J28" s="82"/>
+      <c r="J28" s="87"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="82"/>
+      <c r="A29" s="87"/>
       <c r="B29" s="50" t="s">
         <v>165</v>
       </c>
       <c r="C29" s="48" t="s">
         <v>193</v>
       </c>
-      <c r="D29" s="80"/>
+      <c r="D29" s="85"/>
       <c r="E29" s="48" t="s">
         <v>165</v>
       </c>
       <c r="F29" s="48" t="s">
         <v>214</v>
       </c>
-      <c r="G29" s="80"/>
+      <c r="G29" s="85"/>
       <c r="H29" s="48" t="s">
         <v>165</v>
       </c>
       <c r="I29" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="J29" s="82"/>
+      <c r="J29" s="87"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="82"/>
+      <c r="A30" s="87"/>
       <c r="B30" s="50" t="s">
         <v>166</v>
       </c>
       <c r="C30" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="D30" s="80"/>
+      <c r="D30" s="85"/>
       <c r="E30" s="48" t="s">
         <v>166</v>
       </c>
       <c r="F30" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="G30" s="80"/>
+      <c r="G30" s="85"/>
       <c r="H30" s="48" t="s">
         <v>166</v>
       </c>
       <c r="I30" s="48" t="s">
         <v>206</v>
       </c>
-      <c r="J30" s="82"/>
+      <c r="J30" s="87"/>
     </row>
     <row r="31" spans="1:10" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="82"/>
+      <c r="A31" s="87"/>
       <c r="B31" s="50" t="s">
         <v>167</v>
       </c>
       <c r="C31" s="48"/>
-      <c r="D31" s="81"/>
+      <c r="D31" s="86"/>
       <c r="E31" s="48" t="s">
         <v>167</v>
       </c>
       <c r="F31" s="48"/>
-      <c r="G31" s="81"/>
+      <c r="G31" s="86"/>
       <c r="H31" s="48" t="s">
         <v>167</v>
       </c>
       <c r="I31" s="48"/>
-      <c r="J31" s="82"/>
+      <c r="J31" s="87"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" s="82"/>
+      <c r="A32" s="87"/>
       <c r="B32" s="52"/>
       <c r="C32" s="49"/>
       <c r="D32" s="49"/>
@@ -5825,100 +5865,100 @@
       <c r="G32" s="49"/>
       <c r="H32" s="49"/>
       <c r="I32" s="49"/>
-      <c r="J32" s="82"/>
+      <c r="J32" s="87"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="82"/>
+      <c r="A33" s="87"/>
       <c r="B33" s="50" t="s">
         <v>163</v>
       </c>
       <c r="C33" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="79"/>
+      <c r="D33" s="84"/>
       <c r="E33" s="48" t="s">
         <v>163</v>
       </c>
       <c r="F33" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="G33" s="79"/>
+      <c r="G33" s="84"/>
       <c r="H33" s="48" t="s">
         <v>163</v>
       </c>
       <c r="I33" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="J33" s="82"/>
+      <c r="J33" s="87"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="82"/>
+      <c r="A34" s="87"/>
       <c r="B34" s="50" t="s">
         <v>165</v>
       </c>
       <c r="C34" s="48" t="s">
         <v>195</v>
       </c>
-      <c r="D34" s="80"/>
+      <c r="D34" s="85"/>
       <c r="E34" s="48" t="s">
         <v>165</v>
       </c>
       <c r="F34" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="G34" s="80"/>
+      <c r="G34" s="85"/>
       <c r="H34" s="48" t="s">
         <v>165</v>
       </c>
       <c r="I34" s="48" t="s">
         <v>179</v>
       </c>
-      <c r="J34" s="82"/>
+      <c r="J34" s="87"/>
     </row>
     <row r="35" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="82"/>
+      <c r="A35" s="87"/>
       <c r="B35" s="50" t="s">
         <v>166</v>
       </c>
       <c r="C35" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="D35" s="80"/>
+      <c r="D35" s="85"/>
       <c r="E35" s="48" t="s">
         <v>166</v>
       </c>
       <c r="F35" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="G35" s="80"/>
+      <c r="G35" s="85"/>
       <c r="H35" s="48" t="s">
         <v>166</v>
       </c>
       <c r="I35" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="J35" s="82"/>
+      <c r="J35" s="87"/>
     </row>
     <row r="36" spans="1:10" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="82"/>
+      <c r="A36" s="87"/>
       <c r="B36" s="50" t="s">
         <v>167</v>
       </c>
       <c r="C36" s="48"/>
-      <c r="D36" s="81"/>
+      <c r="D36" s="86"/>
       <c r="E36" s="48" t="s">
         <v>167</v>
       </c>
       <c r="F36" s="48"/>
-      <c r="G36" s="81"/>
+      <c r="G36" s="86"/>
       <c r="H36" s="48" t="s">
         <v>167</v>
       </c>
       <c r="I36" s="48"/>
-      <c r="J36" s="82"/>
+      <c r="J36" s="87"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A37" s="82"/>
+      <c r="A37" s="87"/>
       <c r="B37" s="52"/>
       <c r="C37" s="49"/>
       <c r="D37" s="54"/>
@@ -5927,100 +5967,100 @@
       <c r="G37" s="49"/>
       <c r="H37" s="49"/>
       <c r="I37" s="49"/>
-      <c r="J37" s="82"/>
+      <c r="J37" s="87"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="82"/>
+      <c r="A38" s="87"/>
       <c r="B38" s="50" t="s">
         <v>163</v>
       </c>
       <c r="C38" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D38" s="79"/>
+      <c r="D38" s="84"/>
       <c r="E38" s="48" t="s">
         <v>163</v>
       </c>
       <c r="F38" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="G38" s="79"/>
+      <c r="G38" s="84"/>
       <c r="H38" s="48" t="s">
         <v>163</v>
       </c>
       <c r="I38" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="J38" s="82"/>
+      <c r="J38" s="87"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" s="82"/>
+      <c r="A39" s="87"/>
       <c r="B39" s="50" t="s">
         <v>165</v>
       </c>
       <c r="C39" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="D39" s="80"/>
+      <c r="D39" s="85"/>
       <c r="E39" s="48" t="s">
         <v>165</v>
       </c>
       <c r="F39" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="G39" s="80"/>
+      <c r="G39" s="85"/>
       <c r="H39" s="48" t="s">
         <v>165</v>
       </c>
       <c r="I39" s="48" t="s">
         <v>208</v>
       </c>
-      <c r="J39" s="82"/>
+      <c r="J39" s="87"/>
     </row>
     <row r="40" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="82"/>
+      <c r="A40" s="87"/>
       <c r="B40" s="50" t="s">
         <v>166</v>
       </c>
       <c r="C40" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="D40" s="80"/>
+      <c r="D40" s="85"/>
       <c r="E40" s="48" t="s">
         <v>166</v>
       </c>
       <c r="F40" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="G40" s="80"/>
+      <c r="G40" s="85"/>
       <c r="H40" s="48" t="s">
         <v>166</v>
       </c>
       <c r="I40" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="J40" s="82"/>
+      <c r="J40" s="87"/>
     </row>
     <row r="41" spans="1:10" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="82"/>
+      <c r="A41" s="87"/>
       <c r="B41" s="50" t="s">
         <v>167</v>
       </c>
       <c r="C41" s="48"/>
-      <c r="D41" s="81"/>
+      <c r="D41" s="86"/>
       <c r="E41" s="48" t="s">
         <v>167</v>
       </c>
       <c r="F41" s="48"/>
-      <c r="G41" s="81"/>
+      <c r="G41" s="86"/>
       <c r="H41" s="48" t="s">
         <v>167</v>
       </c>
       <c r="I41" s="48"/>
-      <c r="J41" s="82"/>
+      <c r="J41" s="87"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A42" s="82"/>
+      <c r="A42" s="87"/>
       <c r="B42" s="52"/>
       <c r="C42" s="49"/>
       <c r="D42" s="49"/>
@@ -6029,100 +6069,100 @@
       <c r="G42" s="49"/>
       <c r="H42" s="49"/>
       <c r="I42" s="49"/>
-      <c r="J42" s="82"/>
+      <c r="J42" s="87"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A43" s="82"/>
+      <c r="A43" s="87"/>
       <c r="B43" s="50" t="s">
         <v>163</v>
       </c>
       <c r="C43" s="48" t="s">
         <v>176</v>
       </c>
-      <c r="D43" s="79"/>
+      <c r="D43" s="84"/>
       <c r="E43" s="50" t="s">
         <v>163</v>
       </c>
       <c r="F43" s="48" t="s">
         <v>176</v>
       </c>
-      <c r="G43" s="79"/>
+      <c r="G43" s="84"/>
       <c r="H43" s="50" t="s">
         <v>163</v>
       </c>
       <c r="I43" s="48" t="s">
         <v>176</v>
       </c>
-      <c r="J43" s="82"/>
+      <c r="J43" s="87"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A44" s="82"/>
+      <c r="A44" s="87"/>
       <c r="B44" s="50" t="s">
         <v>165</v>
       </c>
       <c r="C44" s="48" t="s">
         <v>198</v>
       </c>
-      <c r="D44" s="80"/>
+      <c r="D44" s="85"/>
       <c r="E44" s="50" t="s">
         <v>165</v>
       </c>
       <c r="F44" s="48" t="s">
         <v>219</v>
       </c>
-      <c r="G44" s="80"/>
+      <c r="G44" s="85"/>
       <c r="H44" s="50" t="s">
         <v>165</v>
       </c>
       <c r="I44" s="48" t="s">
         <v>199</v>
       </c>
-      <c r="J44" s="82"/>
+      <c r="J44" s="87"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A45" s="82"/>
+      <c r="A45" s="87"/>
       <c r="B45" s="50" t="s">
         <v>166</v>
       </c>
       <c r="C45" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="D45" s="80"/>
+      <c r="D45" s="85"/>
       <c r="E45" s="50" t="s">
         <v>166</v>
       </c>
       <c r="F45" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="G45" s="80"/>
+      <c r="G45" s="85"/>
       <c r="H45" s="50" t="s">
         <v>166</v>
       </c>
       <c r="I45" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="J45" s="82"/>
+      <c r="J45" s="87"/>
     </row>
     <row r="46" spans="1:10" ht="88" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="82"/>
+      <c r="A46" s="87"/>
       <c r="B46" s="50" t="s">
         <v>167</v>
       </c>
       <c r="C46" s="48"/>
-      <c r="D46" s="81"/>
+      <c r="D46" s="86"/>
       <c r="E46" s="50" t="s">
         <v>167</v>
       </c>
       <c r="F46" s="48"/>
-      <c r="G46" s="81"/>
+      <c r="G46" s="86"/>
       <c r="H46" s="50" t="s">
         <v>167</v>
       </c>
       <c r="I46" s="48"/>
-      <c r="J46" s="82"/>
+      <c r="J46" s="87"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A47" s="82"/>
+      <c r="A47" s="87"/>
       <c r="B47" s="52"/>
       <c r="C47" s="49"/>
       <c r="D47" s="49"/>
@@ -6131,10 +6171,17 @@
       <c r="G47" s="49"/>
       <c r="H47" s="52"/>
       <c r="I47" s="49"/>
-      <c r="J47" s="82"/>
+      <c r="J47" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="D33:D36"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="D18:D21"/>
     <mergeCell ref="D43:D46"/>
     <mergeCell ref="A1:A47"/>
     <mergeCell ref="J1:J47"/>
@@ -6151,13 +6198,6 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="D33:D36"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="D18:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Tidied up the code, moved classes to main package. User/Admin/Newsagent/Customer finished
</commit_message>
<xml_diff>
--- a/User Stories/NataliaUserStories.xlsx
+++ b/User Stories/NataliaUserStories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cad1acabf18afac6/Desktop/Software Design with AI for Cloud/Year_3/agile-labs3/Newsagent-Project/User Stories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="725" documentId="13_ncr:1_{7B2E17FA-F2A9-4DCC-A803-850E080333ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F5E785B-7E42-4AC8-9638-B6F5BA389E8F}"/>
+  <xr:revisionPtr revIDLastSave="776" documentId="13_ncr:1_{7B2E17FA-F2A9-4DCC-A803-850E080333ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41922FBE-6C9F-4E5B-AD8A-78B43F9BD1FD}"/>
   <bookViews>
     <workbookView xWindow="14740" yWindow="2750" windowWidth="22950" windowHeight="16250" activeTab="2" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
   </bookViews>
@@ -16,8 +16,7 @@
     <sheet name="AdminUserStories" sheetId="1" r:id="rId1"/>
     <sheet name="NewsagentUserStories" sheetId="2" r:id="rId2"/>
     <sheet name="UMLs" sheetId="3" r:id="rId3"/>
-    <sheet name="JUnit" sheetId="5" r:id="rId4"/>
-    <sheet name="MySQL Tests" sheetId="4" r:id="rId5"/>
+    <sheet name="MySQL Tests" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="266">
   <si>
     <t>As an admin</t>
   </si>
@@ -426,9 +425,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>+generateInvoice() : void</t>
-  </si>
-  <si>
     <t>- username : String</t>
   </si>
   <si>
@@ -549,12 +545,6 @@
     <t>Customer Table</t>
   </si>
   <si>
-    <t>Admin Table</t>
-  </si>
-  <si>
-    <t>Newsagent Table</t>
-  </si>
-  <si>
     <t>#2</t>
   </si>
   <si>
@@ -600,15 +590,6 @@
     <t>SELECT * FROM customerDetails;</t>
   </si>
   <si>
-    <t>INSERT INTO newsagentDetails VALUES (NULL, "newsagent2", "Newsagent2", "newsagent");</t>
-  </si>
-  <si>
-    <t>SELECT * FROM newsagentDetails;</t>
-  </si>
-  <si>
-    <t>SELECT * FROM adminDetails;</t>
-  </si>
-  <si>
     <t>INSERT INTO customerDetails VALUES (NULL, "Adrian", "Kochatek", "2 Athlone", "0874124578");</t>
   </si>
   <si>
@@ -645,69 +626,30 @@
     <t>DELETE FROM customerDetails WHERE address="Roscommon";</t>
   </si>
   <si>
-    <t>INSERT INTO newsagentDetails VALUES (NULL, "newsagent", "Newsagent123", "newsagent");</t>
-  </si>
-  <si>
     <t>Insert second newsagent into table</t>
   </si>
   <si>
     <t>Read newsagent username, role where newsagentID=2</t>
   </si>
   <si>
-    <t>SELECT username, role FROM newsagentDetails WHERE newsagentID="2";</t>
-  </si>
-  <si>
     <t>Search newsagent by role</t>
   </si>
   <si>
-    <t>SELECT * FROM newsagentDetails WHERE role="newsagent";</t>
-  </si>
-  <si>
-    <t>UPDATE newsagentDetails SET username="oldNewsagent" WHERE newsagentID="2";</t>
-  </si>
-  <si>
     <t>Update newsagent password for username oldNewsagent</t>
   </si>
   <si>
-    <t>UPDATE newsagentDetails SET newsagentPassword="oldPassword" WHERE username="oldNewsagent";</t>
-  </si>
-  <si>
-    <t>INSERT INTO adminDetails VALUES (NULL, "admin", "Admin123", "admin");</t>
-  </si>
-  <si>
-    <t>INSERT INTO adminDetails VALUES (NULL, "admin2", "Admin2", "admin");</t>
-  </si>
-  <si>
     <t>Read admin ID, name where role=admin</t>
   </si>
   <si>
-    <t>SELECT adminID, username FROM adminDetails WHERE role="admin";</t>
-  </si>
-  <si>
     <t>Search admin by ID=2</t>
   </si>
   <si>
-    <t>SELECT * FROM adminDetails WHERE adminID="2";</t>
-  </si>
-  <si>
-    <t>UPDATE adminDetails SET username="oldAdmin" WHERE adminID="2";</t>
-  </si>
-  <si>
     <t>Update admin password for adminID=2</t>
   </si>
   <si>
-    <t>UPDATE adminDetails SET adminPassword="oldPassword" WHERE adminID="2";</t>
-  </si>
-  <si>
     <t>Delete admin where username=oldAdmin</t>
   </si>
   <si>
-    <t>DELETE FROM adminDetails WHERE username="oldAdmin";</t>
-  </si>
-  <si>
-    <t>DELETE FROM newsagentDetails WHERE newsagentID="2";</t>
-  </si>
-  <si>
     <t>- address : String</t>
   </si>
   <si>
@@ -756,9 +698,6 @@
     <t>+updateCustomer (int id)</t>
   </si>
   <si>
-    <t>+generateDeliveryReport() : void</t>
-  </si>
-  <si>
     <t>+createCustomer(firstName: String, lastName: String, address: String, phoneNo: String)</t>
   </si>
   <si>
@@ -841,6 +780,63 @@
   </si>
   <si>
     <t>+doesCustomerExist(int id) : boolean</t>
+  </si>
+  <si>
+    <t>INSERT INTO userdetails VALUES (NULL, "admin", "Admin123", "admin");</t>
+  </si>
+  <si>
+    <t>INSERT INTO userdetails VALUES (NULL, "admin2", "Admin2", "admin");</t>
+  </si>
+  <si>
+    <t>SELECT adminID, username FROM userdetails WHERE role="admin";</t>
+  </si>
+  <si>
+    <t>UPDATE userdetails SET adminPassword="oldPassword" WHERE adminID="2";</t>
+  </si>
+  <si>
+    <t>DELETE FROM userdetails WHERE username="oldAdmin";</t>
+  </si>
+  <si>
+    <t>INSERT INTO userdetails VALUES (NULL, "newsagent", "Newsagent123", "newsagent");</t>
+  </si>
+  <si>
+    <t>INSERT INTO userdetails VALUES (NULL, "newsagent2", "Newsagent2", "newsagent");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Newsagent </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin </t>
+  </si>
+  <si>
+    <t>SELECT * FROM userdetails where role="newsagent";</t>
+  </si>
+  <si>
+    <t>SELECT * FROM userdetails where role="admin";</t>
+  </si>
+  <si>
+    <t>SELECT username, role FROM userdetails WHERE userID="2";</t>
+  </si>
+  <si>
+    <t>SELECT * FROM userdetails WHERE userID="2";</t>
+  </si>
+  <si>
+    <t>SELECT * FROM userdetails WHERE role="newsagent";</t>
+  </si>
+  <si>
+    <t>UPDATE userdetails SET username="oldNewsagent" WHERE userID="2";</t>
+  </si>
+  <si>
+    <t>UPDATE userdetails SET username="oldAdmin" WHERE userID="2";</t>
+  </si>
+  <si>
+    <t>UPDATE userdetails SET newsagentPassword="oldPassword" WHERE username="oldNewsagent";</t>
+  </si>
+  <si>
+    <t>DELETE FROM userdetails WHERE userID="2";</t>
+  </si>
+  <si>
+    <t>+doesUserExist(int id) : boolean</t>
   </si>
 </sst>
 </file>
@@ -1041,7 +1037,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1191,7 +1187,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1261,15 +1256,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1285,6 +1274,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1312,50 +1302,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>37354</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>74706</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2779060</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>155841</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44D60117-9839-A68D-6CE1-7C2F4067F98A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3227295" y="4549588"/>
-          <a:ext cx="2741706" cy="3442900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>22411</xdr:colOff>
       <xdr:row>25</xdr:row>
@@ -1381,7 +1327,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1425,7 +1371,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1469,7 +1415,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1489,22 +1435,66 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>37354</xdr:colOff>
+      <xdr:colOff>29884</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>82178</xdr:rowOff>
+      <xdr:rowOff>74706</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2786530</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>156094</xdr:rowOff>
+      <xdr:colOff>2797826</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>112060</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D69D7EB-90AA-C860-9755-92A026E64656}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="179296" y="4736353"/>
+          <a:ext cx="2767942" cy="4893236"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>22411</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>82177</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2876177</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>161073</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{152B75F1-05F8-30A3-377D-4F0DA0F3F660}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E5DE07E-89C2-447E-5DD4-85A419A9153C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1520,8 +1510,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="186766" y="4743825"/>
-          <a:ext cx="2749176" cy="4182740"/>
+          <a:off x="3212352" y="4930589"/>
+          <a:ext cx="2853766" cy="5121543"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3366,16 +3356,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="58">
+      <c r="A2" s="57">
         <v>1</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="60" t="s">
-        <v>150</v>
-      </c>
-      <c r="D2" s="60" t="s">
+      <c r="C2" s="59" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="59" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="15" t="s">
@@ -3386,10 +3376,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="59"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
+      <c r="A3" s="58"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
       <c r="E3" s="15" t="s">
         <v>47</v>
       </c>
@@ -3398,50 +3388,50 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="59"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
       <c r="E4" s="15" t="s">
         <v>49</v>
       </c>
       <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="59"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
       <c r="E5" s="15" t="s">
         <v>50</v>
       </c>
       <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="59"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
+      <c r="A6" s="58"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
       <c r="E6" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="59"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
+      <c r="A7" s="58"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
       <c r="E7" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="59"/>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
+      <c r="A8" s="58"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
       <c r="E8" s="15" t="s">
         <v>37</v>
       </c>
@@ -3456,16 +3446,16 @@
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="58">
+      <c r="A10" s="57">
         <v>2</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="60" t="s">
+      <c r="C10" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="60" t="s">
+      <c r="D10" s="59" t="s">
         <v>81</v>
       </c>
       <c r="E10" s="14" t="s">
@@ -3476,60 +3466,60 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="59"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
+      <c r="A11" s="58"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
       <c r="E11" s="15" t="s">
         <v>87</v>
       </c>
       <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="59"/>
-      <c r="B12" s="61"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
+      <c r="A12" s="58"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
       <c r="E12" s="15" t="s">
         <v>90</v>
       </c>
       <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="59"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
+      <c r="A13" s="58"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
       <c r="E13" s="15" t="s">
         <v>88</v>
       </c>
       <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="59"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
+      <c r="A14" s="58"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
       <c r="E14" s="15" t="s">
         <v>89</v>
       </c>
       <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="59"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
       <c r="E15" s="15" t="s">
         <v>83</v>
       </c>
       <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="72"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
+      <c r="A16" s="71"/>
+      <c r="B16" s="72"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="72"/>
       <c r="E16" s="15" t="s">
         <v>14</v>
       </c>
@@ -3544,16 +3534,16 @@
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="58">
+      <c r="A18" s="57">
         <v>3</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="60" t="s">
+      <c r="C18" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="60" t="s">
+      <c r="D18" s="59" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="15" t="s">
@@ -3564,20 +3554,20 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="59"/>
-      <c r="B19" s="61"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
+      <c r="A19" s="58"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
       <c r="E19" s="15" t="s">
         <v>91</v>
       </c>
       <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="72"/>
-      <c r="B20" s="73"/>
-      <c r="C20" s="73"/>
-      <c r="D20" s="73"/>
+      <c r="A20" s="71"/>
+      <c r="B20" s="72"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="72"/>
       <c r="E20" s="11" t="s">
         <v>51</v>
       </c>
@@ -3592,16 +3582,16 @@
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="58">
+      <c r="A22" s="57">
         <v>4</v>
       </c>
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="60" t="s">
+      <c r="C22" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="60" t="s">
+      <c r="D22" s="59" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="15" t="s">
@@ -3612,60 +3602,60 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="59"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="61"/>
+      <c r="A23" s="58"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
       <c r="E23" s="15" t="s">
         <v>96</v>
       </c>
       <c r="F23" s="21"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="59"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
+      <c r="A24" s="58"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
       <c r="E24" s="15" t="s">
         <v>97</v>
       </c>
       <c r="F24" s="21"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="59"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
+      <c r="A25" s="58"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
       <c r="E25" s="15" t="s">
         <v>98</v>
       </c>
       <c r="F25" s="21"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="59"/>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
+      <c r="A26" s="58"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="60"/>
       <c r="E26" s="15" t="s">
         <v>92</v>
       </c>
       <c r="F26" s="21"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="59"/>
-      <c r="B27" s="61"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
+      <c r="A27" s="58"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="60"/>
       <c r="E27" s="15" t="s">
         <v>93</v>
       </c>
       <c r="F27" s="21"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="72"/>
-      <c r="B28" s="73"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="73"/>
+      <c r="A28" s="71"/>
+      <c r="B28" s="72"/>
+      <c r="C28" s="72"/>
+      <c r="D28" s="72"/>
       <c r="E28" s="15" t="s">
         <v>11</v>
       </c>
@@ -3680,16 +3670,16 @@
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="58">
+      <c r="A30" s="57">
         <v>5</v>
       </c>
-      <c r="B30" s="60" t="s">
+      <c r="B30" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="60" t="s">
+      <c r="C30" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="60" t="s">
+      <c r="D30" s="59" t="s">
         <v>82</v>
       </c>
       <c r="E30" s="15" t="s">
@@ -3698,20 +3688,20 @@
       <c r="F30" s="21"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="59"/>
-      <c r="B31" s="61"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="61"/>
+      <c r="A31" s="58"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="60"/>
       <c r="E31" s="15" t="s">
         <v>94</v>
       </c>
       <c r="F31" s="21"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="72"/>
-      <c r="B32" s="73"/>
-      <c r="C32" s="73"/>
-      <c r="D32" s="73"/>
+      <c r="A32" s="71"/>
+      <c r="B32" s="72"/>
+      <c r="C32" s="72"/>
+      <c r="D32" s="72"/>
       <c r="E32" s="15" t="s">
         <v>95</v>
       </c>
@@ -3726,16 +3716,16 @@
       <c r="F33" s="7"/>
     </row>
     <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="58">
+      <c r="A34" s="57">
         <v>6</v>
       </c>
-      <c r="B34" s="60" t="s">
+      <c r="B34" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="60" t="s">
+      <c r="C34" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="60" t="s">
+      <c r="D34" s="59" t="s">
         <v>16</v>
       </c>
       <c r="E34" s="15" t="s">
@@ -3746,10 +3736,10 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="72"/>
-      <c r="B35" s="73"/>
-      <c r="C35" s="73"/>
-      <c r="D35" s="73"/>
+      <c r="A35" s="71"/>
+      <c r="B35" s="72"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="72"/>
       <c r="E35" s="15" t="s">
         <v>100</v>
       </c>
@@ -3764,70 +3754,70 @@
       <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="77">
+      <c r="A37" s="76">
         <v>7</v>
       </c>
-      <c r="B37" s="76" t="s">
+      <c r="B37" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="76" t="s">
+      <c r="C37" s="75" t="s">
         <v>68</v>
       </c>
-      <c r="D37" s="76" t="s">
+      <c r="D37" s="75" t="s">
         <v>69</v>
       </c>
       <c r="E37" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="F37" s="60" t="s">
+      <c r="F37" s="59" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="77"/>
-      <c r="B38" s="76"/>
-      <c r="C38" s="76"/>
-      <c r="D38" s="76"/>
+      <c r="A38" s="76"/>
+      <c r="B38" s="75"/>
+      <c r="C38" s="75"/>
+      <c r="D38" s="75"/>
       <c r="E38" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="F38" s="61"/>
+      <c r="F38" s="60"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="77"/>
-      <c r="B39" s="76"/>
-      <c r="C39" s="76"/>
-      <c r="D39" s="76"/>
+      <c r="A39" s="76"/>
+      <c r="B39" s="75"/>
+      <c r="C39" s="75"/>
+      <c r="D39" s="75"/>
       <c r="E39" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="F39" s="73"/>
+      <c r="F39" s="72"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="77"/>
-      <c r="B40" s="76"/>
-      <c r="C40" s="76"/>
-      <c r="D40" s="76"/>
+      <c r="A40" s="76"/>
+      <c r="B40" s="75"/>
+      <c r="C40" s="75"/>
+      <c r="D40" s="75"/>
       <c r="E40" s="21" t="s">
         <v>72</v>
       </c>
       <c r="F40" s="21"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="77"/>
-      <c r="B41" s="76"/>
-      <c r="C41" s="76"/>
-      <c r="D41" s="76"/>
+      <c r="A41" s="76"/>
+      <c r="B41" s="75"/>
+      <c r="C41" s="75"/>
+      <c r="D41" s="75"/>
       <c r="E41" s="21" t="s">
         <v>73</v>
       </c>
       <c r="F41" s="21"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="77"/>
-      <c r="B42" s="76"/>
-      <c r="C42" s="76"/>
-      <c r="D42" s="76"/>
+      <c r="A42" s="76"/>
+      <c r="B42" s="75"/>
+      <c r="C42" s="75"/>
+      <c r="D42" s="75"/>
       <c r="E42" s="21" t="s">
         <v>75</v>
       </c>
@@ -3842,82 +3832,82 @@
       <c r="F43" s="7"/>
     </row>
     <row r="44" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="78">
+      <c r="A44" s="77">
         <v>8</v>
       </c>
-      <c r="B44" s="60" t="s">
+      <c r="B44" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="60" t="s">
+      <c r="C44" s="59" t="s">
+        <v>151</v>
+      </c>
+      <c r="D44" s="59" t="s">
         <v>152</v>
-      </c>
-      <c r="D44" s="60" t="s">
-        <v>153</v>
       </c>
       <c r="E44" s="21" t="s">
         <v>39</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="79"/>
-      <c r="B45" s="61"/>
-      <c r="C45" s="61"/>
-      <c r="D45" s="61"/>
+      <c r="A45" s="78"/>
+      <c r="B45" s="60"/>
+      <c r="C45" s="60"/>
+      <c r="D45" s="60"/>
       <c r="E45" s="21" t="s">
         <v>47</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="79"/>
-      <c r="B46" s="61"/>
-      <c r="C46" s="61"/>
-      <c r="D46" s="61"/>
+      <c r="A46" s="78"/>
+      <c r="B46" s="60"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
       <c r="E46" s="21" t="s">
         <v>49</v>
       </c>
       <c r="F46" s="21"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="79"/>
-      <c r="B47" s="61"/>
-      <c r="C47" s="61"/>
-      <c r="D47" s="61"/>
+      <c r="A47" s="78"/>
+      <c r="B47" s="60"/>
+      <c r="C47" s="60"/>
+      <c r="D47" s="60"/>
       <c r="E47" s="21" t="s">
         <v>50</v>
       </c>
       <c r="F47" s="21"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" s="79"/>
-      <c r="B48" s="61"/>
-      <c r="C48" s="61"/>
-      <c r="D48" s="61"/>
+      <c r="A48" s="78"/>
+      <c r="B48" s="60"/>
+      <c r="C48" s="60"/>
+      <c r="D48" s="60"/>
       <c r="E48" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="F48" s="21"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" s="78"/>
+      <c r="B49" s="60"/>
+      <c r="C49" s="60"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="F48" s="21"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="79"/>
-      <c r="B49" s="61"/>
-      <c r="C49" s="61"/>
-      <c r="D49" s="61"/>
-      <c r="E49" s="21" t="s">
-        <v>155</v>
-      </c>
       <c r="F49" s="21"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="80"/>
-      <c r="B50" s="73"/>
-      <c r="C50" s="73"/>
-      <c r="D50" s="73"/>
+      <c r="A50" s="79"/>
+      <c r="B50" s="72"/>
+      <c r="C50" s="72"/>
+      <c r="D50" s="72"/>
       <c r="E50" s="21" t="s">
         <v>37</v>
       </c>
@@ -3932,82 +3922,82 @@
       <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="78">
+      <c r="A52" s="77">
         <v>9</v>
       </c>
-      <c r="B52" s="60" t="s">
+      <c r="B52" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C52" s="60" t="s">
+      <c r="C52" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="D52" s="59" t="s">
         <v>160</v>
-      </c>
-      <c r="D52" s="60" t="s">
-        <v>161</v>
       </c>
       <c r="E52" s="21" t="s">
         <v>39</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="79"/>
-      <c r="B53" s="61"/>
-      <c r="C53" s="61"/>
-      <c r="D53" s="61"/>
+      <c r="A53" s="78"/>
+      <c r="B53" s="60"/>
+      <c r="C53" s="60"/>
+      <c r="D53" s="60"/>
       <c r="E53" s="21" t="s">
         <v>47</v>
       </c>
       <c r="F53" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="79"/>
-      <c r="B54" s="61"/>
-      <c r="C54" s="61"/>
-      <c r="D54" s="61"/>
+      <c r="A54" s="78"/>
+      <c r="B54" s="60"/>
+      <c r="C54" s="60"/>
+      <c r="D54" s="60"/>
       <c r="E54" s="21" t="s">
         <v>49</v>
       </c>
       <c r="F54" s="21"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" s="79"/>
-      <c r="B55" s="61"/>
-      <c r="C55" s="61"/>
-      <c r="D55" s="61"/>
+      <c r="A55" s="78"/>
+      <c r="B55" s="60"/>
+      <c r="C55" s="60"/>
+      <c r="D55" s="60"/>
       <c r="E55" s="21" t="s">
         <v>50</v>
       </c>
       <c r="F55" s="21"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="79"/>
-      <c r="B56" s="61"/>
-      <c r="C56" s="61"/>
-      <c r="D56" s="61"/>
+      <c r="A56" s="78"/>
+      <c r="B56" s="60"/>
+      <c r="C56" s="60"/>
+      <c r="D56" s="60"/>
       <c r="E56" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="F56" s="21"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" s="78"/>
+      <c r="B57" s="60"/>
+      <c r="C57" s="60"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="F56" s="21"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A57" s="79"/>
-      <c r="B57" s="61"/>
-      <c r="C57" s="61"/>
-      <c r="D57" s="61"/>
-      <c r="E57" s="21" t="s">
-        <v>155</v>
-      </c>
       <c r="F57" s="21"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="80"/>
-      <c r="B58" s="73"/>
-      <c r="C58" s="73"/>
-      <c r="D58" s="73"/>
+      <c r="A58" s="79"/>
+      <c r="B58" s="72"/>
+      <c r="C58" s="72"/>
+      <c r="D58" s="72"/>
       <c r="E58" s="21" t="s">
         <v>37</v>
       </c>
@@ -4030,40 +4020,40 @@
       <c r="F64" s="7"/>
     </row>
     <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="66">
+      <c r="A65" s="65">
         <v>10</v>
       </c>
-      <c r="B65" s="69" t="s">
+      <c r="B65" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="C65" s="69" t="s">
+      <c r="C65" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="D65" s="69" t="s">
+      <c r="D65" s="68" t="s">
         <v>33</v>
       </c>
       <c r="E65" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F65" s="74" t="s">
+      <c r="F65" s="73" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66" s="67"/>
-      <c r="B66" s="70"/>
-      <c r="C66" s="70"/>
-      <c r="D66" s="70"/>
+      <c r="A66" s="66"/>
+      <c r="B66" s="69"/>
+      <c r="C66" s="69"/>
+      <c r="D66" s="69"/>
       <c r="E66" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="F66" s="75"/>
+      <c r="F66" s="74"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" s="68"/>
-      <c r="B67" s="71"/>
-      <c r="C67" s="71"/>
-      <c r="D67" s="71"/>
+      <c r="A67" s="67"/>
+      <c r="B67" s="70"/>
+      <c r="C67" s="70"/>
+      <c r="D67" s="70"/>
       <c r="E67" s="6"/>
       <c r="F67" s="31"/>
     </row>
@@ -4076,16 +4066,16 @@
       <c r="F68" s="7"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="66">
+      <c r="A69" s="65">
         <v>11</v>
       </c>
-      <c r="B69" s="69" t="s">
+      <c r="B69" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="C69" s="69" t="s">
+      <c r="C69" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="D69" s="69" t="s">
+      <c r="D69" s="68" t="s">
         <v>26</v>
       </c>
       <c r="E69" s="17" t="s">
@@ -4094,20 +4084,20 @@
       <c r="F69" s="31"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="67"/>
-      <c r="B70" s="70"/>
-      <c r="C70" s="70"/>
-      <c r="D70" s="70"/>
+      <c r="A70" s="66"/>
+      <c r="B70" s="69"/>
+      <c r="C70" s="69"/>
+      <c r="D70" s="69"/>
       <c r="E70" s="17" t="s">
         <v>28</v>
       </c>
       <c r="F70" s="31"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" s="68"/>
-      <c r="B71" s="71"/>
-      <c r="C71" s="71"/>
-      <c r="D71" s="71"/>
+      <c r="A71" s="67"/>
+      <c r="B71" s="70"/>
+      <c r="C71" s="70"/>
+      <c r="D71" s="70"/>
       <c r="E71" s="17" t="s">
         <v>29</v>
       </c>
@@ -4121,16 +4111,16 @@
       <c r="E74" s="9"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="64">
+      <c r="A75" s="63">
         <v>6</v>
       </c>
-      <c r="B75" s="62" t="s">
+      <c r="B75" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C75" s="62" t="s">
+      <c r="C75" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="D75" s="62" t="s">
+      <c r="D75" s="61" t="s">
         <v>19</v>
       </c>
       <c r="E75" s="12" t="s">
@@ -4138,10 +4128,10 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A76" s="65"/>
-      <c r="B76" s="63"/>
-      <c r="C76" s="63"/>
-      <c r="D76" s="63"/>
+      <c r="A76" s="64"/>
+      <c r="B76" s="62"/>
+      <c r="C76" s="62"/>
+      <c r="D76" s="62"/>
       <c r="E76" s="12" t="s">
         <v>31</v>
       </c>
@@ -4299,16 +4289,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="58">
+      <c r="A2" s="57">
         <v>1</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="59" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="14" t="s">
@@ -4319,10 +4309,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="59"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
+      <c r="A3" s="58"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
       <c r="E3" s="15" t="s">
         <v>60</v>
       </c>
@@ -4331,70 +4321,70 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="59"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
       <c r="E4" s="15" t="s">
         <v>64</v>
       </c>
       <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="59"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
       <c r="E5" s="15" t="s">
         <v>65</v>
       </c>
       <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="59"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
+      <c r="A6" s="58"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
       <c r="E6" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="59"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
+      <c r="A7" s="58"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
       <c r="E7" s="15" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
       <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="59"/>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
+      <c r="A8" s="58"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
       <c r="E8" s="15" t="s">
         <v>61</v>
       </c>
       <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="59"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
+      <c r="A9" s="58"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
       <c r="E9" s="15" t="s">
         <v>62</v>
       </c>
       <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="72"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
       <c r="E10" s="15" t="s">
         <v>14</v>
       </c>
@@ -4409,16 +4399,16 @@
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="58">
+      <c r="A12" s="57">
         <v>2</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="60" t="s">
+      <c r="C12" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="59" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="15" t="s">
@@ -4429,40 +4419,40 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="59"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
+      <c r="A13" s="58"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
       <c r="E13" s="15" t="s">
         <v>102</v>
       </c>
       <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="59"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
+      <c r="A14" s="58"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
       <c r="E14" s="15" t="s">
         <v>103</v>
       </c>
       <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="59"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
       <c r="E15" s="15" t="s">
         <v>104</v>
       </c>
       <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="72"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
+      <c r="A16" s="71"/>
+      <c r="B16" s="72"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="72"/>
       <c r="E16" s="11" t="s">
         <v>51</v>
       </c>
@@ -4477,16 +4467,16 @@
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="58">
+      <c r="A18" s="57">
         <v>3</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="60" t="s">
+      <c r="C18" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="60" t="s">
+      <c r="D18" s="59" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="15" t="s">
@@ -4497,50 +4487,50 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="59"/>
-      <c r="B19" s="61"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
+      <c r="A19" s="58"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
       <c r="E19" s="15" t="s">
         <v>102</v>
       </c>
       <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="59"/>
-      <c r="B20" s="61"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
+      <c r="A20" s="58"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
       <c r="E20" s="15" t="s">
         <v>106</v>
       </c>
       <c r="F20" s="21"/>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="59"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="60"/>
       <c r="E21" s="15" t="s">
         <v>107</v>
       </c>
       <c r="F21" s="21"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="59"/>
-      <c r="B22" s="61"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
+      <c r="A22" s="58"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
       <c r="E22" s="15" t="s">
         <v>109</v>
       </c>
       <c r="F22" s="21"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="59"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="61"/>
+      <c r="A23" s="58"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
       <c r="E23" s="15" t="s">
         <v>108</v>
       </c>
@@ -4555,16 +4545,16 @@
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="58">
+      <c r="A25" s="57">
         <v>4</v>
       </c>
-      <c r="B25" s="60" t="s">
+      <c r="B25" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="60" t="s">
+      <c r="C25" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="60" t="s">
+      <c r="D25" s="59" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="15" t="s">
@@ -4573,10 +4563,10 @@
       <c r="F25" s="21"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="59"/>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
+      <c r="A26" s="58"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="60"/>
       <c r="E26" s="15" t="s">
         <v>111</v>
       </c>
@@ -4591,16 +4581,16 @@
       <c r="F27" s="7"/>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="58">
+      <c r="A28" s="57">
         <v>5</v>
       </c>
-      <c r="B28" s="60" t="s">
+      <c r="B28" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="60" t="s">
+      <c r="C28" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="60" t="s">
+      <c r="D28" s="59" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="15" t="s">
@@ -4611,10 +4601,10 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="59"/>
-      <c r="B29" s="61"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="61"/>
+      <c r="A29" s="58"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="60"/>
       <c r="E29" s="15" t="s">
         <v>17</v>
       </c>
@@ -4629,16 +4619,16 @@
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="58">
+      <c r="A31" s="57">
         <v>6</v>
       </c>
-      <c r="B31" s="60" t="s">
+      <c r="B31" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="60" t="s">
+      <c r="C31" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="D31" s="60" t="s">
+      <c r="D31" s="59" t="s">
         <v>43</v>
       </c>
       <c r="E31" s="14" t="s">
@@ -4649,30 +4639,30 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="59"/>
-      <c r="B32" s="61"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61"/>
+      <c r="A32" s="58"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="60"/>
       <c r="E32" s="15" t="s">
         <v>116</v>
       </c>
       <c r="F32" s="21"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="59"/>
-      <c r="B33" s="61"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
       <c r="E33" s="15" t="s">
         <v>114</v>
       </c>
       <c r="F33" s="21"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="72"/>
-      <c r="B34" s="73"/>
-      <c r="C34" s="73"/>
-      <c r="D34" s="73"/>
+      <c r="A34" s="71"/>
+      <c r="B34" s="72"/>
+      <c r="C34" s="72"/>
+      <c r="D34" s="72"/>
       <c r="E34" s="15" t="s">
         <v>22</v>
       </c>
@@ -4687,16 +4677,16 @@
       <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="58">
+      <c r="A36" s="57">
         <v>7</v>
       </c>
-      <c r="B36" s="60" t="s">
+      <c r="B36" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="60" t="s">
+      <c r="C36" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="60" t="s">
+      <c r="D36" s="59" t="s">
         <v>24</v>
       </c>
       <c r="E36" s="15" t="s">
@@ -4705,20 +4695,20 @@
       <c r="F36" s="21"/>
     </row>
     <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="59"/>
-      <c r="B37" s="61"/>
-      <c r="C37" s="61"/>
-      <c r="D37" s="61"/>
+      <c r="A37" s="58"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="60"/>
       <c r="E37" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F37" s="21"/>
     </row>
     <row r="38" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="72"/>
-      <c r="B38" s="73"/>
-      <c r="C38" s="73"/>
-      <c r="D38" s="73"/>
+      <c r="A38" s="71"/>
+      <c r="B38" s="72"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="72"/>
       <c r="E38" s="15" t="s">
         <v>36</v>
       </c>
@@ -4733,16 +4723,16 @@
       <c r="F39" s="7"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="58">
+      <c r="A40" s="57">
         <v>8</v>
       </c>
-      <c r="B40" s="60" t="s">
+      <c r="B40" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="60" t="s">
-        <v>149</v>
-      </c>
-      <c r="D40" s="60" t="s">
+      <c r="C40" s="59" t="s">
+        <v>148</v>
+      </c>
+      <c r="D40" s="59" t="s">
         <v>117</v>
       </c>
       <c r="E40" s="21" t="s">
@@ -4751,70 +4741,70 @@
       <c r="F40" s="21"/>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="59"/>
-      <c r="B41" s="61"/>
-      <c r="C41" s="61"/>
-      <c r="D41" s="61"/>
+      <c r="A41" s="58"/>
+      <c r="B41" s="60"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
       <c r="E41" s="21" t="s">
         <v>119</v>
       </c>
       <c r="F41" s="21"/>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="59"/>
-      <c r="B42" s="61"/>
-      <c r="C42" s="61"/>
-      <c r="D42" s="61"/>
+      <c r="A42" s="58"/>
+      <c r="B42" s="60"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="60"/>
       <c r="E42" s="21" t="s">
         <v>120</v>
       </c>
       <c r="F42" s="21"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="59"/>
-      <c r="B43" s="61"/>
-      <c r="C43" s="61"/>
-      <c r="D43" s="61"/>
+      <c r="A43" s="58"/>
+      <c r="B43" s="60"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="60"/>
       <c r="E43" s="21" t="s">
         <v>121</v>
       </c>
       <c r="F43" s="21"/>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="59"/>
-      <c r="B44" s="61"/>
-      <c r="C44" s="61"/>
-      <c r="D44" s="61"/>
+      <c r="A44" s="58"/>
+      <c r="B44" s="60"/>
+      <c r="C44" s="60"/>
+      <c r="D44" s="60"/>
       <c r="E44" s="21" t="s">
         <v>123</v>
       </c>
       <c r="F44" s="21"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="59"/>
-      <c r="B45" s="61"/>
-      <c r="C45" s="61"/>
-      <c r="D45" s="61"/>
+      <c r="A45" s="58"/>
+      <c r="B45" s="60"/>
+      <c r="C45" s="60"/>
+      <c r="D45" s="60"/>
       <c r="E45" s="21" t="s">
         <v>124</v>
       </c>
       <c r="F45" s="21"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="59"/>
-      <c r="B46" s="61"/>
-      <c r="C46" s="61"/>
-      <c r="D46" s="61"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="60"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
       <c r="E46" s="21" t="s">
         <v>122</v>
       </c>
       <c r="F46" s="21"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="59"/>
-      <c r="B47" s="61"/>
-      <c r="C47" s="61"/>
-      <c r="D47" s="61"/>
+      <c r="A47" s="58"/>
+      <c r="B47" s="60"/>
+      <c r="C47" s="60"/>
+      <c r="D47" s="60"/>
       <c r="E47" s="14" t="s">
         <v>75</v>
       </c>
@@ -4871,8 +4861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD0B509-A153-4B31-95B8-BC32DC1B6A3B}">
   <dimension ref="B2:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4898,293 +4888,295 @@
         <v>127</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H2" s="43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J2" s="43" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="35" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="J3" s="35" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J4" s="36" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H5" s="36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J5" s="36" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J6" s="36" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="39"/>
       <c r="D7" s="36"/>
       <c r="F7" s="39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H7" s="37"/>
       <c r="J7" s="39"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>205</v>
+      </c>
+      <c r="H8" s="40" t="s">
+        <v>210</v>
+      </c>
+      <c r="J8" s="40"/>
+    </row>
+    <row r="9" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B9" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>204</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="J9" s="39" t="s">
         <v>228</v>
       </c>
-      <c r="D8" s="35" t="s">
-        <v>227</v>
-      </c>
-      <c r="F8" s="40" t="s">
-        <v>224</v>
-      </c>
-      <c r="H8" s="40" t="s">
-        <v>229</v>
-      </c>
-      <c r="J8" s="40"/>
-    </row>
-    <row r="9" spans="2:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B9" s="34" t="s">
-        <v>252</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>253</v>
-      </c>
-      <c r="F9" s="36" t="s">
-        <v>223</v>
-      </c>
-      <c r="H9" s="36" t="s">
-        <v>254</v>
-      </c>
-      <c r="J9" s="39" t="s">
-        <v>248</v>
-      </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="38"/>
       <c r="D10" s="36"/>
       <c r="F10" s="36" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="H10" s="36" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="81" t="s">
-        <v>239</v>
-      </c>
-      <c r="D11" s="82" t="s">
-        <v>148</v>
+      <c r="B11" s="80" t="s">
+        <v>219</v>
+      </c>
+      <c r="D11" s="80" t="s">
+        <v>147</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="H11" s="38" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="81"/>
-      <c r="D12" s="82"/>
+      <c r="B12" s="80"/>
+      <c r="D12" s="80"/>
       <c r="F12" s="38" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="H12" s="38" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="J12" s="55" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="34" t="s">
-        <v>237</v>
+      <c r="B13" s="36" t="s">
+        <v>218</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="F13" s="38"/>
       <c r="H13" s="38" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="32" t="s">
-        <v>262</v>
+      <c r="B14" s="38" t="s">
+        <v>242</v>
       </c>
       <c r="D14" s="56" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="F14" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="H14" s="38" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="86" t="s">
+        <v>222</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>220</v>
+      </c>
+      <c r="F15" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="H14" s="38" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="57" t="s">
-        <v>242</v>
-      </c>
-      <c r="D15" s="36" t="s">
-        <v>240</v>
-      </c>
-      <c r="F15" s="38" t="s">
-        <v>134</v>
-      </c>
       <c r="H15" s="38" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B16" s="32" t="s">
-        <v>128</v>
-      </c>
+      <c r="B16" s="86"/>
       <c r="D16" s="36"/>
       <c r="F16" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="H16" s="38" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="F17" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="H16" s="38" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B17" s="32" t="s">
+      <c r="H17" s="39" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="D18" s="38" t="s">
+        <v>237</v>
+      </c>
+      <c r="F18" s="38" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="38" t="s">
+        <v>241</v>
+      </c>
+      <c r="D19" s="38" t="s">
         <v>238</v>
       </c>
-      <c r="D17" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="F17" s="38" t="s">
-        <v>136</v>
-      </c>
-      <c r="H17" s="39" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D18" s="38" t="s">
-        <v>257</v>
-      </c>
-      <c r="F18" s="38" t="s">
+      <c r="F19" s="38" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="32" t="s">
-        <v>264</v>
-      </c>
-      <c r="D19" s="38" t="s">
-        <v>258</v>
-      </c>
-      <c r="F19" s="38" t="s">
+      <c r="H19" s="55" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="80" t="s">
+        <v>239</v>
+      </c>
+      <c r="D20" s="80" t="s">
+        <v>239</v>
+      </c>
+      <c r="F20" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="H19" s="55" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B20" s="32" t="s">
-        <v>260</v>
-      </c>
-      <c r="D20" s="82" t="s">
-        <v>259</v>
-      </c>
-      <c r="F20" s="38" t="s">
+    </row>
+    <row r="21" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="80"/>
+      <c r="D21" s="80"/>
+      <c r="F21" s="38" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="32" t="s">
-        <v>261</v>
-      </c>
-      <c r="D21" s="83"/>
-      <c r="F21" s="38" t="s">
+    <row r="22" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="39" t="s">
+        <v>246</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="F22" s="38" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="81" t="s">
-        <v>259</v>
-      </c>
-      <c r="F22" s="38" t="s">
-        <v>141</v>
-      </c>
-    </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B23" s="81"/>
-      <c r="D23" s="55" t="s">
-        <v>226</v>
-      </c>
       <c r="F23" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B24" s="32" t="s">
-        <v>266</v>
+      <c r="B24" s="55" t="s">
+        <v>207</v>
+      </c>
+      <c r="D24" s="55" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="F25" s="55" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -5192,7 +5184,7 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B20:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5200,25 +5192,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E08554-D8B2-4838-942A-41D15992982E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A678BF3-4A56-4A1E-B2DF-017A74834050}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5234,25 +5212,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="87"/>
-      <c r="B1" s="88" t="s">
-        <v>168</v>
-      </c>
-      <c r="C1" s="88"/>
+      <c r="A1" s="84"/>
+      <c r="B1" s="85" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" s="85"/>
       <c r="D1" s="47"/>
-      <c r="E1" s="88" t="s">
-        <v>169</v>
-      </c>
-      <c r="F1" s="88"/>
+      <c r="E1" s="85" t="s">
+        <v>255</v>
+      </c>
+      <c r="F1" s="85"/>
       <c r="G1" s="47"/>
-      <c r="H1" s="88" t="s">
-        <v>170</v>
-      </c>
-      <c r="I1" s="88"/>
-      <c r="J1" s="87"/>
+      <c r="H1" s="85" t="s">
+        <v>254</v>
+      </c>
+      <c r="I1" s="85"/>
+      <c r="J1" s="84"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="87"/>
+      <c r="A2" s="84"/>
       <c r="B2" s="51"/>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
@@ -5261,100 +5239,100 @@
       <c r="G2" s="46"/>
       <c r="H2" s="46"/>
       <c r="I2" s="46"/>
-      <c r="J2" s="87"/>
+      <c r="J2" s="84"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="87"/>
+      <c r="A3" s="84"/>
       <c r="B3" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="D3" s="81"/>
+      <c r="E3" s="48" t="s">
+        <v>162</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="G3" s="81"/>
+      <c r="H3" s="48" t="s">
+        <v>162</v>
+      </c>
+      <c r="I3" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="J3" s="84"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="84"/>
+      <c r="B4" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="48" t="s">
-        <v>163</v>
-      </c>
-      <c r="F3" s="48" t="s">
+      <c r="C4" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="D4" s="82"/>
+      <c r="E4" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="G3" s="84"/>
-      <c r="H3" s="48" t="s">
-        <v>163</v>
-      </c>
-      <c r="I3" s="48" t="s">
+      <c r="F4" s="48" t="s">
+        <v>178</v>
+      </c>
+      <c r="G4" s="82"/>
+      <c r="H4" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="J3" s="87"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="87"/>
-      <c r="B4" s="50" t="s">
+      <c r="I4" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="J4" s="84"/>
+    </row>
+    <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="84"/>
+      <c r="B5" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="C4" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="D4" s="85"/>
-      <c r="E4" s="48" t="s">
+      <c r="C5" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="D5" s="82"/>
+      <c r="E5" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="F4" s="48" t="s">
-        <v>181</v>
-      </c>
-      <c r="G4" s="85"/>
-      <c r="H4" s="48" t="s">
+      <c r="F5" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="G5" s="82"/>
+      <c r="H5" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="I4" s="48" t="s">
-        <v>182</v>
-      </c>
-      <c r="J4" s="87"/>
-    </row>
-    <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="87"/>
-      <c r="B5" s="50" t="s">
+      <c r="I5" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="J5" s="84"/>
+    </row>
+    <row r="6" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="84"/>
+      <c r="B6" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="C5" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="48" t="s">
+      <c r="C6" s="48"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="F5" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="G5" s="85"/>
-      <c r="H5" s="48" t="s">
+      <c r="F6" s="48"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="I5" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="J5" s="87"/>
-    </row>
-    <row r="6" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="87"/>
-      <c r="B6" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="F6" s="48"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="48" t="s">
-        <v>167</v>
-      </c>
       <c r="I6" s="48"/>
-      <c r="J6" s="87"/>
+      <c r="J6" s="84"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="87"/>
+      <c r="A7" s="84"/>
       <c r="B7" s="52"/>
       <c r="C7" s="49"/>
       <c r="D7" s="49"/>
@@ -5363,100 +5341,100 @@
       <c r="G7" s="49"/>
       <c r="H7" s="49"/>
       <c r="I7" s="49"/>
-      <c r="J7" s="87"/>
+      <c r="J7" s="84"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="87"/>
+      <c r="A8" s="84"/>
       <c r="B8" s="50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="D8" s="84"/>
+        <v>168</v>
+      </c>
+      <c r="D8" s="81"/>
       <c r="E8" s="48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F8" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="G8" s="84"/>
+        <v>168</v>
+      </c>
+      <c r="G8" s="81"/>
       <c r="H8" s="48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I8" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="J8" s="87"/>
+        <v>168</v>
+      </c>
+      <c r="J8" s="84"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="87"/>
+      <c r="A9" s="84"/>
       <c r="B9" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="D9" s="82"/>
+      <c r="E9" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F9" s="48" t="s">
+        <v>178</v>
+      </c>
+      <c r="G9" s="82"/>
+      <c r="H9" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="I9" s="48" t="s">
+        <v>195</v>
+      </c>
+      <c r="J9" s="84"/>
+    </row>
+    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="84"/>
+      <c r="B10" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="C9" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="D9" s="85"/>
-      <c r="E9" s="48" t="s">
+      <c r="C10" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="D10" s="82"/>
+      <c r="E10" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="F9" s="48" t="s">
-        <v>181</v>
-      </c>
-      <c r="G9" s="85"/>
-      <c r="H9" s="48" t="s">
+      <c r="F10" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="G10" s="82"/>
+      <c r="H10" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="I9" s="48" t="s">
-        <v>202</v>
-      </c>
-      <c r="J9" s="87"/>
-    </row>
-    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="87"/>
-      <c r="B10" s="50" t="s">
+      <c r="I10" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="J10" s="84"/>
+    </row>
+    <row r="11" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="84"/>
+      <c r="B11" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="D10" s="85"/>
-      <c r="E10" s="48" t="s">
+      <c r="C11" s="48"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="F10" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="G10" s="85"/>
-      <c r="H10" s="48" t="s">
+      <c r="F11" s="48"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="I10" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="J10" s="87"/>
-    </row>
-    <row r="11" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="87"/>
-      <c r="B11" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="F11" s="48"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="48" t="s">
-        <v>167</v>
-      </c>
       <c r="I11" s="48"/>
-      <c r="J11" s="87"/>
+      <c r="J11" s="84"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="87"/>
+      <c r="A12" s="84"/>
       <c r="B12" s="52"/>
       <c r="C12" s="49"/>
       <c r="D12" s="49"/>
@@ -5465,92 +5443,92 @@
       <c r="G12" s="49"/>
       <c r="H12" s="49"/>
       <c r="I12" s="49"/>
-      <c r="J12" s="87"/>
+      <c r="J12" s="84"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="87"/>
+      <c r="A13" s="84"/>
       <c r="B13" s="50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="D13" s="84"/>
+        <v>169</v>
+      </c>
+      <c r="D13" s="81"/>
       <c r="E13" s="48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F13" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="G13" s="84"/>
+        <v>169</v>
+      </c>
+      <c r="G13" s="81"/>
       <c r="H13" s="48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I13" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="J13" s="87"/>
+        <v>169</v>
+      </c>
+      <c r="J13" s="84"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="87"/>
+      <c r="A14" s="84"/>
       <c r="B14" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="D14" s="82"/>
+      <c r="E14" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F14" s="48"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="I14" s="48"/>
+      <c r="J14" s="84"/>
+    </row>
+    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="84"/>
+      <c r="B15" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="C14" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="D14" s="85"/>
-      <c r="E14" s="48" t="s">
+      <c r="C15" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="D15" s="82"/>
+      <c r="E15" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="F14" s="48"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="48" t="s">
+      <c r="F15" s="21"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="I14" s="48"/>
-      <c r="J14" s="87"/>
-    </row>
-    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="87"/>
-      <c r="B15" s="50" t="s">
+      <c r="I15" s="21"/>
+      <c r="J15" s="84"/>
+    </row>
+    <row r="16" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="84"/>
+      <c r="B16" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="D15" s="85"/>
-      <c r="E15" s="48" t="s">
+      <c r="C16" s="48"/>
+      <c r="D16" s="83"/>
+      <c r="E16" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="48" t="s">
+      <c r="F16" s="48"/>
+      <c r="G16" s="83"/>
+      <c r="H16" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="I15" s="21"/>
-      <c r="J15" s="87"/>
-    </row>
-    <row r="16" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="87"/>
-      <c r="B16" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="86"/>
-      <c r="E16" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="F16" s="48"/>
-      <c r="G16" s="86"/>
-      <c r="H16" s="48" t="s">
-        <v>167</v>
-      </c>
       <c r="I16" s="48"/>
-      <c r="J16" s="87"/>
+      <c r="J16" s="84"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="87"/>
+      <c r="A17" s="84"/>
       <c r="B17" s="52"/>
       <c r="C17" s="49"/>
       <c r="D17" s="49"/>
@@ -5559,100 +5537,100 @@
       <c r="G17" s="49"/>
       <c r="H17" s="49"/>
       <c r="I17" s="49"/>
-      <c r="J17" s="87"/>
+      <c r="J17" s="84"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="87"/>
+      <c r="A18" s="84"/>
       <c r="B18" s="50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>173</v>
-      </c>
-      <c r="D18" s="84"/>
+        <v>170</v>
+      </c>
+      <c r="D18" s="81"/>
       <c r="E18" s="48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F18" s="48" t="s">
-        <v>173</v>
-      </c>
-      <c r="G18" s="84"/>
+        <v>170</v>
+      </c>
+      <c r="G18" s="81"/>
       <c r="H18" s="48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I18" s="48" t="s">
-        <v>173</v>
-      </c>
-      <c r="J18" s="87"/>
+        <v>170</v>
+      </c>
+      <c r="J18" s="84"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="87"/>
+      <c r="A19" s="84"/>
       <c r="B19" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="D19" s="82"/>
+      <c r="E19" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F19" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="G19" s="82"/>
+      <c r="H19" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="I19" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="J19" s="84"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="84"/>
+      <c r="B20" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="C19" s="48" t="s">
-        <v>183</v>
-      </c>
-      <c r="D19" s="85"/>
-      <c r="E19" s="48" t="s">
+      <c r="C20" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="D20" s="82"/>
+      <c r="E20" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="F19" s="48" t="s">
-        <v>183</v>
-      </c>
-      <c r="G19" s="85"/>
-      <c r="H19" s="48" t="s">
+      <c r="F20" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="G20" s="82"/>
+      <c r="H20" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="I19" s="48" t="s">
-        <v>183</v>
-      </c>
-      <c r="J19" s="87"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="87"/>
-      <c r="B20" s="50" t="s">
+      <c r="I20" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="J20" s="84"/>
+    </row>
+    <row r="21" spans="1:10" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="84"/>
+      <c r="B21" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="C20" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="D20" s="85"/>
-      <c r="E20" s="48" t="s">
+      <c r="C21" s="48"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="F20" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="G20" s="85"/>
-      <c r="H20" s="48" t="s">
+      <c r="F21" s="48"/>
+      <c r="G21" s="83"/>
+      <c r="H21" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="I20" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="J20" s="87"/>
-    </row>
-    <row r="21" spans="1:10" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="87"/>
-      <c r="B21" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="F21" s="48"/>
-      <c r="G21" s="86"/>
-      <c r="H21" s="48" t="s">
-        <v>167</v>
-      </c>
       <c r="I21" s="48"/>
-      <c r="J21" s="87"/>
+      <c r="J21" s="84"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="87"/>
+      <c r="A22" s="84"/>
       <c r="B22" s="52"/>
       <c r="C22" s="49"/>
       <c r="D22" s="49"/>
@@ -5661,100 +5639,100 @@
       <c r="G22" s="49"/>
       <c r="H22" s="49"/>
       <c r="I22" s="49"/>
-      <c r="J22" s="87"/>
+      <c r="J22" s="84"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="87"/>
+      <c r="A23" s="84"/>
       <c r="B23" s="50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>174</v>
-      </c>
-      <c r="D23" s="84"/>
+        <v>171</v>
+      </c>
+      <c r="D23" s="81"/>
       <c r="E23" s="48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F23" s="48" t="s">
-        <v>174</v>
-      </c>
-      <c r="G23" s="84"/>
+        <v>171</v>
+      </c>
+      <c r="G23" s="81"/>
       <c r="H23" s="48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I23" s="48" t="s">
-        <v>174</v>
-      </c>
-      <c r="J23" s="87"/>
+        <v>171</v>
+      </c>
+      <c r="J23" s="84"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="87"/>
+      <c r="A24" s="84"/>
       <c r="B24" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="C24" s="48" t="s">
+        <v>186</v>
+      </c>
+      <c r="D24" s="82"/>
+      <c r="E24" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F24" s="48" t="s">
+        <v>199</v>
+      </c>
+      <c r="G24" s="82"/>
+      <c r="H24" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="I24" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="J24" s="84"/>
+    </row>
+    <row r="25" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="84"/>
+      <c r="B25" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="C24" s="48" t="s">
-        <v>192</v>
-      </c>
-      <c r="D24" s="85"/>
-      <c r="E24" s="48" t="s">
+      <c r="C25" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="D25" s="82"/>
+      <c r="E25" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="F24" s="48" t="s">
-        <v>212</v>
-      </c>
-      <c r="G24" s="85"/>
-      <c r="H24" s="48" t="s">
+      <c r="F25" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="G25" s="82"/>
+      <c r="H25" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="I24" s="48" t="s">
-        <v>203</v>
-      </c>
-      <c r="J24" s="87"/>
-    </row>
-    <row r="25" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="87"/>
-      <c r="B25" s="50" t="s">
+      <c r="I25" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="J25" s="84"/>
+    </row>
+    <row r="26" spans="1:10" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="84"/>
+      <c r="B26" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="C25" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="D25" s="85"/>
-      <c r="E25" s="48" t="s">
+      <c r="C26" s="48"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="F25" s="21" t="s">
-        <v>213</v>
-      </c>
-      <c r="G25" s="85"/>
-      <c r="H25" s="48" t="s">
+      <c r="F26" s="48"/>
+      <c r="G26" s="83"/>
+      <c r="H26" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="I25" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="J25" s="87"/>
-    </row>
-    <row r="26" spans="1:10" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="87"/>
-      <c r="B26" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="C26" s="48"/>
-      <c r="D26" s="86"/>
-      <c r="E26" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="F26" s="48"/>
-      <c r="G26" s="86"/>
-      <c r="H26" s="48" t="s">
-        <v>167</v>
-      </c>
       <c r="I26" s="48"/>
-      <c r="J26" s="87"/>
+      <c r="J26" s="84"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="87"/>
+      <c r="A27" s="84"/>
       <c r="B27" s="52"/>
       <c r="C27" s="49"/>
       <c r="D27" s="49"/>
@@ -5763,100 +5741,100 @@
       <c r="G27" s="49"/>
       <c r="H27" s="49"/>
       <c r="I27" s="49"/>
-      <c r="J27" s="87"/>
+      <c r="J27" s="84"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="87"/>
+      <c r="A28" s="84"/>
       <c r="B28" s="50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C28" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="D28" s="84"/>
+        <v>172</v>
+      </c>
+      <c r="D28" s="81"/>
       <c r="E28" s="48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F28" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="G28" s="84"/>
+        <v>172</v>
+      </c>
+      <c r="G28" s="81"/>
       <c r="H28" s="48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I28" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="J28" s="87"/>
+        <v>172</v>
+      </c>
+      <c r="J28" s="84"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="87"/>
+      <c r="A29" s="84"/>
       <c r="B29" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="C29" s="48" t="s">
+        <v>187</v>
+      </c>
+      <c r="D29" s="82"/>
+      <c r="E29" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F29" s="48" t="s">
+        <v>200</v>
+      </c>
+      <c r="G29" s="82"/>
+      <c r="H29" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="I29" s="48" t="s">
+        <v>197</v>
+      </c>
+      <c r="J29" s="84"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="84"/>
+      <c r="B30" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="C29" s="48" t="s">
-        <v>193</v>
-      </c>
-      <c r="D29" s="85"/>
-      <c r="E29" s="48" t="s">
+      <c r="C30" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="D30" s="82"/>
+      <c r="E30" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="F29" s="48" t="s">
-        <v>214</v>
-      </c>
-      <c r="G29" s="85"/>
-      <c r="H29" s="48" t="s">
+      <c r="F30" s="48" t="s">
+        <v>259</v>
+      </c>
+      <c r="G30" s="82"/>
+      <c r="H30" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="I29" s="48" t="s">
-        <v>205</v>
-      </c>
-      <c r="J29" s="87"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="87"/>
-      <c r="B30" s="50" t="s">
+      <c r="I30" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="J30" s="84"/>
+    </row>
+    <row r="31" spans="1:10" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="84"/>
+      <c r="B31" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="C30" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="D30" s="85"/>
-      <c r="E30" s="48" t="s">
+      <c r="C31" s="48"/>
+      <c r="D31" s="83"/>
+      <c r="E31" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="F30" s="48" t="s">
-        <v>215</v>
-      </c>
-      <c r="G30" s="85"/>
-      <c r="H30" s="48" t="s">
+      <c r="F31" s="48"/>
+      <c r="G31" s="83"/>
+      <c r="H31" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="I30" s="48" t="s">
-        <v>206</v>
-      </c>
-      <c r="J30" s="87"/>
-    </row>
-    <row r="31" spans="1:10" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="87"/>
-      <c r="B31" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="C31" s="48"/>
-      <c r="D31" s="86"/>
-      <c r="E31" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="F31" s="48"/>
-      <c r="G31" s="86"/>
-      <c r="H31" s="48" t="s">
-        <v>167</v>
-      </c>
       <c r="I31" s="48"/>
-      <c r="J31" s="87"/>
+      <c r="J31" s="84"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" s="87"/>
+      <c r="A32" s="84"/>
       <c r="B32" s="52"/>
       <c r="C32" s="49"/>
       <c r="D32" s="49"/>
@@ -5865,100 +5843,100 @@
       <c r="G32" s="49"/>
       <c r="H32" s="49"/>
       <c r="I32" s="49"/>
-      <c r="J32" s="87"/>
+      <c r="J32" s="84"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="87"/>
+      <c r="A33" s="84"/>
       <c r="B33" s="50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C33" s="48" t="s">
-        <v>174</v>
-      </c>
-      <c r="D33" s="84"/>
+        <v>171</v>
+      </c>
+      <c r="D33" s="81"/>
       <c r="E33" s="48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F33" s="48" t="s">
-        <v>174</v>
-      </c>
-      <c r="G33" s="84"/>
+        <v>171</v>
+      </c>
+      <c r="G33" s="81"/>
       <c r="H33" s="48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I33" s="48" t="s">
-        <v>174</v>
-      </c>
-      <c r="J33" s="87"/>
+        <v>171</v>
+      </c>
+      <c r="J33" s="84"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="87"/>
+      <c r="A34" s="84"/>
       <c r="B34" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="C34" s="48" t="s">
+        <v>189</v>
+      </c>
+      <c r="D34" s="82"/>
+      <c r="E34" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F34" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G34" s="82"/>
+      <c r="H34" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="I34" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="J34" s="84"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35" s="84"/>
+      <c r="B35" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="C34" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="D34" s="85"/>
-      <c r="E34" s="48" t="s">
+      <c r="C35" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="D35" s="82"/>
+      <c r="E35" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="F34" s="48" t="s">
-        <v>178</v>
-      </c>
-      <c r="G34" s="85"/>
-      <c r="H34" s="48" t="s">
+      <c r="F35" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="G35" s="82"/>
+      <c r="H35" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="I34" s="48" t="s">
-        <v>179</v>
-      </c>
-      <c r="J34" s="87"/>
-    </row>
-    <row r="35" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="87"/>
-      <c r="B35" s="50" t="s">
+      <c r="I35" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="J35" s="84"/>
+    </row>
+    <row r="36" spans="1:10" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="84"/>
+      <c r="B36" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="C35" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="D35" s="85"/>
-      <c r="E35" s="48" t="s">
+      <c r="C36" s="48"/>
+      <c r="D36" s="83"/>
+      <c r="E36" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="F35" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="G35" s="85"/>
-      <c r="H35" s="48" t="s">
+      <c r="F36" s="48"/>
+      <c r="G36" s="83"/>
+      <c r="H36" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="I35" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="J35" s="87"/>
-    </row>
-    <row r="36" spans="1:10" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="87"/>
-      <c r="B36" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="C36" s="48"/>
-      <c r="D36" s="86"/>
-      <c r="E36" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="F36" s="48"/>
-      <c r="G36" s="86"/>
-      <c r="H36" s="48" t="s">
-        <v>167</v>
-      </c>
       <c r="I36" s="48"/>
-      <c r="J36" s="87"/>
+      <c r="J36" s="84"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A37" s="87"/>
+      <c r="A37" s="84"/>
       <c r="B37" s="52"/>
       <c r="C37" s="49"/>
       <c r="D37" s="54"/>
@@ -5967,100 +5945,100 @@
       <c r="G37" s="49"/>
       <c r="H37" s="49"/>
       <c r="I37" s="49"/>
-      <c r="J37" s="87"/>
+      <c r="J37" s="84"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="87"/>
+      <c r="A38" s="84"/>
       <c r="B38" s="50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C38" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="D38" s="84"/>
+        <v>172</v>
+      </c>
+      <c r="D38" s="81"/>
       <c r="E38" s="48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F38" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="G38" s="84"/>
+        <v>172</v>
+      </c>
+      <c r="G38" s="81"/>
       <c r="H38" s="48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I38" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="J38" s="87"/>
+        <v>172</v>
+      </c>
+      <c r="J38" s="84"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" s="87"/>
+      <c r="A39" s="84"/>
       <c r="B39" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="C39" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="D39" s="82"/>
+      <c r="E39" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F39" s="48" t="s">
+        <v>201</v>
+      </c>
+      <c r="G39" s="82"/>
+      <c r="H39" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="I39" s="48" t="s">
+        <v>198</v>
+      </c>
+      <c r="J39" s="84"/>
+    </row>
+    <row r="40" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="84"/>
+      <c r="B40" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="C39" s="48" t="s">
-        <v>177</v>
-      </c>
-      <c r="D39" s="85"/>
-      <c r="E39" s="48" t="s">
+      <c r="C40" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="D40" s="82"/>
+      <c r="E40" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="F39" s="48" t="s">
-        <v>217</v>
-      </c>
-      <c r="G39" s="85"/>
-      <c r="H39" s="48" t="s">
+      <c r="F40" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="G40" s="82"/>
+      <c r="H40" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="I39" s="48" t="s">
-        <v>208</v>
-      </c>
-      <c r="J39" s="87"/>
-    </row>
-    <row r="40" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="87"/>
-      <c r="B40" s="50" t="s">
+      <c r="I40" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="J40" s="84"/>
+    </row>
+    <row r="41" spans="1:10" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="84"/>
+      <c r="B41" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="C40" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="D40" s="85"/>
-      <c r="E40" s="48" t="s">
+      <c r="C41" s="48"/>
+      <c r="D41" s="83"/>
+      <c r="E41" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="F40" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="G40" s="85"/>
-      <c r="H40" s="48" t="s">
+      <c r="F41" s="48"/>
+      <c r="G41" s="83"/>
+      <c r="H41" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="I40" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="J40" s="87"/>
-    </row>
-    <row r="41" spans="1:10" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="87"/>
-      <c r="B41" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="C41" s="48"/>
-      <c r="D41" s="86"/>
-      <c r="E41" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="F41" s="48"/>
-      <c r="G41" s="86"/>
-      <c r="H41" s="48" t="s">
-        <v>167</v>
-      </c>
       <c r="I41" s="48"/>
-      <c r="J41" s="87"/>
+      <c r="J41" s="84"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A42" s="87"/>
+      <c r="A42" s="84"/>
       <c r="B42" s="52"/>
       <c r="C42" s="49"/>
       <c r="D42" s="49"/>
@@ -6069,100 +6047,100 @@
       <c r="G42" s="49"/>
       <c r="H42" s="49"/>
       <c r="I42" s="49"/>
-      <c r="J42" s="87"/>
+      <c r="J42" s="84"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A43" s="87"/>
+      <c r="A43" s="84"/>
       <c r="B43" s="50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C43" s="48" t="s">
-        <v>176</v>
-      </c>
-      <c r="D43" s="84"/>
+        <v>173</v>
+      </c>
+      <c r="D43" s="81"/>
       <c r="E43" s="50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F43" s="48" t="s">
-        <v>176</v>
-      </c>
-      <c r="G43" s="84"/>
+        <v>173</v>
+      </c>
+      <c r="G43" s="81"/>
       <c r="H43" s="50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I43" s="48" t="s">
-        <v>176</v>
-      </c>
-      <c r="J43" s="87"/>
+        <v>173</v>
+      </c>
+      <c r="J43" s="84"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A44" s="87"/>
+      <c r="A44" s="84"/>
       <c r="B44" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="C44" s="48" t="s">
+        <v>192</v>
+      </c>
+      <c r="D44" s="82"/>
+      <c r="E44" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="F44" s="48" t="s">
+        <v>202</v>
+      </c>
+      <c r="G44" s="82"/>
+      <c r="H44" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="I44" s="48" t="s">
+        <v>193</v>
+      </c>
+      <c r="J44" s="84"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A45" s="84"/>
+      <c r="B45" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="C44" s="48" t="s">
-        <v>198</v>
-      </c>
-      <c r="D44" s="85"/>
-      <c r="E44" s="50" t="s">
+      <c r="C45" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="D45" s="82"/>
+      <c r="E45" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="F44" s="48" t="s">
-        <v>219</v>
-      </c>
-      <c r="G44" s="85"/>
-      <c r="H44" s="50" t="s">
+      <c r="F45" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="G45" s="82"/>
+      <c r="H45" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="I44" s="48" t="s">
-        <v>199</v>
-      </c>
-      <c r="J44" s="87"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A45" s="87"/>
-      <c r="B45" s="50" t="s">
+      <c r="I45" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="J45" s="84"/>
+    </row>
+    <row r="46" spans="1:10" ht="88" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="84"/>
+      <c r="B46" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="C45" s="21" t="s">
-        <v>200</v>
-      </c>
-      <c r="D45" s="85"/>
-      <c r="E45" s="50" t="s">
+      <c r="C46" s="48"/>
+      <c r="D46" s="83"/>
+      <c r="E46" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="F45" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="G45" s="85"/>
-      <c r="H45" s="50" t="s">
+      <c r="F46" s="48"/>
+      <c r="G46" s="83"/>
+      <c r="H46" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="I45" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="J45" s="87"/>
-    </row>
-    <row r="46" spans="1:10" ht="88" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="87"/>
-      <c r="B46" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="C46" s="48"/>
-      <c r="D46" s="86"/>
-      <c r="E46" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="F46" s="48"/>
-      <c r="G46" s="86"/>
-      <c r="H46" s="50" t="s">
-        <v>167</v>
-      </c>
       <c r="I46" s="48"/>
-      <c r="J46" s="87"/>
+      <c r="J46" s="84"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A47" s="87"/>
+      <c r="A47" s="84"/>
       <c r="B47" s="52"/>
       <c r="C47" s="49"/>
       <c r="D47" s="49"/>
@@ -6171,7 +6149,7 @@
       <c r="G47" s="49"/>
       <c r="H47" s="52"/>
       <c r="I47" s="49"/>
-      <c r="J47" s="87"/>
+      <c r="J47" s="84"/>
     </row>
   </sheetData>
   <mergeCells count="23">

</xml_diff>

<commit_message>
Changed methods visibility and created Options UML
</commit_message>
<xml_diff>
--- a/User Stories/NataliaUserStories.xlsx
+++ b/User Stories/NataliaUserStories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cad1acabf18afac6/Desktop/Software Design with AI for Cloud/Year_3/agile-labs3/Newsagent-Project/User Stories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="776" documentId="13_ncr:1_{7B2E17FA-F2A9-4DCC-A803-850E080333ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41922FBE-6C9F-4E5B-AD8A-78B43F9BD1FD}"/>
+  <xr:revisionPtr revIDLastSave="872" documentId="13_ncr:1_{7B2E17FA-F2A9-4DCC-A803-850E080333ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5866974-206C-410C-BA3A-9C18AA288D91}"/>
   <bookViews>
-    <workbookView xWindow="14740" yWindow="2750" windowWidth="22950" windowHeight="16250" activeTab="2" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminUserStories" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="278">
   <si>
     <t>As an admin</t>
   </si>
@@ -837,6 +837,42 @@
   </si>
   <si>
     <t>+doesUserExist(int id) : boolean</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>- Scanner : static</t>
+  </si>
+  <si>
+    <t>+ Connection : static</t>
+  </si>
+  <si>
+    <t>+ Options()</t>
+  </si>
+  <si>
+    <t>+ loginScreen() : static void</t>
+  </si>
+  <si>
+    <t>- authenticatePassword(String username, String password) : boolean static</t>
+  </si>
+  <si>
+    <t>- authenticateUsername (String uesrname): boolean static</t>
+  </si>
+  <si>
+    <t>- User getUser(String username, String password, String role) : static</t>
+  </si>
+  <si>
+    <t>- adminOptions() : void</t>
+  </si>
+  <si>
+    <t>- newsagentOptions() : void</t>
+  </si>
+  <si>
+    <t>- driverOptions() : void</t>
+  </si>
+  <si>
+    <t>- logOut() : void</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1073,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1187,16 +1223,62 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1211,51 +1293,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1274,7 +1311,12 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1311,7 +1353,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>2578803</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>112059</xdr:rowOff>
+      <xdr:rowOff>112058</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1399,7 +1441,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>2196353</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>66756</xdr:rowOff>
+      <xdr:rowOff>66755</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1443,7 +1485,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>2797826</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>112060</xdr:rowOff>
+      <xdr:rowOff>112061</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3024,6 +3066,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3327,17 +3373,17 @@
       <selection activeCell="C69" sqref="C69:C71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.90625" style="24" customWidth="1"/>
-    <col min="2" max="2" width="13.08984375" customWidth="1"/>
-    <col min="3" max="3" width="28.453125" customWidth="1"/>
-    <col min="4" max="4" width="35.1796875" customWidth="1"/>
-    <col min="5" max="5" width="57.81640625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="39.453125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="2.9296875" style="24" customWidth="1"/>
+    <col min="2" max="2" width="13.06640625" customWidth="1"/>
+    <col min="3" max="3" width="28.46484375" customWidth="1"/>
+    <col min="4" max="4" width="35.19921875" customWidth="1"/>
+    <col min="5" max="5" width="57.796875" style="11" customWidth="1"/>
+    <col min="6" max="6" width="39.46484375" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="22"/>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -3355,17 +3401,17 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="57">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="65">
         <v>1</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="58" t="s">
         <v>149</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="58" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="15" t="s">
@@ -3375,11 +3421,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="58"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="66"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="15" t="s">
         <v>47</v>
       </c>
@@ -3387,57 +3433,57 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="58"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="66"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="15" t="s">
         <v>49</v>
       </c>
       <c r="F4" s="21"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="58"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="66"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
       <c r="E5" s="15" t="s">
         <v>50</v>
       </c>
       <c r="F5" s="21"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="58"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="66"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
       <c r="E6" s="15" t="s">
         <v>150</v>
       </c>
       <c r="F6" s="21"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="58"/>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="66"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
       <c r="E7" s="15" t="s">
         <v>154</v>
       </c>
       <c r="F7" s="21"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="58"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="66"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
       <c r="E8" s="15" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="21"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="25"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -3445,17 +3491,17 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="57">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="65">
         <v>2</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="59" t="s">
+      <c r="C10" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="59" t="s">
+      <c r="D10" s="58" t="s">
         <v>81</v>
       </c>
       <c r="E10" s="14" t="s">
@@ -3465,67 +3511,67 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="58"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="66"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
       <c r="E11" s="15" t="s">
         <v>87</v>
       </c>
       <c r="F11" s="21"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="58"/>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="66"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
       <c r="E12" s="15" t="s">
         <v>90</v>
       </c>
       <c r="F12" s="21"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="58"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="66"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
       <c r="E13" s="15" t="s">
         <v>88</v>
       </c>
       <c r="F13" s="21"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="58"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="66"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
       <c r="E14" s="15" t="s">
         <v>89</v>
       </c>
       <c r="F14" s="21"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="58"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="66"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
       <c r="E15" s="15" t="s">
         <v>83</v>
       </c>
       <c r="F15" s="21"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="71"/>
-      <c r="B16" s="72"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="67"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
       <c r="E16" s="15" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="21"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="23"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -3533,17 +3579,17 @@
       <c r="E17" s="16"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="57">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="65">
         <v>3</v>
       </c>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="59" t="s">
+      <c r="C18" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="59" t="s">
+      <c r="D18" s="58" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="15" t="s">
@@ -3553,27 +3599,27 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="58"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="66"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
       <c r="E19" s="15" t="s">
         <v>91</v>
       </c>
       <c r="F19" s="21"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="71"/>
-      <c r="B20" s="72"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="72"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="67"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
       <c r="E20" s="11" t="s">
         <v>51</v>
       </c>
       <c r="F20" s="21"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="23"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -3581,17 +3627,17 @@
       <c r="E21" s="16"/>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="57">
+    <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="65">
         <v>4</v>
       </c>
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="59" t="s">
+      <c r="C22" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="59" t="s">
+      <c r="D22" s="58" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="15" t="s">
@@ -3601,67 +3647,67 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="58"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="66"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
       <c r="E23" s="15" t="s">
         <v>96</v>
       </c>
       <c r="F23" s="21"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="58"/>
-      <c r="B24" s="60"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="60"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="66"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
       <c r="E24" s="15" t="s">
         <v>97</v>
       </c>
       <c r="F24" s="21"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="58"/>
-      <c r="B25" s="60"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="66"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
       <c r="E25" s="15" t="s">
         <v>98</v>
       </c>
       <c r="F25" s="21"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="58"/>
-      <c r="B26" s="60"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="60"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="66"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
       <c r="E26" s="15" t="s">
         <v>92</v>
       </c>
       <c r="F26" s="21"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="58"/>
-      <c r="B27" s="60"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="60"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="66"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
       <c r="E27" s="15" t="s">
         <v>93</v>
       </c>
       <c r="F27" s="21"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="71"/>
-      <c r="B28" s="72"/>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" s="67"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="60"/>
       <c r="E28" s="15" t="s">
         <v>11</v>
       </c>
       <c r="F28" s="21"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="23"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -3669,17 +3715,17 @@
       <c r="E29" s="16"/>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="57">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="65">
         <v>5</v>
       </c>
-      <c r="B30" s="59" t="s">
+      <c r="B30" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="59" t="s">
+      <c r="C30" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="59" t="s">
+      <c r="D30" s="58" t="s">
         <v>82</v>
       </c>
       <c r="E30" s="15" t="s">
@@ -3687,27 +3733,27 @@
       </c>
       <c r="F30" s="21"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="58"/>
-      <c r="B31" s="60"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="60"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" s="66"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
       <c r="E31" s="15" t="s">
         <v>94</v>
       </c>
       <c r="F31" s="21"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="71"/>
-      <c r="B32" s="72"/>
-      <c r="C32" s="72"/>
-      <c r="D32" s="72"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" s="67"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="60"/>
       <c r="E32" s="15" t="s">
         <v>95</v>
       </c>
       <c r="F32" s="21"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="23"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -3715,17 +3761,17 @@
       <c r="E33" s="16"/>
       <c r="F33" s="7"/>
     </row>
-    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="57">
+    <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A34" s="65">
         <v>6</v>
       </c>
-      <c r="B34" s="59" t="s">
+      <c r="B34" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="59" t="s">
+      <c r="C34" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="59" t="s">
+      <c r="D34" s="58" t="s">
         <v>16</v>
       </c>
       <c r="E34" s="15" t="s">
@@ -3735,17 +3781,17 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="71"/>
-      <c r="B35" s="72"/>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" s="67"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="60"/>
       <c r="E35" s="15" t="s">
         <v>100</v>
       </c>
       <c r="F35" s="21"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="26"/>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
@@ -3753,77 +3799,77 @@
       <c r="E36" s="19"/>
       <c r="F36" s="7"/>
     </row>
-    <row r="37" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="76">
+    <row r="37" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="68">
         <v>7</v>
       </c>
-      <c r="B37" s="75" t="s">
+      <c r="B37" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="75" t="s">
+      <c r="C37" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="D37" s="75" t="s">
+      <c r="D37" s="64" t="s">
         <v>69</v>
       </c>
       <c r="E37" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="F37" s="59" t="s">
+      <c r="F37" s="58" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="76"/>
-      <c r="B38" s="75"/>
-      <c r="C38" s="75"/>
-      <c r="D38" s="75"/>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" s="68"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="64"/>
       <c r="E38" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="F38" s="60"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="76"/>
-      <c r="B39" s="75"/>
-      <c r="C39" s="75"/>
-      <c r="D39" s="75"/>
+      <c r="F38" s="59"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" s="68"/>
+      <c r="B39" s="64"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="64"/>
       <c r="E39" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="F39" s="72"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="76"/>
-      <c r="B40" s="75"/>
-      <c r="C40" s="75"/>
-      <c r="D40" s="75"/>
+      <c r="F39" s="60"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" s="68"/>
+      <c r="B40" s="64"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="64"/>
       <c r="E40" s="21" t="s">
         <v>72</v>
       </c>
       <c r="F40" s="21"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="76"/>
-      <c r="B41" s="75"/>
-      <c r="C41" s="75"/>
-      <c r="D41" s="75"/>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" s="68"/>
+      <c r="B41" s="64"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="64"/>
       <c r="E41" s="21" t="s">
         <v>73</v>
       </c>
       <c r="F41" s="21"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="76"/>
-      <c r="B42" s="75"/>
-      <c r="C42" s="75"/>
-      <c r="D42" s="75"/>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="68"/>
+      <c r="B42" s="64"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="64"/>
       <c r="E42" s="21" t="s">
         <v>75</v>
       </c>
       <c r="F42" s="21"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="27"/>
       <c r="B43" s="20"/>
       <c r="C43" s="44"/>
@@ -3831,17 +3877,17 @@
       <c r="E43" s="45"/>
       <c r="F43" s="7"/>
     </row>
-    <row r="44" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="77">
+    <row r="44" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="61">
         <v>8</v>
       </c>
-      <c r="B44" s="59" t="s">
+      <c r="B44" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="59" t="s">
+      <c r="C44" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="D44" s="59" t="s">
+      <c r="D44" s="58" t="s">
         <v>152</v>
       </c>
       <c r="E44" s="21" t="s">
@@ -3851,11 +3897,11 @@
         <v>155</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="78"/>
-      <c r="B45" s="60"/>
-      <c r="C45" s="60"/>
-      <c r="D45" s="60"/>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" s="62"/>
+      <c r="B45" s="59"/>
+      <c r="C45" s="59"/>
+      <c r="D45" s="59"/>
       <c r="E45" s="21" t="s">
         <v>47</v>
       </c>
@@ -3863,57 +3909,57 @@
         <v>156</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="78"/>
-      <c r="B46" s="60"/>
-      <c r="C46" s="60"/>
-      <c r="D46" s="60"/>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46" s="62"/>
+      <c r="B46" s="59"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="59"/>
       <c r="E46" s="21" t="s">
         <v>49</v>
       </c>
       <c r="F46" s="21"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="78"/>
-      <c r="B47" s="60"/>
-      <c r="C47" s="60"/>
-      <c r="D47" s="60"/>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47" s="62"/>
+      <c r="B47" s="59"/>
+      <c r="C47" s="59"/>
+      <c r="D47" s="59"/>
       <c r="E47" s="21" t="s">
         <v>50</v>
       </c>
       <c r="F47" s="21"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" s="78"/>
-      <c r="B48" s="60"/>
-      <c r="C48" s="60"/>
-      <c r="D48" s="60"/>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48" s="62"/>
+      <c r="B48" s="59"/>
+      <c r="C48" s="59"/>
+      <c r="D48" s="59"/>
       <c r="E48" s="21" t="s">
         <v>153</v>
       </c>
       <c r="F48" s="21"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="78"/>
-      <c r="B49" s="60"/>
-      <c r="C49" s="60"/>
-      <c r="D49" s="60"/>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49" s="62"/>
+      <c r="B49" s="59"/>
+      <c r="C49" s="59"/>
+      <c r="D49" s="59"/>
       <c r="E49" s="21" t="s">
         <v>154</v>
       </c>
       <c r="F49" s="21"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="79"/>
-      <c r="B50" s="72"/>
-      <c r="C50" s="72"/>
-      <c r="D50" s="72"/>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50" s="63"/>
+      <c r="B50" s="60"/>
+      <c r="C50" s="60"/>
+      <c r="D50" s="60"/>
       <c r="E50" s="21" t="s">
         <v>37</v>
       </c>
       <c r="F50" s="21"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="27"/>
       <c r="B51" s="20"/>
       <c r="C51" s="44"/>
@@ -3921,17 +3967,17 @@
       <c r="E51" s="45"/>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="77">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52" s="61">
         <v>9</v>
       </c>
-      <c r="B52" s="59" t="s">
+      <c r="B52" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C52" s="59" t="s">
+      <c r="C52" s="58" t="s">
         <v>159</v>
       </c>
-      <c r="D52" s="59" t="s">
+      <c r="D52" s="58" t="s">
         <v>160</v>
       </c>
       <c r="E52" s="21" t="s">
@@ -3941,11 +3987,11 @@
         <v>157</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="78"/>
-      <c r="B53" s="60"/>
-      <c r="C53" s="60"/>
-      <c r="D53" s="60"/>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53" s="62"/>
+      <c r="B53" s="59"/>
+      <c r="C53" s="59"/>
+      <c r="D53" s="59"/>
       <c r="E53" s="21" t="s">
         <v>47</v>
       </c>
@@ -3953,57 +3999,57 @@
         <v>158</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="78"/>
-      <c r="B54" s="60"/>
-      <c r="C54" s="60"/>
-      <c r="D54" s="60"/>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54" s="62"/>
+      <c r="B54" s="59"/>
+      <c r="C54" s="59"/>
+      <c r="D54" s="59"/>
       <c r="E54" s="21" t="s">
         <v>49</v>
       </c>
       <c r="F54" s="21"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" s="78"/>
-      <c r="B55" s="60"/>
-      <c r="C55" s="60"/>
-      <c r="D55" s="60"/>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55" s="62"/>
+      <c r="B55" s="59"/>
+      <c r="C55" s="59"/>
+      <c r="D55" s="59"/>
       <c r="E55" s="21" t="s">
         <v>50</v>
       </c>
       <c r="F55" s="21"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="78"/>
-      <c r="B56" s="60"/>
-      <c r="C56" s="60"/>
-      <c r="D56" s="60"/>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56" s="62"/>
+      <c r="B56" s="59"/>
+      <c r="C56" s="59"/>
+      <c r="D56" s="59"/>
       <c r="E56" s="21" t="s">
         <v>153</v>
       </c>
       <c r="F56" s="21"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A57" s="78"/>
-      <c r="B57" s="60"/>
-      <c r="C57" s="60"/>
-      <c r="D57" s="60"/>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57" s="62"/>
+      <c r="B57" s="59"/>
+      <c r="C57" s="59"/>
+      <c r="D57" s="59"/>
       <c r="E57" s="21" t="s">
         <v>154</v>
       </c>
       <c r="F57" s="21"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="79"/>
-      <c r="B58" s="72"/>
-      <c r="C58" s="72"/>
-      <c r="D58" s="72"/>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58" s="63"/>
+      <c r="B58" s="60"/>
+      <c r="C58" s="60"/>
+      <c r="D58" s="60"/>
       <c r="E58" s="21" t="s">
         <v>37</v>
       </c>
       <c r="F58" s="21"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="27"/>
       <c r="B59" s="20"/>
       <c r="C59" s="44"/>
@@ -4011,7 +4057,7 @@
       <c r="E59" s="45"/>
       <c r="F59" s="7"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="23"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
@@ -4019,45 +4065,45 @@
       <c r="E64" s="16"/>
       <c r="F64" s="7"/>
     </row>
-    <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="65">
+    <row r="65" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A65" s="71">
         <v>10</v>
       </c>
-      <c r="B65" s="68" t="s">
+      <c r="B65" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="C65" s="68" t="s">
+      <c r="C65" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="D65" s="68" t="s">
+      <c r="D65" s="74" t="s">
         <v>33</v>
       </c>
       <c r="E65" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F65" s="73" t="s">
+      <c r="F65" s="69" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66" s="66"/>
-      <c r="B66" s="69"/>
-      <c r="C66" s="69"/>
-      <c r="D66" s="69"/>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A66" s="72"/>
+      <c r="B66" s="75"/>
+      <c r="C66" s="75"/>
+      <c r="D66" s="75"/>
       <c r="E66" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="F66" s="74"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" s="67"/>
-      <c r="B67" s="70"/>
-      <c r="C67" s="70"/>
-      <c r="D67" s="70"/>
+      <c r="F66" s="70"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A67" s="73"/>
+      <c r="B67" s="76"/>
+      <c r="C67" s="76"/>
+      <c r="D67" s="76"/>
       <c r="E67" s="6"/>
       <c r="F67" s="31"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="23"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
@@ -4065,17 +4111,17 @@
       <c r="E68" s="16"/>
       <c r="F68" s="7"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="65">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A69" s="71">
         <v>11</v>
       </c>
-      <c r="B69" s="68" t="s">
+      <c r="B69" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="C69" s="68" t="s">
+      <c r="C69" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="D69" s="68" t="s">
+      <c r="D69" s="74" t="s">
         <v>26</v>
       </c>
       <c r="E69" s="17" t="s">
@@ -4083,67 +4129,67 @@
       </c>
       <c r="F69" s="31"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="66"/>
-      <c r="B70" s="69"/>
-      <c r="C70" s="69"/>
-      <c r="D70" s="69"/>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A70" s="72"/>
+      <c r="B70" s="75"/>
+      <c r="C70" s="75"/>
+      <c r="D70" s="75"/>
       <c r="E70" s="17" t="s">
         <v>28</v>
       </c>
       <c r="F70" s="31"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" s="67"/>
-      <c r="B71" s="70"/>
-      <c r="C71" s="70"/>
-      <c r="D71" s="70"/>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A71" s="73"/>
+      <c r="B71" s="76"/>
+      <c r="C71" s="76"/>
+      <c r="D71" s="76"/>
       <c r="E71" s="17" t="s">
         <v>29</v>
       </c>
       <c r="F71" s="31"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="23"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="9"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="63">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A75" s="79">
         <v>6</v>
       </c>
-      <c r="B75" s="61" t="s">
+      <c r="B75" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="C75" s="61" t="s">
+      <c r="C75" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="D75" s="61" t="s">
+      <c r="D75" s="77" t="s">
         <v>19</v>
       </c>
       <c r="E75" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A76" s="64"/>
-      <c r="B76" s="62"/>
-      <c r="C76" s="62"/>
-      <c r="D76" s="62"/>
+    <row r="76" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A76" s="80"/>
+      <c r="B76" s="78"/>
+      <c r="C76" s="78"/>
+      <c r="D76" s="78"/>
       <c r="E76" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="23"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="9"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" s="28">
         <v>7</v>
       </c>
@@ -4160,7 +4206,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="29"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -4169,7 +4215,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="29"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -4178,7 +4224,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A81" s="30"/>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
@@ -4187,7 +4233,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A82" s="23"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -4196,40 +4242,6 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="C44:C50"/>
-    <mergeCell ref="B44:B50"/>
-    <mergeCell ref="D44:D50"/>
-    <mergeCell ref="A44:A50"/>
-    <mergeCell ref="A52:A58"/>
-    <mergeCell ref="B52:B58"/>
-    <mergeCell ref="C52:C58"/>
-    <mergeCell ref="D52:D58"/>
-    <mergeCell ref="C37:C42"/>
-    <mergeCell ref="D37:D42"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="B37:B42"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="D65:D67"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C22:C28"/>
-    <mergeCell ref="D22:D28"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="B2:B8"/>
     <mergeCell ref="C2:C8"/>
@@ -4246,6 +4258,40 @@
     <mergeCell ref="B10:B16"/>
     <mergeCell ref="C10:C16"/>
     <mergeCell ref="D10:D16"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C22:C28"/>
+    <mergeCell ref="D22:D28"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="D65:D67"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="D37:D42"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="B37:B42"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="C44:C50"/>
+    <mergeCell ref="B44:B50"/>
+    <mergeCell ref="D44:D50"/>
+    <mergeCell ref="A44:A50"/>
+    <mergeCell ref="A52:A58"/>
+    <mergeCell ref="B52:B58"/>
+    <mergeCell ref="C52:C58"/>
+    <mergeCell ref="D52:D58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4260,17 +4306,17 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.90625" style="24" customWidth="1"/>
-    <col min="2" max="2" width="23.453125" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" customWidth="1"/>
+    <col min="1" max="1" width="2.9296875" style="24" customWidth="1"/>
+    <col min="2" max="2" width="23.46484375" customWidth="1"/>
+    <col min="3" max="3" width="27.796875" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="52.6328125" customWidth="1"/>
-    <col min="6" max="6" width="44.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.59765625" customWidth="1"/>
+    <col min="6" max="6" width="44.19921875" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="22"/>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -4288,17 +4334,17 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="57">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="65">
         <v>1</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="58" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="14" t="s">
@@ -4308,11 +4354,11 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="58"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="66"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="15" t="s">
         <v>60</v>
       </c>
@@ -4320,77 +4366,77 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="58"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="66"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="15" t="s">
         <v>64</v>
       </c>
       <c r="F4" s="21"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="58"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="66"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
       <c r="E5" s="15" t="s">
         <v>65</v>
       </c>
       <c r="F5" s="21"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="58"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="66"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
       <c r="E6" s="15" t="s">
         <v>161</v>
       </c>
       <c r="F6" s="21"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="58"/>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="66"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
       <c r="E7" s="15" t="s">
         <v>245</v>
       </c>
       <c r="F7" s="21"/>
     </row>
-    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="58"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
+    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="66"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
       <c r="E8" s="15" t="s">
         <v>61</v>
       </c>
       <c r="F8" s="21"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="58"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="66"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
       <c r="E9" s="15" t="s">
         <v>62</v>
       </c>
       <c r="F9" s="21"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="71"/>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="67"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
       <c r="E10" s="15" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="21"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="23"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -4398,17 +4444,17 @@
       <c r="E11" s="16"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="57">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="65">
         <v>2</v>
       </c>
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="59" t="s">
+      <c r="D12" s="58" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="15" t="s">
@@ -4418,47 +4464,47 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="58"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="66"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
       <c r="E13" s="15" t="s">
         <v>102</v>
       </c>
       <c r="F13" s="21"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="58"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="66"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
       <c r="E14" s="15" t="s">
         <v>103</v>
       </c>
       <c r="F14" s="21"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="58"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="66"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
       <c r="E15" s="15" t="s">
         <v>104</v>
       </c>
       <c r="F15" s="21"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="71"/>
-      <c r="B16" s="72"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="67"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
       <c r="E16" s="11" t="s">
         <v>51</v>
       </c>
       <c r="F16" s="21"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="23"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -4466,17 +4512,17 @@
       <c r="E17" s="16"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="57">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="65">
         <v>3</v>
       </c>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="59" t="s">
+      <c r="C18" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="59" t="s">
+      <c r="D18" s="58" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="15" t="s">
@@ -4486,57 +4532,57 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="58"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="66"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
       <c r="E19" s="15" t="s">
         <v>102</v>
       </c>
       <c r="F19" s="21"/>
     </row>
-    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="58"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="66"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
       <c r="E20" s="15" t="s">
         <v>106</v>
       </c>
       <c r="F20" s="21"/>
     </row>
-    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="58"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="60"/>
+    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="66"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
       <c r="E21" s="15" t="s">
         <v>107</v>
       </c>
       <c r="F21" s="21"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="58"/>
-      <c r="B22" s="60"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="66"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
       <c r="E22" s="15" t="s">
         <v>109</v>
       </c>
       <c r="F22" s="21"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="58"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="66"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
       <c r="E23" s="15" t="s">
         <v>108</v>
       </c>
       <c r="F23" s="21"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="23"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -4544,17 +4590,17 @@
       <c r="E24" s="16"/>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="57">
+    <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A25" s="65">
         <v>4</v>
       </c>
-      <c r="B25" s="59" t="s">
+      <c r="B25" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="59" t="s">
+      <c r="C25" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="59" t="s">
+      <c r="D25" s="58" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="15" t="s">
@@ -4562,17 +4608,17 @@
       </c>
       <c r="F25" s="21"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="58"/>
-      <c r="B26" s="60"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="60"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="66"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
       <c r="E26" s="15" t="s">
         <v>111</v>
       </c>
       <c r="F26" s="21"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="23"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -4580,17 +4626,17 @@
       <c r="E27" s="16"/>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="57">
+    <row r="28" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A28" s="65">
         <v>5</v>
       </c>
-      <c r="B28" s="59" t="s">
+      <c r="B28" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="59" t="s">
+      <c r="C28" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="59" t="s">
+      <c r="D28" s="58" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="15" t="s">
@@ -4600,17 +4646,17 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="58"/>
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="66"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
       <c r="E29" s="15" t="s">
         <v>17</v>
       </c>
       <c r="F29" s="21"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="23"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -4618,17 +4664,17 @@
       <c r="E30" s="16"/>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="57">
+    <row r="31" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="65">
         <v>6</v>
       </c>
-      <c r="B31" s="59" t="s">
+      <c r="B31" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="59" t="s">
+      <c r="C31" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="D31" s="59" t="s">
+      <c r="D31" s="58" t="s">
         <v>43</v>
       </c>
       <c r="E31" s="14" t="s">
@@ -4638,37 +4684,37 @@
         <v>115</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="58"/>
-      <c r="B32" s="60"/>
-      <c r="C32" s="60"/>
-      <c r="D32" s="60"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" s="66"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
       <c r="E32" s="15" t="s">
         <v>116</v>
       </c>
       <c r="F32" s="21"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="58"/>
-      <c r="B33" s="60"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" s="66"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
       <c r="E33" s="15" t="s">
         <v>114</v>
       </c>
       <c r="F33" s="21"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="71"/>
-      <c r="B34" s="72"/>
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" s="67"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="60"/>
       <c r="E34" s="15" t="s">
         <v>22</v>
       </c>
       <c r="F34" s="21"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="23"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -4676,17 +4722,17 @@
       <c r="E35" s="16"/>
       <c r="F35" s="7"/>
     </row>
-    <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="57">
+    <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A36" s="65">
         <v>7</v>
       </c>
-      <c r="B36" s="59" t="s">
+      <c r="B36" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="59" t="s">
+      <c r="C36" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="59" t="s">
+      <c r="D36" s="58" t="s">
         <v>24</v>
       </c>
       <c r="E36" s="15" t="s">
@@ -4694,27 +4740,27 @@
       </c>
       <c r="F36" s="21"/>
     </row>
-    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="58"/>
-      <c r="B37" s="60"/>
-      <c r="C37" s="60"/>
-      <c r="D37" s="60"/>
+    <row r="37" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A37" s="66"/>
+      <c r="B37" s="59"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="59"/>
       <c r="E37" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F37" s="21"/>
     </row>
-    <row r="38" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="71"/>
-      <c r="B38" s="72"/>
-      <c r="C38" s="72"/>
-      <c r="D38" s="72"/>
+    <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A38" s="67"/>
+      <c r="B38" s="60"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="60"/>
       <c r="E38" s="15" t="s">
         <v>36</v>
       </c>
       <c r="F38" s="21"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="23"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -4722,17 +4768,17 @@
       <c r="E39" s="16"/>
       <c r="F39" s="7"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="57">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" s="65">
         <v>8</v>
       </c>
-      <c r="B40" s="59" t="s">
+      <c r="B40" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="59" t="s">
+      <c r="C40" s="58" t="s">
         <v>148</v>
       </c>
-      <c r="D40" s="59" t="s">
+      <c r="D40" s="58" t="s">
         <v>117</v>
       </c>
       <c r="E40" s="21" t="s">
@@ -4740,77 +4786,77 @@
       </c>
       <c r="F40" s="21"/>
     </row>
-    <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="58"/>
-      <c r="B41" s="60"/>
-      <c r="C41" s="60"/>
-      <c r="D41" s="60"/>
+    <row r="41" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A41" s="66"/>
+      <c r="B41" s="59"/>
+      <c r="C41" s="59"/>
+      <c r="D41" s="59"/>
       <c r="E41" s="21" t="s">
         <v>119</v>
       </c>
       <c r="F41" s="21"/>
     </row>
-    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="58"/>
-      <c r="B42" s="60"/>
-      <c r="C42" s="60"/>
-      <c r="D42" s="60"/>
+    <row r="42" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A42" s="66"/>
+      <c r="B42" s="59"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="59"/>
       <c r="E42" s="21" t="s">
         <v>120</v>
       </c>
       <c r="F42" s="21"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="58"/>
-      <c r="B43" s="60"/>
-      <c r="C43" s="60"/>
-      <c r="D43" s="60"/>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" s="66"/>
+      <c r="B43" s="59"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="59"/>
       <c r="E43" s="21" t="s">
         <v>121</v>
       </c>
       <c r="F43" s="21"/>
     </row>
-    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="58"/>
-      <c r="B44" s="60"/>
-      <c r="C44" s="60"/>
-      <c r="D44" s="60"/>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" s="66"/>
+      <c r="B44" s="59"/>
+      <c r="C44" s="59"/>
+      <c r="D44" s="59"/>
       <c r="E44" s="21" t="s">
         <v>123</v>
       </c>
       <c r="F44" s="21"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="58"/>
-      <c r="B45" s="60"/>
-      <c r="C45" s="60"/>
-      <c r="D45" s="60"/>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" s="66"/>
+      <c r="B45" s="59"/>
+      <c r="C45" s="59"/>
+      <c r="D45" s="59"/>
       <c r="E45" s="21" t="s">
         <v>124</v>
       </c>
       <c r="F45" s="21"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="58"/>
-      <c r="B46" s="60"/>
-      <c r="C46" s="60"/>
-      <c r="D46" s="60"/>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46" s="66"/>
+      <c r="B46" s="59"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="59"/>
       <c r="E46" s="21" t="s">
         <v>122</v>
       </c>
       <c r="F46" s="21"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="58"/>
-      <c r="B47" s="60"/>
-      <c r="C47" s="60"/>
-      <c r="D47" s="60"/>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47" s="66"/>
+      <c r="B47" s="59"/>
+      <c r="C47" s="59"/>
+      <c r="D47" s="59"/>
       <c r="E47" s="14" t="s">
         <v>75</v>
       </c>
       <c r="F47" s="21"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="23"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -4820,6 +4866,30 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="C2:C10"/>
+    <mergeCell ref="D2:D10"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="A31:A34"/>
     <mergeCell ref="A40:A47"/>
     <mergeCell ref="B40:B47"/>
     <mergeCell ref="C40:C47"/>
@@ -4828,30 +4898,6 @@
     <mergeCell ref="C36:C38"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="C2:C10"/>
-    <mergeCell ref="D2:D10"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="D12:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4859,27 +4905,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD0B509-A153-4B31-95B8-BC32DC1B6A3B}">
-  <dimension ref="B2:J25"/>
+  <dimension ref="B2:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.08984375" customWidth="1"/>
-    <col min="2" max="2" width="40.453125" style="32" customWidth="1"/>
-    <col min="3" max="3" width="3.08984375" style="32" customWidth="1"/>
-    <col min="4" max="4" width="41.7265625" style="34" customWidth="1"/>
-    <col min="5" max="5" width="3.81640625" style="32" customWidth="1"/>
-    <col min="6" max="6" width="37.90625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="3.6328125" style="32" customWidth="1"/>
-    <col min="8" max="8" width="40.6328125" style="32" customWidth="1"/>
-    <col min="9" max="9" width="3.26953125" customWidth="1"/>
-    <col min="10" max="10" width="31.54296875" style="32" customWidth="1"/>
+    <col min="1" max="1" width="2.06640625" customWidth="1"/>
+    <col min="2" max="2" width="40.46484375" style="32" customWidth="1"/>
+    <col min="3" max="3" width="3.06640625" style="32" customWidth="1"/>
+    <col min="4" max="4" width="41.73046875" style="34" customWidth="1"/>
+    <col min="5" max="5" width="3.796875" style="32" customWidth="1"/>
+    <col min="6" max="6" width="37.9296875" style="32" customWidth="1"/>
+    <col min="7" max="7" width="3.59765625" style="32" customWidth="1"/>
+    <col min="8" max="8" width="40.59765625" style="32" customWidth="1"/>
+    <col min="9" max="9" width="3.265625" customWidth="1"/>
+    <col min="10" max="10" width="31.53125" style="32" customWidth="1"/>
+    <col min="11" max="11" width="3.265625" customWidth="1"/>
+    <col min="12" max="12" width="32.53125" style="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B2" s="41" t="s">
         <v>126</v>
       </c>
@@ -4896,8 +4944,11 @@
       <c r="J2" s="43" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="L2" s="43" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B3" s="35" t="s">
         <v>229</v>
       </c>
@@ -4913,8 +4964,11 @@
       <c r="J3" s="35" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="L3" s="40" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B4" s="38" t="s">
         <v>128</v>
       </c>
@@ -4930,8 +4984,11 @@
       <c r="J4" s="36" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="L4" s="38" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B5" s="38" t="s">
         <v>130</v>
       </c>
@@ -4947,8 +5004,9 @@
       <c r="J5" s="36" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="L5" s="39"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B6" s="38" t="s">
         <v>129</v>
       </c>
@@ -4964,8 +5022,11 @@
       <c r="J6" s="36" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="L6" s="40" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B7" s="39"/>
       <c r="D7" s="36"/>
       <c r="F7" s="39" t="s">
@@ -4973,8 +5034,11 @@
       </c>
       <c r="H7" s="37"/>
       <c r="J7" s="39"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="L7" s="38" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B8" s="40" t="s">
         <v>209</v>
       </c>
@@ -4988,112 +5052,131 @@
         <v>210</v>
       </c>
       <c r="J8" s="40"/>
-    </row>
-    <row r="9" spans="2:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B9" s="36" t="s">
+      <c r="L8" s="38" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B9" s="81" t="s">
         <v>232</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="81" t="s">
         <v>233</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="81" t="s">
         <v>204</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="81" t="s">
         <v>234</v>
       </c>
       <c r="J9" s="39" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="38"/>
-      <c r="D10" s="36"/>
-      <c r="F10" s="36" t="s">
+      <c r="L9" s="38" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="F10" s="81"/>
+      <c r="H10" s="81"/>
+      <c r="L10" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B11" s="81" t="s">
+        <v>219</v>
+      </c>
+      <c r="D11" s="81" t="s">
+        <v>147</v>
+      </c>
+      <c r="F11" s="36" t="s">
         <v>242</v>
       </c>
-      <c r="H10" s="36" t="s">
+      <c r="H11" s="36" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="80" t="s">
-        <v>219</v>
-      </c>
-      <c r="D11" s="80" t="s">
-        <v>147</v>
-      </c>
-      <c r="F11" s="36" t="s">
+      <c r="L11" s="38" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="F12" s="36" t="s">
         <v>243</v>
       </c>
-      <c r="H11" s="38" t="s">
+      <c r="H12" s="38" t="s">
         <v>235</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="F12" s="38" t="s">
-        <v>206</v>
-      </c>
-      <c r="H12" s="38" t="s">
-        <v>211</v>
       </c>
       <c r="J12" s="55" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="L12" s="81" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B13" s="36" t="s">
         <v>218</v>
       </c>
       <c r="D13" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="F13" s="38"/>
+      <c r="F13" s="38" t="s">
+        <v>206</v>
+      </c>
       <c r="H13" s="38" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+        <v>211</v>
+      </c>
+      <c r="L13" s="81"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B14" s="38" t="s">
         <v>242</v>
       </c>
       <c r="D14" s="56" t="s">
         <v>221</v>
       </c>
-      <c r="F14" s="38" t="s">
-        <v>132</v>
-      </c>
+      <c r="F14" s="38"/>
       <c r="H14" s="38" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="86" t="s">
+        <v>212</v>
+      </c>
+      <c r="L14" s="81" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="57" t="s">
         <v>222</v>
       </c>
       <c r="D15" s="36" t="s">
         <v>220</v>
       </c>
       <c r="F15" s="38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H15" s="38" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B16" s="86"/>
+        <v>213</v>
+      </c>
+      <c r="L15" s="81"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B16" s="57"/>
       <c r="D16" s="36"/>
       <c r="F16" s="38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H16" s="38" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+        <v>214</v>
+      </c>
+      <c r="L16" s="81" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="38" t="s">
         <v>244</v>
       </c>
@@ -5101,13 +5184,14 @@
         <v>236</v>
       </c>
       <c r="F17" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="H17" s="39" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+      <c r="H17" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="L17" s="88"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B18" s="38" t="s">
         <v>240</v>
       </c>
@@ -5115,10 +5199,14 @@
         <v>237</v>
       </c>
       <c r="F18" s="38" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+      <c r="H18" s="39" t="s">
+        <v>216</v>
+      </c>
+      <c r="L18" s="87"/>
+    </row>
+    <row r="19" spans="2:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="38" t="s">
         <v>241</v>
       </c>
@@ -5126,65 +5214,78 @@
         <v>238</v>
       </c>
       <c r="F19" s="38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H19" s="55" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B20" s="80" t="s">
+      <c r="L19" s="55" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B20" s="81" t="s">
         <v>239</v>
       </c>
-      <c r="D20" s="80" t="s">
+      <c r="D20" s="81" t="s">
         <v>239</v>
       </c>
       <c r="F20" s="38" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="81"/>
+      <c r="D21" s="81"/>
+      <c r="F21" s="38" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="80"/>
-      <c r="D21" s="80"/>
-      <c r="F21" s="38" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" s="39" t="s">
         <v>246</v>
       </c>
-      <c r="D22" s="32" t="s">
+      <c r="D22" s="39" t="s">
         <v>265</v>
       </c>
       <c r="F22" s="38" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="F23" s="38" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="F23" s="39" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B24" s="55" t="s">
         <v>207</v>
       </c>
       <c r="D24" s="55" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F24" s="39" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.45">
       <c r="F25" s="55" t="s">
         <v>207</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="11">
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="B20:B21"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="L14:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5199,38 +5300,38 @@
       <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="1.26953125" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="53"/>
+    <col min="1" max="1" width="1.265625" customWidth="1"/>
+    <col min="2" max="2" width="8.73046875" style="53"/>
     <col min="3" max="3" width="73" customWidth="1"/>
-    <col min="4" max="4" width="3.36328125" customWidth="1"/>
-    <col min="6" max="6" width="58.453125" customWidth="1"/>
-    <col min="7" max="7" width="3.36328125" customWidth="1"/>
-    <col min="9" max="9" width="63.36328125" customWidth="1"/>
-    <col min="10" max="10" width="2.1796875" customWidth="1"/>
+    <col min="4" max="4" width="3.33203125" customWidth="1"/>
+    <col min="6" max="6" width="58.46484375" customWidth="1"/>
+    <col min="7" max="7" width="3.33203125" customWidth="1"/>
+    <col min="9" max="9" width="63.33203125" customWidth="1"/>
+    <col min="10" max="10" width="2.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="84"/>
-      <c r="B1" s="85" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A1" s="85"/>
+      <c r="B1" s="86" t="s">
         <v>167</v>
       </c>
-      <c r="C1" s="85"/>
+      <c r="C1" s="86"/>
       <c r="D1" s="47"/>
-      <c r="E1" s="85" t="s">
+      <c r="E1" s="86" t="s">
         <v>255</v>
       </c>
-      <c r="F1" s="85"/>
+      <c r="F1" s="86"/>
       <c r="G1" s="47"/>
-      <c r="H1" s="85" t="s">
+      <c r="H1" s="86" t="s">
         <v>254</v>
       </c>
-      <c r="I1" s="85"/>
-      <c r="J1" s="84"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="84"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="85"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A2" s="85"/>
       <c r="B2" s="51"/>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
@@ -5239,100 +5340,100 @@
       <c r="G2" s="46"/>
       <c r="H2" s="46"/>
       <c r="I2" s="46"/>
-      <c r="J2" s="84"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="84"/>
+      <c r="J2" s="85"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A3" s="85"/>
       <c r="B3" s="50" t="s">
         <v>162</v>
       </c>
       <c r="C3" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="D3" s="81"/>
+      <c r="D3" s="82"/>
       <c r="E3" s="48" t="s">
         <v>162</v>
       </c>
       <c r="F3" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="G3" s="81"/>
+      <c r="G3" s="82"/>
       <c r="H3" s="48" t="s">
         <v>162</v>
       </c>
       <c r="I3" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="J3" s="84"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="84"/>
+      <c r="J3" s="85"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" s="85"/>
       <c r="B4" s="50" t="s">
         <v>164</v>
       </c>
       <c r="C4" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="D4" s="82"/>
+      <c r="D4" s="83"/>
       <c r="E4" s="48" t="s">
         <v>164</v>
       </c>
       <c r="F4" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="G4" s="82"/>
+      <c r="G4" s="83"/>
       <c r="H4" s="48" t="s">
         <v>164</v>
       </c>
       <c r="I4" s="48" t="s">
         <v>179</v>
       </c>
-      <c r="J4" s="84"/>
-    </row>
-    <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="84"/>
+      <c r="J4" s="85"/>
+    </row>
+    <row r="5" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="85"/>
       <c r="B5" s="50" t="s">
         <v>165</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="D5" s="82"/>
+      <c r="D5" s="83"/>
       <c r="E5" s="48" t="s">
         <v>165</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="G5" s="82"/>
+      <c r="G5" s="83"/>
       <c r="H5" s="48" t="s">
         <v>165</v>
       </c>
       <c r="I5" s="21" t="s">
         <v>252</v>
       </c>
-      <c r="J5" s="84"/>
-    </row>
-    <row r="6" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="84"/>
+      <c r="J5" s="85"/>
+    </row>
+    <row r="6" spans="1:10" ht="31.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="85"/>
       <c r="B6" s="50" t="s">
         <v>166</v>
       </c>
       <c r="C6" s="48"/>
-      <c r="D6" s="83"/>
+      <c r="D6" s="84"/>
       <c r="E6" s="48" t="s">
         <v>166</v>
       </c>
       <c r="F6" s="48"/>
-      <c r="G6" s="83"/>
+      <c r="G6" s="84"/>
       <c r="H6" s="48" t="s">
         <v>166</v>
       </c>
       <c r="I6" s="48"/>
-      <c r="J6" s="84"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="84"/>
+      <c r="J6" s="85"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" s="85"/>
       <c r="B7" s="52"/>
       <c r="C7" s="49"/>
       <c r="D7" s="49"/>
@@ -5341,100 +5442,100 @@
       <c r="G7" s="49"/>
       <c r="H7" s="49"/>
       <c r="I7" s="49"/>
-      <c r="J7" s="84"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="84"/>
+      <c r="J7" s="85"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" s="85"/>
       <c r="B8" s="50" t="s">
         <v>162</v>
       </c>
       <c r="C8" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="D8" s="81"/>
+      <c r="D8" s="82"/>
       <c r="E8" s="48" t="s">
         <v>162</v>
       </c>
       <c r="F8" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="G8" s="81"/>
+      <c r="G8" s="82"/>
       <c r="H8" s="48" t="s">
         <v>162</v>
       </c>
       <c r="I8" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="J8" s="84"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="84"/>
+      <c r="J8" s="85"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" s="85"/>
       <c r="B9" s="50" t="s">
         <v>164</v>
       </c>
       <c r="C9" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="D9" s="82"/>
+      <c r="D9" s="83"/>
       <c r="E9" s="48" t="s">
         <v>164</v>
       </c>
       <c r="F9" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="G9" s="82"/>
+      <c r="G9" s="83"/>
       <c r="H9" s="48" t="s">
         <v>164</v>
       </c>
       <c r="I9" s="48" t="s">
         <v>195</v>
       </c>
-      <c r="J9" s="84"/>
-    </row>
-    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="84"/>
+      <c r="J9" s="85"/>
+    </row>
+    <row r="10" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="85"/>
       <c r="B10" s="50" t="s">
         <v>165</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="D10" s="82"/>
+      <c r="D10" s="83"/>
       <c r="E10" s="48" t="s">
         <v>165</v>
       </c>
       <c r="F10" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="G10" s="82"/>
+      <c r="G10" s="83"/>
       <c r="H10" s="48" t="s">
         <v>165</v>
       </c>
       <c r="I10" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="J10" s="84"/>
-    </row>
-    <row r="11" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="84"/>
+      <c r="J10" s="85"/>
+    </row>
+    <row r="11" spans="1:10" ht="31.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="85"/>
       <c r="B11" s="50" t="s">
         <v>166</v>
       </c>
       <c r="C11" s="48"/>
-      <c r="D11" s="83"/>
+      <c r="D11" s="84"/>
       <c r="E11" s="48" t="s">
         <v>166</v>
       </c>
       <c r="F11" s="48"/>
-      <c r="G11" s="83"/>
+      <c r="G11" s="84"/>
       <c r="H11" s="48" t="s">
         <v>166</v>
       </c>
       <c r="I11" s="48"/>
-      <c r="J11" s="84"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="84"/>
+      <c r="J11" s="85"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="85"/>
       <c r="B12" s="52"/>
       <c r="C12" s="49"/>
       <c r="D12" s="49"/>
@@ -5443,92 +5544,92 @@
       <c r="G12" s="49"/>
       <c r="H12" s="49"/>
       <c r="I12" s="49"/>
-      <c r="J12" s="84"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="84"/>
+      <c r="J12" s="85"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" s="85"/>
       <c r="B13" s="50" t="s">
         <v>162</v>
       </c>
       <c r="C13" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="D13" s="81"/>
+      <c r="D13" s="82"/>
       <c r="E13" s="48" t="s">
         <v>162</v>
       </c>
       <c r="F13" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="G13" s="81"/>
+      <c r="G13" s="82"/>
       <c r="H13" s="48" t="s">
         <v>162</v>
       </c>
       <c r="I13" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="J13" s="84"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="84"/>
+      <c r="J13" s="85"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" s="85"/>
       <c r="B14" s="50" t="s">
         <v>164</v>
       </c>
       <c r="C14" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="D14" s="82"/>
+      <c r="D14" s="83"/>
       <c r="E14" s="48" t="s">
         <v>164</v>
       </c>
       <c r="F14" s="48"/>
-      <c r="G14" s="82"/>
+      <c r="G14" s="83"/>
       <c r="H14" s="48" t="s">
         <v>164</v>
       </c>
       <c r="I14" s="48"/>
-      <c r="J14" s="84"/>
-    </row>
-    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="84"/>
+      <c r="J14" s="85"/>
+    </row>
+    <row r="15" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="85"/>
       <c r="B15" s="50" t="s">
         <v>165</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="D15" s="82"/>
+      <c r="D15" s="83"/>
       <c r="E15" s="48" t="s">
         <v>165</v>
       </c>
       <c r="F15" s="21"/>
-      <c r="G15" s="82"/>
+      <c r="G15" s="83"/>
       <c r="H15" s="48" t="s">
         <v>165</v>
       </c>
       <c r="I15" s="21"/>
-      <c r="J15" s="84"/>
-    </row>
-    <row r="16" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="84"/>
+      <c r="J15" s="85"/>
+    </row>
+    <row r="16" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="85"/>
       <c r="B16" s="50" t="s">
         <v>166</v>
       </c>
       <c r="C16" s="48"/>
-      <c r="D16" s="83"/>
+      <c r="D16" s="84"/>
       <c r="E16" s="48" t="s">
         <v>166</v>
       </c>
       <c r="F16" s="48"/>
-      <c r="G16" s="83"/>
+      <c r="G16" s="84"/>
       <c r="H16" s="48" t="s">
         <v>166</v>
       </c>
       <c r="I16" s="48"/>
-      <c r="J16" s="84"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="84"/>
+      <c r="J16" s="85"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A17" s="85"/>
       <c r="B17" s="52"/>
       <c r="C17" s="49"/>
       <c r="D17" s="49"/>
@@ -5537,100 +5638,100 @@
       <c r="G17" s="49"/>
       <c r="H17" s="49"/>
       <c r="I17" s="49"/>
-      <c r="J17" s="84"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="84"/>
+      <c r="J17" s="85"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A18" s="85"/>
       <c r="B18" s="50" t="s">
         <v>162</v>
       </c>
       <c r="C18" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="D18" s="81"/>
+      <c r="D18" s="82"/>
       <c r="E18" s="48" t="s">
         <v>162</v>
       </c>
       <c r="F18" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="G18" s="81"/>
+      <c r="G18" s="82"/>
       <c r="H18" s="48" t="s">
         <v>162</v>
       </c>
       <c r="I18" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="J18" s="84"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="84"/>
+      <c r="J18" s="85"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A19" s="85"/>
       <c r="B19" s="50" t="s">
         <v>164</v>
       </c>
       <c r="C19" s="48" t="s">
         <v>180</v>
       </c>
-      <c r="D19" s="82"/>
+      <c r="D19" s="83"/>
       <c r="E19" s="48" t="s">
         <v>164</v>
       </c>
       <c r="F19" s="48" t="s">
         <v>180</v>
       </c>
-      <c r="G19" s="82"/>
+      <c r="G19" s="83"/>
       <c r="H19" s="48" t="s">
         <v>164</v>
       </c>
       <c r="I19" s="48" t="s">
         <v>180</v>
       </c>
-      <c r="J19" s="84"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="84"/>
+      <c r="J19" s="85"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A20" s="85"/>
       <c r="B20" s="50" t="s">
         <v>165</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="D20" s="82"/>
+      <c r="D20" s="83"/>
       <c r="E20" s="48" t="s">
         <v>165</v>
       </c>
       <c r="F20" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="G20" s="82"/>
+      <c r="G20" s="83"/>
       <c r="H20" s="48" t="s">
         <v>165</v>
       </c>
       <c r="I20" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="J20" s="84"/>
-    </row>
-    <row r="21" spans="1:10" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="84"/>
+      <c r="J20" s="85"/>
+    </row>
+    <row r="21" spans="1:10" ht="81.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="85"/>
       <c r="B21" s="50" t="s">
         <v>166</v>
       </c>
       <c r="C21" s="48"/>
-      <c r="D21" s="83"/>
+      <c r="D21" s="84"/>
       <c r="E21" s="48" t="s">
         <v>166</v>
       </c>
       <c r="F21" s="48"/>
-      <c r="G21" s="83"/>
+      <c r="G21" s="84"/>
       <c r="H21" s="48" t="s">
         <v>166</v>
       </c>
       <c r="I21" s="48"/>
-      <c r="J21" s="84"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="84"/>
+      <c r="J21" s="85"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A22" s="85"/>
       <c r="B22" s="52"/>
       <c r="C22" s="49"/>
       <c r="D22" s="49"/>
@@ -5639,100 +5740,100 @@
       <c r="G22" s="49"/>
       <c r="H22" s="49"/>
       <c r="I22" s="49"/>
-      <c r="J22" s="84"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="84"/>
+      <c r="J22" s="85"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A23" s="85"/>
       <c r="B23" s="50" t="s">
         <v>162</v>
       </c>
       <c r="C23" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="D23" s="81"/>
+      <c r="D23" s="82"/>
       <c r="E23" s="48" t="s">
         <v>162</v>
       </c>
       <c r="F23" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="G23" s="81"/>
+      <c r="G23" s="82"/>
       <c r="H23" s="48" t="s">
         <v>162</v>
       </c>
       <c r="I23" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="J23" s="84"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="84"/>
+      <c r="J23" s="85"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A24" s="85"/>
       <c r="B24" s="50" t="s">
         <v>164</v>
       </c>
       <c r="C24" s="48" t="s">
         <v>186</v>
       </c>
-      <c r="D24" s="82"/>
+      <c r="D24" s="83"/>
       <c r="E24" s="48" t="s">
         <v>164</v>
       </c>
       <c r="F24" s="48" t="s">
         <v>199</v>
       </c>
-      <c r="G24" s="82"/>
+      <c r="G24" s="83"/>
       <c r="H24" s="48" t="s">
         <v>164</v>
       </c>
       <c r="I24" s="48" t="s">
         <v>196</v>
       </c>
-      <c r="J24" s="84"/>
-    </row>
-    <row r="25" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="84"/>
+      <c r="J24" s="85"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A25" s="85"/>
       <c r="B25" s="50" t="s">
         <v>165</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="D25" s="82"/>
+      <c r="D25" s="83"/>
       <c r="E25" s="48" t="s">
         <v>165</v>
       </c>
       <c r="F25" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="G25" s="82"/>
+      <c r="G25" s="83"/>
       <c r="H25" s="48" t="s">
         <v>165</v>
       </c>
       <c r="I25" s="21" t="s">
         <v>258</v>
       </c>
-      <c r="J25" s="84"/>
-    </row>
-    <row r="26" spans="1:10" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="84"/>
+      <c r="J25" s="85"/>
+    </row>
+    <row r="26" spans="1:10" ht="66.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="85"/>
       <c r="B26" s="50" t="s">
         <v>166</v>
       </c>
       <c r="C26" s="48"/>
-      <c r="D26" s="83"/>
+      <c r="D26" s="84"/>
       <c r="E26" s="48" t="s">
         <v>166</v>
       </c>
       <c r="F26" s="48"/>
-      <c r="G26" s="83"/>
+      <c r="G26" s="84"/>
       <c r="H26" s="48" t="s">
         <v>166</v>
       </c>
       <c r="I26" s="48"/>
-      <c r="J26" s="84"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="84"/>
+      <c r="J26" s="85"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A27" s="85"/>
       <c r="B27" s="52"/>
       <c r="C27" s="49"/>
       <c r="D27" s="49"/>
@@ -5741,100 +5842,100 @@
       <c r="G27" s="49"/>
       <c r="H27" s="49"/>
       <c r="I27" s="49"/>
-      <c r="J27" s="84"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="84"/>
+      <c r="J27" s="85"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A28" s="85"/>
       <c r="B28" s="50" t="s">
         <v>162</v>
       </c>
       <c r="C28" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="D28" s="81"/>
+      <c r="D28" s="82"/>
       <c r="E28" s="48" t="s">
         <v>162</v>
       </c>
       <c r="F28" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="G28" s="81"/>
+      <c r="G28" s="82"/>
       <c r="H28" s="48" t="s">
         <v>162</v>
       </c>
       <c r="I28" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="J28" s="84"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="84"/>
+      <c r="J28" s="85"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A29" s="85"/>
       <c r="B29" s="50" t="s">
         <v>164</v>
       </c>
       <c r="C29" s="48" t="s">
         <v>187</v>
       </c>
-      <c r="D29" s="82"/>
+      <c r="D29" s="83"/>
       <c r="E29" s="48" t="s">
         <v>164</v>
       </c>
       <c r="F29" s="48" t="s">
         <v>200</v>
       </c>
-      <c r="G29" s="82"/>
+      <c r="G29" s="83"/>
       <c r="H29" s="48" t="s">
         <v>164</v>
       </c>
       <c r="I29" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="J29" s="84"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="84"/>
+      <c r="J29" s="85"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A30" s="85"/>
       <c r="B30" s="50" t="s">
         <v>165</v>
       </c>
       <c r="C30" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="D30" s="82"/>
+      <c r="D30" s="83"/>
       <c r="E30" s="48" t="s">
         <v>165</v>
       </c>
       <c r="F30" s="48" t="s">
         <v>259</v>
       </c>
-      <c r="G30" s="82"/>
+      <c r="G30" s="83"/>
       <c r="H30" s="48" t="s">
         <v>165</v>
       </c>
       <c r="I30" s="48" t="s">
         <v>260</v>
       </c>
-      <c r="J30" s="84"/>
-    </row>
-    <row r="31" spans="1:10" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="84"/>
+      <c r="J30" s="85"/>
+    </row>
+    <row r="31" spans="1:10" ht="63.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="85"/>
       <c r="B31" s="50" t="s">
         <v>166</v>
       </c>
       <c r="C31" s="48"/>
-      <c r="D31" s="83"/>
+      <c r="D31" s="84"/>
       <c r="E31" s="48" t="s">
         <v>166</v>
       </c>
       <c r="F31" s="48"/>
-      <c r="G31" s="83"/>
+      <c r="G31" s="84"/>
       <c r="H31" s="48" t="s">
         <v>166</v>
       </c>
       <c r="I31" s="48"/>
-      <c r="J31" s="84"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" s="84"/>
+      <c r="J31" s="85"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A32" s="85"/>
       <c r="B32" s="52"/>
       <c r="C32" s="49"/>
       <c r="D32" s="49"/>
@@ -5843,100 +5944,100 @@
       <c r="G32" s="49"/>
       <c r="H32" s="49"/>
       <c r="I32" s="49"/>
-      <c r="J32" s="84"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="84"/>
+      <c r="J32" s="85"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A33" s="85"/>
       <c r="B33" s="50" t="s">
         <v>162</v>
       </c>
       <c r="C33" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="D33" s="81"/>
+      <c r="D33" s="82"/>
       <c r="E33" s="48" t="s">
         <v>162</v>
       </c>
       <c r="F33" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="G33" s="81"/>
+      <c r="G33" s="82"/>
       <c r="H33" s="48" t="s">
         <v>162</v>
       </c>
       <c r="I33" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="J33" s="84"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="84"/>
+      <c r="J33" s="85"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A34" s="85"/>
       <c r="B34" s="50" t="s">
         <v>164</v>
       </c>
       <c r="C34" s="48" t="s">
         <v>189</v>
       </c>
-      <c r="D34" s="82"/>
+      <c r="D34" s="83"/>
       <c r="E34" s="48" t="s">
         <v>164</v>
       </c>
       <c r="F34" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="G34" s="82"/>
+      <c r="G34" s="83"/>
       <c r="H34" s="48" t="s">
         <v>164</v>
       </c>
       <c r="I34" s="48" t="s">
         <v>176</v>
       </c>
-      <c r="J34" s="84"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" s="84"/>
+      <c r="J34" s="85"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A35" s="85"/>
       <c r="B35" s="50" t="s">
         <v>165</v>
       </c>
       <c r="C35" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="D35" s="82"/>
+      <c r="D35" s="83"/>
       <c r="E35" s="48" t="s">
         <v>165</v>
       </c>
       <c r="F35" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="G35" s="82"/>
+      <c r="G35" s="83"/>
       <c r="H35" s="48" t="s">
         <v>165</v>
       </c>
       <c r="I35" s="21" t="s">
         <v>261</v>
       </c>
-      <c r="J35" s="84"/>
-    </row>
-    <row r="36" spans="1:10" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="84"/>
+      <c r="J35" s="85"/>
+    </row>
+    <row r="36" spans="1:10" ht="80.55" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="85"/>
       <c r="B36" s="50" t="s">
         <v>166</v>
       </c>
       <c r="C36" s="48"/>
-      <c r="D36" s="83"/>
+      <c r="D36" s="84"/>
       <c r="E36" s="48" t="s">
         <v>166</v>
       </c>
       <c r="F36" s="48"/>
-      <c r="G36" s="83"/>
+      <c r="G36" s="84"/>
       <c r="H36" s="48" t="s">
         <v>166</v>
       </c>
       <c r="I36" s="48"/>
-      <c r="J36" s="84"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A37" s="84"/>
+      <c r="J36" s="85"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A37" s="85"/>
       <c r="B37" s="52"/>
       <c r="C37" s="49"/>
       <c r="D37" s="54"/>
@@ -5945,100 +6046,100 @@
       <c r="G37" s="49"/>
       <c r="H37" s="49"/>
       <c r="I37" s="49"/>
-      <c r="J37" s="84"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="84"/>
+      <c r="J37" s="85"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A38" s="85"/>
       <c r="B38" s="50" t="s">
         <v>162</v>
       </c>
       <c r="C38" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="D38" s="81"/>
+      <c r="D38" s="82"/>
       <c r="E38" s="48" t="s">
         <v>162</v>
       </c>
       <c r="F38" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="G38" s="81"/>
+      <c r="G38" s="82"/>
       <c r="H38" s="48" t="s">
         <v>162</v>
       </c>
       <c r="I38" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="J38" s="84"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" s="84"/>
+      <c r="J38" s="85"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A39" s="85"/>
       <c r="B39" s="50" t="s">
         <v>164</v>
       </c>
       <c r="C39" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="D39" s="82"/>
+      <c r="D39" s="83"/>
       <c r="E39" s="48" t="s">
         <v>164</v>
       </c>
       <c r="F39" s="48" t="s">
         <v>201</v>
       </c>
-      <c r="G39" s="82"/>
+      <c r="G39" s="83"/>
       <c r="H39" s="48" t="s">
         <v>164</v>
       </c>
       <c r="I39" s="48" t="s">
         <v>198</v>
       </c>
-      <c r="J39" s="84"/>
-    </row>
-    <row r="40" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="84"/>
+      <c r="J39" s="85"/>
+    </row>
+    <row r="40" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="85"/>
       <c r="B40" s="50" t="s">
         <v>165</v>
       </c>
       <c r="C40" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="D40" s="82"/>
+      <c r="D40" s="83"/>
       <c r="E40" s="48" t="s">
         <v>165</v>
       </c>
       <c r="F40" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="G40" s="82"/>
+      <c r="G40" s="83"/>
       <c r="H40" s="48" t="s">
         <v>165</v>
       </c>
       <c r="I40" s="21" t="s">
         <v>263</v>
       </c>
-      <c r="J40" s="84"/>
-    </row>
-    <row r="41" spans="1:10" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="84"/>
+      <c r="J40" s="85"/>
+    </row>
+    <row r="41" spans="1:10" ht="65.55" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="85"/>
       <c r="B41" s="50" t="s">
         <v>166</v>
       </c>
       <c r="C41" s="48"/>
-      <c r="D41" s="83"/>
+      <c r="D41" s="84"/>
       <c r="E41" s="48" t="s">
         <v>166</v>
       </c>
       <c r="F41" s="48"/>
-      <c r="G41" s="83"/>
+      <c r="G41" s="84"/>
       <c r="H41" s="48" t="s">
         <v>166</v>
       </c>
       <c r="I41" s="48"/>
-      <c r="J41" s="84"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A42" s="84"/>
+      <c r="J41" s="85"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A42" s="85"/>
       <c r="B42" s="52"/>
       <c r="C42" s="49"/>
       <c r="D42" s="49"/>
@@ -6047,100 +6148,100 @@
       <c r="G42" s="49"/>
       <c r="H42" s="49"/>
       <c r="I42" s="49"/>
-      <c r="J42" s="84"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A43" s="84"/>
+      <c r="J42" s="85"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A43" s="85"/>
       <c r="B43" s="50" t="s">
         <v>162</v>
       </c>
       <c r="C43" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="D43" s="81"/>
+      <c r="D43" s="82"/>
       <c r="E43" s="50" t="s">
         <v>162</v>
       </c>
       <c r="F43" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="G43" s="81"/>
+      <c r="G43" s="82"/>
       <c r="H43" s="50" t="s">
         <v>162</v>
       </c>
       <c r="I43" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="J43" s="84"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A44" s="84"/>
+      <c r="J43" s="85"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A44" s="85"/>
       <c r="B44" s="50" t="s">
         <v>164</v>
       </c>
       <c r="C44" s="48" t="s">
         <v>192</v>
       </c>
-      <c r="D44" s="82"/>
+      <c r="D44" s="83"/>
       <c r="E44" s="50" t="s">
         <v>164</v>
       </c>
       <c r="F44" s="48" t="s">
         <v>202</v>
       </c>
-      <c r="G44" s="82"/>
+      <c r="G44" s="83"/>
       <c r="H44" s="50" t="s">
         <v>164</v>
       </c>
       <c r="I44" s="48" t="s">
         <v>193</v>
       </c>
-      <c r="J44" s="84"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A45" s="84"/>
+      <c r="J44" s="85"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A45" s="85"/>
       <c r="B45" s="50" t="s">
         <v>165</v>
       </c>
       <c r="C45" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="D45" s="82"/>
+      <c r="D45" s="83"/>
       <c r="E45" s="50" t="s">
         <v>165</v>
       </c>
       <c r="F45" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="G45" s="82"/>
+      <c r="G45" s="83"/>
       <c r="H45" s="50" t="s">
         <v>165</v>
       </c>
       <c r="I45" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="J45" s="84"/>
-    </row>
-    <row r="46" spans="1:10" ht="88" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="84"/>
+      <c r="J45" s="85"/>
+    </row>
+    <row r="46" spans="1:10" ht="88.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="85"/>
       <c r="B46" s="50" t="s">
         <v>166</v>
       </c>
       <c r="C46" s="48"/>
-      <c r="D46" s="83"/>
+      <c r="D46" s="84"/>
       <c r="E46" s="50" t="s">
         <v>166</v>
       </c>
       <c r="F46" s="48"/>
-      <c r="G46" s="83"/>
+      <c r="G46" s="84"/>
       <c r="H46" s="50" t="s">
         <v>166</v>
       </c>
       <c r="I46" s="48"/>
-      <c r="J46" s="84"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A47" s="84"/>
+      <c r="J46" s="85"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A47" s="85"/>
       <c r="B47" s="52"/>
       <c r="C47" s="49"/>
       <c r="D47" s="49"/>
@@ -6149,17 +6250,10 @@
       <c r="G47" s="49"/>
       <c r="H47" s="52"/>
       <c r="I47" s="49"/>
-      <c r="J47" s="84"/>
+      <c r="J47" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="D33:D36"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="D18:D21"/>
     <mergeCell ref="D43:D46"/>
     <mergeCell ref="A1:A47"/>
     <mergeCell ref="J1:J47"/>
@@ -6176,6 +6270,13 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="D33:D36"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="D18:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>